<commit_message>
added AMC & GME
</commit_message>
<xml_diff>
--- a/Biopharma.xlsx
+++ b/Biopharma.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Desktop\CODE\models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235FAAE9-6186-487B-83D2-315A7E372D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA0B0D3-E133-4C11-BAE5-652A1E23B969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8100" yWindow="510" windowWidth="20310" windowHeight="14910" xr2:uid="{17641224-F2C3-441B-B85B-BB32567FE633}"/>
+    <workbookView xWindow="7770" yWindow="390" windowWidth="20745" windowHeight="14490" xr2:uid="{17641224-F2C3-441B-B85B-BB32567FE633}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -43,6 +43,7 @@
     <externalReference r:id="rId26"/>
     <externalReference r:id="rId27"/>
     <externalReference r:id="rId28"/>
+    <externalReference r:id="rId29"/>
   </externalReferences>
   <definedNames>
     <definedName name="AUD">FX!$C$5</definedName>
@@ -72,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="292">
   <si>
     <t>Exarta</t>
   </si>
@@ -1987,6 +1988,81 @@
           </cell>
         </row>
       </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink26.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Master Pipeline"/>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+      <sheetName val="Stribild"/>
+      <sheetName val="Truvada"/>
+      <sheetName val="Viread"/>
+      <sheetName val="Ranexa"/>
+      <sheetName val="Atripla"/>
+      <sheetName val="IMS Monthly"/>
+      <sheetName val="IMS"/>
+      <sheetName val="Rx"/>
+      <sheetName val="HBV"/>
+      <sheetName val="darusentan"/>
+      <sheetName val="Letairis"/>
+      <sheetName val="Hepsera"/>
+      <sheetName val="HIV"/>
+      <sheetName val="GS 9137"/>
+      <sheetName val="GS 9132"/>
+      <sheetName val="GS9190"/>
+      <sheetName val="sofosbuvir"/>
+      <sheetName val="idelasilib"/>
+      <sheetName val="GS 9451"/>
+      <sheetName val="Cayston"/>
+      <sheetName val="Tamiflu"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1">
+        <row r="3">
+          <cell r="J3">
+            <v>1262</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="J5">
+            <v>6752</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="J6">
+            <v>26208</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2781,10 +2857,10 @@
   <dimension ref="B2:T141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D52" sqref="D52"/>
+      <selection pane="bottomRight" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3176,7 +3252,7 @@
         <v>-25217</v>
       </c>
       <c r="G15" s="6">
-        <f t="shared" ref="G15:G18" si="1">E15-F15</f>
+        <f t="shared" ref="G15:G19" si="1">E15-F15</f>
         <v>128243</v>
       </c>
       <c r="H15" s="3" t="s">
@@ -3237,65 +3313,80 @@
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="7">
+        <v>60.9</v>
+      </c>
+      <c r="E18" s="6">
+        <f>+D18*[26]Main!$J$3</f>
+        <v>76855.8</v>
+      </c>
+      <c r="F18" s="6">
+        <f>+[26]Main!$J$5-[26]Main!$J$6</f>
+        <v>-19456</v>
+      </c>
+      <c r="G18" s="6">
+        <f>E18-F18</f>
+        <v>96311.8</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B19" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D19" s="7">
         <v>175.1</v>
       </c>
-      <c r="E18" s="6">
-        <f>D18*[14]Main!$J$3*EUR</f>
+      <c r="E19" s="6">
+        <f>D19*[14]Main!$J$3*EUR</f>
         <v>77446.648629173942</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F19" s="6">
         <f>([14]Main!$J$5-[14]Main!$J$6)*EUR</f>
         <v>-9387.644400000001</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G19" s="6">
         <f t="shared" si="1"/>
         <v>86834.293029173947</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H19" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B19" s="5" t="s">
+    <row r="20" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B20" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D20" s="3">
         <v>255.99</v>
       </c>
-      <c r="E19" s="6">
-        <f>D19*[15]Main!$J$3*AUD</f>
+      <c r="E20" s="6">
+        <f>D20*[15]Main!$J$3*AUD</f>
         <v>80031.808981488444</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F20" s="6">
         <f>[15]Main!$J$5-[15]Main!$J$6</f>
         <v>-3998.1000000000004</v>
       </c>
-      <c r="G19" s="6">
-        <f>E19-F19</f>
+      <c r="G20" s="6">
+        <f>E20-F20</f>
         <v>84029.90898148845</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H20" s="3" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B20" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" s="3">
-        <v>58.53</v>
       </c>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.2">
@@ -4908,14 +4999,14 @@
     <hyperlink ref="B11" r:id="rId6" xr:uid="{8513C491-1620-4390-AB90-9384BB1A043B}"/>
     <hyperlink ref="B15" r:id="rId7" xr:uid="{83DA0EB3-074A-48C7-ADA5-0A0973E8354D}"/>
     <hyperlink ref="B6" r:id="rId8" xr:uid="{615921E7-8A8A-4F41-A8F3-1AF78A43F1AC}"/>
-    <hyperlink ref="B18" r:id="rId9" xr:uid="{A38EC1E4-9170-422B-A9F5-3B6EB77DF40A}"/>
+    <hyperlink ref="B19" r:id="rId9" xr:uid="{A38EC1E4-9170-422B-A9F5-3B6EB77DF40A}"/>
     <hyperlink ref="B9" r:id="rId10" xr:uid="{CCC45DFB-BF73-4A15-8527-F4C3C617F472}"/>
-    <hyperlink ref="B19" r:id="rId11" xr:uid="{FC86E1B4-4BA7-43A8-8FCA-CC27867A7922}"/>
+    <hyperlink ref="B20" r:id="rId11" xr:uid="{FC86E1B4-4BA7-43A8-8FCA-CC27867A7922}"/>
     <hyperlink ref="B12" r:id="rId12" xr:uid="{F9D09B0D-FACB-4CCA-872E-286E56965815}"/>
     <hyperlink ref="B14" r:id="rId13" xr:uid="{5A59EF45-A9EA-44F3-BECB-EFED8413DCF6}"/>
     <hyperlink ref="B16" r:id="rId14" xr:uid="{316E9202-338F-4301-AEBE-A9FA398A76CC}"/>
     <hyperlink ref="B5" r:id="rId15" xr:uid="{0888F4DA-9569-4326-990C-43015A33BD61}"/>
-    <hyperlink ref="B20" r:id="rId16" xr:uid="{C2959A9B-7367-43D7-934F-562A915DC4DD}"/>
+    <hyperlink ref="B18" r:id="rId16" xr:uid="{C2959A9B-7367-43D7-934F-562A915DC4DD}"/>
     <hyperlink ref="B21" r:id="rId17" xr:uid="{A069369A-FB97-4A4A-A581-321FA79E4250}"/>
     <hyperlink ref="B22" r:id="rId18" xr:uid="{6EF35D30-7113-4CE8-9077-C5BE97F74D36}"/>
     <hyperlink ref="B23" r:id="rId19" xr:uid="{1F769FA7-6B90-4B6B-9BCC-7D6679675B06}"/>

</xml_diff>

<commit_message>
regn, trading updates, crypto updates
</commit_message>
<xml_diff>
--- a/Biopharma.xlsx
+++ b/Biopharma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D905AC5E-1996-43F9-A6A0-44168A70297D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B6CDA3-A590-45F9-B449-0FC739CCDEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26595" yWindow="1830" windowWidth="26250" windowHeight="17190" xr2:uid="{17641224-F2C3-441B-B85B-BB32567FE633}"/>
+    <workbookView xWindow="-46845" yWindow="2400" windowWidth="26445" windowHeight="16230" xr2:uid="{17641224-F2C3-441B-B85B-BB32567FE633}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -56,6 +56,7 @@
     <externalReference r:id="rId39"/>
     <externalReference r:id="rId40"/>
     <externalReference r:id="rId41"/>
+    <externalReference r:id="rId42"/>
   </externalReferences>
   <definedNames>
     <definedName name="AUD">FX!$C$5</definedName>
@@ -85,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="334">
   <si>
     <t>Exarta</t>
   </si>
@@ -2221,6 +2222,49 @@
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
+      <sheetName val="Consta"/>
+      <sheetName val="Vivitrol"/>
+      <sheetName val="Byetta LAR"/>
+      <sheetName val="Discontinued - ALKS27"/>
+      <sheetName val="Jansenn Contract"/>
+      <sheetName val="ALKS33"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="L3">
+            <v>164.25427500000001</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="L5">
+            <v>759.97699999999998</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="L6">
+            <v>294.53699999999998</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink25.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
@@ -2246,7 +2290,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink26.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2277,7 +2321,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink27.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2307,18 +2351,47 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink28.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="N3">
+            <v>9.4141049999999993</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="N5">
+            <v>11.249000000000001</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="N6">
+            <v>18.713000000000001</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink29.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2356,70 +2429,6 @@
       <sheetData sheetId="5"/>
       <sheetData sheetId="6"/>
       <sheetData sheetId="7"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink28.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Main"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="L3">
-            <v>40.004356999999999</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="L5">
-            <v>277.88299999999998</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="L6">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink29.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Main"/>
-      <sheetName val="Model"/>
-      <sheetName val="Yutrepia"/>
-      <sheetName val="Generic"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="J3">
-            <v>64.344476</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="J5">
-            <v>111.794</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="J6">
-            <v>19.475999999999999</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2536,17 +2545,17 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="M3">
-            <v>44.710678000000001</v>
+          <cell r="L3">
+            <v>40.004356999999999</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="M5">
-            <v>120.43700000000001</v>
+          <cell r="L5">
+            <v>277.88299999999998</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="M6">
+          <cell r="L6">
             <v>0</v>
           </cell>
         </row>
@@ -2561,25 +2570,31 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
+      <sheetName val="Model"/>
+      <sheetName val="Yutrepia"/>
+      <sheetName val="Generic"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="M3">
-            <v>184.19892899999999</v>
+          <cell r="J3">
+            <v>64.344476</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="M5">
-            <v>67.233999999999995</v>
+          <cell r="J5">
+            <v>111.794</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="M6">
-            <v>126.736</v>
+          <cell r="J6">
+            <v>19.475999999999999</v>
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2594,18 +2609,18 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="N3">
-            <v>20.079526999999999</v>
+          <cell r="M3">
+            <v>44.710678000000001</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="N5">
-            <v>16.64</v>
+          <cell r="M5">
+            <v>120.43700000000001</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="N6">
-            <v>0.69799999999999995</v>
+          <cell r="M6">
+            <v>0</v>
           </cell>
         </row>
       </sheetData>
@@ -2623,18 +2638,18 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="L3">
-            <v>48.69059</v>
+          <cell r="M3">
+            <v>184.19892899999999</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="L5">
-            <v>18.687999999999999</v>
+          <cell r="M5">
+            <v>67.233999999999995</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="L6">
-            <v>5.4249999999999998</v>
+          <cell r="M6">
+            <v>126.736</v>
           </cell>
         </row>
       </sheetData>
@@ -2652,18 +2667,18 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="M3">
-            <v>20.500177000000001</v>
+          <cell r="N3">
+            <v>20.079526999999999</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="M5">
-            <v>131.17699999999999</v>
+          <cell r="N5">
+            <v>16.64</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="M6">
-            <v>0</v>
+          <cell r="N6">
+            <v>0.69799999999999995</v>
           </cell>
         </row>
       </sheetData>
@@ -2681,18 +2696,18 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="M3">
-            <v>21.362773000000001</v>
+          <cell r="L3">
+            <v>48.69059</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="M5">
-            <v>55.28</v>
+          <cell r="L5">
+            <v>18.687999999999999</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="M6">
-            <v>0</v>
+          <cell r="L6">
+            <v>5.4249999999999998</v>
           </cell>
         </row>
       </sheetData>
@@ -2706,39 +2721,25 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
-      <sheetName val="Model"/>
-      <sheetName val="Consta"/>
-      <sheetName val="Vivitrol"/>
-      <sheetName val="Byetta LAR"/>
-      <sheetName val="Discontinued - ALKS27"/>
-      <sheetName val="Jansenn Contract"/>
-      <sheetName val="ALKS33"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="L3">
-            <v>164.25427500000001</v>
+          <cell r="M3">
+            <v>20.500177000000001</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="L5">
-            <v>759.97699999999998</v>
+          <cell r="M5">
+            <v>131.17699999999999</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="L6">
-            <v>294.53699999999998</v>
+          <cell r="M6">
+            <v>0</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2753,21 +2754,66 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="N3">
-            <v>9.4141049999999993</v>
+          <cell r="M3">
+            <v>21.362773000000001</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="N5">
-            <v>11.249000000000001</v>
+          <cell r="M5">
+            <v>55.28</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="N6">
-            <v>18.713000000000001</v>
+          <cell r="M6">
+            <v>0</v>
           </cell>
         </row>
       </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink38.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+      <sheetName val="Dupixent"/>
+      <sheetName val="Eylea"/>
+      <sheetName val="Arcalyst"/>
+      <sheetName val="Zaltrap"/>
+      <sheetName val="VEGF Trap"/>
+      <sheetName val="REGN727"/>
+      <sheetName val="REGN88"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="K3">
+            <v>109.51814600000002</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="K5">
+            <v>13982.3</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="K6">
+            <v>1980.7</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3519,10 +3565,10 @@
   <dimension ref="B2:AB151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C109" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C140" sqref="C140"/>
+      <selection pane="bottomRight" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4303,39 +4349,61 @@
     </row>
     <row r="23" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="7">
+        <v>630</v>
+      </c>
+      <c r="E23" s="6">
+        <f>+[38]Main!$K$3</f>
+        <v>109.51814600000002</v>
+      </c>
+      <c r="F23" s="6">
+        <f>+D23*E23</f>
+        <v>68996.431980000008</v>
+      </c>
+      <c r="G23" s="6">
+        <f>+[38]Main!$K$5-[38]Main!$K$6</f>
+        <v>12001.599999999999</v>
+      </c>
+      <c r="H23" s="6">
+        <f>F23-G23</f>
+        <v>56994.83198000001</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="J23" s="18">
+        <v>44782</v>
+      </c>
+    </row>
+    <row r="24" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B24" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D24" s="3">
         <v>10.46</v>
       </c>
-      <c r="F23" s="6">
-        <f>D23*[18]Main!$M$3</f>
+      <c r="F24" s="6">
+        <f>D24*[18]Main!$M$3</f>
         <v>12680.93945768</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G24" s="6">
         <f>[18]Main!$M$5-[18]Main!$M$6</f>
         <v>-18665.5</v>
       </c>
-      <c r="H23" s="6">
-        <f>F23-G23</f>
+      <c r="H24" s="6">
+        <f>F24-G24</f>
         <v>31346.43945768</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="I24" s="3" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B24" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="3">
-        <v>580.95000000000005</v>
       </c>
     </row>
     <row r="25" spans="2:27" x14ac:dyDescent="0.2">
@@ -4792,7 +4860,7 @@
         <v>28.03</v>
       </c>
       <c r="E52" s="6">
-        <f>+[36]Main!$L$3</f>
+        <f>+[24]Main!$L$3</f>
         <v>164.25427500000001</v>
       </c>
       <c r="F52" s="6">
@@ -4800,7 +4868,7 @@
         <v>4604.0473282500006</v>
       </c>
       <c r="G52" s="6">
-        <f>+[36]Main!$L$5-[36]Main!$L$6</f>
+        <f>+[24]Main!$L$5-[24]Main!$L$6</f>
         <v>465.44</v>
       </c>
       <c r="H52" s="6">
@@ -5351,11 +5419,11 @@
         <v>10.119999999999999</v>
       </c>
       <c r="F94" s="6">
-        <f>+D94*[24]Main!$N$3</f>
+        <f>+D94*[25]Main!$N$3</f>
         <v>3152.1980120399994</v>
       </c>
       <c r="G94" s="6">
-        <f>+[24]Main!$N$5-[24]Main!$N$6</f>
+        <f>+[25]Main!$N$5-[25]Main!$N$6</f>
         <v>869.93499999999995</v>
       </c>
       <c r="H94" s="6">
@@ -5736,11 +5804,11 @@
         <v>15.65</v>
       </c>
       <c r="F126" s="6">
-        <f>D126*[25]Main!$L$3</f>
+        <f>D126*[26]Main!$L$3</f>
         <v>1253.1559559500001</v>
       </c>
       <c r="G126" s="6">
-        <f>+[25]Main!$L$5-[25]Main!$L$6</f>
+        <f>+[26]Main!$L$5-[26]Main!$L$6</f>
         <v>112.015</v>
       </c>
       <c r="H126" s="6">
@@ -5762,11 +5830,11 @@
         <v>16.93</v>
       </c>
       <c r="F127" s="6">
-        <f>+D127*[26]Main!$L$3</f>
+        <f>+D127*[27]Main!$L$3</f>
         <v>1228.5485933099999</v>
       </c>
       <c r="G127" s="6">
-        <f>+[26]Main!$L$5-[26]Main!$L$6</f>
+        <f>+[27]Main!$L$5-[27]Main!$L$6</f>
         <v>153.25991400000001</v>
       </c>
       <c r="H127" s="6">
@@ -5937,7 +6005,7 @@
         <v>3.95</v>
       </c>
       <c r="E137" s="6">
-        <f>+[37]Main!$N$3</f>
+        <f>+[28]Main!$N$3</f>
         <v>9.4141049999999993</v>
       </c>
       <c r="F137" s="6">
@@ -5945,7 +6013,7 @@
         <v>37.185714749999995</v>
       </c>
       <c r="G137" s="6">
-        <f>+[37]Main!$N$5-[37]Main!$N$6</f>
+        <f>+[28]Main!$N$5-[28]Main!$N$6</f>
         <v>-7.4640000000000004</v>
       </c>
       <c r="H137" s="6">
@@ -6015,11 +6083,11 @@
         <v>7.06</v>
       </c>
       <c r="F141" s="6">
-        <f>D141*[27]Main!$J$3</f>
+        <f>D141*[29]Main!$J$3</f>
         <v>725.62786605999997</v>
       </c>
       <c r="G141" s="6">
-        <f>[27]Main!$J$5-[27]Main!$J$6</f>
+        <f>[29]Main!$J$5-[29]Main!$J$6</f>
         <v>197.79600000000002</v>
       </c>
       <c r="H141" s="8">
@@ -6041,11 +6109,11 @@
         <v>14.68</v>
       </c>
       <c r="F142" s="6">
-        <f>D142*[28]Main!$L$3</f>
+        <f>D142*[30]Main!$L$3</f>
         <v>587.26396075999992</v>
       </c>
       <c r="G142" s="6">
-        <f>[28]Main!$L$5-[28]Main!$L$6</f>
+        <f>[30]Main!$L$5-[30]Main!$L$6</f>
         <v>277.88299999999998</v>
       </c>
       <c r="H142" s="8">
@@ -6067,11 +6135,11 @@
         <v>4.8600000000000003</v>
       </c>
       <c r="F143" s="6">
-        <f>D143*[29]Main!$J$3</f>
+        <f>D143*[31]Main!$J$3</f>
         <v>312.71415336000001</v>
       </c>
       <c r="G143" s="8">
-        <f>+[29]Main!$J$5-[29]Main!$J$6</f>
+        <f>+[31]Main!$J$5-[31]Main!$J$6</f>
         <v>92.317999999999998</v>
       </c>
       <c r="H143" s="8">
@@ -6093,11 +6161,11 @@
         <v>7.57</v>
       </c>
       <c r="F144" s="6">
-        <f>D144*[30]Main!$M$3</f>
+        <f>D144*[32]Main!$M$3</f>
         <v>338.45983246000003</v>
       </c>
       <c r="G144" s="6">
-        <f>[30]Main!$M$5-[30]Main!$M$6</f>
+        <f>[32]Main!$M$5-[32]Main!$M$6</f>
         <v>120.43700000000001</v>
       </c>
       <c r="H144" s="8">
@@ -6119,11 +6187,11 @@
         <v>0.7</v>
       </c>
       <c r="F145" s="6">
-        <f>D145*[31]Main!$M$3</f>
+        <f>D145*[33]Main!$M$3</f>
         <v>128.9392503</v>
       </c>
       <c r="G145" s="6">
-        <f>[31]Main!$M$5-[31]Main!$M$6</f>
+        <f>[33]Main!$M$5-[33]Main!$M$6</f>
         <v>-59.50200000000001</v>
       </c>
       <c r="H145" s="8">
@@ -6145,11 +6213,11 @@
         <v>1.98</v>
       </c>
       <c r="F146" s="6">
-        <f>D146*[32]Main!$N$3</f>
+        <f>D146*[34]Main!$N$3</f>
         <v>39.757463459999997</v>
       </c>
       <c r="G146" s="6">
-        <f>[32]Main!$N$5-[32]Main!$N$6</f>
+        <f>[34]Main!$N$5-[34]Main!$N$6</f>
         <v>15.942</v>
       </c>
       <c r="H146" s="8">
@@ -6171,11 +6239,11 @@
         <v>0.62</v>
       </c>
       <c r="F147" s="6">
-        <f>D147*[33]Main!$L$3</f>
+        <f>D147*[35]Main!$L$3</f>
         <v>30.1881658</v>
       </c>
       <c r="G147" s="6">
-        <f>[33]Main!$L$5-[33]Main!$L$6</f>
+        <f>[35]Main!$L$5-[35]Main!$L$6</f>
         <v>13.262999999999998</v>
       </c>
       <c r="H147" s="8">
@@ -6197,11 +6265,11 @@
         <v>6.12</v>
       </c>
       <c r="F148" s="6">
-        <f>D148*[34]Main!$M$3</f>
+        <f>D148*[36]Main!$M$3</f>
         <v>125.46108324000001</v>
       </c>
       <c r="G148" s="6">
-        <f>[34]Main!$M$5-[34]Main!$M$6</f>
+        <f>[36]Main!$M$5-[36]Main!$M$6</f>
         <v>131.17699999999999</v>
       </c>
       <c r="H148" s="8">
@@ -6223,11 +6291,11 @@
         <v>0.98</v>
       </c>
       <c r="F149" s="6">
-        <f>D149*[35]Main!$M$3</f>
+        <f>D149*[37]Main!$M$3</f>
         <v>20.935517539999999</v>
       </c>
       <c r="G149" s="6">
-        <f>[35]Main!$M$5-[35]Main!$M$6</f>
+        <f>[37]Main!$M$5-[37]Main!$M$6</f>
         <v>55.28</v>
       </c>
       <c r="H149" s="8">
@@ -6284,7 +6352,7 @@
     <hyperlink ref="B19" r:id="rId16" xr:uid="{C2959A9B-7367-43D7-934F-562A915DC4DD}"/>
     <hyperlink ref="B22" r:id="rId17" xr:uid="{A069369A-FB97-4A4A-A581-321FA79E4250}"/>
     <hyperlink ref="B35" r:id="rId18" xr:uid="{6EF35D30-7113-4CE8-9077-C5BE97F74D36}"/>
-    <hyperlink ref="B24" r:id="rId19" xr:uid="{1F769FA7-6B90-4B6B-9BCC-7D6679675B06}"/>
+    <hyperlink ref="B23" r:id="rId19" xr:uid="{1F769FA7-6B90-4B6B-9BCC-7D6679675B06}"/>
     <hyperlink ref="B25" r:id="rId20" xr:uid="{6108C865-F45B-4849-97C5-0C40AD61A72B}"/>
     <hyperlink ref="B26" r:id="rId21" xr:uid="{FBD4E7AC-5982-43A1-83EA-3F3AB2E91655}"/>
     <hyperlink ref="B27" r:id="rId22" xr:uid="{53091BB6-5763-4DDE-A659-5638BD3CADCA}"/>
@@ -6303,7 +6371,7 @@
     <hyperlink ref="B49" r:id="rId35" xr:uid="{A1C90F9B-FBBF-4C72-9A11-3798F692A0D2}"/>
     <hyperlink ref="B50" r:id="rId36" xr:uid="{F7B6503D-1F84-47C4-B87E-BDA7159D1B9F}"/>
     <hyperlink ref="B44" r:id="rId37" xr:uid="{D0EE43E7-C3F5-4256-99AE-DDCA9EC11DCF}"/>
-    <hyperlink ref="B23" r:id="rId38" xr:uid="{1C25970A-A568-4869-A34A-5C6C7551D812}"/>
+    <hyperlink ref="B24" r:id="rId38" xr:uid="{1C25970A-A568-4869-A34A-5C6C7551D812}"/>
     <hyperlink ref="B126" r:id="rId39" xr:uid="{C3A06396-38CD-486E-9F4F-233A79292B4F}"/>
     <hyperlink ref="B94" r:id="rId40" xr:uid="{B83625D8-44D2-4842-9139-F29C8D5F2D8E}"/>
     <hyperlink ref="B127" r:id="rId41" xr:uid="{5FF32E6A-C6C7-4793-8271-BD230B9C7641}"/>

</xml_diff>

<commit_message>
updated trading sheet and other models
</commit_message>
<xml_diff>
--- a/Biopharma.xlsx
+++ b/Biopharma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C79175-659D-4374-859E-0AC76C23A1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA86B51-E3CC-45A1-A4F6-0FAE09592FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53265" yWindow="1950" windowWidth="25395" windowHeight="18930" xr2:uid="{17641224-F2C3-441B-B85B-BB32567FE633}"/>
+    <workbookView xWindow="9300" yWindow="1200" windowWidth="24495" windowHeight="17940" xr2:uid="{17641224-F2C3-441B-B85B-BB32567FE633}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="359">
   <si>
     <t>Exarta</t>
   </si>
@@ -1133,6 +1133,36 @@
   </si>
   <si>
     <t>ACLX</t>
+  </si>
+  <si>
+    <t>SyntheticGestalt</t>
+  </si>
+  <si>
+    <t>11m</t>
+  </si>
+  <si>
+    <t>Neomorph</t>
+  </si>
+  <si>
+    <t>Moonlake Immunotherapeutics</t>
+  </si>
+  <si>
+    <t>IL-17 A/F mab</t>
+  </si>
+  <si>
+    <t>Iveric</t>
+  </si>
+  <si>
+    <t>ISEE</t>
+  </si>
+  <si>
+    <t>Ablynx</t>
+  </si>
+  <si>
+    <t>Centocor</t>
+  </si>
+  <si>
+    <t>Medarex</t>
   </si>
 </sst>
 </file>
@@ -1185,7 +1215,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1205,40 +1235,8 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1249,13 +1247,7 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1551,8 +1543,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="RX Rank"/>
-      <sheetName val="RX Alpha"/>
+      <sheetName val="Master"/>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
       <sheetName val="Lovenox"/>
@@ -1573,24 +1564,24 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
+      <sheetData sheetId="1">
         <row r="3">
-          <cell r="L3">
-            <v>1254.9000000000001</v>
+          <cell r="K3">
+            <v>1251</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="L5">
-            <v>10098</v>
+          <cell r="K5">
+            <v>0</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="L6">
-            <v>20306</v>
+          <cell r="K6">
+            <v>12190</v>
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
@@ -1606,7 +1597,6 @@
       <sheetData sheetId="15"/>
       <sheetData sheetId="16"/>
       <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1616,6 +1606,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
+      <sheetName val="Master"/>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
       <sheetName val="Crestor"/>
@@ -1639,43 +1630,44 @@
       <sheetName val="Failures"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0">
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1">
         <row r="3">
           <cell r="L3">
-            <v>1561</v>
+            <v>1560</v>
           </cell>
         </row>
         <row r="5">
           <cell r="L5">
-            <v>5823</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="6">
           <cell r="L6">
-            <v>31040</v>
+            <v>24689</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2999,9 +2991,9 @@
       <sheetName val="IP"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
       <sheetData sheetId="3">
         <row r="3">
           <cell r="L3">
@@ -3019,40 +3011,40 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
-      <sheetData sheetId="33" refreshError="1"/>
-      <sheetData sheetId="34" refreshError="1"/>
-      <sheetData sheetId="35" refreshError="1"/>
-      <sheetData sheetId="36" refreshError="1"/>
-      <sheetData sheetId="37" refreshError="1"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+      <sheetData sheetId="37"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3126,7 +3118,7 @@
       <sheetName val="Crixivan"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="3">
           <cell r="J3">
@@ -3144,27 +3136,27 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3177,24 +3169,25 @@
       <sheetName val="IMS Dollars"/>
       <sheetName val="Sandoz"/>
       <sheetName val="IMS Alpha"/>
+      <sheetName val="Master"/>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
-      <sheetName val="Diovan"/>
-      <sheetName val="Diovan Model"/>
+      <sheetName val="Cosentyx"/>
+      <sheetName val="Entresto"/>
+      <sheetName val="Lucentis"/>
+      <sheetName val="Gilenya"/>
+      <sheetName val="Exjade"/>
+      <sheetName val="Sandostatin"/>
       <sheetName val="Gleevec"/>
+      <sheetName val="Tekturna"/>
+      <sheetName val="Galvus"/>
+      <sheetName val="Tasigna"/>
+      <sheetName val="Xolair"/>
       <sheetName val="Zometa"/>
-      <sheetName val="Lucentis"/>
       <sheetName val="Femara"/>
-      <sheetName val="Sandostatin"/>
-      <sheetName val="Exjade"/>
-      <sheetName val="Tekturna"/>
-      <sheetName val="Lamisil"/>
+      <sheetName val="indacaterol"/>
       <sheetName val="Focalin"/>
       <sheetName val="Aclasta"/>
-      <sheetName val="indacaterol"/>
-      <sheetName val="Galvus"/>
-      <sheetName val="Tasigna"/>
-      <sheetName val="FTY720"/>
       <sheetName val="Exforge"/>
       <sheetName val="Lotrel"/>
       <sheetName val="Afinitor"/>
@@ -3202,30 +3195,30 @@
       <sheetName val="Consumer"/>
       <sheetName val="Vaccines"/>
       <sheetName val="Menveo"/>
-      <sheetName val="Xolair"/>
+      <sheetName val="Diovan"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
-      <sheetData sheetId="3">
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4">
         <row r="3">
-          <cell r="L3">
-            <v>2212.5849010000002</v>
+          <cell r="K3">
+            <v>2182.7885879999999</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="L5">
+          <cell r="K5">
             <v>0</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="L6">
-            <v>10678</v>
+          <cell r="K6">
+            <v>9519</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
       <sheetData sheetId="6"/>
       <sheetData sheetId="7"/>
@@ -3250,6 +3243,7 @@
       <sheetData sheetId="26"/>
       <sheetData sheetId="27"/>
       <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3259,7 +3253,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Master Pipeline"/>
+      <sheetName val="Master"/>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
       <sheetName val="Opdivo"/>
@@ -3282,43 +3276,43 @@
       <sheetName val="brivanib"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="3">
-          <cell r="L3">
-            <v>2129.0642710000002</v>
+          <cell r="K3">
+            <v>2135.2551579999999</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="L5">
-            <v>14968</v>
+          <cell r="K5">
+            <v>13228</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="L6">
-            <v>44972</v>
+          <cell r="K6">
+            <v>42060</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3621,13 +3615,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3750AF13-821E-4BF9-92BC-DEDDF3C9498E}">
-  <dimension ref="A2:AB154"/>
+  <dimension ref="A2:AB155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomRight" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3646,22 +3640,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="P2" s="28" t="s">
+      <c r="P2" s="14" t="s">
         <v>322</v>
       </c>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
-      <c r="U2" s="28"/>
-      <c r="V2" s="28" t="s">
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14" t="s">
         <v>321</v>
       </c>
-      <c r="W2" s="28"/>
-      <c r="X2" s="28"/>
-      <c r="Y2" s="28"/>
-      <c r="Z2" s="28"/>
-      <c r="AA2" s="28"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14"/>
+      <c r="AA2" s="14"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
@@ -3756,7 +3750,7 @@
       <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="7">
         <v>169.99</v>
       </c>
       <c r="E4" s="6">
@@ -3778,14 +3772,14 @@
       <c r="I4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="18">
+      <c r="J4" s="9">
         <v>44804</v>
       </c>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -3797,7 +3791,7 @@
       <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="7">
         <v>138.28</v>
       </c>
       <c r="E5" s="6">
@@ -3819,14 +3813,14 @@
       <c r="I5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="18">
+      <c r="J5" s="9">
         <v>44771</v>
       </c>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -3860,74 +3854,74 @@
       <c r="I6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J6" s="9">
         <v>44774</v>
       </c>
       <c r="K6" s="7">
         <f>+[3]Model!$DM$84</f>
         <v>193.79899328583781</v>
       </c>
-      <c r="L6" s="22">
+      <c r="L6" s="10">
         <f>K6/D6-1</f>
         <v>-0.33379514167810986</v>
       </c>
-      <c r="M6" s="22">
+      <c r="M6" s="10">
         <f>[3]Model!$DM$80</f>
         <v>0.01</v>
       </c>
-      <c r="N6" s="22">
+      <c r="N6" s="10">
         <f>[3]Model!$DM$81</f>
         <v>-0.01</v>
       </c>
-      <c r="O6" s="22">
+      <c r="O6" s="10">
         <f>[3]Model!$DM$82</f>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="P6" s="24">
+      <c r="P6" s="12">
         <f t="shared" ref="P6:U6" si="1">($G$6/$H$6)/V6</f>
         <v>34.06702797542119</v>
       </c>
-      <c r="Q6" s="24">
+      <c r="Q6" s="12">
         <f t="shared" si="1"/>
         <v>34.35232826787027</v>
       </c>
-      <c r="R6" s="24">
+      <c r="R6" s="12">
         <f t="shared" si="1"/>
         <v>17.483163429324609</v>
       </c>
-      <c r="S6" s="24">
+      <c r="S6" s="12">
         <f t="shared" si="1"/>
         <v>15.227617414114208</v>
       </c>
-      <c r="T6" s="24">
+      <c r="T6" s="12">
         <f t="shared" si="1"/>
         <v>12.992954223035117</v>
       </c>
-      <c r="U6" s="24">
+      <c r="U6" s="12">
         <f t="shared" si="1"/>
         <v>12.568938996312276</v>
       </c>
-      <c r="V6" s="23">
+      <c r="V6" s="11">
         <f>+[3]Model!DC67</f>
         <v>8.8854650460225582</v>
       </c>
-      <c r="W6" s="23">
+      <c r="W6" s="11">
         <f>+[3]Model!DD67</f>
         <v>8.8116701708569245</v>
       </c>
-      <c r="X6" s="23">
+      <c r="X6" s="11">
         <f>+[3]Model!DE67</f>
         <v>17.313879580268342</v>
       </c>
-      <c r="Y6" s="23">
+      <c r="Y6" s="11">
         <f>+[3]Model!DF67</f>
         <v>19.878447039056095</v>
       </c>
-      <c r="Z6" s="23">
+      <c r="Z6" s="11">
         <f>+[3]Model!DG67</f>
         <v>23.297348786222955</v>
       </c>
-      <c r="AA6" s="23">
+      <c r="AA6" s="11">
         <f>+[3]Model!DH67</f>
         <v>24.083288683817315</v>
       </c>
@@ -3945,7 +3939,7 @@
       <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="7">
         <v>303.35000000000002</v>
       </c>
       <c r="E7" s="6">
@@ -3967,14 +3961,14 @@
       <c r="I7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="18">
+      <c r="J7" s="9">
         <v>44772</v>
       </c>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
       <c r="AB7" s="1">
         <v>1896</v>
       </c>
@@ -4011,17 +4005,17 @@
       <c r="I8" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="9">
         <v>44770</v>
       </c>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="A9" t="s">
         <v>345</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -4052,18 +4046,18 @@
       <c r="I9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="9">
         <v>44776</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
+      <c r="A10" t="s">
         <v>345</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" t="s">
         <v>328</v>
       </c>
       <c r="D10" s="7">
@@ -4088,24 +4082,12 @@
       <c r="I10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="18">
+      <c r="J10" s="9">
         <v>44776</v>
       </c>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="21"/>
-      <c r="S10" s="21"/>
-      <c r="T10" s="21"/>
-      <c r="U10" s="21"/>
-      <c r="V10" s="21"/>
-      <c r="W10" s="21"/>
-      <c r="X10" s="21"/>
-      <c r="Y10" s="21"/>
-      <c r="Z10" s="21"/>
-      <c r="AA10" s="21"/>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+      <c r="A11" t="s">
         <v>345</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -4136,12 +4118,12 @@
       <c r="I11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J11" s="18">
+      <c r="J11" s="9">
         <v>44778</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
+      <c r="A12" t="s">
         <v>345</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -4154,23 +4136,30 @@
         <v>81.06</v>
       </c>
       <c r="E12" s="6">
-        <f>D12*[8]Main!$L$3</f>
-        <v>179352.13207506001</v>
+        <f>+D12*H12</f>
+        <v>176936.84294328</v>
       </c>
       <c r="F12" s="6">
-        <f>[8]Main!$L$5-[8]Main!$L$6</f>
-        <v>-10678</v>
+        <f>+[8]Main!$K$5-[8]Main!$K$6</f>
+        <v>-9519</v>
       </c>
       <c r="G12" s="6">
         <f>E12-F12</f>
-        <v>190030.13207506001</v>
+        <v>186455.84294328</v>
+      </c>
+      <c r="H12" s="6">
+        <f>+[8]Main!$K$3</f>
+        <v>2182.7885879999999</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>16</v>
+        <v>311</v>
+      </c>
+      <c r="J12" s="9">
+        <v>44808</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
+      <c r="A13" t="s">
         <v>345</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -4183,23 +4172,30 @@
         <v>73.77</v>
       </c>
       <c r="E13" s="6">
-        <f>D13*[9]Main!$L$3</f>
-        <v>157061.07127166999</v>
+        <f>+D13*H13</f>
+        <v>157517.77300565998</v>
       </c>
       <c r="F13" s="6">
-        <f>[9]Main!$L$5-[9]Main!$L$6</f>
-        <v>-30004</v>
+        <f>+[9]Main!$K$5-[9]Main!$K$6</f>
+        <v>-28832</v>
       </c>
       <c r="G13" s="6">
         <f>E13-F13</f>
-        <v>187065.07127166999</v>
+        <v>186349.77300565998</v>
+      </c>
+      <c r="H13" s="6">
+        <f>+[9]Main!$K$3</f>
+        <v>2135.2551579999999</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>16</v>
+        <v>311</v>
+      </c>
+      <c r="J13" s="9">
+        <v>44810</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
+      <c r="A14" t="s">
         <v>345</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -4208,11 +4204,11 @@
       <c r="C14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="7">
         <v>246.73</v>
       </c>
       <c r="E14" s="6">
-        <f>D14*[10]Main!$K$3</f>
+        <f>+D14*H14</f>
         <v>131753.82</v>
       </c>
       <c r="F14" s="6">
@@ -4223,12 +4219,19 @@
         <f t="shared" si="0"/>
         <v>162063.82</v>
       </c>
+      <c r="H14" s="6">
+        <f>+[10]Main!$K$3</f>
+        <v>534</v>
+      </c>
       <c r="I14" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="J14" s="9">
+        <v>44810</v>
+      </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
+      <c r="A15" t="s">
         <v>345</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -4241,19 +4244,26 @@
         <v>49.2</v>
       </c>
       <c r="E15" s="6">
-        <f>D15*[11]Main!$L$3*2</f>
-        <v>123482.16000000002</v>
+        <f>D15*[11]Main!$K$3*2</f>
+        <v>123098.40000000001</v>
       </c>
       <c r="F15" s="6">
-        <f>([11]Main!$L$5-[11]Main!$L$6)*EUR</f>
-        <v>-10384.598400000001</v>
+        <f>([11]Main!$K$5-[11]Main!$K$6)*EUR</f>
+        <v>-12400.887000000001</v>
       </c>
       <c r="G15" s="6">
         <f t="shared" ref="G15:G23" si="2">E15-F15</f>
-        <v>133866.75840000002</v>
+        <v>135499.28700000001</v>
+      </c>
+      <c r="H15" s="6">
+        <f>+[11]Main!$K$3</f>
+        <v>1251</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>23</v>
+        <v>311</v>
+      </c>
+      <c r="J15" s="9">
+        <v>44810</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.2">
@@ -4270,23 +4280,30 @@
         <v>66</v>
       </c>
       <c r="E16" s="6">
-        <f>D16*[12]Main!$L$3</f>
-        <v>103026</v>
+        <f>+D16*H16</f>
+        <v>102960</v>
       </c>
       <c r="F16" s="6">
         <f>[12]Main!$L$5-[12]Main!$L$6</f>
-        <v>-25217</v>
+        <v>-24689</v>
       </c>
       <c r="G16" s="6">
         <f t="shared" si="2"/>
-        <v>128243</v>
+        <v>127649</v>
+      </c>
+      <c r="H16" s="6">
+        <f>+[12]Main!$L$3</f>
+        <v>1560</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="J16" s="9">
+        <v>44812</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>345</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -4317,12 +4334,12 @@
       <c r="I17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J17" s="18">
+      <c r="J17" s="9">
         <v>44792</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>345</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -4353,13 +4370,13 @@
       <c r="I18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J18" s="18">
+      <c r="J18" s="9">
         <f>+J17</f>
         <v>44792</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>345</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -4390,12 +4407,12 @@
       <c r="I19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J19" s="18">
+      <c r="J19" s="9">
         <v>44780</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A20" s="10" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>345</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -4423,8 +4440,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>345</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -4452,17 +4469,17 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>345</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="5" t="s">
         <v>49</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="7">
         <v>263.08999999999997</v>
       </c>
       <c r="E22" s="6">
@@ -4481,8 +4498,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>345</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -4513,12 +4530,12 @@
       <c r="I23" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="J23" s="18">
+      <c r="J23" s="9">
         <v>44782</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>345</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -4527,12 +4544,12 @@
       <c r="C24" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="7">
         <v>128.03</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A25" s="10" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>345</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -4545,8 +4562,8 @@
         <v>3311</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A26" s="10" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>345</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -4559,8 +4576,8 @@
         <v>13.12</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A27" s="10" t="s">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>345</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -4569,43 +4586,19 @@
       <c r="C27" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="P27" s="27"/>
-      <c r="Q27" s="27"/>
-      <c r="R27" s="27"/>
-      <c r="S27" s="27"/>
-      <c r="T27" s="27"/>
-      <c r="U27" s="27"/>
-      <c r="V27" s="27"/>
-      <c r="W27" s="27"/>
-      <c r="X27" s="27"/>
-      <c r="Y27" s="27"/>
-      <c r="Z27" s="27"/>
-      <c r="AA27" s="27"/>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>345</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" t="s">
         <v>265</v>
       </c>
-      <c r="P28" s="9"/>
-      <c r="Q28" s="9"/>
-      <c r="R28" s="9"/>
-      <c r="S28" s="9"/>
-      <c r="T28" s="9"/>
-      <c r="U28" s="9"/>
-      <c r="V28" s="9"/>
-      <c r="W28" s="9"/>
-      <c r="X28" s="9"/>
-      <c r="Y28" s="9"/>
-      <c r="Z28" s="9"/>
-      <c r="AA28" s="9"/>
-    </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>345</v>
       </c>
@@ -4619,53 +4612,29 @@
         <v>125.14</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" t="s">
         <v>268</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="P30" s="11"/>
-      <c r="Q30" s="11"/>
-      <c r="R30" s="11"/>
-      <c r="S30" s="11"/>
-      <c r="T30" s="11"/>
-      <c r="U30" s="11"/>
-      <c r="V30" s="11"/>
-      <c r="W30" s="11"/>
-      <c r="X30" s="11"/>
-      <c r="Y30" s="11"/>
-      <c r="Z30" s="11"/>
-      <c r="AA30" s="11"/>
-    </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" t="s">
         <v>266</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" t="s">
         <v>267</v>
       </c>
-      <c r="P31" s="11"/>
-      <c r="Q31" s="11"/>
-      <c r="R31" s="11"/>
-      <c r="S31" s="11"/>
-      <c r="T31" s="11"/>
-      <c r="U31" s="11"/>
-      <c r="V31" s="11"/>
-      <c r="W31" s="11"/>
-      <c r="X31" s="11"/>
-      <c r="Y31" s="11"/>
-      <c r="Z31" s="11"/>
-      <c r="AA31" s="11"/>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>345</v>
       </c>
@@ -4679,30 +4648,18 @@
         <v>3060</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A33" s="10" t="s">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>345</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" t="s">
         <v>270</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" t="s">
         <v>271</v>
       </c>
-      <c r="P33" s="11"/>
-      <c r="Q33" s="11"/>
-      <c r="R33" s="11"/>
-      <c r="S33" s="11"/>
-      <c r="T33" s="11"/>
-      <c r="U33" s="11"/>
-      <c r="V33" s="11"/>
-      <c r="W33" s="11"/>
-      <c r="X33" s="11"/>
-      <c r="Y33" s="11"/>
-      <c r="Z33" s="11"/>
-      <c r="AA33" s="11"/>
-    </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>345</v>
       </c>
@@ -4716,8 +4673,8 @@
         <v>165.45</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A35" s="10" t="s">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>345</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -4730,532 +4687,428 @@
         <v>63.83</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A36" s="10" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>345</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" t="s">
         <v>272</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36" t="s">
         <v>273</v>
       </c>
       <c r="D36" s="6"/>
-      <c r="P36" s="11"/>
-      <c r="Q36" s="11"/>
-      <c r="R36" s="11"/>
-      <c r="S36" s="11"/>
-      <c r="T36" s="11"/>
-      <c r="U36" s="11"/>
-      <c r="V36" s="11"/>
-      <c r="W36" s="11"/>
-      <c r="X36" s="11"/>
-      <c r="Y36" s="11"/>
-      <c r="Z36" s="11"/>
-      <c r="AA36" s="11"/>
-    </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>345</v>
+      </c>
       <c r="B37" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D37" s="6">
+        <v>1978</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>345</v>
+      </c>
+      <c r="B38" t="s">
+        <v>276</v>
+      </c>
+      <c r="C38" t="s">
+        <v>277</v>
+      </c>
+      <c r="D38" s="6"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D39" s="3">
+        <v>39.35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>345</v>
+      </c>
+      <c r="B40" t="s">
+        <v>274</v>
+      </c>
+      <c r="C40" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B41" t="s">
+        <v>287</v>
+      </c>
+      <c r="C41" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D42" s="6">
         <v>4360</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B38" s="1" t="s">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B43" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D43" s="3">
         <v>76.08</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B39" s="5" t="s">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B44" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D44" s="3">
         <v>71.27</v>
       </c>
-      <c r="E39" s="6">
-        <f>+D39*[19]Main!$K$3</f>
+      <c r="E44" s="6">
+        <f>+D44*[19]Main!$K$3</f>
         <v>15786.66213397</v>
       </c>
-      <c r="F39" s="6">
+      <c r="F44" s="6">
         <f>+[19]Main!$K$5-[19]Main!$K$6</f>
         <v>2721</v>
       </c>
-      <c r="G39" s="6">
-        <f>E39-F39</f>
+      <c r="G44" s="6">
+        <f>E44-F44</f>
         <v>13065.66213397</v>
       </c>
-      <c r="I39" s="3" t="s">
+      <c r="I44" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B40" s="5" t="s">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B45" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D45" s="3">
         <v>28.54</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B41" s="1" t="s">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B46" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D46" s="3">
         <v>349.96</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B42" s="5" t="s">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B47" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D47" s="3">
         <v>10.46</v>
       </c>
-      <c r="E42" s="6">
-        <f>D42*[20]Main!$M$3</f>
+      <c r="E47" s="6">
+        <f>D47*[20]Main!$M$3</f>
         <v>12680.93945768</v>
       </c>
-      <c r="F42" s="6">
+      <c r="F47" s="6">
         <f>[20]Main!$M$5-[20]Main!$M$6</f>
         <v>-18665.5</v>
       </c>
-      <c r="G42" s="6">
-        <f>E42-F42</f>
+      <c r="G47" s="6">
+        <f>E47-F47</f>
         <v>31346.43945768</v>
       </c>
-      <c r="I42" s="3" t="s">
+      <c r="I47" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B43" s="5" t="s">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B48" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D48" s="3">
         <v>137.09</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B44" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D44" s="3">
-        <v>39.35</v>
-      </c>
-    </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B45" s="10" t="s">
-        <v>274</v>
-      </c>
-      <c r="C45" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="P45" s="11"/>
-      <c r="Q45" s="11"/>
-      <c r="R45" s="11"/>
-      <c r="S45" s="11"/>
-      <c r="T45" s="11"/>
-      <c r="U45" s="11"/>
-      <c r="V45" s="11"/>
-      <c r="W45" s="11"/>
-      <c r="X45" s="11"/>
-      <c r="Y45" s="11"/>
-      <c r="Z45" s="11"/>
-      <c r="AA45" s="11"/>
-    </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B46" s="5" t="s">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B49" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D49" s="3">
         <v>132.13999999999999</v>
       </c>
-      <c r="E46" s="6">
-        <f>D46*[21]Main!$L$3</f>
+      <c r="E49" s="6">
+        <f>D49*[21]Main!$L$3</f>
         <v>13539.443113239999</v>
       </c>
-      <c r="F46" s="6">
+      <c r="F49" s="6">
         <f>[21]Main!$L$5-[21]Main!$L$6</f>
         <v>5643.241</v>
       </c>
-      <c r="G46" s="6">
-        <f>E46-F46</f>
+      <c r="G49" s="6">
+        <f>E49-F49</f>
         <v>7896.2021132399987</v>
       </c>
-      <c r="I46" s="3" t="s">
+      <c r="I49" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B47" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D47" s="6">
-        <v>1978</v>
-      </c>
-    </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B48" s="1" t="s">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B50" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D50" s="3">
         <v>11.57</v>
       </c>
     </row>
-    <row r="49" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B49" s="1" t="s">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B51" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D49" s="3">
+      <c r="D51" s="3">
         <v>145.13999999999999</v>
       </c>
     </row>
-    <row r="50" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B50" s="5" t="s">
+    <row r="52" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B52" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D50" s="3">
+      <c r="D52" s="3">
         <v>219.38</v>
       </c>
-      <c r="E50" s="6">
-        <f>D50*[22]Main!$K$3</f>
+      <c r="E52" s="6">
+        <f>D52*[22]Main!$K$3</f>
         <v>10464.426000000001</v>
       </c>
-      <c r="F50" s="6">
+      <c r="F52" s="6">
         <f>[22]Main!$K$5-[22]Main!$K$6</f>
         <v>3027</v>
       </c>
-      <c r="G50" s="6">
-        <f>E50-F50</f>
+      <c r="G52" s="6">
+        <f>E52-F52</f>
         <v>7437.4260000000013</v>
       </c>
-      <c r="I50" s="3" t="s">
+      <c r="I52" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B51" s="5" t="s">
+    <row r="53" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B53" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D51" s="7">
+      <c r="D53" s="7">
         <v>57</v>
       </c>
-      <c r="E51" s="6">
-        <f>+D51*[23]Main!$L$3</f>
+      <c r="E53" s="6">
+        <f>+D53*[23]Main!$L$3</f>
         <v>6071.7436259999995</v>
       </c>
-      <c r="F51" s="6">
+      <c r="F53" s="6">
         <f>+[23]Main!$L$5-[23]Main!$L$6</f>
         <v>776.13</v>
       </c>
-      <c r="G51" s="6">
-        <f>+E51-F51</f>
+      <c r="G53" s="6">
+        <f>+E53-F53</f>
         <v>5295.6136259999994</v>
       </c>
-      <c r="I51" s="3" t="s">
+      <c r="I53" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B52" s="5" t="s">
+    <row r="54" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B54" s="5" t="s">
         <v>306</v>
       </c>
-      <c r="C52" s="10" t="s">
+      <c r="C54" t="s">
         <v>307</v>
       </c>
-      <c r="D52" s="6">
+      <c r="D54" s="6">
         <v>1721.48</v>
       </c>
-      <c r="E52" s="6">
-        <f>+D52*H52/100*GBP</f>
+      <c r="E54" s="6">
+        <f>+D54*H54/100*GBP</f>
         <v>4746.2735717200003</v>
       </c>
-      <c r="F52" s="6">
+      <c r="F54" s="6">
         <f>+[24]Main!$K$5-[24]Main!$K$6</f>
         <v>-337</v>
       </c>
-      <c r="G52" s="6">
-        <f>+E52-F52</f>
+      <c r="G54" s="6">
+        <f>+E54-F54</f>
         <v>5083.2735717200003</v>
       </c>
-      <c r="H52" s="6">
+      <c r="H54" s="6">
         <f>+[24]Main!$K$3</f>
         <v>233</v>
       </c>
-      <c r="I52" s="3" t="s">
+      <c r="I54" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P52" s="15"/>
-      <c r="Q52" s="15"/>
-      <c r="R52" s="15"/>
-      <c r="S52" s="15"/>
-      <c r="T52" s="15"/>
-      <c r="U52" s="15"/>
-      <c r="V52" s="15"/>
-      <c r="W52" s="15"/>
-      <c r="X52" s="15"/>
-      <c r="Y52" s="15"/>
-      <c r="Z52" s="15"/>
-      <c r="AA52" s="15"/>
-    </row>
-    <row r="53" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B53" s="5" t="s">
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B55" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D53" s="3">
+      <c r="D55" s="3">
         <v>28.03</v>
       </c>
-      <c r="E53" s="6">
-        <f>+H53*D53</f>
+      <c r="E55" s="6">
+        <f>+H55*D55</f>
         <v>4604.0473282500006</v>
       </c>
-      <c r="F53" s="6">
+      <c r="F55" s="6">
         <f>+[25]Main!$L$5-[25]Main!$L$6</f>
         <v>465.44</v>
       </c>
-      <c r="G53" s="6">
-        <f>+E53-F53</f>
+      <c r="G55" s="6">
+        <f>+E55-F55</f>
         <v>4138.607328250001</v>
       </c>
-      <c r="H53" s="6">
+      <c r="H55" s="6">
         <f>+[25]Main!$L$3</f>
         <v>164.25427500000001</v>
       </c>
-      <c r="I53" s="3" t="s">
+      <c r="I55" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="J53" s="18">
+      <c r="J55" s="9">
         <v>44782</v>
       </c>
     </row>
-    <row r="54" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B54" s="1" t="s">
+    <row r="56" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B56" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D54" s="3">
+      <c r="D56" s="3">
         <v>93.28</v>
       </c>
     </row>
-    <row r="55" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B55" s="1" t="s">
+    <row r="57" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B57" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D55" s="3">
+      <c r="D57" s="3">
         <v>142.91</v>
       </c>
     </row>
-    <row r="56" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B56" s="10" t="s">
+    <row r="58" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
         <v>280</v>
       </c>
-      <c r="C56" s="10" t="s">
+      <c r="C58" t="s">
         <v>280</v>
       </c>
-      <c r="P56" s="12"/>
-      <c r="Q56" s="12"/>
-      <c r="R56" s="12"/>
-      <c r="S56" s="12"/>
-      <c r="T56" s="12"/>
-      <c r="U56" s="12"/>
-      <c r="V56" s="12"/>
-      <c r="W56" s="12"/>
-      <c r="X56" s="12"/>
-      <c r="Y56" s="12"/>
-      <c r="Z56" s="12"/>
-      <c r="AA56" s="12"/>
-    </row>
-    <row r="57" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B57" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="C57" s="10" t="s">
-        <v>288</v>
-      </c>
-      <c r="P57" s="12"/>
-      <c r="Q57" s="12"/>
-      <c r="R57" s="12"/>
-      <c r="S57" s="12"/>
-      <c r="T57" s="12"/>
-      <c r="U57" s="12"/>
-      <c r="V57" s="12"/>
-      <c r="W57" s="12"/>
-      <c r="X57" s="12"/>
-      <c r="Y57" s="12"/>
-      <c r="Z57" s="12"/>
-      <c r="AA57" s="12"/>
-    </row>
-    <row r="58" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B58" s="1" t="s">
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B59" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D58" s="3">
+      <c r="D59" s="3">
         <v>7.71</v>
       </c>
     </row>
-    <row r="59" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B59" s="10" t="s">
+    <row r="60" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
         <v>285</v>
       </c>
-      <c r="C59" s="10" t="s">
+      <c r="C60" t="s">
         <v>286</v>
       </c>
-      <c r="P59" s="12"/>
-      <c r="Q59" s="12"/>
-      <c r="R59" s="12"/>
-      <c r="S59" s="12"/>
-      <c r="T59" s="12"/>
-      <c r="U59" s="12"/>
-      <c r="V59" s="12"/>
-      <c r="W59" s="12"/>
-      <c r="X59" s="12"/>
-      <c r="Y59" s="12"/>
-      <c r="Z59" s="12"/>
-      <c r="AA59" s="12"/>
-    </row>
-    <row r="60" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B60" s="10" t="s">
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
         <v>283</v>
       </c>
-      <c r="C60" s="10" t="s">
+      <c r="C61" t="s">
         <v>284</v>
       </c>
-      <c r="P60" s="12"/>
-      <c r="Q60" s="12"/>
-      <c r="R60" s="12"/>
-      <c r="S60" s="12"/>
-      <c r="T60" s="12"/>
-      <c r="U60" s="12"/>
-      <c r="V60" s="12"/>
-      <c r="W60" s="12"/>
-      <c r="X60" s="12"/>
-      <c r="Y60" s="12"/>
-      <c r="Z60" s="12"/>
-      <c r="AA60" s="12"/>
-    </row>
-    <row r="61" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B61" s="10" t="s">
+    </row>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
         <v>281</v>
       </c>
-      <c r="C61" s="10" t="s">
+      <c r="C62" t="s">
         <v>282</v>
       </c>
-      <c r="P61" s="12"/>
-      <c r="Q61" s="12"/>
-      <c r="R61" s="12"/>
-      <c r="S61" s="12"/>
-      <c r="T61" s="12"/>
-      <c r="U61" s="12"/>
-      <c r="V61" s="12"/>
-      <c r="W61" s="12"/>
-      <c r="X61" s="12"/>
-      <c r="Y61" s="12"/>
-      <c r="Z61" s="12"/>
-      <c r="AA61" s="12"/>
-    </row>
-    <row r="62" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B62" s="10" t="s">
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
         <v>278</v>
       </c>
-      <c r="C62" s="10" t="s">
+      <c r="C63" t="s">
         <v>279</v>
       </c>
-      <c r="P62" s="12"/>
-      <c r="Q62" s="12"/>
-      <c r="R62" s="12"/>
-      <c r="S62" s="12"/>
-      <c r="T62" s="12"/>
-      <c r="U62" s="12"/>
-      <c r="V62" s="12"/>
-      <c r="W62" s="12"/>
-      <c r="X62" s="12"/>
-      <c r="Y62" s="12"/>
-      <c r="Z62" s="12"/>
-      <c r="AA62" s="12"/>
-    </row>
-    <row r="63" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B63" s="10" t="s">
-        <v>276</v>
-      </c>
-      <c r="C63" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="P63" s="12"/>
-      <c r="Q63" s="12"/>
-      <c r="R63" s="12"/>
-      <c r="S63" s="12"/>
-      <c r="T63" s="12"/>
-      <c r="U63" s="12"/>
-      <c r="V63" s="12"/>
-      <c r="W63" s="12"/>
-      <c r="X63" s="12"/>
-      <c r="Y63" s="12"/>
-      <c r="Z63" s="12"/>
-      <c r="AA63" s="12"/>
-    </row>
-    <row r="64" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B64" s="10" t="s">
+    </row>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
         <v>262</v>
       </c>
-      <c r="C64" s="10" t="s">
+      <c r="C64" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5513,27 +5366,15 @@
       </c>
     </row>
     <row r="88" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B88" s="10" t="s">
+      <c r="B88" t="s">
         <v>317</v>
       </c>
-      <c r="C88" s="10" t="s">
+      <c r="C88" t="s">
         <v>318</v>
       </c>
       <c r="D88" s="3">
         <v>4.26</v>
       </c>
-      <c r="P88" s="19"/>
-      <c r="Q88" s="19"/>
-      <c r="R88" s="19"/>
-      <c r="S88" s="19"/>
-      <c r="T88" s="19"/>
-      <c r="U88" s="19"/>
-      <c r="V88" s="19"/>
-      <c r="W88" s="19"/>
-      <c r="X88" s="19"/>
-      <c r="Y88" s="19"/>
-      <c r="Z88" s="19"/>
-      <c r="AA88" s="19"/>
       <c r="AB88" s="1">
         <v>2011</v>
       </c>
@@ -5641,7 +5482,7 @@
         <v>35.770000000000003</v>
       </c>
     </row>
-    <row r="97" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B97" s="1" t="s">
         <v>165</v>
       </c>
@@ -5652,7 +5493,7 @@
         <v>14.27</v>
       </c>
     </row>
-    <row r="98" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B98" s="1" t="s">
         <v>167</v>
       </c>
@@ -5663,7 +5504,7 @@
         <v>7.36</v>
       </c>
     </row>
-    <row r="99" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B99" s="1" t="s">
         <v>169</v>
       </c>
@@ -5674,7 +5515,7 @@
         <v>9.35</v>
       </c>
     </row>
-    <row r="100" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B100" s="1" t="s">
         <v>171</v>
       </c>
@@ -5685,7 +5526,7 @@
         <v>43.98</v>
       </c>
     </row>
-    <row r="101" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B101" s="1" t="s">
         <v>173</v>
       </c>
@@ -5696,7 +5537,7 @@
         <v>5.18</v>
       </c>
     </row>
-    <row r="102" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B102" s="1" t="s">
         <v>175</v>
       </c>
@@ -5707,7 +5548,7 @@
         <v>53.72</v>
       </c>
     </row>
-    <row r="103" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B103" s="1" t="s">
         <v>177</v>
       </c>
@@ -5718,27 +5559,15 @@
         <v>21.04</v>
       </c>
     </row>
-    <row r="104" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B104" s="10" t="s">
+    <row r="104" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B104" t="s">
         <v>319</v>
       </c>
-      <c r="C104" s="10" t="s">
+      <c r="C104" t="s">
         <v>320</v>
       </c>
-      <c r="P104" s="20"/>
-      <c r="Q104" s="20"/>
-      <c r="R104" s="20"/>
-      <c r="S104" s="20"/>
-      <c r="T104" s="20"/>
-      <c r="U104" s="20"/>
-      <c r="V104" s="20"/>
-      <c r="W104" s="20"/>
-      <c r="X104" s="20"/>
-      <c r="Y104" s="20"/>
-      <c r="Z104" s="20"/>
-      <c r="AA104" s="20"/>
-    </row>
-    <row r="105" spans="2:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="105" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B105" s="1" t="s">
         <v>179</v>
       </c>
@@ -5749,7 +5578,7 @@
         <v>20.7</v>
       </c>
     </row>
-    <row r="106" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B106" s="1" t="s">
         <v>181</v>
       </c>
@@ -5760,7 +5589,7 @@
         <v>18.579999999999998</v>
       </c>
     </row>
-    <row r="107" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B107" s="1" t="s">
         <v>183</v>
       </c>
@@ -5771,7 +5600,7 @@
         <v>16.12</v>
       </c>
     </row>
-    <row r="108" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B108" s="1" t="s">
         <v>185</v>
       </c>
@@ -5782,7 +5611,7 @@
         <v>28.41</v>
       </c>
     </row>
-    <row r="109" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B109" s="1" t="s">
         <v>187</v>
       </c>
@@ -5793,753 +5622,704 @@
         <v>33.86</v>
       </c>
     </row>
-    <row r="110" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B110" s="1" t="s">
+    <row r="110" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B110" t="s">
+        <v>354</v>
+      </c>
+      <c r="C110" t="s">
+        <v>355</v>
+      </c>
+      <c r="D110" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B111" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C110" s="1" t="s">
+      <c r="C111" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="D110" s="3">
+      <c r="D111" s="3">
         <v>38.35</v>
       </c>
     </row>
-    <row r="111" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B111" s="1" t="s">
+    <row r="112" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B112" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="C111" s="1" t="s">
+      <c r="C112" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D111" s="3">
+      <c r="D112" s="3">
         <v>9.6199999999999992</v>
       </c>
     </row>
-    <row r="112" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B112" s="1" t="s">
+    <row r="113" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B113" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="C113" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="D112" s="3">
+      <c r="D113" s="3">
         <v>25.49</v>
       </c>
     </row>
-    <row r="113" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B113" s="10" t="s">
+    <row r="114" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B114" t="s">
         <v>300</v>
       </c>
-      <c r="C113" s="10" t="s">
+      <c r="C114" t="s">
         <v>301</v>
       </c>
-      <c r="P113" s="14"/>
-      <c r="Q113" s="14"/>
-      <c r="R113" s="14"/>
-      <c r="S113" s="14"/>
-      <c r="T113" s="14"/>
-      <c r="U113" s="14"/>
-      <c r="V113" s="14"/>
-      <c r="W113" s="14"/>
-      <c r="X113" s="14"/>
-      <c r="Y113" s="14"/>
-      <c r="Z113" s="14"/>
-      <c r="AA113" s="14"/>
-    </row>
-    <row r="114" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B114" s="1" t="s">
+    </row>
+    <row r="115" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B115" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C114" s="1" t="s">
+      <c r="C115" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="D114" s="3">
+      <c r="D115" s="3">
         <v>11.42</v>
       </c>
     </row>
-    <row r="115" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B115" s="1" t="s">
+    <row r="116" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B116" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C115" s="1" t="s">
+      <c r="C116" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="D115" s="3">
+      <c r="D116" s="3">
         <v>26.64</v>
       </c>
     </row>
-    <row r="116" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B116" s="1" t="s">
+    <row r="117" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B117" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C116" s="1" t="s">
+      <c r="C117" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="D116" s="3">
+      <c r="D117" s="3">
         <v>30.48</v>
       </c>
     </row>
-    <row r="117" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B117" s="1" t="s">
+    <row r="118" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B118" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="C118" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="D117" s="3">
+      <c r="D118" s="3">
         <v>12.98</v>
       </c>
     </row>
-    <row r="118" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B118" s="1" t="s">
+    <row r="119" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B119" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C118" s="1" t="s">
+      <c r="C119" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="D118" s="3">
+      <c r="D119" s="3">
         <v>10.96</v>
       </c>
     </row>
-    <row r="119" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B119" s="1" t="s">
+    <row r="120" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B120" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="C120" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="D119" s="3">
+      <c r="D120" s="3">
         <v>2.42</v>
       </c>
     </row>
-    <row r="120" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B120" s="1" t="s">
+    <row r="121" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B121" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="C121" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="D120" s="7">
+      <c r="D121" s="7">
         <v>55.5</v>
       </c>
     </row>
-    <row r="121" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B121" s="1" t="s">
+    <row r="122" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B122" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C121" s="1" t="s">
+      <c r="C122" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="D121" s="3">
+      <c r="D122" s="3">
         <v>10.63</v>
       </c>
     </row>
-    <row r="122" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B122" s="1" t="s">
+    <row r="123" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B123" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C122" s="1" t="s">
+      <c r="C123" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="D122" s="3">
+      <c r="D123" s="3">
         <v>33.130000000000003</v>
       </c>
     </row>
-    <row r="123" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B123" s="1" t="s">
+    <row r="124" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B124" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C123" s="1" t="s">
+      <c r="C124" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="D123" s="3">
+      <c r="D124" s="3">
         <v>31.52</v>
       </c>
     </row>
-    <row r="124" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B124" s="1" t="s">
+    <row r="125" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B125" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="C124" s="1" t="s">
+      <c r="C125" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="D124" s="3">
+      <c r="D125" s="3">
         <v>7.62</v>
       </c>
     </row>
-    <row r="125" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B125" s="1" t="s">
+    <row r="126" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B126" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C125" s="1" t="s">
+      <c r="C126" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="D125" s="3">
+      <c r="D126" s="3">
         <v>28.55</v>
       </c>
     </row>
-    <row r="126" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B126" s="1" t="s">
+    <row r="127" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B127" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="C126" s="1" t="s">
+      <c r="C127" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="D126" s="3">
+      <c r="D127" s="3">
         <v>27.02</v>
       </c>
     </row>
-    <row r="127" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B127" s="5" t="s">
+    <row r="128" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B128" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="C127" s="10" t="s">
+      <c r="C128" t="s">
         <v>298</v>
       </c>
-      <c r="D127" s="3">
+      <c r="D128" s="3">
         <v>15.65</v>
       </c>
-      <c r="E127" s="6">
-        <f>D127*[27]Main!$L$3</f>
+      <c r="E128" s="6">
+        <f>D128*[27]Main!$L$3</f>
         <v>1253.1559559500001</v>
       </c>
-      <c r="F127" s="6">
+      <c r="F128" s="6">
         <f>+[27]Main!$L$5-[27]Main!$L$6</f>
         <v>112.015</v>
       </c>
-      <c r="G127" s="6">
-        <f>+E127-F127</f>
+      <c r="G128" s="6">
+        <f>+E128-F128</f>
         <v>1141.14095595</v>
       </c>
-      <c r="I127" s="3" t="s">
+      <c r="I128" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="128" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B128" s="5" t="s">
+    <row r="129" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B129" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="C128" s="10" t="s">
+      <c r="C129" t="s">
         <v>309</v>
       </c>
-      <c r="D128" s="3">
+      <c r="D129" s="3">
         <v>16.93</v>
       </c>
-      <c r="E128" s="6">
-        <f>+D128*[28]Main!$L$3</f>
+      <c r="E129" s="6">
+        <f>+D129*[28]Main!$L$3</f>
         <v>1228.5485933099999</v>
       </c>
-      <c r="F128" s="6">
+      <c r="F129" s="6">
         <f>+[28]Main!$L$5-[28]Main!$L$6</f>
         <v>153.25991400000001</v>
       </c>
-      <c r="G128" s="6">
-        <f>+E128-F128</f>
+      <c r="G129" s="6">
+        <f>+E129-F129</f>
         <v>1075.2886793099999</v>
       </c>
-      <c r="I128" s="3" t="s">
+      <c r="I129" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J128" s="18">
+      <c r="J129" s="9">
         <v>44771</v>
       </c>
-      <c r="K128" s="18"/>
-      <c r="L128" s="18"/>
-      <c r="M128" s="18"/>
-      <c r="N128" s="18"/>
-      <c r="O128" s="18"/>
-      <c r="P128" s="16"/>
-      <c r="Q128" s="16"/>
-      <c r="R128" s="16"/>
-      <c r="S128" s="16"/>
-      <c r="T128" s="16"/>
-      <c r="U128" s="16"/>
-      <c r="V128" s="16"/>
-      <c r="W128" s="16"/>
-      <c r="X128" s="16"/>
-      <c r="Y128" s="16"/>
-      <c r="Z128" s="16"/>
-      <c r="AA128" s="16"/>
-    </row>
-    <row r="129" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B129" s="1" t="s">
+      <c r="K129" s="9"/>
+      <c r="L129" s="9"/>
+      <c r="M129" s="9"/>
+      <c r="N129" s="9"/>
+      <c r="O129" s="9"/>
+    </row>
+    <row r="130" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B130" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C129" s="1" t="s">
+      <c r="C130" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D129" s="3">
+      <c r="D130" s="3">
         <v>3.17</v>
       </c>
     </row>
-    <row r="130" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B130" s="1" t="s">
+    <row r="131" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B131" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="C130" s="1" t="s">
+      <c r="C131" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="D130" s="3">
+      <c r="D131" s="3">
         <v>8.76</v>
       </c>
     </row>
-    <row r="131" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B131" s="1" t="s">
+    <row r="132" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B132" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C131" s="1" t="s">
+      <c r="C132" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="D131" s="3">
+      <c r="D132" s="3">
         <v>18.010000000000002</v>
       </c>
     </row>
-    <row r="132" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B132" s="10" t="s">
+    <row r="133" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B133" t="s">
         <v>314</v>
       </c>
-      <c r="C132" s="10" t="s">
+      <c r="C133" t="s">
         <v>315</v>
       </c>
-      <c r="D132" s="3">
+      <c r="D133" s="3">
         <v>3.92</v>
       </c>
-      <c r="E132" s="3">
+      <c r="E133" s="3">
         <v>630</v>
       </c>
-      <c r="P132" s="17"/>
-      <c r="Q132" s="17"/>
-      <c r="R132" s="17"/>
-      <c r="S132" s="17"/>
-      <c r="T132" s="17"/>
-      <c r="U132" s="17"/>
-      <c r="V132" s="17"/>
-      <c r="W132" s="17"/>
-      <c r="X132" s="17"/>
-      <c r="Y132" s="17"/>
-      <c r="Z132" s="17"/>
-      <c r="AA132" s="17"/>
-    </row>
-    <row r="133" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B133" s="10" t="s">
+    </row>
+    <row r="134" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B134" t="s">
         <v>312</v>
       </c>
-      <c r="C133" s="10" t="s">
+      <c r="C134" t="s">
         <v>313</v>
       </c>
-      <c r="D133" s="3">
+      <c r="D134" s="3">
         <v>11.93</v>
       </c>
-      <c r="E133" s="3">
+      <c r="E134" s="3">
         <v>516</v>
       </c>
-      <c r="P133" s="17"/>
-      <c r="Q133" s="17"/>
-      <c r="R133" s="17"/>
-      <c r="S133" s="17"/>
-      <c r="T133" s="17"/>
-      <c r="U133" s="17"/>
-      <c r="V133" s="17"/>
-      <c r="W133" s="17"/>
-      <c r="X133" s="17"/>
-      <c r="Y133" s="17"/>
-      <c r="Z133" s="17"/>
-      <c r="AA133" s="17"/>
-    </row>
-    <row r="134" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B134" s="1" t="s">
+    </row>
+    <row r="135" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B135" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="C134" s="1" t="s">
+      <c r="C135" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="D134" s="3">
+      <c r="D135" s="3">
         <v>5.46</v>
       </c>
     </row>
-    <row r="135" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B135" s="1" t="s">
+    <row r="136" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B136" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="C135" s="1" t="s">
+      <c r="C136" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D135" s="7">
+      <c r="D136" s="7">
         <v>36.6</v>
       </c>
     </row>
-    <row r="136" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B136" s="1" t="s">
+    <row r="137" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B137" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="C136" s="1" t="s">
+      <c r="C137" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="D136" s="7">
+      <c r="D137" s="7">
         <v>40.24</v>
       </c>
     </row>
-    <row r="137" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B137" s="1" t="s">
+    <row r="138" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B138" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C137" s="1" t="s">
+      <c r="C138" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D137" s="3">
+      <c r="D138" s="3">
         <v>22.11</v>
       </c>
     </row>
-    <row r="138" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B138" s="5" t="s">
+    <row r="139" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B139" s="5" t="s">
         <v>332</v>
       </c>
-      <c r="C138" s="10" t="s">
+      <c r="C139" t="s">
         <v>333</v>
       </c>
-      <c r="D138" s="3">
+      <c r="D139" s="3">
         <v>3.95</v>
       </c>
-      <c r="E138" s="6">
-        <f>+D138*H138</f>
+      <c r="E139" s="6">
+        <f>+D139*H139</f>
         <v>37.185714749999995</v>
       </c>
-      <c r="F138" s="6">
+      <c r="F139" s="6">
         <f>+[29]Main!$N$5-[29]Main!$N$6</f>
         <v>-7.4640000000000004</v>
       </c>
-      <c r="G138" s="6">
-        <f>+E138-F138</f>
+      <c r="G139" s="6">
+        <f>+E139-F139</f>
         <v>44.649714749999994</v>
       </c>
-      <c r="H138" s="6">
+      <c r="H139" s="6">
         <f>+[29]Main!$N$3</f>
         <v>9.4141049999999993</v>
       </c>
-      <c r="I138" s="3" t="s">
+      <c r="I139" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="J138" s="18">
+      <c r="J139" s="9">
         <v>44780</v>
       </c>
-      <c r="P138" s="25"/>
-      <c r="Q138" s="25"/>
-      <c r="R138" s="25"/>
-      <c r="S138" s="25"/>
-      <c r="T138" s="25"/>
-      <c r="U138" s="25"/>
-      <c r="V138" s="25"/>
-      <c r="W138" s="25"/>
-      <c r="X138" s="25"/>
-      <c r="Y138" s="25"/>
-      <c r="Z138" s="25"/>
-      <c r="AA138" s="25"/>
-    </row>
-    <row r="139" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B139" s="1" t="s">
+    </row>
+    <row r="140" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B140" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C139" s="1" t="s">
+      <c r="C140" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="D139" s="3">
+      <c r="D140" s="3">
         <v>10.31</v>
       </c>
     </row>
-    <row r="140" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B140" s="1" t="s">
+    <row r="141" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B141" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C140" s="1" t="s">
+      <c r="C141" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="D140" s="7">
+      <c r="D141" s="7">
         <v>1.3</v>
       </c>
     </row>
-    <row r="141" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B141" s="1" t="s">
+    <row r="142" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B142" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="C141" s="1" t="s">
+      <c r="C142" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="D141" s="3">
+      <c r="D142" s="3">
         <v>3.35</v>
       </c>
     </row>
-    <row r="142" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B142" s="5" t="s">
+    <row r="143" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B143" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="C142" s="1" t="s">
+      <c r="C143" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="D142" s="3">
+      <c r="D143" s="3">
         <v>7.06</v>
       </c>
-      <c r="E142" s="6">
-        <f>D142*[30]Main!$J$3</f>
+      <c r="E143" s="6">
+        <f>D143*[30]Main!$J$3</f>
         <v>725.62786605999997</v>
       </c>
-      <c r="F142" s="6">
+      <c r="F143" s="6">
         <f>[30]Main!$J$5-[30]Main!$J$6</f>
         <v>197.79600000000002</v>
       </c>
-      <c r="G142" s="8">
-        <f>+E142-F142</f>
+      <c r="G143" s="8">
+        <f>+E143-F143</f>
         <v>527.83186605999992</v>
       </c>
-      <c r="I142" s="3" t="s">
+      <c r="I143" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="143" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B143" s="5" t="s">
+    <row r="144" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B144" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="C143" s="1" t="s">
+      <c r="C144" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="D143" s="3">
+      <c r="D144" s="3">
         <v>14.68</v>
       </c>
-      <c r="E143" s="6">
-        <f>D143*[31]Main!$L$3</f>
+      <c r="E144" s="6">
+        <f>D144*[31]Main!$L$3</f>
         <v>587.26396075999992</v>
       </c>
-      <c r="F143" s="6">
+      <c r="F144" s="6">
         <f>[31]Main!$L$5-[31]Main!$L$6</f>
         <v>277.88299999999998</v>
       </c>
-      <c r="G143" s="8">
-        <f>+E143-F143</f>
+      <c r="G144" s="8">
+        <f>+E144-F144</f>
         <v>309.38096075999994</v>
       </c>
-      <c r="I143" s="3" t="s">
+      <c r="I144" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="144" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B144" s="5" t="s">
+    <row r="145" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B145" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="C144" s="1" t="s">
+      <c r="C145" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="D144" s="3">
+      <c r="D145" s="3">
         <v>4.8600000000000003</v>
       </c>
-      <c r="E144" s="6">
-        <f>D144*[32]Main!$J$3</f>
+      <c r="E145" s="6">
+        <f>D145*[32]Main!$J$3</f>
         <v>312.71415336000001</v>
       </c>
-      <c r="F144" s="8">
+      <c r="F145" s="8">
         <f>+[32]Main!$J$5-[32]Main!$J$6</f>
         <v>92.317999999999998</v>
       </c>
-      <c r="G144" s="8">
-        <f>+E144-F144</f>
+      <c r="G145" s="8">
+        <f>+E145-F145</f>
         <v>220.39615336000003</v>
       </c>
-      <c r="I144" s="3" t="s">
+      <c r="I145" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="145" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B145" s="5" t="s">
+    <row r="146" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B146" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="C145" s="1" t="s">
+      <c r="C146" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="D145" s="3">
+      <c r="D146" s="3">
         <v>7.57</v>
       </c>
-      <c r="E145" s="6">
-        <f>D145*[33]Main!$M$3</f>
+      <c r="E146" s="6">
+        <f>D146*[33]Main!$M$3</f>
         <v>338.45983246000003</v>
       </c>
-      <c r="F145" s="6">
+      <c r="F146" s="6">
         <f>[33]Main!$M$5-[33]Main!$M$6</f>
         <v>120.43700000000001</v>
       </c>
-      <c r="G145" s="8">
-        <f t="shared" ref="G145:G150" si="3">+E145-F145</f>
+      <c r="G146" s="8">
+        <f t="shared" ref="G146:G151" si="3">+E146-F146</f>
         <v>218.02283246000002</v>
       </c>
-      <c r="I145" s="3" t="s">
+      <c r="I146" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="146" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B146" s="5" t="s">
+    <row r="147" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B147" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="C146" s="1" t="s">
+      <c r="C147" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="D146" s="7">
+      <c r="D147" s="7">
         <v>0.7</v>
       </c>
-      <c r="E146" s="6">
-        <f>D146*[34]Main!$M$3</f>
+      <c r="E147" s="6">
+        <f>D147*[34]Main!$M$3</f>
         <v>128.9392503</v>
       </c>
-      <c r="F146" s="6">
+      <c r="F147" s="6">
         <f>[34]Main!$M$5-[34]Main!$M$6</f>
         <v>-59.50200000000001</v>
       </c>
-      <c r="G146" s="8">
+      <c r="G147" s="8">
         <f t="shared" si="3"/>
         <v>188.44125030000001</v>
       </c>
-      <c r="I146" s="3" t="s">
+      <c r="I147" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="147" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B147" s="5" t="s">
+    <row r="148" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B148" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="C147" s="1" t="s">
+      <c r="C148" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="D147" s="3">
+      <c r="D148" s="3">
         <v>1.98</v>
       </c>
-      <c r="E147" s="6">
-        <f>D147*[35]Main!$N$3</f>
+      <c r="E148" s="6">
+        <f>D148*[35]Main!$N$3</f>
         <v>39.757463459999997</v>
       </c>
-      <c r="F147" s="6">
+      <c r="F148" s="6">
         <f>[35]Main!$N$5-[35]Main!$N$6</f>
         <v>15.942</v>
       </c>
-      <c r="G147" s="8">
+      <c r="G148" s="8">
         <f t="shared" si="3"/>
         <v>23.815463459999997</v>
       </c>
-      <c r="I147" s="3" t="s">
+      <c r="I148" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="148" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B148" s="5" t="s">
+    <row r="149" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B149" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="C148" s="1" t="s">
+      <c r="C149" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="D148" s="3">
+      <c r="D149" s="3">
         <v>0.62</v>
       </c>
-      <c r="E148" s="6">
-        <f>D148*[36]Main!$L$3</f>
+      <c r="E149" s="6">
+        <f>D149*[36]Main!$L$3</f>
         <v>30.1881658</v>
       </c>
-      <c r="F148" s="6">
+      <c r="F149" s="6">
         <f>[36]Main!$L$5-[36]Main!$L$6</f>
         <v>13.262999999999998</v>
       </c>
-      <c r="G148" s="8">
+      <c r="G149" s="8">
         <f t="shared" si="3"/>
         <v>16.925165800000002</v>
       </c>
-      <c r="I148" s="3" t="s">
+      <c r="I149" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="149" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B149" s="5" t="s">
+    <row r="150" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B150" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="C149" s="1" t="s">
+      <c r="C150" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="D149" s="3">
+      <c r="D150" s="3">
         <v>6.12</v>
       </c>
-      <c r="E149" s="6">
-        <f>D149*[37]Main!$M$3</f>
+      <c r="E150" s="6">
+        <f>D150*[37]Main!$M$3</f>
         <v>125.46108324000001</v>
       </c>
-      <c r="F149" s="6">
+      <c r="F150" s="6">
         <f>[37]Main!$M$5-[37]Main!$M$6</f>
         <v>131.17699999999999</v>
       </c>
-      <c r="G149" s="8">
+      <c r="G150" s="8">
         <f t="shared" si="3"/>
         <v>-5.7159167599999847</v>
       </c>
-      <c r="I149" s="3" t="s">
+      <c r="I150" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="150" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B150" s="5" t="s">
+    <row r="151" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B151" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="C150" s="1" t="s">
+      <c r="C151" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="D150" s="3">
+      <c r="D151" s="3">
         <v>0.98</v>
       </c>
-      <c r="E150" s="6">
-        <f>D150*[38]Main!$M$3</f>
+      <c r="E151" s="6">
+        <f>D151*[38]Main!$M$3</f>
         <v>20.935517539999999</v>
       </c>
-      <c r="F150" s="6">
+      <c r="F151" s="6">
         <f>[38]Main!$M$5-[38]Main!$M$6</f>
         <v>55.28</v>
       </c>
-      <c r="G150" s="8">
+      <c r="G151" s="8">
         <f t="shared" si="3"/>
         <v>-34.344482460000002</v>
       </c>
-      <c r="I150" s="3" t="s">
+      <c r="I151" s="3" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="151" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B151" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="C151" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="D151" s="3">
-        <v>0.61</v>
       </c>
     </row>
     <row r="152" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B152" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D152" s="3">
-        <v>5.55</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="153" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B153" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D153" s="3">
+        <v>5.55</v>
+      </c>
+    </row>
+    <row r="154" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B154" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="C153" s="10" t="s">
+      <c r="C154" t="s">
         <v>344</v>
       </c>
-      <c r="D153" s="7">
+      <c r="D154" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="154" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B154" s="10" t="s">
+    <row r="155" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B155" t="s">
         <v>347</v>
       </c>
-      <c r="C154" s="10" t="s">
+      <c r="C155" t="s">
         <v>348</v>
       </c>
     </row>
@@ -6566,34 +6346,34 @@
     <hyperlink ref="B5" r:id="rId15" xr:uid="{0888F4DA-9569-4326-990C-43015A33BD61}"/>
     <hyperlink ref="B19" r:id="rId16" xr:uid="{C2959A9B-7367-43D7-934F-562A915DC4DD}"/>
     <hyperlink ref="B22" r:id="rId17" xr:uid="{A069369A-FB97-4A4A-A581-321FA79E4250}"/>
-    <hyperlink ref="B39" r:id="rId18" xr:uid="{6EF35D30-7113-4CE8-9077-C5BE97F74D36}"/>
+    <hyperlink ref="B44" r:id="rId18" xr:uid="{6EF35D30-7113-4CE8-9077-C5BE97F74D36}"/>
     <hyperlink ref="B23" r:id="rId19" xr:uid="{1F769FA7-6B90-4B6B-9BCC-7D6679675B06}"/>
     <hyperlink ref="B24" r:id="rId20" xr:uid="{6108C865-F45B-4849-97C5-0C40AD61A72B}"/>
     <hyperlink ref="B25" r:id="rId21" xr:uid="{FBD4E7AC-5982-43A1-83EA-3F3AB2E91655}"/>
-    <hyperlink ref="B43" r:id="rId22" xr:uid="{53091BB6-5763-4DDE-A659-5638BD3CADCA}"/>
-    <hyperlink ref="B40" r:id="rId23" xr:uid="{10922C8B-4C13-4E76-B998-3ADD8CC60E47}"/>
+    <hyperlink ref="B48" r:id="rId22" xr:uid="{53091BB6-5763-4DDE-A659-5638BD3CADCA}"/>
+    <hyperlink ref="B45" r:id="rId23" xr:uid="{10922C8B-4C13-4E76-B998-3ADD8CC60E47}"/>
     <hyperlink ref="B26" r:id="rId24" xr:uid="{61277D68-67DC-475B-9B61-B7E2F3017110}"/>
-    <hyperlink ref="B144" r:id="rId25" xr:uid="{14A63DAF-63A6-4B91-A2AF-AE28EA251457}"/>
-    <hyperlink ref="B147" r:id="rId26" xr:uid="{4ACA7C7F-E42A-4687-A776-AB8065DB40FF}"/>
-    <hyperlink ref="B143" r:id="rId27" xr:uid="{B3421391-7EC0-4253-8F62-5ED45A5BFA02}"/>
-    <hyperlink ref="B148" r:id="rId28" xr:uid="{F6A45FC7-B73C-4143-9CAB-B3ADA19B5FD7}"/>
-    <hyperlink ref="B145" r:id="rId29" xr:uid="{BBD267CB-7407-4913-9D05-6A6AA380019F}"/>
-    <hyperlink ref="B150" r:id="rId30" xr:uid="{85368858-6D0F-4ABE-975C-AE5530342445}"/>
-    <hyperlink ref="B142" r:id="rId31" xr:uid="{8B5BC1F5-14D4-45A0-B224-31FAF227EAF3}"/>
-    <hyperlink ref="B149" r:id="rId32" xr:uid="{D5FB3BFE-F0A8-4C09-90A1-9F506EF0ADE4}"/>
-    <hyperlink ref="B146" r:id="rId33" xr:uid="{11598046-2AED-42E7-ACA5-251A20A59427}"/>
+    <hyperlink ref="B145" r:id="rId25" xr:uid="{14A63DAF-63A6-4B91-A2AF-AE28EA251457}"/>
+    <hyperlink ref="B148" r:id="rId26" xr:uid="{4ACA7C7F-E42A-4687-A776-AB8065DB40FF}"/>
+    <hyperlink ref="B144" r:id="rId27" xr:uid="{B3421391-7EC0-4253-8F62-5ED45A5BFA02}"/>
+    <hyperlink ref="B149" r:id="rId28" xr:uid="{F6A45FC7-B73C-4143-9CAB-B3ADA19B5FD7}"/>
+    <hyperlink ref="B146" r:id="rId29" xr:uid="{BBD267CB-7407-4913-9D05-6A6AA380019F}"/>
+    <hyperlink ref="B151" r:id="rId30" xr:uid="{85368858-6D0F-4ABE-975C-AE5530342445}"/>
+    <hyperlink ref="B143" r:id="rId31" xr:uid="{8B5BC1F5-14D4-45A0-B224-31FAF227EAF3}"/>
+    <hyperlink ref="B150" r:id="rId32" xr:uid="{D5FB3BFE-F0A8-4C09-90A1-9F506EF0ADE4}"/>
+    <hyperlink ref="B147" r:id="rId33" xr:uid="{11598046-2AED-42E7-ACA5-251A20A59427}"/>
     <hyperlink ref="B18" r:id="rId34" xr:uid="{DD499110-DFB7-4D1A-B234-8AA2514ADD29}"/>
-    <hyperlink ref="B50" r:id="rId35" xr:uid="{A1C90F9B-FBBF-4C72-9A11-3798F692A0D2}"/>
-    <hyperlink ref="B51" r:id="rId36" xr:uid="{F7B6503D-1F84-47C4-B87E-BDA7159D1B9F}"/>
-    <hyperlink ref="B46" r:id="rId37" xr:uid="{D0EE43E7-C3F5-4256-99AE-DDCA9EC11DCF}"/>
-    <hyperlink ref="B42" r:id="rId38" xr:uid="{1C25970A-A568-4869-A34A-5C6C7551D812}"/>
-    <hyperlink ref="B127" r:id="rId39" xr:uid="{C3A06396-38CD-486E-9F4F-233A79292B4F}"/>
+    <hyperlink ref="B52" r:id="rId35" xr:uid="{A1C90F9B-FBBF-4C72-9A11-3798F692A0D2}"/>
+    <hyperlink ref="B53" r:id="rId36" xr:uid="{F7B6503D-1F84-47C4-B87E-BDA7159D1B9F}"/>
+    <hyperlink ref="B49" r:id="rId37" xr:uid="{D0EE43E7-C3F5-4256-99AE-DDCA9EC11DCF}"/>
+    <hyperlink ref="B47" r:id="rId38" xr:uid="{1C25970A-A568-4869-A34A-5C6C7551D812}"/>
+    <hyperlink ref="B128" r:id="rId39" xr:uid="{C3A06396-38CD-486E-9F4F-233A79292B4F}"/>
     <hyperlink ref="B95" r:id="rId40" xr:uid="{B83625D8-44D2-4842-9139-F29C8D5F2D8E}"/>
-    <hyperlink ref="B128" r:id="rId41" xr:uid="{5FF32E6A-C6C7-4793-8271-BD230B9C7641}"/>
-    <hyperlink ref="B52" r:id="rId42" xr:uid="{E5739E03-9FE4-4D05-90C8-36ABF7D078CB}"/>
+    <hyperlink ref="B129" r:id="rId41" xr:uid="{5FF32E6A-C6C7-4793-8271-BD230B9C7641}"/>
+    <hyperlink ref="B54" r:id="rId42" xr:uid="{E5739E03-9FE4-4D05-90C8-36ABF7D078CB}"/>
     <hyperlink ref="B10" r:id="rId43" xr:uid="{F2359CF1-2AD9-4995-B3BE-132C87B2B53D}"/>
-    <hyperlink ref="B53" r:id="rId44" xr:uid="{25285F59-771C-40DB-8B78-E1E454C61406}"/>
-    <hyperlink ref="B138" r:id="rId45" xr:uid="{C000061C-001D-4088-90A4-B672D181D3C5}"/>
+    <hyperlink ref="B55" r:id="rId44" xr:uid="{25285F59-771C-40DB-8B78-E1E454C61406}"/>
+    <hyperlink ref="B139" r:id="rId45" xr:uid="{C000061C-001D-4088-90A4-B672D181D3C5}"/>
     <hyperlink ref="B27" r:id="rId46" xr:uid="{98C5B53F-658C-427A-AF31-B4D604AF2D15}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6658,27 +6438,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED149DB-8F62-4CB2-88E6-87DDBD9316FC}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -6701,22 +6481,22 @@
         <v>341</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>291</v>
       </c>
@@ -6727,22 +6507,22 @@
         <v>292</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>334</v>
       </c>
@@ -6761,8 +6541,32 @@
       <c r="G10" t="s">
         <v>339</v>
       </c>
-      <c r="H10" s="26">
+      <c r="H10" s="13">
         <v>44599</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>349</v>
+      </c>
+      <c r="E11" t="s">
+        <v>336</v>
+      </c>
+      <c r="F11" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>352</v>
+      </c>
+      <c r="I13" t="s">
+        <v>353</v>
       </c>
     </row>
   </sheetData>
@@ -6775,13 +6579,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60F650EA-F83A-4483-B12E-DBBE9EC4FA2A}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6825,6 +6629,30 @@
         <v>331</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>356</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>357</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>358</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" location="Main!A1" display="Main" xr:uid="{D25979DB-5EBB-4C30-9F58-BD318CF0CEE3}"/>

</xml_diff>

<commit_message>
a few new ones, TMO
</commit_message>
<xml_diff>
--- a/Biopharma.xlsx
+++ b/Biopharma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16243105-8E6D-48CA-8964-F18BD2C60D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3004547-AE53-422B-8B12-9012266C0449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="77910" yWindow="750" windowWidth="25035" windowHeight="19590" xr2:uid="{17641224-F2C3-441B-B85B-BB32567FE633}"/>
+    <workbookView xWindow="25440" yWindow="1050" windowWidth="16080" windowHeight="19590" xr2:uid="{17641224-F2C3-441B-B85B-BB32567FE633}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="386">
   <si>
     <t>Exarta</t>
   </si>
@@ -1182,6 +1182,72 @@
   </si>
   <si>
     <t>CYDY</t>
+  </si>
+  <si>
+    <t>Celltrion</t>
+  </si>
+  <si>
+    <t>068270 KS</t>
+  </si>
+  <si>
+    <t>Vifor</t>
+  </si>
+  <si>
+    <t>VIFN SW</t>
+  </si>
+  <si>
+    <t>Divi Labs</t>
+  </si>
+  <si>
+    <t>DIVI IN</t>
+  </si>
+  <si>
+    <t>CSPC</t>
+  </si>
+  <si>
+    <t>1093 HK</t>
+  </si>
+  <si>
+    <t>Yunnan Baiyao</t>
+  </si>
+  <si>
+    <t>000538 CH</t>
+  </si>
+  <si>
+    <t>Cipla</t>
+  </si>
+  <si>
+    <t>CIPLA</t>
+  </si>
+  <si>
+    <t>Recordati</t>
+  </si>
+  <si>
+    <t>REC IM</t>
+  </si>
+  <si>
+    <t>Ipsen</t>
+  </si>
+  <si>
+    <t>IPN</t>
+  </si>
+  <si>
+    <t>SK Bioscience</t>
+  </si>
+  <si>
+    <t>302440 KS</t>
+  </si>
+  <si>
+    <t>Shanghai Junshi</t>
+  </si>
+  <si>
+    <t>1877 HK</t>
+  </si>
+  <si>
+    <t>Orion</t>
+  </si>
+  <si>
+    <t>ORNBV FH</t>
   </si>
 </sst>
 </file>
@@ -1234,7 +1300,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1271,6 +1337,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1700,6 +1767,93 @@
       <sheetName val="Master"/>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
+      <sheetName val="Biktarvy"/>
+      <sheetName val="Descovy"/>
+      <sheetName val="Genvoya"/>
+      <sheetName val="Veklury"/>
+      <sheetName val="Stribild"/>
+      <sheetName val="Trodelvy"/>
+      <sheetName val="Truvada"/>
+      <sheetName val="Viread"/>
+      <sheetName val="Ranexa"/>
+      <sheetName val="Atripla"/>
+      <sheetName val="Harvoni"/>
+      <sheetName val="IMS Monthly"/>
+      <sheetName val="IMS"/>
+      <sheetName val="Rx"/>
+      <sheetName val="HBV"/>
+      <sheetName val="darusentan"/>
+      <sheetName val="Letairis"/>
+      <sheetName val="Hepsera"/>
+      <sheetName val="HIV"/>
+      <sheetName val="GS 9137"/>
+      <sheetName val="GS 9132"/>
+      <sheetName val="GS9190"/>
+      <sheetName val="sofosbuvir"/>
+      <sheetName val="idelasilib"/>
+      <sheetName val="GS 9451"/>
+      <sheetName val="Cayston"/>
+      <sheetName val="Tamiflu"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1">
+        <row r="3">
+          <cell r="J3">
+            <v>1253.3673940000001</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="J5">
+            <v>7000</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="J6">
+            <v>26216</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink14.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Master"/>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
       <sheetName val="Advair"/>
       <sheetName val="Relovair"/>
       <sheetName val="Consumer"/>
@@ -1819,93 +1973,6 @@
       <sheetData sheetId="49" refreshError="1"/>
       <sheetData sheetId="50" refreshError="1"/>
       <sheetData sheetId="51" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink14.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Master"/>
-      <sheetName val="Main"/>
-      <sheetName val="Model"/>
-      <sheetName val="Biktarvy"/>
-      <sheetName val="Descovy"/>
-      <sheetName val="Genvoya"/>
-      <sheetName val="Veklury"/>
-      <sheetName val="Stribild"/>
-      <sheetName val="Trodelvy"/>
-      <sheetName val="Truvada"/>
-      <sheetName val="Viread"/>
-      <sheetName val="Ranexa"/>
-      <sheetName val="Atripla"/>
-      <sheetName val="Harvoni"/>
-      <sheetName val="IMS Monthly"/>
-      <sheetName val="IMS"/>
-      <sheetName val="Rx"/>
-      <sheetName val="HBV"/>
-      <sheetName val="darusentan"/>
-      <sheetName val="Letairis"/>
-      <sheetName val="Hepsera"/>
-      <sheetName val="HIV"/>
-      <sheetName val="GS 9137"/>
-      <sheetName val="GS 9132"/>
-      <sheetName val="GS9190"/>
-      <sheetName val="sofosbuvir"/>
-      <sheetName val="idelasilib"/>
-      <sheetName val="GS 9451"/>
-      <sheetName val="Cayston"/>
-      <sheetName val="Tamiflu"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1">
-        <row r="3">
-          <cell r="J3">
-            <v>1253.3673940000001</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="J5">
-            <v>7000</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="J6">
-            <v>26216</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3774,13 +3841,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3750AF13-821E-4BF9-92BC-DEDDF3C9498E}">
-  <dimension ref="A1:AC158"/>
+  <dimension ref="A1:AC169"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I19" sqref="I19"/>
+      <selection pane="bottomRight" activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3801,14 +3868,14 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B1" s="1">
-        <f ca="1">RANDBETWEEN(1,B145)</f>
-        <v>23</v>
+        <f ca="1">RANDBETWEEN(1,B156)</f>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="K2" s="9">
         <f>MIN(K4:K24)</f>
-        <v>44792</v>
+        <v>44804</v>
       </c>
       <c r="Q2" s="15" t="s">
         <v>321</v>
@@ -4004,7 +4071,7 @@
         <v>344</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" ref="B6:B69" si="1">B5+1</f>
+        <f t="shared" ref="B6:B80" si="1">B5+1</f>
         <v>3</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -4545,7 +4612,7 @@
         <v>76330.07429460001</v>
       </c>
       <c r="G17" s="6">
-        <f>+[14]Main!$J$5-[14]Main!$J$6</f>
+        <f>+[13]Main!$J$5-[13]Main!$J$6</f>
         <v>-19216</v>
       </c>
       <c r="H17" s="6">
@@ -4553,7 +4620,7 @@
         <v>95546.07429460001</v>
       </c>
       <c r="I17" s="6">
-        <f>+[14]Main!$J$3</f>
+        <f>+[13]Main!$J$3</f>
         <v>1253.3673940000001</v>
       </c>
       <c r="J17" s="3" t="s">
@@ -4585,7 +4652,7 @@
         <v>62427.75</v>
       </c>
       <c r="G18" s="6">
-        <f>([13]Main!$K$6-[13]Main!$K$7)*GBP</f>
+        <f>([14]Main!$K$6-[14]Main!$K$7)*GBP</f>
         <v>-22956.02</v>
       </c>
       <c r="H18" s="6">
@@ -4593,14 +4660,14 @@
         <v>85383.77</v>
       </c>
       <c r="I18" s="6">
-        <f>+[13]Main!$K$4</f>
+        <f>+[14]Main!$K$4</f>
         <v>4025</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>16</v>
       </c>
       <c r="K18" s="9">
-        <v>44792</v>
+        <v>44821</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -4625,7 +4692,7 @@
         <v>63478.365159999994</v>
       </c>
       <c r="G19" s="6">
-        <f>([13]Main!$K$6-[13]Main!$K$7)*GBP</f>
+        <f>([14]Main!$K$6-[14]Main!$K$7)*GBP</f>
         <v>-22956.02</v>
       </c>
       <c r="H19" s="6">
@@ -4633,7 +4700,7 @@
         <v>86434.385159999991</v>
       </c>
       <c r="I19" s="6">
-        <f>+[13]Main!$K$4</f>
+        <f>+[14]Main!$K$4</f>
         <v>4025</v>
       </c>
       <c r="J19" s="3" t="s">
@@ -4641,7 +4708,7 @@
       </c>
       <c r="K19" s="9">
         <f>+K18</f>
-        <v>44792</v>
+        <v>44821</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -5196,44 +5263,27 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E44" s="3">
-        <v>76.08</v>
-      </c>
+      <c r="C44" s="16" t="s">
+        <v>364</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>365</v>
+      </c>
+      <c r="E44" s="6"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B45" s="1">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="C45" s="5" t="s">
-        <v>50</v>
+      <c r="C45" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="E45" s="3">
-        <v>71.27</v>
-      </c>
-      <c r="F45" s="6">
-        <f>+E45*[22]Main!$K$3</f>
-        <v>15786.66213397</v>
-      </c>
-      <c r="G45" s="6">
-        <f>+[22]Main!$K$5-[22]Main!$K$6</f>
-        <v>2721</v>
-      </c>
-      <c r="H45" s="6">
-        <f>F45-G45</f>
-        <v>13065.66213397</v>
-      </c>
-      <c r="J45" s="3" t="s">
-        <v>16</v>
+        <v>76.08</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
@@ -5242,13 +5292,28 @@
         <v>43</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="E46" s="3">
-        <v>28.54</v>
+        <v>71.27</v>
+      </c>
+      <c r="F46" s="6">
+        <f>+E46*[22]Main!$K$3</f>
+        <v>15786.66213397</v>
+      </c>
+      <c r="G46" s="6">
+        <f>+[22]Main!$K$5-[22]Main!$K$6</f>
+        <v>2721</v>
+      </c>
+      <c r="H46" s="6">
+        <f>F46-G46</f>
+        <v>13065.66213397</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
@@ -5256,14 +5321,14 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>64</v>
+      <c r="C47" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E47" s="3">
-        <v>349.96</v>
+        <v>28.54</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
@@ -5271,14 +5336,14 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="C48" s="5" t="s">
-        <v>58</v>
+      <c r="C48" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E48" s="7">
-        <v>137.09</v>
+        <v>65</v>
+      </c>
+      <c r="E48" s="3">
+        <v>349.96</v>
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.2">
@@ -5287,28 +5352,13 @@
         <v>46</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="E49" s="7">
-        <v>132.13999999999999</v>
-      </c>
-      <c r="F49" s="6">
-        <f>E49*[23]Main!$L$3</f>
-        <v>13539.443113239999</v>
-      </c>
-      <c r="G49" s="6">
-        <f>[23]Main!$L$5-[23]Main!$L$6</f>
-        <v>5643.241</v>
-      </c>
-      <c r="H49" s="6">
-        <f>F49-G49</f>
-        <v>7896.2021132399987</v>
-      </c>
-      <c r="J49" s="3" t="s">
-        <v>16</v>
+        <v>137.09</v>
       </c>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.2">
@@ -5316,14 +5366,29 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>86</v>
+      <c r="C50" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E50" s="3">
-        <v>11.57</v>
+        <v>81</v>
+      </c>
+      <c r="E50" s="7">
+        <v>132.13999999999999</v>
+      </c>
+      <c r="F50" s="6">
+        <f>E50*[23]Main!$L$3</f>
+        <v>13539.443113239999</v>
+      </c>
+      <c r="G50" s="6">
+        <f>[23]Main!$L$5-[23]Main!$L$6</f>
+        <v>5643.241</v>
+      </c>
+      <c r="H50" s="6">
+        <f>F50-G50</f>
+        <v>7896.2021132399987</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.2">
@@ -5332,13 +5397,13 @@
         <v>48</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E51" s="3">
-        <v>145.13999999999999</v>
+        <v>11.57</v>
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.2">
@@ -5346,1916 +5411,2051 @@
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C52" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E52" s="3">
+        <v>145.13999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B53" s="1">
+        <f>B80+1</f>
+        <v>75</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E53" s="3">
+        <v>82.53</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B54" s="1">
+        <f>B52+1</f>
+        <v>50</v>
+      </c>
+      <c r="C54" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E52" s="7">
+      <c r="E54" s="7">
         <v>219.38</v>
       </c>
-      <c r="F52" s="6">
-        <f>E52*[24]Main!$K$3</f>
+      <c r="F54" s="6">
+        <f>E54*[24]Main!$K$3</f>
         <v>10464.426000000001</v>
       </c>
-      <c r="G52" s="6">
+      <c r="G54" s="6">
         <f>[24]Main!$K$5-[24]Main!$K$6</f>
         <v>3027</v>
       </c>
-      <c r="H52" s="6">
-        <f>F52-G52</f>
+      <c r="H54" s="6">
+        <f>F54-G54</f>
         <v>7437.4260000000013</v>
       </c>
-      <c r="J52" s="3" t="s">
+      <c r="J54" s="3" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B53" s="1">
-        <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E53" s="7">
-        <v>57</v>
-      </c>
-      <c r="F53" s="6">
-        <f>+E53*[25]Main!$L$3</f>
-        <v>6071.7436259999995</v>
-      </c>
-      <c r="G53" s="6">
-        <f>+[25]Main!$L$5-[25]Main!$L$6</f>
-        <v>776.13</v>
-      </c>
-      <c r="H53" s="6">
-        <f>+F53-G53</f>
-        <v>5295.6136259999994</v>
-      </c>
-      <c r="J53" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B54" s="1">
-        <f t="shared" si="1"/>
-        <v>51</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="D54" t="s">
-        <v>361</v>
-      </c>
-      <c r="E54" s="3">
-        <v>3.42</v>
-      </c>
-      <c r="F54" s="6">
-        <f>+E54*I54</f>
-        <v>2379.9056977800001</v>
-      </c>
-      <c r="G54" s="6">
-        <f>+[26]Main!$K$5-[26]Main!$K$6</f>
-        <v>1840.732</v>
-      </c>
-      <c r="H54" s="6">
-        <f>+F54-G54</f>
-        <v>539.17369778000011</v>
-      </c>
-      <c r="I54" s="6">
-        <f>+[26]Main!$K$3</f>
-        <v>695.87885900000003</v>
-      </c>
-      <c r="J54" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="K54" s="9">
-        <v>44816</v>
       </c>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B55" s="1">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="D55" t="s">
-        <v>306</v>
-      </c>
-      <c r="E55" s="6">
-        <v>1721.48</v>
+        <v>136</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E55" s="7">
+        <v>57</v>
       </c>
       <c r="F55" s="6">
-        <f>+E55*I55/100*GBP</f>
-        <v>4746.2735717200003</v>
+        <f>+E55*[25]Main!$L$3</f>
+        <v>6071.7436259999995</v>
       </c>
       <c r="G55" s="6">
-        <f>+[27]Main!$K$5-[27]Main!$K$6</f>
-        <v>-337</v>
+        <f>+[25]Main!$L$5-[25]Main!$L$6</f>
+        <v>776.13</v>
       </c>
       <c r="H55" s="6">
         <f>+F55-G55</f>
-        <v>5083.2735717200003</v>
-      </c>
-      <c r="I55" s="6">
-        <f>+[27]Main!$K$3</f>
-        <v>233</v>
+        <v>5295.6136259999994</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B56" s="1">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>139</v>
+        <v>360</v>
+      </c>
+      <c r="D56" t="s">
+        <v>361</v>
       </c>
       <c r="E56" s="3">
-        <v>28.03</v>
+        <v>3.42</v>
       </c>
       <c r="F56" s="6">
-        <f>+I56*E56</f>
-        <v>4604.0473282500006</v>
+        <f>+E56*I56</f>
+        <v>2379.9056977800001</v>
       </c>
       <c r="G56" s="6">
-        <f>+[28]Main!$L$5-[28]Main!$L$6</f>
-        <v>465.44</v>
+        <f>+[26]Main!$K$5-[26]Main!$K$6</f>
+        <v>1840.732</v>
       </c>
       <c r="H56" s="6">
         <f>+F56-G56</f>
-        <v>4138.607328250001</v>
+        <v>539.17369778000011</v>
       </c>
       <c r="I56" s="6">
-        <f>+[28]Main!$L$3</f>
-        <v>164.25427500000001</v>
+        <f>+[26]Main!$K$3</f>
+        <v>695.87885900000003</v>
       </c>
       <c r="J56" s="3" t="s">
         <v>310</v>
       </c>
       <c r="K56" s="9">
-        <v>44782</v>
+        <v>44816</v>
       </c>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B57" s="1">
         <f t="shared" si="1"/>
-        <v>54</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E57" s="3">
-        <v>93.28</v>
+        <v>53</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="D57" t="s">
+        <v>306</v>
+      </c>
+      <c r="E57" s="6">
+        <v>1721.48</v>
+      </c>
+      <c r="F57" s="6">
+        <f>+E57*I57/100*GBP</f>
+        <v>4746.2735717200003</v>
+      </c>
+      <c r="G57" s="6">
+        <f>+[27]Main!$K$5-[27]Main!$K$6</f>
+        <v>-337</v>
+      </c>
+      <c r="H57" s="6">
+        <f>+F57-G57</f>
+        <v>5083.2735717200003</v>
+      </c>
+      <c r="I57" s="6">
+        <f>+[27]Main!$K$3</f>
+        <v>233</v>
+      </c>
+      <c r="J57" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B58" s="1">
         <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>94</v>
+        <v>54</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>138</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>95</v>
+        <v>139</v>
       </c>
       <c r="E58" s="3">
-        <v>142.91</v>
+        <v>28.03</v>
+      </c>
+      <c r="F58" s="6">
+        <f>+I58*E58</f>
+        <v>4604.0473282500006</v>
+      </c>
+      <c r="G58" s="6">
+        <f>+[28]Main!$L$5-[28]Main!$L$6</f>
+        <v>465.44</v>
+      </c>
+      <c r="H58" s="6">
+        <f>+F58-G58</f>
+        <v>4138.607328250001</v>
+      </c>
+      <c r="I58" s="6">
+        <f>+[28]Main!$L$3</f>
+        <v>164.25427500000001</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="K58" s="9">
+        <v>44782</v>
       </c>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B59" s="1">
         <f t="shared" si="1"/>
-        <v>56</v>
-      </c>
-      <c r="C59" t="s">
-        <v>279</v>
-      </c>
-      <c r="D59" t="s">
-        <v>279</v>
+        <v>55</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E59" s="3">
+        <v>93.28</v>
       </c>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B60" s="1">
         <f t="shared" si="1"/>
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E60" s="3">
-        <v>7.71</v>
+        <v>376</v>
+      </c>
+      <c r="D60" s="16" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B61" s="1">
-        <f t="shared" si="1"/>
-        <v>58</v>
-      </c>
-      <c r="C61" t="s">
-        <v>284</v>
-      </c>
-      <c r="D61" t="s">
-        <v>285</v>
+        <f>B59+1</f>
+        <v>56</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E61" s="3">
+        <v>142.91</v>
       </c>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B62" s="1">
         <f t="shared" si="1"/>
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C62" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D62" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B63" s="1">
         <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="C63" t="s">
-        <v>280</v>
-      </c>
-      <c r="D63" t="s">
-        <v>281</v>
+        <v>58</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E63" s="3">
+        <v>7.71</v>
       </c>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B64" s="1">
         <f t="shared" si="1"/>
-        <v>61</v>
-      </c>
-      <c r="C64" t="s">
-        <v>277</v>
-      </c>
-      <c r="D64" t="s">
-        <v>278</v>
+        <v>59</v>
+      </c>
+      <c r="C64" s="16" t="s">
+        <v>380</v>
+      </c>
+      <c r="D64" s="16" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B65" s="1">
         <f t="shared" si="1"/>
-        <v>62</v>
-      </c>
-      <c r="C65" t="s">
-        <v>261</v>
-      </c>
-      <c r="D65" t="s">
-        <v>262</v>
+        <v>60</v>
+      </c>
+      <c r="C65" s="16" t="s">
+        <v>382</v>
+      </c>
+      <c r="D65" s="16" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B66" s="1">
         <f t="shared" si="1"/>
-        <v>63</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E66" s="3">
-        <v>11.04</v>
+        <v>61</v>
+      </c>
+      <c r="C66" s="16" t="s">
+        <v>384</v>
+      </c>
+      <c r="D66" s="16" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B67" s="1">
         <f t="shared" si="1"/>
-        <v>64</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E67" s="3">
-        <v>44.14</v>
+        <v>62</v>
+      </c>
+      <c r="C67" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="D67" s="16" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B68" s="1">
         <f t="shared" si="1"/>
-        <v>65</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E68" s="3">
-        <v>35.26</v>
+        <v>63</v>
+      </c>
+      <c r="C68" t="s">
+        <v>284</v>
+      </c>
+      <c r="D68" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B69" s="1">
         <f t="shared" si="1"/>
-        <v>66</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E69" s="3">
-        <v>82.53</v>
+        <v>64</v>
+      </c>
+      <c r="C69" t="s">
+        <v>366</v>
+      </c>
+      <c r="D69" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B70" s="1">
-        <f t="shared" ref="B70:B133" si="4">B69+1</f>
-        <v>67</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E70" s="3">
-        <v>24.78</v>
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="C70" t="s">
+        <v>370</v>
+      </c>
+      <c r="D70" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B71" s="1">
-        <f t="shared" si="4"/>
-        <v>68</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E71" s="3">
-        <v>4.72</v>
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="C71" t="s">
+        <v>372</v>
+      </c>
+      <c r="D71" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B72" s="1">
-        <f t="shared" si="4"/>
-        <v>69</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E72" s="3">
-        <v>24.53</v>
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+      <c r="C72" t="s">
+        <v>368</v>
+      </c>
+      <c r="D72" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B73" s="1">
-        <f t="shared" si="4"/>
-        <v>70</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E73" s="3">
-        <v>23.02</v>
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="C73" t="s">
+        <v>282</v>
+      </c>
+      <c r="D73" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B74" s="1">
-        <f t="shared" si="4"/>
-        <v>71</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E74" s="3">
-        <v>29.12</v>
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="C74" t="s">
+        <v>280</v>
+      </c>
+      <c r="D74" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B75" s="1">
-        <f t="shared" si="4"/>
-        <v>72</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E75" s="3">
-        <v>33.17</v>
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="C75" t="s">
+        <v>277</v>
+      </c>
+      <c r="D75" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B76" s="1">
-        <f t="shared" si="4"/>
-        <v>73</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E76" s="3">
-        <v>53.21</v>
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="C76" t="s">
+        <v>374</v>
+      </c>
+      <c r="D76" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B77" s="1">
-        <f t="shared" si="4"/>
-        <v>74</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E77" s="3">
-        <v>46.23</v>
+        <f>B75+1</f>
+        <v>71</v>
+      </c>
+      <c r="C77" t="s">
+        <v>261</v>
+      </c>
+      <c r="D77" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B78" s="1">
-        <f t="shared" si="4"/>
-        <v>75</v>
+        <f t="shared" si="1"/>
+        <v>72</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E78" s="7">
-        <v>70</v>
+        <v>99</v>
+      </c>
+      <c r="E78" s="3">
+        <v>11.04</v>
       </c>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B79" s="1">
-        <f t="shared" si="4"/>
-        <v>76</v>
+        <f t="shared" si="1"/>
+        <v>73</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="E79" s="3">
-        <v>18.559999999999999</v>
+        <v>44.14</v>
       </c>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B80" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E80" s="3">
+        <v>35.26</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B81" s="1">
+        <f>B53+1</f>
+        <v>76</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E81" s="3">
+        <v>24.78</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B82" s="1">
+        <f t="shared" ref="B82:B144" si="4">B81+1</f>
         <v>77</v>
       </c>
-      <c r="C80" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E80" s="3">
-        <v>15.75</v>
-      </c>
-    </row>
-    <row r="81" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B81" s="1">
+      <c r="C82" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E82" s="3">
+        <v>4.72</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B83" s="1">
         <f t="shared" si="4"/>
         <v>78</v>
       </c>
-      <c r="C81" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E81" s="3">
-        <v>19.510000000000002</v>
-      </c>
-    </row>
-    <row r="82" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B82" s="1">
+      <c r="C83" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E83" s="3">
+        <v>24.53</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B84" s="1">
         <f t="shared" si="4"/>
         <v>79</v>
       </c>
-      <c r="C82" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E82" s="3">
-        <v>66.97</v>
-      </c>
-    </row>
-    <row r="83" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B83" s="1">
+      <c r="C84" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E84" s="3">
+        <v>23.02</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B85" s="1">
         <f t="shared" si="4"/>
         <v>80</v>
       </c>
-      <c r="C83" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E83" s="3">
-        <v>54.94</v>
-      </c>
-    </row>
-    <row r="84" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B84" s="1">
+      <c r="C85" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E85" s="3">
+        <v>29.12</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B86" s="1">
         <f t="shared" si="4"/>
         <v>81</v>
       </c>
-      <c r="C84" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E84" s="3">
-        <v>38.840000000000003</v>
-      </c>
-    </row>
-    <row r="85" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B85" s="1">
+      <c r="C86" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E86" s="3">
+        <v>33.17</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B87" s="1">
         <f t="shared" si="4"/>
         <v>82</v>
       </c>
-      <c r="C85" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E85" s="3">
-        <v>83.92</v>
-      </c>
-    </row>
-    <row r="86" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B86" s="1">
+      <c r="C87" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E87" s="3">
+        <v>53.21</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B88" s="1">
         <f t="shared" si="4"/>
         <v>83</v>
       </c>
-      <c r="C86" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E86" s="3">
-        <v>60.72</v>
-      </c>
-    </row>
-    <row r="87" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B87" s="1">
+      <c r="C88" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E88" s="3">
+        <v>46.23</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B89" s="1">
         <f t="shared" si="4"/>
         <v>84</v>
       </c>
-      <c r="C87" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E87" s="7">
-        <v>12.2</v>
-      </c>
-    </row>
-    <row r="88" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B88" s="1">
+      <c r="C89" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E89" s="7">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B90" s="1">
         <f t="shared" si="4"/>
         <v>85</v>
       </c>
-      <c r="C88" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E88" s="3">
-        <v>2.37</v>
-      </c>
-    </row>
-    <row r="89" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B89" s="1">
+      <c r="C90" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E90" s="3">
+        <v>18.559999999999999</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B91" s="1">
         <f t="shared" si="4"/>
         <v>86</v>
       </c>
-      <c r="C89" t="s">
-        <v>316</v>
-      </c>
-      <c r="D89" t="s">
-        <v>317</v>
-      </c>
-      <c r="E89" s="3">
-        <v>4.26</v>
-      </c>
-      <c r="AC89" s="1">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="90" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B90" s="1">
+      <c r="C91" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E91" s="3">
+        <v>15.75</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B92" s="1">
         <f t="shared" si="4"/>
         <v>87</v>
       </c>
-      <c r="C90" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E90" s="3">
-        <v>42.98</v>
-      </c>
-    </row>
-    <row r="91" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B91" s="1">
+      <c r="C92" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E92" s="3">
+        <v>19.510000000000002</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B93" s="1">
         <f t="shared" si="4"/>
         <v>88</v>
       </c>
-      <c r="C91" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E91" s="3">
-        <v>23.92</v>
-      </c>
-    </row>
-    <row r="92" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B92" s="1">
+      <c r="C93" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E93" s="3">
+        <v>66.97</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B94" s="1">
         <f t="shared" si="4"/>
         <v>89</v>
       </c>
-      <c r="C92" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E92" s="3">
-        <v>53.29</v>
-      </c>
-    </row>
-    <row r="93" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B93" s="1">
+      <c r="C94" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E94" s="3">
+        <v>54.94</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B95" s="1">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
-      <c r="C93" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E93" s="3">
-        <v>74.459999999999994</v>
-      </c>
-    </row>
-    <row r="94" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B94" s="1">
+      <c r="C95" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E95" s="3">
+        <v>38.840000000000003</v>
+      </c>
+    </row>
+    <row r="96" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B96" s="1">
         <f t="shared" si="4"/>
         <v>91</v>
       </c>
-      <c r="C94" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E94" s="3">
-        <v>48.63</v>
-      </c>
-    </row>
-    <row r="95" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B95" s="1">
+      <c r="C96" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E96" s="3">
+        <v>83.92</v>
+      </c>
+    </row>
+    <row r="97" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="B97" s="1">
         <f t="shared" si="4"/>
         <v>92</v>
       </c>
-      <c r="C95" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E95" s="3">
-        <v>27.73</v>
-      </c>
-    </row>
-    <row r="96" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B96" s="1">
+      <c r="C97" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E97" s="3">
+        <v>60.72</v>
+      </c>
+    </row>
+    <row r="98" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="B98" s="1">
         <f t="shared" si="4"/>
         <v>93</v>
       </c>
-      <c r="C96" s="5" t="s">
+      <c r="C98" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E98" s="7">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="99" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="B99" s="1">
+        <f t="shared" si="4"/>
+        <v>94</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E99" s="3">
+        <v>2.37</v>
+      </c>
+    </row>
+    <row r="100" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="B100" s="1">
+        <f t="shared" si="4"/>
+        <v>95</v>
+      </c>
+      <c r="C100" t="s">
+        <v>316</v>
+      </c>
+      <c r="D100" t="s">
+        <v>317</v>
+      </c>
+      <c r="E100" s="3">
+        <v>4.26</v>
+      </c>
+      <c r="AC100" s="1">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="101" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="B101" s="1">
+        <f t="shared" si="4"/>
+        <v>96</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E101" s="3">
+        <v>42.98</v>
+      </c>
+    </row>
+    <row r="102" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="B102" s="1">
+        <f t="shared" si="4"/>
+        <v>97</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E102" s="3">
+        <v>23.92</v>
+      </c>
+    </row>
+    <row r="103" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="B103" s="1">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E103" s="3">
+        <v>53.29</v>
+      </c>
+    </row>
+    <row r="104" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="B104" s="1">
+        <f t="shared" si="4"/>
+        <v>99</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E104" s="3">
+        <v>74.459999999999994</v>
+      </c>
+    </row>
+    <row r="105" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="B105" s="1">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E105" s="3">
+        <v>48.63</v>
+      </c>
+    </row>
+    <row r="106" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="B106" s="1">
+        <f t="shared" si="4"/>
+        <v>101</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E106" s="3">
+        <v>27.73</v>
+      </c>
+    </row>
+    <row r="107" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="B107" s="1">
+        <f t="shared" si="4"/>
+        <v>102</v>
+      </c>
+      <c r="C107" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="D96" s="1" t="s">
+      <c r="D107" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="E96" s="3">
+      <c r="E107" s="3">
         <v>10.119999999999999</v>
       </c>
-      <c r="F96" s="6">
-        <f>+E96*[29]Main!$N$3</f>
+      <c r="F107" s="6">
+        <f>+E107*[29]Main!$N$3</f>
         <v>3152.1980120399994</v>
       </c>
-      <c r="G96" s="6">
+      <c r="G107" s="6">
         <f>+[29]Main!$N$5-[29]Main!$N$6</f>
         <v>869.93499999999995</v>
       </c>
-      <c r="H96" s="6">
-        <f>+F96-G96</f>
+      <c r="H107" s="6">
+        <f>+F107-G107</f>
         <v>2282.2630120399995</v>
       </c>
-      <c r="J96" s="3" t="s">
+      <c r="J107" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B97" s="1">
-        <f t="shared" si="4"/>
-        <v>94</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E97" s="3">
-        <v>35.770000000000003</v>
-      </c>
-    </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B98" s="1">
-        <f t="shared" si="4"/>
-        <v>95</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E98" s="3">
-        <v>14.27</v>
-      </c>
-    </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B99" s="1">
-        <f t="shared" si="4"/>
-        <v>96</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="E99" s="3">
-        <v>7.36</v>
-      </c>
-    </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B100" s="1">
-        <f t="shared" si="4"/>
-        <v>97</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E100" s="3">
-        <v>9.35</v>
-      </c>
-    </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B101" s="1">
-        <f t="shared" si="4"/>
-        <v>98</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E101" s="3">
-        <v>43.98</v>
-      </c>
-    </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B102" s="1">
-        <f t="shared" si="4"/>
-        <v>99</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E102" s="3">
-        <v>5.18</v>
-      </c>
-    </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B103" s="1">
-        <f t="shared" si="4"/>
-        <v>100</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="E103" s="3">
-        <v>53.72</v>
-      </c>
-    </row>
-    <row r="104" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B104" s="1">
-        <f t="shared" si="4"/>
-        <v>101</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="E104" s="3">
-        <v>21.04</v>
-      </c>
-    </row>
-    <row r="105" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B105" s="1">
-        <f t="shared" si="4"/>
-        <v>102</v>
-      </c>
-      <c r="C105" t="s">
-        <v>318</v>
-      </c>
-      <c r="D105" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="106" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B106" s="1">
+    <row r="108" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="B108" s="1">
         <f t="shared" si="4"/>
         <v>103</v>
       </c>
-      <c r="C106" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="E106" s="7">
-        <v>20.7</v>
-      </c>
-    </row>
-    <row r="107" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B107" s="1">
+      <c r="C108" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E108" s="3">
+        <v>35.770000000000003</v>
+      </c>
+    </row>
+    <row r="109" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="B109" s="1">
         <f t="shared" si="4"/>
         <v>104</v>
       </c>
-      <c r="C107" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E107" s="3">
-        <v>18.579999999999998</v>
-      </c>
-    </row>
-    <row r="108" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B108" s="1">
+      <c r="C109" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E109" s="3">
+        <v>14.27</v>
+      </c>
+    </row>
+    <row r="110" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="B110" s="1">
         <f t="shared" si="4"/>
         <v>105</v>
       </c>
-      <c r="C108" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E108" s="3">
-        <v>16.12</v>
-      </c>
-    </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B109" s="1">
+      <c r="C110" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E110" s="3">
+        <v>7.36</v>
+      </c>
+    </row>
+    <row r="111" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="B111" s="1">
         <f t="shared" si="4"/>
         <v>106</v>
       </c>
-      <c r="C109" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="E109" s="3">
-        <v>28.41</v>
-      </c>
-    </row>
-    <row r="110" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B110" s="1">
+      <c r="C111" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E111" s="3">
+        <v>9.35</v>
+      </c>
+    </row>
+    <row r="112" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="B112" s="1">
         <f t="shared" si="4"/>
         <v>107</v>
       </c>
-      <c r="C110" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="E110" s="3">
-        <v>33.86</v>
-      </c>
-    </row>
-    <row r="111" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B111" s="1">
-        <f t="shared" si="4"/>
-        <v>108</v>
-      </c>
-      <c r="C111" t="s">
-        <v>353</v>
-      </c>
-      <c r="D111" t="s">
-        <v>354</v>
-      </c>
-      <c r="E111" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="112" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B112" s="1">
-        <f t="shared" si="4"/>
-        <v>109</v>
-      </c>
       <c r="C112" s="1" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="E112" s="3">
-        <v>38.35</v>
+        <v>43.98</v>
       </c>
     </row>
     <row r="113" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B113" s="1">
         <f t="shared" si="4"/>
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>301</v>
+        <v>172</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="E113" s="3">
-        <v>9.6199999999999992</v>
+        <v>5.18</v>
       </c>
     </row>
     <row r="114" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B114" s="1">
         <f t="shared" si="4"/>
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="E114" s="3">
-        <v>25.49</v>
+        <v>53.72</v>
       </c>
     </row>
     <row r="115" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B115" s="1">
         <f t="shared" si="4"/>
-        <v>112</v>
-      </c>
-      <c r="C115" t="s">
-        <v>299</v>
-      </c>
-      <c r="D115" t="s">
-        <v>300</v>
+        <v>110</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E115" s="3">
+        <v>21.04</v>
       </c>
     </row>
     <row r="116" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B116" s="1">
         <f t="shared" si="4"/>
-        <v>113</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="E116" s="3">
-        <v>11.42</v>
+        <v>111</v>
+      </c>
+      <c r="C116" t="s">
+        <v>318</v>
+      </c>
+      <c r="D116" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="117" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B117" s="1">
         <f t="shared" si="4"/>
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E117" s="3">
-        <v>26.64</v>
+        <v>179</v>
+      </c>
+      <c r="E117" s="7">
+        <v>20.7</v>
       </c>
     </row>
     <row r="118" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B118" s="1">
         <f t="shared" si="4"/>
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="E118" s="3">
-        <v>30.48</v>
+        <v>18.579999999999998</v>
       </c>
     </row>
     <row r="119" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B119" s="1">
         <f t="shared" si="4"/>
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="E119" s="3">
-        <v>12.98</v>
+        <v>16.12</v>
       </c>
     </row>
     <row r="120" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B120" s="1">
         <f t="shared" si="4"/>
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="E120" s="3">
-        <v>10.96</v>
+        <v>28.41</v>
       </c>
     </row>
     <row r="121" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B121" s="1">
         <f t="shared" si="4"/>
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="E121" s="3">
-        <v>2.42</v>
+        <v>33.86</v>
       </c>
     </row>
     <row r="122" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B122" s="1">
         <f t="shared" si="4"/>
-        <v>119</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>206</v>
+        <v>117</v>
+      </c>
+      <c r="C122" t="s">
+        <v>353</v>
+      </c>
+      <c r="D122" t="s">
+        <v>354</v>
       </c>
       <c r="E122" s="7">
-        <v>55.5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="123" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B123" s="1">
         <f t="shared" si="4"/>
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
       <c r="E123" s="3">
-        <v>10.63</v>
+        <v>38.35</v>
       </c>
     </row>
     <row r="124" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B124" s="1">
         <f t="shared" si="4"/>
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>209</v>
+        <v>301</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="E124" s="3">
-        <v>33.130000000000003</v>
+        <v>9.6199999999999992</v>
       </c>
     </row>
     <row r="125" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B125" s="1">
         <f t="shared" si="4"/>
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="E125" s="3">
-        <v>31.52</v>
+        <v>25.49</v>
       </c>
     </row>
     <row r="126" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B126" s="1">
         <f t="shared" si="4"/>
-        <v>123</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="E126" s="3">
-        <v>7.62</v>
+        <v>121</v>
+      </c>
+      <c r="C126" t="s">
+        <v>299</v>
+      </c>
+      <c r="D126" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="127" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B127" s="1">
         <f t="shared" si="4"/>
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>215</v>
+        <v>193</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>216</v>
+        <v>194</v>
       </c>
       <c r="E127" s="3">
-        <v>28.55</v>
+        <v>11.42</v>
       </c>
     </row>
     <row r="128" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B128" s="1">
         <f t="shared" si="4"/>
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>217</v>
+        <v>195</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>218</v>
+        <v>196</v>
       </c>
       <c r="E128" s="3">
-        <v>27.02</v>
+        <v>26.64</v>
       </c>
     </row>
     <row r="129" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B129" s="1">
         <f t="shared" si="4"/>
-        <v>126</v>
-      </c>
-      <c r="C129" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="D129" t="s">
-        <v>297</v>
+        <v>124</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="E129" s="3">
-        <v>15.65</v>
-      </c>
-      <c r="F129" s="6">
-        <f>E129*[30]Main!$L$3</f>
-        <v>1253.1559559500001</v>
-      </c>
-      <c r="G129" s="6">
-        <f>+[30]Main!$L$5-[30]Main!$L$6</f>
-        <v>112.015</v>
-      </c>
-      <c r="H129" s="6">
-        <f>+F129-G129</f>
-        <v>1141.14095595</v>
-      </c>
-      <c r="J129" s="3" t="s">
-        <v>16</v>
+        <v>30.48</v>
       </c>
     </row>
     <row r="130" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B130" s="1">
         <f t="shared" si="4"/>
-        <v>127</v>
-      </c>
-      <c r="C130" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="D130" t="s">
-        <v>308</v>
+        <v>125</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>200</v>
       </c>
       <c r="E130" s="3">
-        <v>16.93</v>
-      </c>
-      <c r="F130" s="6">
-        <f>+E130*[31]Main!$L$3</f>
-        <v>1228.5485933099999</v>
-      </c>
-      <c r="G130" s="6">
-        <f>+[31]Main!$L$5-[31]Main!$L$6</f>
-        <v>153.25991400000001</v>
-      </c>
-      <c r="H130" s="6">
-        <f>+F130-G130</f>
-        <v>1075.2886793099999</v>
-      </c>
-      <c r="J130" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K130" s="9">
-        <v>44771</v>
-      </c>
-      <c r="L130" s="9"/>
-      <c r="M130" s="9"/>
-      <c r="N130" s="9"/>
-      <c r="O130" s="9"/>
-      <c r="P130" s="9"/>
+        <v>12.98</v>
+      </c>
     </row>
     <row r="131" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B131" s="1">
         <f t="shared" si="4"/>
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="E131" s="3">
-        <v>3.17</v>
+        <v>10.96</v>
       </c>
     </row>
     <row r="132" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B132" s="1">
         <f t="shared" si="4"/>
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="E132" s="3">
-        <v>8.76</v>
+        <v>2.42</v>
       </c>
     </row>
     <row r="133" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B133" s="1">
         <f t="shared" si="4"/>
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="E133" s="3">
-        <v>18.010000000000002</v>
+        <v>206</v>
+      </c>
+      <c r="E133" s="7">
+        <v>55.5</v>
       </c>
     </row>
     <row r="134" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B134" s="1">
-        <f t="shared" ref="B134:B158" si="5">B133+1</f>
-        <v>131</v>
-      </c>
-      <c r="C134" t="s">
-        <v>313</v>
-      </c>
-      <c r="D134" t="s">
-        <v>314</v>
+        <f t="shared" si="4"/>
+        <v>129</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>208</v>
       </c>
       <c r="E134" s="3">
-        <v>3.92</v>
-      </c>
-      <c r="F134" s="3">
-        <v>630</v>
+        <v>10.63</v>
       </c>
     </row>
     <row r="135" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B135" s="1">
-        <f t="shared" si="5"/>
-        <v>132</v>
-      </c>
-      <c r="C135" t="s">
-        <v>311</v>
-      </c>
-      <c r="D135" t="s">
-        <v>312</v>
+        <f t="shared" si="4"/>
+        <v>130</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>210</v>
       </c>
       <c r="E135" s="3">
-        <v>11.93</v>
-      </c>
-      <c r="F135" s="3">
-        <v>516</v>
+        <v>33.130000000000003</v>
       </c>
     </row>
     <row r="136" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B136" s="1">
-        <f t="shared" si="5"/>
-        <v>133</v>
+        <f t="shared" si="4"/>
+        <v>131</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="E136" s="3">
-        <v>5.46</v>
+        <v>31.52</v>
       </c>
     </row>
     <row r="137" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B137" s="1">
-        <f t="shared" si="5"/>
-        <v>134</v>
+        <f t="shared" si="4"/>
+        <v>132</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="E137" s="7">
-        <v>36.6</v>
+        <v>214</v>
+      </c>
+      <c r="E137" s="3">
+        <v>7.62</v>
       </c>
     </row>
     <row r="138" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B138" s="1">
-        <f t="shared" si="5"/>
-        <v>135</v>
+        <f t="shared" si="4"/>
+        <v>133</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="E138" s="7">
-        <v>40.24</v>
+        <v>216</v>
+      </c>
+      <c r="E138" s="3">
+        <v>28.55</v>
       </c>
     </row>
     <row r="139" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B139" s="1">
-        <f t="shared" si="5"/>
-        <v>136</v>
+        <f t="shared" si="4"/>
+        <v>134</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="E139" s="3">
-        <v>22.11</v>
+        <v>27.02</v>
       </c>
     </row>
     <row r="140" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B140" s="1">
-        <f t="shared" si="5"/>
-        <v>137</v>
+        <f t="shared" si="4"/>
+        <v>135</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>331</v>
+        <v>296</v>
       </c>
       <c r="D140" t="s">
-        <v>332</v>
+        <v>297</v>
       </c>
       <c r="E140" s="3">
-        <v>3.95</v>
+        <v>15.65</v>
       </c>
       <c r="F140" s="6">
-        <f>+E140*I140</f>
-        <v>37.185714749999995</v>
+        <f>E140*[30]Main!$L$3</f>
+        <v>1253.1559559500001</v>
       </c>
       <c r="G140" s="6">
-        <f>+[32]Main!$N$5-[32]Main!$N$6</f>
-        <v>-7.4640000000000004</v>
+        <f>+[30]Main!$L$5-[30]Main!$L$6</f>
+        <v>112.015</v>
       </c>
       <c r="H140" s="6">
         <f>+F140-G140</f>
-        <v>44.649714749999994</v>
-      </c>
-      <c r="I140" s="6">
-        <f>+[32]Main!$N$3</f>
-        <v>9.4141049999999993</v>
+        <v>1141.14095595</v>
       </c>
       <c r="J140" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="K140" s="9">
-        <v>44780</v>
+        <v>16</v>
       </c>
     </row>
     <row r="141" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B141" s="1">
-        <f t="shared" si="5"/>
-        <v>138</v>
-      </c>
-      <c r="C141" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="D141" s="1" t="s">
-        <v>234</v>
+        <f t="shared" si="4"/>
+        <v>136</v>
+      </c>
+      <c r="C141" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="D141" t="s">
+        <v>308</v>
       </c>
       <c r="E141" s="3">
-        <v>10.31</v>
-      </c>
+        <v>16.93</v>
+      </c>
+      <c r="F141" s="6">
+        <f>+E141*[31]Main!$L$3</f>
+        <v>1228.5485933099999</v>
+      </c>
+      <c r="G141" s="6">
+        <f>+[31]Main!$L$5-[31]Main!$L$6</f>
+        <v>153.25991400000001</v>
+      </c>
+      <c r="H141" s="6">
+        <f>+F141-G141</f>
+        <v>1075.2886793099999</v>
+      </c>
+      <c r="J141" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K141" s="9">
+        <v>44771</v>
+      </c>
+      <c r="L141" s="9"/>
+      <c r="M141" s="9"/>
+      <c r="N141" s="9"/>
+      <c r="O141" s="9"/>
+      <c r="P141" s="9"/>
     </row>
     <row r="142" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B142" s="1">
-        <f t="shared" si="5"/>
-        <v>139</v>
+        <f t="shared" si="4"/>
+        <v>137</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="E142" s="7">
-        <v>1.3</v>
+        <v>220</v>
+      </c>
+      <c r="E142" s="3">
+        <v>3.17</v>
       </c>
     </row>
     <row r="143" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B143" s="1">
-        <f t="shared" si="5"/>
-        <v>140</v>
+        <f t="shared" si="4"/>
+        <v>138</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
       <c r="E143" s="3">
-        <v>3.35</v>
+        <v>8.76</v>
       </c>
     </row>
     <row r="144" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B144" s="1">
-        <f t="shared" si="5"/>
-        <v>141</v>
-      </c>
-      <c r="C144" s="5" t="s">
-        <v>239</v>
+        <f t="shared" si="4"/>
+        <v>139</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>223</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
       <c r="E144" s="3">
-        <v>7.06</v>
-      </c>
-      <c r="F144" s="6">
-        <f>E144*[33]Main!$J$3</f>
-        <v>725.62786605999997</v>
-      </c>
-      <c r="G144" s="6">
-        <f>[33]Main!$J$5-[33]Main!$J$6</f>
-        <v>197.79600000000002</v>
-      </c>
-      <c r="H144" s="8">
-        <f>+F144-G144</f>
-        <v>527.83186605999992</v>
-      </c>
-      <c r="J144" s="3" t="s">
-        <v>16</v>
+        <v>18.010000000000002</v>
       </c>
     </row>
     <row r="145" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B145" s="1">
-        <f t="shared" si="5"/>
-        <v>142</v>
-      </c>
-      <c r="C145" s="5" t="s">
-        <v>362</v>
-      </c>
-      <c r="D145" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="E145" s="7">
-        <v>0.6</v>
-      </c>
-      <c r="F145" s="6">
-        <f>+E145*I145</f>
-        <v>486.43225439999998</v>
-      </c>
-      <c r="G145" s="6">
-        <f>+[34]Main!$K$5-[34]Main!$K$6</f>
-        <v>-37.984000000000002</v>
-      </c>
-      <c r="H145" s="8">
-        <f t="shared" ref="H145" si="6">+F145-G145</f>
-        <v>524.41625439999996</v>
-      </c>
-      <c r="I145" s="6">
-        <f>+[34]Main!$K$3</f>
-        <v>810.72042399999998</v>
-      </c>
-      <c r="J145" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="K145" s="9">
-        <v>44816</v>
-      </c>
-      <c r="AC145" s="1">
-        <v>2002</v>
+        <f t="shared" ref="B145:B169" si="5">B144+1</f>
+        <v>140</v>
+      </c>
+      <c r="C145" t="s">
+        <v>313</v>
+      </c>
+      <c r="D145" t="s">
+        <v>314</v>
+      </c>
+      <c r="E145" s="3">
+        <v>3.92</v>
+      </c>
+      <c r="F145" s="3">
+        <v>630</v>
       </c>
     </row>
     <row r="146" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B146" s="1">
         <f t="shared" si="5"/>
-        <v>143</v>
-      </c>
-      <c r="C146" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="D146" s="1" t="s">
-        <v>242</v>
+        <v>141</v>
+      </c>
+      <c r="C146" t="s">
+        <v>311</v>
+      </c>
+      <c r="D146" t="s">
+        <v>312</v>
       </c>
       <c r="E146" s="3">
-        <v>14.68</v>
-      </c>
-      <c r="F146" s="6">
-        <f>E146*[35]Main!$L$3</f>
-        <v>587.26396075999992</v>
-      </c>
-      <c r="G146" s="6">
-        <f>[35]Main!$L$5-[35]Main!$L$6</f>
-        <v>277.88299999999998</v>
-      </c>
-      <c r="H146" s="8">
-        <f>+F146-G146</f>
-        <v>309.38096075999994</v>
-      </c>
-      <c r="J146" s="3" t="s">
-        <v>16</v>
+        <v>11.93</v>
+      </c>
+      <c r="F146" s="3">
+        <v>516</v>
       </c>
     </row>
     <row r="147" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B147" s="1">
         <f t="shared" si="5"/>
-        <v>144</v>
-      </c>
-      <c r="C147" s="5" t="s">
-        <v>243</v>
+        <v>142</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>225</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="E147" s="3">
-        <v>4.8600000000000003</v>
-      </c>
-      <c r="F147" s="6">
-        <f>E147*[36]Main!$J$3</f>
-        <v>312.71415336000001</v>
-      </c>
-      <c r="G147" s="8">
-        <f>+[36]Main!$J$5-[36]Main!$J$6</f>
-        <v>92.317999999999998</v>
-      </c>
-      <c r="H147" s="8">
-        <f>+F147-G147</f>
-        <v>220.39615336000003</v>
-      </c>
-      <c r="J147" s="3" t="s">
-        <v>16</v>
+        <v>5.46</v>
       </c>
     </row>
     <row r="148" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B148" s="1">
         <f t="shared" si="5"/>
-        <v>145</v>
-      </c>
-      <c r="C148" s="5" t="s">
-        <v>245</v>
+        <v>143</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>227</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="E148" s="3">
-        <v>7.57</v>
-      </c>
-      <c r="F148" s="6">
-        <f>E148*[37]Main!$M$3</f>
-        <v>338.45983246000003</v>
-      </c>
-      <c r="G148" s="6">
-        <f>[37]Main!$M$5-[37]Main!$M$6</f>
-        <v>120.43700000000001</v>
-      </c>
-      <c r="H148" s="8">
-        <f t="shared" ref="H148:H153" si="7">+F148-G148</f>
-        <v>218.02283246000002</v>
-      </c>
-      <c r="J148" s="3" t="s">
-        <v>16</v>
+        <v>228</v>
+      </c>
+      <c r="E148" s="7">
+        <v>36.6</v>
       </c>
     </row>
     <row r="149" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B149" s="1">
         <f t="shared" si="5"/>
-        <v>146</v>
-      </c>
-      <c r="C149" s="5" t="s">
-        <v>247</v>
+        <v>144</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>229</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
       <c r="E149" s="7">
-        <v>0.7</v>
-      </c>
-      <c r="F149" s="6">
-        <f>E149*[38]Main!$M$3</f>
-        <v>128.9392503</v>
-      </c>
-      <c r="G149" s="6">
-        <f>[38]Main!$M$5-[38]Main!$M$6</f>
-        <v>-59.50200000000001</v>
-      </c>
-      <c r="H149" s="8">
-        <f t="shared" si="7"/>
-        <v>188.44125030000001</v>
-      </c>
-      <c r="J149" s="3" t="s">
-        <v>16</v>
+        <v>40.24</v>
       </c>
     </row>
     <row r="150" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B150" s="1">
         <f t="shared" si="5"/>
-        <v>147</v>
-      </c>
-      <c r="C150" s="5" t="s">
-        <v>249</v>
+        <v>145</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>231</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="E150" s="3">
-        <v>1.98</v>
-      </c>
-      <c r="F150" s="6">
-        <f>E150*[39]Main!$N$3</f>
-        <v>39.757463459999997</v>
-      </c>
-      <c r="G150" s="6">
-        <f>[39]Main!$N$5-[39]Main!$N$6</f>
-        <v>15.942</v>
-      </c>
-      <c r="H150" s="8">
-        <f t="shared" si="7"/>
-        <v>23.815463459999997</v>
-      </c>
-      <c r="J150" s="3" t="s">
-        <v>16</v>
+        <v>22.11</v>
       </c>
     </row>
     <row r="151" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B151" s="1">
         <f t="shared" si="5"/>
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C151" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="D151" s="1" t="s">
-        <v>252</v>
+        <v>331</v>
+      </c>
+      <c r="D151" t="s">
+        <v>332</v>
       </c>
       <c r="E151" s="3">
-        <v>0.62</v>
+        <v>3.95</v>
       </c>
       <c r="F151" s="6">
-        <f>E151*[40]Main!$L$3</f>
-        <v>30.1881658</v>
+        <f>+E151*I151</f>
+        <v>37.185714749999995</v>
       </c>
       <c r="G151" s="6">
-        <f>[40]Main!$L$5-[40]Main!$L$6</f>
-        <v>13.262999999999998</v>
-      </c>
-      <c r="H151" s="8">
-        <f t="shared" si="7"/>
-        <v>16.925165800000002</v>
+        <f>+[32]Main!$N$5-[32]Main!$N$6</f>
+        <v>-7.4640000000000004</v>
+      </c>
+      <c r="H151" s="6">
+        <f>+F151-G151</f>
+        <v>44.649714749999994</v>
+      </c>
+      <c r="I151" s="6">
+        <f>+[32]Main!$N$3</f>
+        <v>9.4141049999999993</v>
       </c>
       <c r="J151" s="3" t="s">
-        <v>16</v>
+        <v>310</v>
+      </c>
+      <c r="K151" s="9">
+        <v>44780</v>
       </c>
     </row>
     <row r="152" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B152" s="1">
         <f t="shared" si="5"/>
-        <v>149</v>
-      </c>
-      <c r="C152" s="5" t="s">
-        <v>253</v>
+        <v>147</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>233</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>254</v>
+        <v>234</v>
       </c>
       <c r="E152" s="3">
-        <v>6.12</v>
-      </c>
-      <c r="F152" s="6">
-        <f>E152*[41]Main!$M$3</f>
-        <v>125.46108324000001</v>
-      </c>
-      <c r="G152" s="6">
-        <f>[41]Main!$M$5-[41]Main!$M$6</f>
-        <v>131.17699999999999</v>
-      </c>
-      <c r="H152" s="8">
-        <f t="shared" si="7"/>
-        <v>-5.7159167599999847</v>
-      </c>
-      <c r="J152" s="3" t="s">
-        <v>16</v>
+        <v>10.31</v>
       </c>
     </row>
     <row r="153" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B153" s="1">
         <f t="shared" si="5"/>
-        <v>150</v>
-      </c>
-      <c r="C153" s="5" t="s">
-        <v>255</v>
+        <v>148</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>235</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="E153" s="3">
-        <v>0.98</v>
-      </c>
-      <c r="F153" s="6">
-        <f>E153*[42]Main!$M$3</f>
-        <v>20.935517539999999</v>
-      </c>
-      <c r="G153" s="6">
-        <f>[42]Main!$M$5-[42]Main!$M$6</f>
-        <v>55.28</v>
-      </c>
-      <c r="H153" s="8">
-        <f t="shared" si="7"/>
-        <v>-34.344482460000002</v>
-      </c>
-      <c r="J153" s="3" t="s">
-        <v>16</v>
+        <v>236</v>
+      </c>
+      <c r="E153" s="7">
+        <v>1.3</v>
       </c>
     </row>
     <row r="154" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B154" s="1">
         <f t="shared" si="5"/>
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="E154" s="3">
-        <v>0.61</v>
+        <v>3.35</v>
       </c>
     </row>
     <row r="155" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B155" s="1">
         <f t="shared" si="5"/>
-        <v>152</v>
-      </c>
-      <c r="C155" s="1" t="s">
-        <v>259</v>
+        <v>150</v>
+      </c>
+      <c r="C155" s="5" t="s">
+        <v>239</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="E155" s="3">
-        <v>5.55</v>
+        <v>7.06</v>
+      </c>
+      <c r="F155" s="6">
+        <f>E155*[33]Main!$J$3</f>
+        <v>725.62786605999997</v>
+      </c>
+      <c r="G155" s="6">
+        <f>[33]Main!$J$5-[33]Main!$J$6</f>
+        <v>197.79600000000002</v>
+      </c>
+      <c r="H155" s="8">
+        <f>+F155-G155</f>
+        <v>527.83186605999992</v>
+      </c>
+      <c r="J155" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="156" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B156" s="1">
         <f t="shared" si="5"/>
-        <v>153</v>
-      </c>
-      <c r="C156" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D156" t="s">
-        <v>359</v>
+        <v>151</v>
+      </c>
+      <c r="C156" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>363</v>
       </c>
       <c r="E156" s="7">
-        <v>4.2</v>
+        <v>0.6</v>
+      </c>
+      <c r="F156" s="6">
+        <f>+E156*I156</f>
+        <v>486.43225439999998</v>
+      </c>
+      <c r="G156" s="6">
+        <f>+[34]Main!$K$5-[34]Main!$K$6</f>
+        <v>-37.984000000000002</v>
+      </c>
+      <c r="H156" s="8">
+        <f t="shared" ref="H156" si="6">+F156-G156</f>
+        <v>524.41625439999996</v>
+      </c>
+      <c r="I156" s="6">
+        <f>+[34]Main!$K$3</f>
+        <v>810.72042399999998</v>
+      </c>
+      <c r="J156" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="K156" s="9">
+        <v>44816</v>
+      </c>
+      <c r="AC156" s="1">
+        <v>2002</v>
       </c>
     </row>
     <row r="157" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B157" s="1">
         <f t="shared" si="5"/>
-        <v>154</v>
-      </c>
-      <c r="C157" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="D157" t="s">
-        <v>343</v>
-      </c>
-      <c r="E157" s="7">
-        <v>4</v>
+        <v>152</v>
+      </c>
+      <c r="C157" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E157" s="3">
+        <v>14.68</v>
+      </c>
+      <c r="F157" s="6">
+        <f>E157*[35]Main!$L$3</f>
+        <v>587.26396075999992</v>
+      </c>
+      <c r="G157" s="6">
+        <f>[35]Main!$L$5-[35]Main!$L$6</f>
+        <v>277.88299999999998</v>
+      </c>
+      <c r="H157" s="8">
+        <f>+F157-G157</f>
+        <v>309.38096075999994</v>
+      </c>
+      <c r="J157" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="158" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B158" s="1">
         <f t="shared" si="5"/>
+        <v>153</v>
+      </c>
+      <c r="C158" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="E158" s="3">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="F158" s="6">
+        <f>E158*[36]Main!$J$3</f>
+        <v>312.71415336000001</v>
+      </c>
+      <c r="G158" s="8">
+        <f>+[36]Main!$J$5-[36]Main!$J$6</f>
+        <v>92.317999999999998</v>
+      </c>
+      <c r="H158" s="8">
+        <f>+F158-G158</f>
+        <v>220.39615336000003</v>
+      </c>
+      <c r="J158" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="159" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="B159" s="1">
+        <f t="shared" si="5"/>
+        <v>154</v>
+      </c>
+      <c r="C159" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E159" s="3">
+        <v>7.57</v>
+      </c>
+      <c r="F159" s="6">
+        <f>E159*[37]Main!$M$3</f>
+        <v>338.45983246000003</v>
+      </c>
+      <c r="G159" s="6">
+        <f>[37]Main!$M$5-[37]Main!$M$6</f>
+        <v>120.43700000000001</v>
+      </c>
+      <c r="H159" s="8">
+        <f t="shared" ref="H159:H164" si="7">+F159-G159</f>
+        <v>218.02283246000002</v>
+      </c>
+      <c r="J159" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="160" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="B160" s="1">
+        <f t="shared" si="5"/>
         <v>155</v>
       </c>
-      <c r="C158" t="s">
+      <c r="C160" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E160" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="F160" s="6">
+        <f>E160*[38]Main!$M$3</f>
+        <v>128.9392503</v>
+      </c>
+      <c r="G160" s="6">
+        <f>[38]Main!$M$5-[38]Main!$M$6</f>
+        <v>-59.50200000000001</v>
+      </c>
+      <c r="H160" s="8">
+        <f t="shared" si="7"/>
+        <v>188.44125030000001</v>
+      </c>
+      <c r="J160" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="161" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B161" s="1">
+        <f t="shared" si="5"/>
+        <v>156</v>
+      </c>
+      <c r="C161" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E161" s="3">
+        <v>1.98</v>
+      </c>
+      <c r="F161" s="6">
+        <f>E161*[39]Main!$N$3</f>
+        <v>39.757463459999997</v>
+      </c>
+      <c r="G161" s="6">
+        <f>[39]Main!$N$5-[39]Main!$N$6</f>
+        <v>15.942</v>
+      </c>
+      <c r="H161" s="8">
+        <f t="shared" si="7"/>
+        <v>23.815463459999997</v>
+      </c>
+      <c r="J161" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="162" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B162" s="1">
+        <f t="shared" si="5"/>
+        <v>157</v>
+      </c>
+      <c r="C162" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E162" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="F162" s="6">
+        <f>E162*[40]Main!$L$3</f>
+        <v>30.1881658</v>
+      </c>
+      <c r="G162" s="6">
+        <f>[40]Main!$L$5-[40]Main!$L$6</f>
+        <v>13.262999999999998</v>
+      </c>
+      <c r="H162" s="8">
+        <f t="shared" si="7"/>
+        <v>16.925165800000002</v>
+      </c>
+      <c r="J162" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="163" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B163" s="1">
+        <f t="shared" si="5"/>
+        <v>158</v>
+      </c>
+      <c r="C163" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E163" s="3">
+        <v>6.12</v>
+      </c>
+      <c r="F163" s="6">
+        <f>E163*[41]Main!$M$3</f>
+        <v>125.46108324000001</v>
+      </c>
+      <c r="G163" s="6">
+        <f>[41]Main!$M$5-[41]Main!$M$6</f>
+        <v>131.17699999999999</v>
+      </c>
+      <c r="H163" s="8">
+        <f t="shared" si="7"/>
+        <v>-5.7159167599999847</v>
+      </c>
+      <c r="J163" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="164" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B164" s="1">
+        <f t="shared" si="5"/>
+        <v>159</v>
+      </c>
+      <c r="C164" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="E164" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="F164" s="6">
+        <f>E164*[42]Main!$M$3</f>
+        <v>20.935517539999999</v>
+      </c>
+      <c r="G164" s="6">
+        <f>[42]Main!$M$5-[42]Main!$M$6</f>
+        <v>55.28</v>
+      </c>
+      <c r="H164" s="8">
+        <f t="shared" si="7"/>
+        <v>-34.344482460000002</v>
+      </c>
+      <c r="J164" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="165" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B165" s="1">
+        <f t="shared" si="5"/>
+        <v>160</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E165" s="3">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="166" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B166" s="1">
+        <f t="shared" si="5"/>
+        <v>161</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="E166" s="3">
+        <v>5.55</v>
+      </c>
+    </row>
+    <row r="167" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B167" s="1">
+        <f t="shared" si="5"/>
+        <v>162</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="D167" t="s">
+        <v>359</v>
+      </c>
+      <c r="E167" s="7">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="168" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B168" s="1">
+        <f t="shared" si="5"/>
+        <v>163</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D168" t="s">
+        <v>343</v>
+      </c>
+      <c r="E168" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="169" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B169" s="1">
+        <f t="shared" si="5"/>
+        <v>164</v>
+      </c>
+      <c r="C169" t="s">
         <v>346</v>
       </c>
-      <c r="D158" t="s">
+      <c r="D169" t="s">
         <v>347</v>
       </c>
-      <c r="E158" s="3">
+      <c r="E169" s="3">
         <v>20.18</v>
       </c>
     </row>
@@ -7282,38 +7482,38 @@
     <hyperlink ref="C5" r:id="rId15" xr:uid="{0888F4DA-9569-4326-990C-43015A33BD61}"/>
     <hyperlink ref="C17" r:id="rId16" xr:uid="{C2959A9B-7367-43D7-934F-562A915DC4DD}"/>
     <hyperlink ref="C22" r:id="rId17" xr:uid="{A069369A-FB97-4A4A-A581-321FA79E4250}"/>
-    <hyperlink ref="C45" r:id="rId18" xr:uid="{6EF35D30-7113-4CE8-9077-C5BE97F74D36}"/>
+    <hyperlink ref="C46" r:id="rId18" xr:uid="{6EF35D30-7113-4CE8-9077-C5BE97F74D36}"/>
     <hyperlink ref="C23" r:id="rId19" xr:uid="{1F769FA7-6B90-4B6B-9BCC-7D6679675B06}"/>
     <hyperlink ref="C27" r:id="rId20" xr:uid="{FBD4E7AC-5982-43A1-83EA-3F3AB2E91655}"/>
-    <hyperlink ref="C48" r:id="rId21" xr:uid="{53091BB6-5763-4DDE-A659-5638BD3CADCA}"/>
-    <hyperlink ref="C46" r:id="rId22" xr:uid="{10922C8B-4C13-4E76-B998-3ADD8CC60E47}"/>
+    <hyperlink ref="C49" r:id="rId21" xr:uid="{53091BB6-5763-4DDE-A659-5638BD3CADCA}"/>
+    <hyperlink ref="C47" r:id="rId22" xr:uid="{10922C8B-4C13-4E76-B998-3ADD8CC60E47}"/>
     <hyperlink ref="C28" r:id="rId23" xr:uid="{61277D68-67DC-475B-9B61-B7E2F3017110}"/>
-    <hyperlink ref="C147" r:id="rId24" xr:uid="{14A63DAF-63A6-4B91-A2AF-AE28EA251457}"/>
-    <hyperlink ref="C150" r:id="rId25" xr:uid="{4ACA7C7F-E42A-4687-A776-AB8065DB40FF}"/>
-    <hyperlink ref="C146" r:id="rId26" xr:uid="{B3421391-7EC0-4253-8F62-5ED45A5BFA02}"/>
-    <hyperlink ref="C151" r:id="rId27" xr:uid="{F6A45FC7-B73C-4143-9CAB-B3ADA19B5FD7}"/>
-    <hyperlink ref="C148" r:id="rId28" xr:uid="{BBD267CB-7407-4913-9D05-6A6AA380019F}"/>
-    <hyperlink ref="C153" r:id="rId29" xr:uid="{85368858-6D0F-4ABE-975C-AE5530342445}"/>
-    <hyperlink ref="C144" r:id="rId30" xr:uid="{8B5BC1F5-14D4-45A0-B224-31FAF227EAF3}"/>
-    <hyperlink ref="C152" r:id="rId31" xr:uid="{D5FB3BFE-F0A8-4C09-90A1-9F506EF0ADE4}"/>
-    <hyperlink ref="C149" r:id="rId32" xr:uid="{11598046-2AED-42E7-ACA5-251A20A59427}"/>
+    <hyperlink ref="C158" r:id="rId24" xr:uid="{14A63DAF-63A6-4B91-A2AF-AE28EA251457}"/>
+    <hyperlink ref="C161" r:id="rId25" xr:uid="{4ACA7C7F-E42A-4687-A776-AB8065DB40FF}"/>
+    <hyperlink ref="C157" r:id="rId26" xr:uid="{B3421391-7EC0-4253-8F62-5ED45A5BFA02}"/>
+    <hyperlink ref="C162" r:id="rId27" xr:uid="{F6A45FC7-B73C-4143-9CAB-B3ADA19B5FD7}"/>
+    <hyperlink ref="C159" r:id="rId28" xr:uid="{BBD267CB-7407-4913-9D05-6A6AA380019F}"/>
+    <hyperlink ref="C164" r:id="rId29" xr:uid="{85368858-6D0F-4ABE-975C-AE5530342445}"/>
+    <hyperlink ref="C155" r:id="rId30" xr:uid="{8B5BC1F5-14D4-45A0-B224-31FAF227EAF3}"/>
+    <hyperlink ref="C163" r:id="rId31" xr:uid="{D5FB3BFE-F0A8-4C09-90A1-9F506EF0ADE4}"/>
+    <hyperlink ref="C160" r:id="rId32" xr:uid="{11598046-2AED-42E7-ACA5-251A20A59427}"/>
     <hyperlink ref="C19" r:id="rId33" xr:uid="{DD499110-DFB7-4D1A-B234-8AA2514ADD29}"/>
-    <hyperlink ref="C52" r:id="rId34" xr:uid="{A1C90F9B-FBBF-4C72-9A11-3798F692A0D2}"/>
-    <hyperlink ref="C53" r:id="rId35" xr:uid="{F7B6503D-1F84-47C4-B87E-BDA7159D1B9F}"/>
-    <hyperlink ref="C49" r:id="rId36" xr:uid="{D0EE43E7-C3F5-4256-99AE-DDCA9EC11DCF}"/>
+    <hyperlink ref="C54" r:id="rId34" xr:uid="{A1C90F9B-FBBF-4C72-9A11-3798F692A0D2}"/>
+    <hyperlink ref="C55" r:id="rId35" xr:uid="{F7B6503D-1F84-47C4-B87E-BDA7159D1B9F}"/>
+    <hyperlink ref="C50" r:id="rId36" xr:uid="{D0EE43E7-C3F5-4256-99AE-DDCA9EC11DCF}"/>
     <hyperlink ref="C25" r:id="rId37" xr:uid="{1C25970A-A568-4869-A34A-5C6C7551D812}"/>
-    <hyperlink ref="C129" r:id="rId38" xr:uid="{C3A06396-38CD-486E-9F4F-233A79292B4F}"/>
-    <hyperlink ref="C96" r:id="rId39" xr:uid="{B83625D8-44D2-4842-9139-F29C8D5F2D8E}"/>
-    <hyperlink ref="C130" r:id="rId40" xr:uid="{5FF32E6A-C6C7-4793-8271-BD230B9C7641}"/>
-    <hyperlink ref="C55" r:id="rId41" xr:uid="{E5739E03-9FE4-4D05-90C8-36ABF7D078CB}"/>
-    <hyperlink ref="C56" r:id="rId42" xr:uid="{25285F59-771C-40DB-8B78-E1E454C61406}"/>
-    <hyperlink ref="C140" r:id="rId43" xr:uid="{C000061C-001D-4088-90A4-B672D181D3C5}"/>
+    <hyperlink ref="C140" r:id="rId38" xr:uid="{C3A06396-38CD-486E-9F4F-233A79292B4F}"/>
+    <hyperlink ref="C107" r:id="rId39" xr:uid="{B83625D8-44D2-4842-9139-F29C8D5F2D8E}"/>
+    <hyperlink ref="C141" r:id="rId40" xr:uid="{5FF32E6A-C6C7-4793-8271-BD230B9C7641}"/>
+    <hyperlink ref="C57" r:id="rId41" xr:uid="{E5739E03-9FE4-4D05-90C8-36ABF7D078CB}"/>
+    <hyperlink ref="C58" r:id="rId42" xr:uid="{25285F59-771C-40DB-8B78-E1E454C61406}"/>
+    <hyperlink ref="C151" r:id="rId43" xr:uid="{C000061C-001D-4088-90A4-B672D181D3C5}"/>
     <hyperlink ref="C29" r:id="rId44" xr:uid="{98C5B53F-658C-427A-AF31-B4D604AF2D15}"/>
     <hyperlink ref="C24" r:id="rId45" xr:uid="{6A1F812B-EA91-4B3C-B4DC-88F792A7D0DE}"/>
     <hyperlink ref="C26" r:id="rId46" xr:uid="{6930A656-C59A-465F-8634-B30B4FEF47BC}"/>
-    <hyperlink ref="C54" r:id="rId47" xr:uid="{559FAD8A-D620-4B93-BE14-CC22630BD57E}"/>
+    <hyperlink ref="C56" r:id="rId47" xr:uid="{559FAD8A-D620-4B93-BE14-CC22630BD57E}"/>
     <hyperlink ref="C10" r:id="rId48" xr:uid="{467EEBCD-6BD7-4E71-B2C9-FCF3DB57F059}"/>
-    <hyperlink ref="C145" r:id="rId49" xr:uid="{6A576FDB-A573-4A00-8381-4BECF13B35A1}"/>
+    <hyperlink ref="C156" r:id="rId49" xr:uid="{6A576FDB-A573-4A00-8381-4BECF13B35A1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId50"/>

</xml_diff>

<commit_message>
several updates, crypto.xlsx, alzheimers, wuxi
</commit_message>
<xml_diff>
--- a/Biopharma.xlsx
+++ b/Biopharma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E632F36A-3254-4699-847A-6B68A9BB650C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4C0A69-E17D-483A-87BB-AF1632F1EA85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28605" yWindow="1440" windowWidth="22515" windowHeight="19365" xr2:uid="{17641224-F2C3-441B-B85B-BB32567FE633}"/>
+    <workbookView xWindow="24570" yWindow="1155" windowWidth="24855" windowHeight="19110" xr2:uid="{17641224-F2C3-441B-B85B-BB32567FE633}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -66,6 +66,8 @@
     <externalReference r:id="rId49"/>
     <externalReference r:id="rId50"/>
     <externalReference r:id="rId51"/>
+    <externalReference r:id="rId52"/>
+    <externalReference r:id="rId53"/>
   </externalReferences>
   <definedNames>
     <definedName name="AUD">FX!$C$5</definedName>
@@ -74,6 +76,7 @@
     <definedName name="DKKUSD">#REF!</definedName>
     <definedName name="EUR">FX!$C$4</definedName>
     <definedName name="GBP">FX!$C$6</definedName>
+    <definedName name="HKD">FX!$C$8</definedName>
     <definedName name="JPY">FX!$C$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -95,8 +98,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="413">
   <si>
     <t>Exarta</t>
   </si>
@@ -1289,9 +1314,6 @@
     <t>Meissa Vaccines</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Vivoryon</t>
   </si>
   <si>
@@ -1308,6 +1330,36 @@
   </si>
   <si>
     <t>Alzheimer's amyloid aggregation inhibitor</t>
+  </si>
+  <si>
+    <t>Aria Pharmaceuticals</t>
+  </si>
+  <si>
+    <t>FogPharma</t>
+  </si>
+  <si>
+    <t>Series C</t>
+  </si>
+  <si>
+    <t>107m</t>
+  </si>
+  <si>
+    <t>Beta-Catenin</t>
+  </si>
+  <si>
+    <t>Pasithea</t>
+  </si>
+  <si>
+    <t>KTTA</t>
+  </si>
+  <si>
+    <t>USD/HKD</t>
+  </si>
+  <si>
+    <t>Cellarity</t>
+  </si>
+  <si>
+    <t>121m</t>
   </si>
 </sst>
 </file>
@@ -1360,7 +1412,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1397,7 +1449,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1549,38 +1600,18 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
+      <sheetName val="Master"/>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
-      <sheetName val="Epo Global Model"/>
-      <sheetName val="Epo Bottoms-Up Model"/>
-      <sheetName val="EPO Pricing - Rebates"/>
-      <sheetName val="EPO Share"/>
-      <sheetName val="EPO Pricing,Reimbursement"/>
-      <sheetName val="IMS EPOs"/>
-      <sheetName val="NDC EPOs"/>
       <sheetName val="Enbrel"/>
-      <sheetName val="Enbrel Top-Down"/>
-      <sheetName val="Enbrel NDC"/>
-      <sheetName val="Enbrel IMS"/>
+      <sheetName val="Lumakras"/>
       <sheetName val="Neulasta"/>
       <sheetName val="Neupogen"/>
-      <sheetName val="G-CSF Top-Down"/>
-      <sheetName val="GCSF IMS"/>
-      <sheetName val="NDC GCSFs"/>
-      <sheetName val="IP"/>
-      <sheetName val="EPO CHF"/>
-      <sheetName val="EPO MDS"/>
-      <sheetName val="Epo Comp"/>
-      <sheetName val="Epo Science"/>
-      <sheetName val="CERA legal"/>
-      <sheetName val="CERA clinical"/>
-      <sheetName val="David Legal"/>
       <sheetName val="Epogen"/>
       <sheetName val="EPO safety"/>
       <sheetName val="Aranesp"/>
       <sheetName val="G-CSF"/>
       <sheetName val="Sensipar"/>
-      <sheetName val="Kepivance"/>
       <sheetName val="Vectibix"/>
       <sheetName val="Denosumab"/>
       <sheetName val="Denosumab trials"/>
@@ -1599,33 +1630,27 @@
       <sheetName val="208"/>
       <sheetName val="714"/>
       <sheetName val="Failures"/>
-      <sheetName val="FG-2216"/>
-      <sheetName val="Affymax"/>
-      <sheetName val="Reimbursement"/>
-      <sheetName val="MDRX Aranesp Sales"/>
-      <sheetName val="MDRX Procrit sales"/>
-      <sheetName val="Capture Rate Thesis"/>
-      <sheetName val="Management"/>
+      <sheetName val="Kepivance"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0">
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
         <row r="3">
-          <cell r="K3">
-            <v>534</v>
+          <cell r="J3">
+            <v>534.93084999999996</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="K5">
-            <v>6544</v>
+          <cell r="J5">
+            <v>7183</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="K6">
-            <v>36854</v>
+          <cell r="J6">
+            <v>36522</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
@@ -1655,32 +1680,6 @@
       <sheetData sheetId="28"/>
       <sheetData sheetId="29"/>
       <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-      <sheetData sheetId="54"/>
-      <sheetData sheetId="55"/>
-      <sheetData sheetId="56"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2077,17 +2076,17 @@
       <sheetData sheetId="0">
         <row r="3">
           <cell r="J3">
-            <v>470.117188</v>
+            <v>982.42</v>
           </cell>
         </row>
         <row r="5">
           <cell r="J5">
-            <v>10436.4</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="6">
           <cell r="J6">
-            <v>9657.7999999999993</v>
+            <v>36575</v>
           </cell>
         </row>
       </sheetData>
@@ -2098,6 +2097,37 @@
 </file>
 
 <file path=xl/externalLinks/externalLink17.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="J3">
+            <v>470.117188</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="J5">
+            <v>10436.4</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="J6">
+            <v>9657.7999999999993</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink18.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2146,7 +2176,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink19.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2199,7 +2229,46 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Master"/>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+      <sheetName val="Humira"/>
+      <sheetName val="Rinvoq"/>
+      <sheetName val="Skyrizi"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="3">
+          <cell r="K3">
+            <v>1768.096495</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="K5">
+            <v>10205</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="K6">
+            <v>72932</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink20.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2244,46 +2313,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Master"/>
-      <sheetName val="Main"/>
-      <sheetName val="Model"/>
-      <sheetName val="Humira"/>
-      <sheetName val="Rinvoq"/>
-      <sheetName val="Skyrizi"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="3">
-          <cell r="K3">
-            <v>1768.096495</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="K5">
-            <v>10205</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="K6">
-            <v>72932</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink21.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2304,37 +2334,6 @@
         </row>
         <row r="6">
           <cell r="J6">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink21.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Main"/>
-      <sheetName val="Model"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="L3">
-            <v>391.199544</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="L5">
-            <v>18059</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="L6">
             <v>0</v>
           </cell>
         </row>
@@ -2355,18 +2354,18 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="M3">
-            <v>1212.5809400000001</v>
+          <cell r="L3">
+            <v>391.199544</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="M5">
-            <v>752.4</v>
+          <cell r="L5">
+            <v>18059</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="M6">
-            <v>19417.900000000001</v>
+          <cell r="L6">
+            <v>0</v>
           </cell>
         </row>
       </sheetData>
@@ -2382,6 +2381,37 @@
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="M3">
+            <v>1212.5809400000001</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="M5">
+            <v>752.4</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="M6">
+            <v>19417.900000000001</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink24.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
       <sheetName val="Comirnaty"/>
     </sheetNames>
     <sheetDataSet>
@@ -2409,7 +2439,38 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink25.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="J3">
+            <v>4263.5283170000002</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="J5">
+            <v>10082.542000000001</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="J6">
+            <v>2347.1640000000002</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink26.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2476,7 +2537,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink27.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2507,7 +2568,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink28.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2546,7 +2607,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink29.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2574,72 +2635,6 @@
       </sheetData>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink28.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Main"/>
-      <sheetName val="Model"/>
-      <sheetName val="Vtama"/>
-      <sheetName val="brepocitinib"/>
-      <sheetName val="IP"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="K3">
-            <v>695.87885900000003</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="K5">
-            <v>2257.7559999999999</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="K6">
-            <v>417.024</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink29.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Main"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="K3">
-            <v>233</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="K5">
-            <v>426</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="K6">
-            <v>763</v>
-          </cell>
-        </row>
-      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2753,6 +2748,72 @@
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
+      <sheetName val="Vtama"/>
+      <sheetName val="brepocitinib"/>
+      <sheetName val="IP"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="K3">
+            <v>695.87885900000003</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="K5">
+            <v>2257.7559999999999</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="K6">
+            <v>417.024</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink31.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="K3">
+            <v>233</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="K5">
+            <v>426</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="K6">
+            <v>763</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink32.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
       <sheetName val="Consta"/>
       <sheetName val="Vivitrol"/>
       <sheetName val="nemvaleukin"/>
@@ -2792,7 +2853,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink33.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2813,66 +2874,6 @@
         </row>
         <row r="6">
           <cell r="N6">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink32.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Main"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="K3">
-            <v>70.354594000000006</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="K5">
-            <v>1178.8610000000001</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="K6">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink33.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Main"/>
-      <sheetName val="nirogacestat"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="J3">
-            <v>58.068182</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="J5">
-            <v>566.44900000000007</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="J6">
             <v>0</v>
           </cell>
         </row>
@@ -2888,6 +2889,66 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="K3">
+            <v>70.354594000000006</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="K5">
+            <v>1178.8610000000001</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="K6">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink35.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="nirogacestat"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="J3">
+            <v>58.068182</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="J5">
+            <v>566.44900000000007</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="J6">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink36.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
       <sheetName val="sabizabulin"/>
     </sheetNames>
     <sheetDataSet>
@@ -2914,7 +2975,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink37.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2955,7 +3016,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink38.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2979,78 +3040,6 @@
           </cell>
         </row>
       </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink37.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Main"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="N3">
-            <v>9.4141049999999993</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="N5">
-            <v>11.249000000000001</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="N6">
-            <v>18.713000000000001</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink38.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Main"/>
-      <sheetName val="Model"/>
-      <sheetName val="CPP-115 Model"/>
-      <sheetName val="LEMS"/>
-      <sheetName val="Firdapse"/>
-      <sheetName val="Ampyra"/>
-      <sheetName val="CPP-115"/>
-      <sheetName val="CPP-109"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="J3">
-            <v>102.780151</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="J5">
-            <v>197.79600000000002</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="J6">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3065,18 +3054,18 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="K3">
-            <v>810.72042399999998</v>
+          <cell r="N3">
+            <v>9.4141049999999993</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="K5">
-            <v>4.2309999999999999</v>
+          <cell r="N5">
+            <v>11.249000000000001</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="K6">
-            <v>42.215000000000003</v>
+          <cell r="N6">
+            <v>18.713000000000001</v>
           </cell>
         </row>
       </sheetData>
@@ -3169,25 +3158,39 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
+      <sheetName val="Model"/>
+      <sheetName val="CPP-115 Model"/>
+      <sheetName val="LEMS"/>
+      <sheetName val="Firdapse"/>
+      <sheetName val="Ampyra"/>
+      <sheetName val="CPP-115"/>
+      <sheetName val="CPP-109"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="L3">
-            <v>40.004356999999999</v>
+          <cell r="J3">
+            <v>102.780151</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="L5">
-            <v>277.88299999999998</v>
+          <cell r="J5">
+            <v>197.79600000000002</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="L6">
+          <cell r="J6">
             <v>0</v>
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3198,31 +3201,25 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
-      <sheetName val="Model"/>
-      <sheetName val="Yutrepia"/>
-      <sheetName val="Generic"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="J3">
-            <v>64.344476</v>
+          <cell r="K3">
+            <v>810.72042399999998</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="J5">
-            <v>111.794</v>
+          <cell r="K5">
+            <v>4.2309999999999999</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="J6">
-            <v>19.475999999999999</v>
+          <cell r="K6">
+            <v>42.215000000000003</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3237,17 +3234,17 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="M3">
-            <v>44.710678000000001</v>
+          <cell r="L3">
+            <v>40.004356999999999</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="M5">
-            <v>120.43700000000001</v>
+          <cell r="L5">
+            <v>277.88299999999998</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="M6">
+          <cell r="L6">
             <v>0</v>
           </cell>
         </row>
@@ -3262,25 +3259,31 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
+      <sheetName val="Model"/>
+      <sheetName val="Yutrepia"/>
+      <sheetName val="Generic"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="M3">
-            <v>184.19892899999999</v>
+          <cell r="J3">
+            <v>64.344476</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="M5">
-            <v>67.233999999999995</v>
+          <cell r="J5">
+            <v>111.794</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="M6">
-            <v>126.736</v>
+          <cell r="J6">
+            <v>19.475999999999999</v>
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3295,18 +3298,18 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="N3">
-            <v>20.079526999999999</v>
+          <cell r="M3">
+            <v>44.710678000000001</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="N5">
-            <v>16.64</v>
+          <cell r="M5">
+            <v>120.43700000000001</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="N6">
-            <v>0.69799999999999995</v>
+          <cell r="M6">
+            <v>0</v>
           </cell>
         </row>
       </sheetData>
@@ -3324,18 +3327,18 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="L3">
-            <v>48.69059</v>
+          <cell r="M3">
+            <v>184.19892899999999</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="L5">
-            <v>18.687999999999999</v>
+          <cell r="M5">
+            <v>67.233999999999995</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="L6">
-            <v>5.4249999999999998</v>
+          <cell r="M6">
+            <v>126.736</v>
           </cell>
         </row>
       </sheetData>
@@ -3353,18 +3356,18 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="M3">
-            <v>20.500177000000001</v>
+          <cell r="N3">
+            <v>20.079526999999999</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="M5">
-            <v>131.17699999999999</v>
+          <cell r="N5">
+            <v>16.64</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="M6">
-            <v>0</v>
+          <cell r="N6">
+            <v>0.69799999999999995</v>
           </cell>
         </row>
       </sheetData>
@@ -3374,6 +3377,64 @@
 </file>
 
 <file path=xl/externalLinks/externalLink47.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="L3">
+            <v>48.69059</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="L5">
+            <v>18.687999999999999</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="L6">
+            <v>5.4249999999999998</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink48.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="M3">
+            <v>20.500177000000001</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="M5">
+            <v>131.17699999999999</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="M6">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink49.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -3735,7 +3796,7 @@
       <sheetName val="brivanib"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1">
         <row r="3">
           <cell r="K3">
@@ -3753,25 +3814,25 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4074,13 +4135,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3750AF13-821E-4BF9-92BC-DEDDF3C9498E}">
-  <dimension ref="A1:AC175"/>
+  <dimension ref="A1:AC176"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J22" sqref="J22"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4089,7 +4150,7 @@
     <col min="2" max="2" width="4.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8" style="3" customWidth="1"/>
     <col min="6" max="8" width="9.140625" style="3"/>
     <col min="9" max="9" width="7.42578125" style="3" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="3"/>
@@ -4102,7 +4163,7 @@
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B1" s="1">
         <f ca="1">RANDBETWEEN(1,B160)</f>
-        <v>119</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
@@ -4700,7 +4761,7 @@
         <v>310</v>
       </c>
       <c r="K13" s="9">
-        <v>44810</v>
+        <v>44839</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.2">
@@ -4718,29 +4779,29 @@
         <v>35</v>
       </c>
       <c r="E14" s="7">
-        <v>246.73</v>
+        <v>230.55</v>
       </c>
       <c r="F14" s="6">
         <f>+E14*I14</f>
-        <v>131753.82</v>
+        <v>123328.3074675</v>
       </c>
       <c r="G14" s="6">
-        <f>[10]Main!$K$5-[10]Main!$K$6</f>
-        <v>-30310</v>
+        <f>[10]Main!$J$5-[10]Main!$J$6</f>
+        <v>-29339</v>
       </c>
       <c r="H14" s="6">
         <f t="shared" si="0"/>
-        <v>162063.82</v>
+        <v>152667.30746749998</v>
       </c>
       <c r="I14" s="6">
-        <f>+[10]Main!$K$3</f>
-        <v>534</v>
+        <f>+[10]Main!$J$3</f>
+        <v>534.93084999999996</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>16</v>
+        <v>310</v>
       </c>
       <c r="K14" s="9">
-        <v>44810</v>
+        <v>44837</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.2">
@@ -4769,7 +4830,7 @@
         <v>-12400.887000000001</v>
       </c>
       <c r="H15" s="6">
-        <f t="shared" ref="H15:H27" si="3">F15-G15</f>
+        <f t="shared" ref="H15:H28" si="3">F15-G15</f>
         <v>135499.28700000001</v>
       </c>
       <c r="I15" s="6">
@@ -4823,7 +4884,7 @@
         <v>44812</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>344</v>
       </c>
@@ -4863,7 +4924,7 @@
         <v>44819</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>344</v>
       </c>
@@ -4903,7 +4964,7 @@
         <v>44821</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>344</v>
       </c>
@@ -4944,7 +5005,7 @@
         <v>44821</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>344</v>
       </c>
@@ -4983,8 +5044,8 @@
         <v>44813</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>344</v>
       </c>
       <c r="B21" s="1">
@@ -4992,38 +5053,38 @@
         <v>18</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>45</v>
+        <v>263</v>
+      </c>
+      <c r="D21" t="s">
+        <v>264</v>
       </c>
       <c r="E21" s="7">
-        <v>255.99</v>
+        <v>47.814999999999998</v>
       </c>
       <c r="F21" s="6">
-        <f>+E21*I21*AUD</f>
-        <v>82472.633374629047</v>
+        <f>+E21*I21*EUR</f>
+        <v>47787.06963279</v>
       </c>
       <c r="G21" s="6">
-        <f>[16]Main!$J$5-[16]Main!$J$6</f>
-        <v>778.60000000000036</v>
+        <f>([16]Main!$J$5-[16]Main!$J$6)</f>
+        <v>-36575</v>
       </c>
       <c r="H21" s="6">
-        <f t="shared" si="3"/>
-        <v>81694.033374629042</v>
+        <f>+F21-G21</f>
+        <v>84362.069632789993</v>
       </c>
       <c r="I21" s="6">
         <f>+[16]Main!$J$3</f>
-        <v>470.117188</v>
+        <v>982.42</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>310</v>
       </c>
       <c r="K21" s="9">
-        <v>44813</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+        <v>44837</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>344</v>
       </c>
@@ -5032,38 +5093,38 @@
         <v>19</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" s="3">
-        <v>13.12</v>
+        <v>45</v>
+      </c>
+      <c r="E22" s="7">
+        <v>255.99</v>
       </c>
       <c r="F22" s="6">
-        <f>+E22*2*I22</f>
-        <v>40559.315495039998</v>
+        <f>+E22*I22*AUD</f>
+        <v>82472.633374629047</v>
       </c>
       <c r="G22" s="6">
-        <f>([17]Main!$K$6-[17]Main!$K$7)/JPY</f>
-        <v>-28305.661165656984</v>
+        <f>[17]Main!$J$5-[17]Main!$J$6</f>
+        <v>778.60000000000036</v>
       </c>
       <c r="H22" s="6">
-        <f>+F22-G22</f>
-        <v>68864.976660696979</v>
+        <f t="shared" si="3"/>
+        <v>81694.033374629042</v>
       </c>
       <c r="I22" s="6">
-        <f>+[17]Main!$K$4</f>
-        <v>1545.7056210000001</v>
+        <f>+[17]Main!$J$3</f>
+        <v>470.117188</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>310</v>
       </c>
       <c r="K22" s="9">
-        <v>44824</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+        <v>44813</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>344</v>
       </c>
@@ -5075,25 +5136,25 @@
         <v>62</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="E23" s="6">
-        <v>3842</v>
+        <v>63</v>
+      </c>
+      <c r="E23" s="3">
+        <v>13.12</v>
       </c>
       <c r="F23" s="6">
-        <f>+E23*I23/JPY</f>
-        <v>41352.280453185704</v>
+        <f>+E23*2*I23</f>
+        <v>40559.315495039998</v>
       </c>
       <c r="G23" s="6">
-        <f>([17]Main!$K$6-[17]Main!$K$7)/JPY</f>
+        <f>([18]Main!$K$6-[18]Main!$K$7)/JPY</f>
         <v>-28305.661165656984</v>
       </c>
       <c r="H23" s="6">
         <f>+F23-G23</f>
-        <v>69657.941618842684</v>
+        <v>68864.976660696979</v>
       </c>
       <c r="I23" s="6">
-        <f>+[17]Main!$K$4</f>
+        <f>+[18]Main!$K$4</f>
         <v>1545.7056210000001</v>
       </c>
       <c r="J23" s="3" t="s">
@@ -5103,7 +5164,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>344</v>
       </c>
@@ -5112,38 +5173,38 @@
         <v>21</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E24" s="7">
-        <v>288</v>
+        <v>345</v>
+      </c>
+      <c r="E24" s="6">
+        <v>3842</v>
       </c>
       <c r="F24" s="6">
-        <f>+E24*[18]Main!$M$3</f>
-        <v>73728</v>
+        <f>+E24*I24/JPY</f>
+        <v>41352.280453185704</v>
       </c>
       <c r="G24" s="6">
-        <f>+[18]Main!$M$5-[18]Main!$M$6</f>
-        <v>9253.4</v>
+        <f>([18]Main!$K$6-[18]Main!$K$7)/JPY</f>
+        <v>-28305.661165656984</v>
       </c>
       <c r="H24" s="6">
-        <f t="shared" si="3"/>
-        <v>64474.6</v>
+        <f>+F24-G24</f>
+        <v>69657.941618842684</v>
       </c>
       <c r="I24" s="6">
-        <f>+[18]Main!$M$3</f>
-        <v>256</v>
+        <f>+[18]Main!$K$4</f>
+        <v>1545.7056210000001</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>16</v>
+        <v>310</v>
       </c>
       <c r="K24" s="9">
-        <v>44813</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+        <v>44824</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>344</v>
       </c>
@@ -5152,38 +5213,38 @@
         <v>22</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E25" s="7">
-        <v>700</v>
+        <v>288</v>
       </c>
       <c r="F25" s="6">
-        <f>+E25*I25</f>
-        <v>76662.702200000014</v>
+        <f>+E25*[19]Main!$M$3</f>
+        <v>73728</v>
       </c>
       <c r="G25" s="6">
-        <f>+[19]Main!$J$5-[19]Main!$J$6</f>
-        <v>12001.599999999999</v>
+        <f>+[19]Main!$M$5-[19]Main!$M$6</f>
+        <v>9253.4</v>
       </c>
       <c r="H25" s="6">
         <f t="shared" si="3"/>
-        <v>64661.102200000016</v>
+        <v>64474.6</v>
       </c>
       <c r="I25" s="6">
-        <f>+[19]Main!$J$3</f>
-        <v>109.51814600000002</v>
+        <f>+[19]Main!$M$3</f>
+        <v>256</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>310</v>
+        <v>16</v>
       </c>
       <c r="K25" s="9">
-        <v>44820</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+        <v>44813</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>344</v>
       </c>
@@ -5191,39 +5252,39 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="C26" s="14" t="s">
-        <v>56</v>
+      <c r="C26" s="5" t="s">
+        <v>52</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E26" s="6">
-        <v>3626</v>
+        <v>53</v>
+      </c>
+      <c r="E26" s="7">
+        <v>700</v>
       </c>
       <c r="F26" s="6">
-        <f>+E26*I26/JPY</f>
-        <v>41524.161733486522</v>
+        <f>+E26*I26</f>
+        <v>76662.702200000014</v>
       </c>
       <c r="G26" s="6">
-        <f>([20]Main!$J$5-[20]Main!$J$6)/JPY</f>
-        <v>4140.0320311955984</v>
+        <f>+[20]Main!$J$5-[20]Main!$J$6</f>
+        <v>12001.599999999999</v>
       </c>
       <c r="H26" s="6">
-        <f>+F26-G26</f>
-        <v>37384.129702290928</v>
+        <f t="shared" si="3"/>
+        <v>64661.102200000016</v>
       </c>
       <c r="I26" s="6">
         <f>+[20]Main!$J$3</f>
-        <v>1644.5904210000001</v>
+        <v>109.51814600000002</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>310</v>
       </c>
       <c r="K26" s="9">
-        <v>44834</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+        <v>44820</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>344</v>
       </c>
@@ -5232,78 +5293,78 @@
         <v>24</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E27" s="7">
-        <v>142</v>
+        <v>57</v>
+      </c>
+      <c r="E27" s="6">
+        <v>3626</v>
       </c>
       <c r="F27" s="6">
-        <f>+E27*I27</f>
-        <v>55550.335248000003</v>
+        <f>+E27*I27/JPY</f>
+        <v>41524.161733486522</v>
       </c>
       <c r="G27" s="6">
-        <f>+[21]Main!$L$5-[21]Main!$L$6</f>
-        <v>18059</v>
+        <f>([21]Main!$J$5-[21]Main!$J$6)/JPY</f>
+        <v>4140.0320311955984</v>
       </c>
       <c r="H27" s="6">
-        <f t="shared" si="3"/>
-        <v>37491.335248000003</v>
+        <f>+F27-G27</f>
+        <v>37384.129702290928</v>
       </c>
       <c r="I27" s="6">
-        <f>+[21]Main!$L$3</f>
-        <v>391.199544</v>
+        <f>+[21]Main!$J$3</f>
+        <v>1644.5904210000001</v>
       </c>
       <c r="J27" s="3" t="s">
         <v>310</v>
       </c>
       <c r="K27" s="9">
-        <v>44814</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+        <v>44834</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>344</v>
       </c>
       <c r="B28" s="1">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>76</v>
+      <c r="C28" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E28" s="3">
-        <v>8.69</v>
+        <v>55</v>
+      </c>
+      <c r="E28" s="7">
+        <v>142</v>
       </c>
       <c r="F28" s="6">
-        <f>E28*[22]Main!$M$3</f>
-        <v>10537.3283686</v>
+        <f>+E28*I28</f>
+        <v>55550.335248000003</v>
       </c>
       <c r="G28" s="6">
-        <f>[22]Main!$M$5-[22]Main!$M$6</f>
-        <v>-18665.5</v>
+        <f>+[22]Main!$L$5-[22]Main!$L$6</f>
+        <v>18059</v>
       </c>
       <c r="H28" s="6">
-        <f>F28-G28</f>
-        <v>29202.8283686</v>
+        <f t="shared" si="3"/>
+        <v>37491.335248000003</v>
       </c>
       <c r="I28" s="6">
-        <f>+[22]Main!$M$3</f>
-        <v>1212.5809400000001</v>
+        <f>+[22]Main!$L$3</f>
+        <v>391.199544</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>310</v>
       </c>
       <c r="K28" s="9">
-        <v>44828</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+        <v>44814</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>344</v>
       </c>
@@ -5312,38 +5373,38 @@
         <v>26</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E29" s="7">
-        <v>150.91</v>
+        <v>77</v>
+      </c>
+      <c r="E29" s="3">
+        <v>8.69</v>
       </c>
       <c r="F29" s="6">
-        <f>+E29*I29</f>
-        <v>36623.653864910004</v>
+        <f>E29*[23]Main!$M$3</f>
+        <v>10537.3283686</v>
       </c>
       <c r="G29" s="6">
-        <f>+[23]Main!$K$5-[23]Main!$K$6</f>
-        <v>8320.9</v>
+        <f>[23]Main!$M$5-[23]Main!$M$6</f>
+        <v>-18665.5</v>
       </c>
       <c r="H29" s="6">
-        <f>+F29-G29</f>
-        <v>28302.753864910002</v>
+        <f>F29-G29</f>
+        <v>29202.8283686</v>
       </c>
       <c r="I29" s="6">
-        <f>+[23]Main!$K$3</f>
-        <v>242.68540100000001</v>
+        <f>+[23]Main!$M$3</f>
+        <v>1212.5809400000001</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>310</v>
       </c>
       <c r="K29" s="9">
-        <v>44815</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+        <v>44828</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>344</v>
       </c>
@@ -5351,17 +5412,39 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="D30" t="s">
-        <v>264</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C30" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E30" s="7">
+        <v>150.91</v>
+      </c>
+      <c r="F30" s="6">
+        <f>+E30*I30</f>
+        <v>36623.653864910004</v>
+      </c>
+      <c r="G30" s="6">
+        <f>+[24]Main!$K$5-[24]Main!$K$6</f>
+        <v>8320.9</v>
+      </c>
+      <c r="H30" s="6">
+        <f>+F30-G30</f>
+        <v>28302.753864910002</v>
+      </c>
+      <c r="I30" s="6">
+        <f>+[24]Main!$K$3</f>
+        <v>242.68540100000001</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="K30" s="9">
+        <v>44815</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>344</v>
       </c>
@@ -5369,14 +5452,42 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="5" t="s">
         <v>267</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E31" s="7">
+        <v>48.3</v>
+      </c>
+      <c r="F31" s="6" cm="1">
+        <f t="array" ref="F31">+E31*I31/HKD</f>
+        <v>26232.919453643313</v>
+      </c>
+      <c r="G31" s="6">
+        <f>([25]Main!$J$5-[25]Main!$J$6)/HKD</f>
+        <v>985.39847133757974</v>
+      </c>
+      <c r="H31" s="6">
+        <f>+F31-G31</f>
+        <v>25247.520982305734</v>
+      </c>
+      <c r="I31" s="6">
+        <f>+[25]Main!$J$3</f>
+        <v>4263.5283170000002</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="K31" s="9">
+        <v>44838</v>
+      </c>
+      <c r="AC31" s="1">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>344</v>
       </c>
@@ -5389,6 +5500,9 @@
       </c>
       <c r="D32" t="s">
         <v>266</v>
+      </c>
+      <c r="E32" s="6">
+        <v>807000</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
@@ -5616,11 +5730,11 @@
         <v>71.27</v>
       </c>
       <c r="F46" s="6">
-        <f>+E46*[24]Main!$K$3</f>
+        <f>+E46*[26]Main!$K$3</f>
         <v>15786.66213397</v>
       </c>
       <c r="G46" s="6">
-        <f>+[24]Main!$K$5-[24]Main!$K$6</f>
+        <f>+[26]Main!$K$5-[26]Main!$K$6</f>
         <v>2721</v>
       </c>
       <c r="H46" s="6">
@@ -5691,11 +5805,11 @@
         <v>132.13999999999999</v>
       </c>
       <c r="F50" s="6">
-        <f>E50*[25]Main!$L$3</f>
+        <f>E50*[27]Main!$L$3</f>
         <v>13539.443113239999</v>
       </c>
       <c r="G50" s="6">
-        <f>[25]Main!$L$5-[25]Main!$L$6</f>
+        <f>[27]Main!$L$5-[27]Main!$L$6</f>
         <v>5643.241</v>
       </c>
       <c r="H50" s="6">
@@ -5781,11 +5895,11 @@
         <v>219.38</v>
       </c>
       <c r="F55" s="6">
-        <f>E55*[26]Main!$K$3</f>
+        <f>E55*[28]Main!$K$3</f>
         <v>10464.426000000001</v>
       </c>
       <c r="G55" s="6">
-        <f>[26]Main!$K$5-[26]Main!$K$6</f>
+        <f>[28]Main!$K$5-[28]Main!$K$6</f>
         <v>3027</v>
       </c>
       <c r="H55" s="6">
@@ -5811,11 +5925,11 @@
         <v>57</v>
       </c>
       <c r="F56" s="6">
-        <f>+E56*[27]Main!$L$3</f>
+        <f>+E56*[29]Main!$L$3</f>
         <v>6071.7436259999995</v>
       </c>
       <c r="G56" s="6">
-        <f>+[27]Main!$L$5-[27]Main!$L$6</f>
+        <f>+[29]Main!$L$5-[29]Main!$L$6</f>
         <v>776.13</v>
       </c>
       <c r="H56" s="6">
@@ -5845,7 +5959,7 @@
         <v>2379.9056977800001</v>
       </c>
       <c r="G57" s="6">
-        <f>+[28]Main!$K$5-[28]Main!$K$6</f>
+        <f>+[30]Main!$K$5-[30]Main!$K$6</f>
         <v>1840.732</v>
       </c>
       <c r="H57" s="6">
@@ -5853,7 +5967,7 @@
         <v>539.17369778000011</v>
       </c>
       <c r="I57" s="6">
-        <f>+[28]Main!$K$3</f>
+        <f>+[30]Main!$K$3</f>
         <v>695.87885900000003</v>
       </c>
       <c r="J57" s="3" t="s">
@@ -5882,7 +5996,7 @@
         <v>4746.2735717200003</v>
       </c>
       <c r="G58" s="6">
-        <f>+[29]Main!$K$5-[29]Main!$K$6</f>
+        <f>+[31]Main!$K$5-[31]Main!$K$6</f>
         <v>-337</v>
       </c>
       <c r="H58" s="6">
@@ -5890,7 +6004,7 @@
         <v>5083.2735717200003</v>
       </c>
       <c r="I58" s="6">
-        <f>+[29]Main!$K$3</f>
+        <f>+[31]Main!$K$3</f>
         <v>233</v>
       </c>
       <c r="J58" s="3" t="s">
@@ -5916,7 +6030,7 @@
         <v>4604.0473282500006</v>
       </c>
       <c r="G59" s="6">
-        <f>+[30]Main!$L$5-[30]Main!$L$6</f>
+        <f>+[32]Main!$L$5-[32]Main!$L$6</f>
         <v>465.44</v>
       </c>
       <c r="H59" s="6">
@@ -5924,7 +6038,7 @@
         <v>4138.607328250001</v>
       </c>
       <c r="I59" s="6">
-        <f>+[30]Main!$L$3</f>
+        <f>+[32]Main!$L$3</f>
         <v>164.25427500000001</v>
       </c>
       <c r="J59" s="3" t="s">
@@ -6651,11 +6765,11 @@
         <v>9.18</v>
       </c>
       <c r="F110" s="6">
-        <f>+E110*[31]Main!$N$3</f>
+        <f>+E110*[33]Main!$N$3</f>
         <v>2859.4049160599998</v>
       </c>
       <c r="G110" s="6">
-        <f>+[31]Main!$N$5-[31]Main!$N$6</f>
+        <f>+[33]Main!$N$5-[33]Main!$N$6</f>
         <v>869.93499999999995</v>
       </c>
       <c r="H110" s="6">
@@ -6685,7 +6799,7 @@
         <v>3249.6786968599999</v>
       </c>
       <c r="G111" s="6">
-        <f>+[32]Main!$K$5-[32]Main!$K$6</f>
+        <f>+[34]Main!$K$5-[34]Main!$K$6</f>
         <v>1178.8610000000001</v>
       </c>
       <c r="H111" s="6">
@@ -6693,7 +6807,7 @@
         <v>2070.8176968600001</v>
       </c>
       <c r="I111" s="6">
-        <f>+[32]Main!$K$3</f>
+        <f>+[34]Main!$K$3</f>
         <v>70.354594000000006</v>
       </c>
       <c r="J111" s="3" t="s">
@@ -6722,7 +6836,7 @@
         <v>1436.0261408599999</v>
       </c>
       <c r="G112" s="6">
-        <f>+[33]Main!$J$5-[33]Main!$J$6</f>
+        <f>+[35]Main!$J$5-[35]Main!$J$6</f>
         <v>566.44900000000007</v>
       </c>
       <c r="H112" s="6">
@@ -6730,7 +6844,7 @@
         <v>869.57714085999987</v>
       </c>
       <c r="I112" s="6">
-        <f>+[33]Main!$J$3</f>
+        <f>+[35]Main!$J$3</f>
         <v>58.068182</v>
       </c>
       <c r="J112" s="3" t="s">
@@ -7102,7 +7216,7 @@
     </row>
     <row r="137" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B137" s="1">
-        <f t="shared" ref="B137:B175" si="5">B136+1</f>
+        <f t="shared" ref="B137:B176" si="5">B136+1</f>
         <v>112</v>
       </c>
       <c r="C137" s="1" t="s">
@@ -7205,11 +7319,11 @@
         <v>15.65</v>
       </c>
       <c r="F143" s="6">
-        <f>E143*[34]Main!$L$3</f>
+        <f>E143*[36]Main!$L$3</f>
         <v>1253.1559559500001</v>
       </c>
       <c r="G143" s="6">
-        <f>+[34]Main!$L$5-[34]Main!$L$6</f>
+        <f>+[36]Main!$L$5-[36]Main!$L$6</f>
         <v>112.015</v>
       </c>
       <c r="H143" s="6">
@@ -7235,11 +7349,11 @@
         <v>11</v>
       </c>
       <c r="F144" s="6">
-        <f>+E144*[35]Main!$L$3</f>
+        <f>+E144*[37]Main!$L$3</f>
         <v>798.23003700000004</v>
       </c>
       <c r="G144" s="6">
-        <f>+[35]Main!$L$5-[35]Main!$L$6</f>
+        <f>+[37]Main!$L$5-[37]Main!$L$6</f>
         <v>153.25991400000001</v>
       </c>
       <c r="H144" s="6">
@@ -7277,7 +7391,7 @@
         <v>897.18233664000002</v>
       </c>
       <c r="G145" s="6">
-        <f>+[36]Main!$J$5-[36]Main!$J$6</f>
+        <f>+[38]Main!$J$5-[38]Main!$J$6</f>
         <v>601.58999999999992</v>
       </c>
       <c r="H145" s="6">
@@ -7285,7 +7399,7 @@
         <v>295.5923366400001</v>
       </c>
       <c r="I145" s="6">
-        <f>+[36]Main!$J$3</f>
+        <f>+[38]Main!$J$3</f>
         <v>121.89977399999999</v>
       </c>
       <c r="J145" s="3" t="s">
@@ -7455,7 +7569,7 @@
         <v>30.407559149999997</v>
       </c>
       <c r="G155" s="6">
-        <f>+[37]Main!$N$5-[37]Main!$N$6</f>
+        <f>+[39]Main!$N$5-[39]Main!$N$6</f>
         <v>-7.4640000000000004</v>
       </c>
       <c r="H155" s="6">
@@ -7463,7 +7577,7 @@
         <v>37.871559149999996</v>
       </c>
       <c r="I155" s="6">
-        <f>+[37]Main!$N$3</f>
+        <f>+[39]Main!$N$3</f>
         <v>9.4141049999999993</v>
       </c>
       <c r="J155" s="3" t="s">
@@ -7533,11 +7647,11 @@
         <v>7.06</v>
       </c>
       <c r="F159" s="6">
-        <f>E159*[38]Main!$J$3</f>
+        <f>E159*[40]Main!$J$3</f>
         <v>725.62786605999997</v>
       </c>
       <c r="G159" s="6">
-        <f>[38]Main!$J$5-[38]Main!$J$6</f>
+        <f>[40]Main!$J$5-[40]Main!$J$6</f>
         <v>197.79600000000002</v>
       </c>
       <c r="H159" s="8">
@@ -7567,7 +7681,7 @@
         <v>486.43225439999998</v>
       </c>
       <c r="G160" s="6">
-        <f>+[39]Main!$K$5-[39]Main!$K$6</f>
+        <f>+[41]Main!$K$5-[41]Main!$K$6</f>
         <v>-37.984000000000002</v>
       </c>
       <c r="H160" s="8">
@@ -7575,7 +7689,7 @@
         <v>524.41625439999996</v>
       </c>
       <c r="I160" s="6">
-        <f>+[39]Main!$K$3</f>
+        <f>+[41]Main!$K$3</f>
         <v>810.72042399999998</v>
       </c>
       <c r="J160" s="3" t="s">
@@ -7603,11 +7717,11 @@
         <v>14.68</v>
       </c>
       <c r="F161" s="6">
-        <f>E161*[40]Main!$L$3</f>
+        <f>E161*[42]Main!$L$3</f>
         <v>587.26396075999992</v>
       </c>
       <c r="G161" s="6">
-        <f>[40]Main!$L$5-[40]Main!$L$6</f>
+        <f>[42]Main!$L$5-[42]Main!$L$6</f>
         <v>277.88299999999998</v>
       </c>
       <c r="H161" s="8">
@@ -7633,11 +7747,11 @@
         <v>4.8600000000000003</v>
       </c>
       <c r="F162" s="6">
-        <f>E162*[41]Main!$J$3</f>
+        <f>E162*[43]Main!$J$3</f>
         <v>312.71415336000001</v>
       </c>
       <c r="G162" s="8">
-        <f>+[41]Main!$J$5-[41]Main!$J$6</f>
+        <f>+[43]Main!$J$5-[43]Main!$J$6</f>
         <v>92.317999999999998</v>
       </c>
       <c r="H162" s="8">
@@ -7663,11 +7777,11 @@
         <v>7.57</v>
       </c>
       <c r="F163" s="6">
-        <f>E163*[42]Main!$M$3</f>
+        <f>E163*[44]Main!$M$3</f>
         <v>338.45983246000003</v>
       </c>
       <c r="G163" s="6">
-        <f>[42]Main!$M$5-[42]Main!$M$6</f>
+        <f>[44]Main!$M$5-[44]Main!$M$6</f>
         <v>120.43700000000001</v>
       </c>
       <c r="H163" s="8">
@@ -7693,11 +7807,11 @@
         <v>0.7</v>
       </c>
       <c r="F164" s="6">
-        <f>E164*[43]Main!$M$3</f>
+        <f>E164*[45]Main!$M$3</f>
         <v>128.9392503</v>
       </c>
       <c r="G164" s="6">
-        <f>[43]Main!$M$5-[43]Main!$M$6</f>
+        <f>[45]Main!$M$5-[45]Main!$M$6</f>
         <v>-59.50200000000001</v>
       </c>
       <c r="H164" s="8">
@@ -7723,11 +7837,11 @@
         <v>1.98</v>
       </c>
       <c r="F165" s="6">
-        <f>E165*[44]Main!$N$3</f>
+        <f>E165*[46]Main!$N$3</f>
         <v>39.757463459999997</v>
       </c>
       <c r="G165" s="6">
-        <f>[44]Main!$N$5-[44]Main!$N$6</f>
+        <f>[46]Main!$N$5-[46]Main!$N$6</f>
         <v>15.942</v>
       </c>
       <c r="H165" s="8">
@@ -7753,11 +7867,11 @@
         <v>0.62</v>
       </c>
       <c r="F166" s="6">
-        <f>E166*[45]Main!$L$3</f>
+        <f>E166*[47]Main!$L$3</f>
         <v>30.1881658</v>
       </c>
       <c r="G166" s="6">
-        <f>[45]Main!$L$5-[45]Main!$L$6</f>
+        <f>[47]Main!$L$5-[47]Main!$L$6</f>
         <v>13.262999999999998</v>
       </c>
       <c r="H166" s="8">
@@ -7783,11 +7897,11 @@
         <v>6.12</v>
       </c>
       <c r="F167" s="6">
-        <f>E167*[46]Main!$M$3</f>
+        <f>E167*[48]Main!$M$3</f>
         <v>125.46108324000001</v>
       </c>
       <c r="G167" s="6">
-        <f>[46]Main!$M$5-[46]Main!$M$6</f>
+        <f>[48]Main!$M$5-[48]Main!$M$6</f>
         <v>131.17699999999999</v>
       </c>
       <c r="H167" s="8">
@@ -7813,11 +7927,11 @@
         <v>0.98</v>
       </c>
       <c r="F168" s="6">
-        <f>E168*[47]Main!$M$3</f>
+        <f>E168*[49]Main!$M$3</f>
         <v>20.935517539999999</v>
       </c>
       <c r="G168" s="6">
-        <f>[47]Main!$M$5-[47]Main!$M$6</f>
+        <f>[49]Main!$M$5-[49]Main!$M$6</f>
         <v>55.28</v>
       </c>
       <c r="H168" s="8">
@@ -7923,17 +8037,29 @@
         <f t="shared" si="5"/>
         <v>150</v>
       </c>
-      <c r="C175" s="16" t="s">
+      <c r="C175" t="s">
+        <v>397</v>
+      </c>
+      <c r="D175" t="s">
         <v>398</v>
-      </c>
-      <c r="D175" s="16" t="s">
-        <v>399</v>
       </c>
       <c r="E175" s="3">
         <v>9.26</v>
       </c>
       <c r="F175" s="3">
         <v>204</v>
+      </c>
+    </row>
+    <row r="176" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B176" s="1">
+        <f t="shared" si="5"/>
+        <v>151</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>409</v>
       </c>
     </row>
   </sheetData>
@@ -7952,18 +8078,18 @@
     <hyperlink ref="C6" r:id="rId8" xr:uid="{615921E7-8A8A-4F41-A8F3-1AF78A43F1AC}"/>
     <hyperlink ref="C20" r:id="rId9" xr:uid="{A38EC1E4-9170-422B-A9F5-3B6EB77DF40A}"/>
     <hyperlink ref="C9" r:id="rId10" xr:uid="{CCC45DFB-BF73-4A15-8527-F4C3C617F472}"/>
-    <hyperlink ref="C21" r:id="rId11" xr:uid="{FC86E1B4-4BA7-43A8-8FCA-CC27867A7922}"/>
+    <hyperlink ref="C22" r:id="rId11" xr:uid="{FC86E1B4-4BA7-43A8-8FCA-CC27867A7922}"/>
     <hyperlink ref="C13" r:id="rId12" xr:uid="{F9D09B0D-FACB-4CCA-872E-286E56965815}"/>
     <hyperlink ref="C15" r:id="rId13" xr:uid="{5A59EF45-A9EA-44F3-BECB-EFED8413DCF6}"/>
     <hyperlink ref="C18" r:id="rId14" xr:uid="{316E9202-338F-4301-AEBE-A9FA398A76CC}"/>
     <hyperlink ref="C5" r:id="rId15" xr:uid="{0888F4DA-9569-4326-990C-43015A33BD61}"/>
     <hyperlink ref="C17" r:id="rId16" xr:uid="{C2959A9B-7367-43D7-934F-562A915DC4DD}"/>
-    <hyperlink ref="C24" r:id="rId17" xr:uid="{A069369A-FB97-4A4A-A581-321FA79E4250}"/>
+    <hyperlink ref="C25" r:id="rId17" xr:uid="{A069369A-FB97-4A4A-A581-321FA79E4250}"/>
     <hyperlink ref="C46" r:id="rId18" xr:uid="{6EF35D30-7113-4CE8-9077-C5BE97F74D36}"/>
-    <hyperlink ref="C25" r:id="rId19" xr:uid="{1F769FA7-6B90-4B6B-9BCC-7D6679675B06}"/>
+    <hyperlink ref="C26" r:id="rId19" xr:uid="{1F769FA7-6B90-4B6B-9BCC-7D6679675B06}"/>
     <hyperlink ref="C49" r:id="rId20" xr:uid="{53091BB6-5763-4DDE-A659-5638BD3CADCA}"/>
     <hyperlink ref="C47" r:id="rId21" xr:uid="{10922C8B-4C13-4E76-B998-3ADD8CC60E47}"/>
-    <hyperlink ref="C22" r:id="rId22" xr:uid="{61277D68-67DC-475B-9B61-B7E2F3017110}"/>
+    <hyperlink ref="C23" r:id="rId22" xr:uid="{61277D68-67DC-475B-9B61-B7E2F3017110}"/>
     <hyperlink ref="C162" r:id="rId23" xr:uid="{14A63DAF-63A6-4B91-A2AF-AE28EA251457}"/>
     <hyperlink ref="C165" r:id="rId24" xr:uid="{4ACA7C7F-E42A-4687-A776-AB8065DB40FF}"/>
     <hyperlink ref="C161" r:id="rId25" xr:uid="{B3421391-7EC0-4253-8F62-5ED45A5BFA02}"/>
@@ -7976,16 +8102,16 @@
     <hyperlink ref="C55" r:id="rId32" xr:uid="{A1C90F9B-FBBF-4C72-9A11-3798F692A0D2}"/>
     <hyperlink ref="C56" r:id="rId33" xr:uid="{F7B6503D-1F84-47C4-B87E-BDA7159D1B9F}"/>
     <hyperlink ref="C50" r:id="rId34" xr:uid="{D0EE43E7-C3F5-4256-99AE-DDCA9EC11DCF}"/>
-    <hyperlink ref="C28" r:id="rId35" xr:uid="{1C25970A-A568-4869-A34A-5C6C7551D812}"/>
+    <hyperlink ref="C29" r:id="rId35" xr:uid="{1C25970A-A568-4869-A34A-5C6C7551D812}"/>
     <hyperlink ref="C143" r:id="rId36" xr:uid="{C3A06396-38CD-486E-9F4F-233A79292B4F}"/>
     <hyperlink ref="C110" r:id="rId37" xr:uid="{B83625D8-44D2-4842-9139-F29C8D5F2D8E}"/>
     <hyperlink ref="C144" r:id="rId38" xr:uid="{5FF32E6A-C6C7-4793-8271-BD230B9C7641}"/>
     <hyperlink ref="C58" r:id="rId39" xr:uid="{E5739E03-9FE4-4D05-90C8-36ABF7D078CB}"/>
     <hyperlink ref="C59" r:id="rId40" xr:uid="{25285F59-771C-40DB-8B78-E1E454C61406}"/>
     <hyperlink ref="C155" r:id="rId41" xr:uid="{C000061C-001D-4088-90A4-B672D181D3C5}"/>
-    <hyperlink ref="C23" r:id="rId42" xr:uid="{98C5B53F-658C-427A-AF31-B4D604AF2D15}"/>
-    <hyperlink ref="C27" r:id="rId43" xr:uid="{6A1F812B-EA91-4B3C-B4DC-88F792A7D0DE}"/>
-    <hyperlink ref="C29" r:id="rId44" xr:uid="{6930A656-C59A-465F-8634-B30B4FEF47BC}"/>
+    <hyperlink ref="C24" r:id="rId42" xr:uid="{98C5B53F-658C-427A-AF31-B4D604AF2D15}"/>
+    <hyperlink ref="C28" r:id="rId43" xr:uid="{6A1F812B-EA91-4B3C-B4DC-88F792A7D0DE}"/>
+    <hyperlink ref="C30" r:id="rId44" xr:uid="{6930A656-C59A-465F-8634-B30B4FEF47BC}"/>
     <hyperlink ref="C57" r:id="rId45" xr:uid="{559FAD8A-D620-4B93-BE14-CC22630BD57E}"/>
     <hyperlink ref="C10" r:id="rId46" xr:uid="{467EEBCD-6BD7-4E71-B2C9-FCF3DB57F059}"/>
     <hyperlink ref="C160" r:id="rId47" xr:uid="{6A576FDB-A573-4A00-8381-4BECF13B35A1}"/>
@@ -7993,19 +8119,21 @@
     <hyperlink ref="C112" r:id="rId49" xr:uid="{51C9506E-5D60-43F8-BADA-7F72A25DAFF6}"/>
     <hyperlink ref="C111" r:id="rId50" xr:uid="{9E4325F2-98CF-4735-96D0-66A9DC5A8E86}"/>
     <hyperlink ref="C145" r:id="rId51" xr:uid="{6D062383-838D-42C7-BFCD-E5C9DC258548}"/>
-    <hyperlink ref="C26" r:id="rId52" xr:uid="{3F36D809-73FC-441C-88D2-EEB42A40734A}"/>
+    <hyperlink ref="C27" r:id="rId52" xr:uid="{3F36D809-73FC-441C-88D2-EEB42A40734A}"/>
+    <hyperlink ref="C21" r:id="rId53" xr:uid="{5D73AAA9-EBCA-4613-83CF-E75D37F58B6D}"/>
+    <hyperlink ref="C31" r:id="rId54" xr:uid="{C216ACFE-A1E7-4490-95CC-33302FDEACB6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId53"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId55"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCF0B2B-B27D-4DF2-80CD-010154B4E660}">
-  <dimension ref="B2:C7"/>
+  <dimension ref="B2:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8058,6 +8186,14 @@
         <v>143.61000000000001</v>
       </c>
     </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>410</v>
+      </c>
+      <c r="C8">
+        <v>7.85</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8065,13 +8201,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED149DB-8F62-4CB2-88E6-87DDBD9316FC}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
+      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8203,22 +8339,52 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
+        <v>399</v>
+      </c>
+      <c r="C15" t="s">
         <v>400</v>
-      </c>
-      <c r="C15" t="s">
-        <v>401</v>
       </c>
       <c r="E15" t="s">
         <v>335</v>
       </c>
       <c r="F15" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="H15" s="13">
         <v>43466</v>
       </c>
       <c r="I15" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
         <v>403</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>404</v>
+      </c>
+      <c r="E17" t="s">
+        <v>405</v>
+      </c>
+      <c r="F17" t="s">
+        <v>406</v>
+      </c>
+      <c r="I17" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>411</v>
+      </c>
+      <c r="E18" t="s">
+        <v>405</v>
+      </c>
+      <c r="F18" t="s">
+        <v>412</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated GME & AMC
</commit_message>
<xml_diff>
--- a/Biopharma.xlsx
+++ b/Biopharma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DCB170-B324-413B-96DC-0432F54E077E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E918FF-6015-4832-B4D8-855B4AECD032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51720" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{17641224-F2C3-441B-B85B-BB32567FE633}"/>
+    <workbookView xWindow="1020" yWindow="1530" windowWidth="27375" windowHeight="17595" xr2:uid="{17641224-F2C3-441B-B85B-BB32567FE633}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="440">
   <si>
     <t>Exarta</t>
   </si>
@@ -1445,6 +1445,12 @@
   </si>
   <si>
     <t>NOVN VX</t>
+  </si>
+  <si>
+    <t>Viridian</t>
+  </si>
+  <si>
+    <t>VRDN</t>
   </si>
 </sst>
 </file>
@@ -1621,12 +1627,12 @@
       <sheetName val="Duragesic"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
       <sheetData sheetId="6">
         <row r="3">
           <cell r="Q3">
@@ -1644,50 +1650,50 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
-      <sheetData sheetId="33" refreshError="1"/>
-      <sheetData sheetId="34" refreshError="1"/>
-      <sheetData sheetId="35" refreshError="1"/>
-      <sheetData sheetId="36" refreshError="1"/>
-      <sheetData sheetId="37" refreshError="1"/>
-      <sheetData sheetId="38" refreshError="1"/>
-      <sheetData sheetId="39" refreshError="1"/>
-      <sheetData sheetId="40" refreshError="1"/>
-      <sheetData sheetId="41" refreshError="1"/>
-      <sheetData sheetId="42" refreshError="1"/>
-      <sheetData sheetId="43" refreshError="1"/>
-      <sheetData sheetId="44" refreshError="1"/>
-      <sheetData sheetId="45" refreshError="1"/>
-      <sheetData sheetId="46" refreshError="1"/>
-      <sheetData sheetId="47" refreshError="1"/>
-      <sheetData sheetId="48" refreshError="1"/>
-      <sheetData sheetId="49" refreshError="1"/>
-      <sheetData sheetId="50" refreshError="1"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+      <sheetData sheetId="37"/>
+      <sheetData sheetId="38"/>
+      <sheetData sheetId="39"/>
+      <sheetData sheetId="40"/>
+      <sheetData sheetId="41"/>
+      <sheetData sheetId="42"/>
+      <sheetData sheetId="43"/>
+      <sheetData sheetId="44"/>
+      <sheetData sheetId="45"/>
+      <sheetData sheetId="46"/>
+      <sheetData sheetId="47"/>
+      <sheetData sheetId="48"/>
+      <sheetData sheetId="49"/>
+      <sheetData sheetId="50"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1720,7 +1726,7 @@
       <sheetName val="brivanib"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="3">
           <cell r="K3">
@@ -1738,25 +1744,25 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1799,7 +1805,7 @@
       <sheetName val="Kepivance"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="3">
           <cell r="J3">
@@ -1817,35 +1823,35 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1875,7 +1881,7 @@
       <sheetName val="Failures"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="3">
           <cell r="K3">
@@ -1893,22 +1899,22 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1950,7 +1956,7 @@
       <sheetName val="Tamiflu"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="3">
           <cell r="J3">
@@ -1968,34 +1974,34 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2060,7 +2066,7 @@
       <sheetName val="Avandia"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="4">
           <cell r="J4">
@@ -2078,57 +2084,57 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
-      <sheetData sheetId="33" refreshError="1"/>
-      <sheetData sheetId="34" refreshError="1"/>
-      <sheetData sheetId="35" refreshError="1"/>
-      <sheetData sheetId="36" refreshError="1"/>
-      <sheetData sheetId="37" refreshError="1"/>
-      <sheetData sheetId="38" refreshError="1"/>
-      <sheetData sheetId="39" refreshError="1"/>
-      <sheetData sheetId="40" refreshError="1"/>
-      <sheetData sheetId="41" refreshError="1"/>
-      <sheetData sheetId="42" refreshError="1"/>
-      <sheetData sheetId="43" refreshError="1"/>
-      <sheetData sheetId="44" refreshError="1"/>
-      <sheetData sheetId="45" refreshError="1"/>
-      <sheetData sheetId="46" refreshError="1"/>
-      <sheetData sheetId="47" refreshError="1"/>
-      <sheetData sheetId="48" refreshError="1"/>
-      <sheetData sheetId="49" refreshError="1"/>
-      <sheetData sheetId="50" refreshError="1"/>
-      <sheetData sheetId="51" refreshError="1"/>
-      <sheetData sheetId="52" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+      <sheetData sheetId="37"/>
+      <sheetData sheetId="38"/>
+      <sheetData sheetId="39"/>
+      <sheetData sheetId="40"/>
+      <sheetData sheetId="41"/>
+      <sheetData sheetId="42"/>
+      <sheetData sheetId="43"/>
+      <sheetData sheetId="44"/>
+      <sheetData sheetId="45"/>
+      <sheetData sheetId="46"/>
+      <sheetData sheetId="47"/>
+      <sheetData sheetId="48"/>
+      <sheetData sheetId="49"/>
+      <sheetData sheetId="50"/>
+      <sheetData sheetId="51"/>
+      <sheetData sheetId="52"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2241,11 +2247,11 @@
       <sheetName val="literature"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1">
         <row r="4">
           <cell r="K4">
-            <v>1545.7056210000001</v>
+            <v>1549.478885</v>
           </cell>
         </row>
         <row r="6">
@@ -2259,15 +2265,15 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2279,34 +2285,29 @@
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
-      <sheetName val="Trikafta"/>
-      <sheetName val="Orkambi"/>
-      <sheetName val="Symdeko"/>
-      <sheetName val="Kalydeco"/>
-      <sheetName val="CTX001"/>
-      <sheetName val="VX-880"/>
-      <sheetName val="VX-121"/>
-      <sheetName val="VX-548"/>
-      <sheetName val="inaxaplin"/>
-      <sheetName val="VX-634"/>
-      <sheetName val="IP"/>
-      <sheetName val="Compounds"/>
+      <sheetName val="Dupixent"/>
+      <sheetName val="Eylea"/>
+      <sheetName val="Arcalyst"/>
+      <sheetName val="Zaltrap"/>
+      <sheetName val="VEGF Trap"/>
+      <sheetName val="REGN727"/>
+      <sheetName val="REGN88"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="M3">
-            <v>256</v>
+          <cell r="J3">
+            <v>109.51814600000002</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="M5">
-            <v>9253.4</v>
+          <cell r="J5">
+            <v>13982.3</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="M6">
-            <v>0</v>
+          <cell r="J6">
+            <v>1980.7</v>
           </cell>
         </row>
       </sheetData>
@@ -2318,11 +2319,6 @@
       <sheetData sheetId="6"/>
       <sheetData sheetId="7"/>
       <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2351,7 +2347,7 @@
       <sheetName val="LY2140023"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="3">
           <cell r="J3">
@@ -2411,20 +2407,20 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2436,29 +2432,34 @@
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
-      <sheetName val="Dupixent"/>
-      <sheetName val="Eylea"/>
-      <sheetName val="Arcalyst"/>
-      <sheetName val="Zaltrap"/>
-      <sheetName val="VEGF Trap"/>
-      <sheetName val="REGN727"/>
-      <sheetName val="REGN88"/>
+      <sheetName val="Trikafta"/>
+      <sheetName val="Orkambi"/>
+      <sheetName val="Symdeko"/>
+      <sheetName val="Kalydeco"/>
+      <sheetName val="CTX001"/>
+      <sheetName val="VX-880"/>
+      <sheetName val="VX-121"/>
+      <sheetName val="VX-548"/>
+      <sheetName val="inaxaplin"/>
+      <sheetName val="VX-634"/>
+      <sheetName val="IP"/>
+      <sheetName val="Compounds"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="J3">
-            <v>109.51814600000002</v>
+          <cell r="M3">
+            <v>256</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="J5">
-            <v>13982.3</v>
+          <cell r="M5">
+            <v>9253.4</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="J6">
-            <v>1980.7</v>
+          <cell r="M6">
+            <v>0</v>
           </cell>
         </row>
       </sheetData>
@@ -2470,6 +2471,11 @@
       <sheetData sheetId="6"/>
       <sheetData sheetId="7"/>
       <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2696,13 +2702,7 @@
         </row>
       </sheetData>
       <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="10">
-          <cell r="C10">
-            <v>1000</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
@@ -2790,7 +2790,7 @@
       <sheetName val="Skyrizi"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="3">
           <cell r="K3">
@@ -2808,10 +2808,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3229,9 +3229,9 @@
       <sheetName val="taspoglutide"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
       <sheetData sheetId="3">
         <row r="3">
           <cell r="J3">
@@ -3249,28 +3249,28 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3635,7 +3635,7 @@
       <sheetName val="Crixivan"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="3">
           <cell r="J3">
@@ -3653,27 +3653,27 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3963,10 +3963,10 @@
       <sheetName val="IP"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
       <sheetData sheetId="4">
         <row r="3">
           <cell r="K3">
@@ -3984,41 +3984,41 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
-      <sheetData sheetId="33" refreshError="1"/>
-      <sheetData sheetId="34" refreshError="1"/>
-      <sheetData sheetId="35" refreshError="1"/>
-      <sheetData sheetId="36" refreshError="1"/>
-      <sheetData sheetId="37" refreshError="1"/>
-      <sheetData sheetId="38" refreshError="1"/>
-      <sheetData sheetId="39" refreshError="1"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+      <sheetData sheetId="37"/>
+      <sheetData sheetId="38"/>
+      <sheetData sheetId="39"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4053,11 +4053,11 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4085,7 +4085,7 @@
       <sheetName val="Zactima"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="3">
           <cell r="K3">
@@ -4103,20 +4103,20 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4158,10 +4158,10 @@
       <sheetName val="Diovan"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
       <sheetData sheetId="4">
         <row r="3">
           <cell r="K3">
@@ -4179,31 +4179,31 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4507,13 +4507,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3750AF13-821E-4BF9-92BC-DEDDF3C9498E}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AC176"/>
+  <dimension ref="A1:AC177"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A22" sqref="A22"/>
+      <selection pane="bottomRight" activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4536,13 +4536,13 @@
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B1" s="1">
         <f ca="1">RANDBETWEEN(1,B160)</f>
-        <v>49</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="K2" s="9">
         <f>MIN(K4:K37)</f>
-        <v>44820</v>
+        <v>44828</v>
       </c>
       <c r="Q2" s="18" t="s">
         <v>321</v>
@@ -5590,7 +5590,7 @@
       </c>
       <c r="F25" s="6">
         <f>+E25*2*I25</f>
-        <v>40559.315495039998</v>
+        <v>40658.325942399999</v>
       </c>
       <c r="G25" s="6">
         <f>([18]Main!$K$6-[18]Main!$K$7)/JPY</f>
@@ -5598,17 +5598,17 @@
       </c>
       <c r="H25" s="6">
         <f>+F25-G25</f>
-        <v>68864.976660696979</v>
+        <v>68963.987108056986</v>
       </c>
       <c r="I25" s="6">
         <f>+[18]Main!$K$4</f>
-        <v>1545.7056210000001</v>
+        <v>1549.478885</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>310</v>
       </c>
       <c r="K25" s="9">
-        <v>44824</v>
+        <v>44882</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -5630,7 +5630,7 @@
       </c>
       <c r="F26" s="6">
         <f>+E26*I26/JPY</f>
-        <v>41352.280453185704</v>
+        <v>41453.226628855926</v>
       </c>
       <c r="G26" s="6">
         <f>([18]Main!$K$6-[18]Main!$K$7)/JPY</f>
@@ -5638,17 +5638,17 @@
       </c>
       <c r="H26" s="6">
         <f>+F26-G26</f>
-        <v>69657.941618842684</v>
+        <v>69758.887794512906</v>
       </c>
       <c r="I26" s="6">
         <f>+[18]Main!$K$4</f>
-        <v>1545.7056210000001</v>
+        <v>1549.478885</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>310</v>
       </c>
       <c r="K26" s="9">
-        <v>44824</v>
+        <v>44882</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -5656,39 +5656,39 @@
         <v>344</v>
       </c>
       <c r="B27" s="1">
-        <f t="shared" ref="B27:B58" si="2">B26+1</f>
+        <f>+B26+1</f>
         <v>19</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E27" s="7">
-        <v>288</v>
+        <v>736.04</v>
       </c>
       <c r="F27" s="6">
-        <f>+E27*[19]Main!$M$3</f>
-        <v>73728</v>
+        <f>+E27*I27</f>
+        <v>80609.73618184001</v>
       </c>
       <c r="G27" s="6">
-        <f>+[19]Main!$M$5-[19]Main!$M$6</f>
-        <v>9253.4</v>
+        <f>+[19]Main!$J$5-[19]Main!$J$6</f>
+        <v>12001.599999999999</v>
       </c>
       <c r="H27" s="6">
         <f>F27-G27</f>
-        <v>64474.6</v>
+        <v>68608.136181840004</v>
       </c>
       <c r="I27" s="6">
-        <f>+[19]Main!$M$3</f>
-        <v>256</v>
+        <f>+[19]Main!$J$3</f>
+        <v>109.51814600000002</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>16</v>
+        <v>310</v>
       </c>
       <c r="K27" s="9">
-        <v>44845</v>
+        <v>44881</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -5696,39 +5696,39 @@
         <v>344</v>
       </c>
       <c r="B28" s="1">
-        <f t="shared" si="2"/>
+        <f>+B27+1</f>
         <v>20</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E28" s="7">
-        <v>700</v>
+        <v>288</v>
       </c>
       <c r="F28" s="6">
-        <f>+E28*I28</f>
-        <v>76662.702200000014</v>
+        <f>+E28*[20]Main!$M$3</f>
+        <v>73728</v>
       </c>
       <c r="G28" s="6">
-        <f>+[20]Main!$J$5-[20]Main!$J$6</f>
-        <v>12001.599999999999</v>
+        <f>+[20]Main!$M$5-[20]Main!$M$6</f>
+        <v>9253.4</v>
       </c>
       <c r="H28" s="6">
         <f>F28-G28</f>
-        <v>64661.102200000016</v>
+        <v>64474.6</v>
       </c>
       <c r="I28" s="6">
-        <f>+[20]Main!$J$3</f>
-        <v>109.51814600000002</v>
+        <f>+[20]Main!$M$3</f>
+        <v>256</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>310</v>
+        <v>16</v>
       </c>
       <c r="K28" s="9">
-        <v>44820</v>
+        <v>44845</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -5736,7 +5736,7 @@
         <v>344</v>
       </c>
       <c r="B29" s="1">
-        <f t="shared" si="2"/>
+        <f>+B28+1</f>
         <v>21</v>
       </c>
       <c r="C29" s="5" t="s">
@@ -5776,7 +5776,7 @@
         <v>344</v>
       </c>
       <c r="B30" s="1">
-        <f t="shared" si="2"/>
+        <f>+B29+1</f>
         <v>22</v>
       </c>
       <c r="C30" s="14" t="s">
@@ -5816,7 +5816,7 @@
         <v>344</v>
       </c>
       <c r="B31" s="1">
-        <f t="shared" si="2"/>
+        <f>+B30+1</f>
         <v>23</v>
       </c>
       <c r="C31" s="5" t="s">
@@ -5856,7 +5856,7 @@
         <v>344</v>
       </c>
       <c r="B32" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="B32:B58" si="2">B31+1</f>
         <v>24</v>
       </c>
       <c r="C32" s="5" t="s">
@@ -7809,7 +7809,7 @@
     </row>
     <row r="135" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B135" s="1">
-        <f t="shared" ref="B135:B176" si="6">B134+1</f>
+        <f t="shared" ref="B135:B177" si="6">B134+1</f>
         <v>127</v>
       </c>
       <c r="C135" s="1" t="s">
@@ -8683,6 +8683,21 @@
       </c>
       <c r="D176" s="1" t="s">
         <v>409</v>
+      </c>
+    </row>
+    <row r="177" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B177" s="1">
+        <f t="shared" si="6"/>
+        <v>169</v>
+      </c>
+      <c r="C177" t="s">
+        <v>438</v>
+      </c>
+      <c r="D177" t="s">
+        <v>439</v>
+      </c>
+      <c r="E177" s="3">
+        <v>20.32</v>
       </c>
     </row>
   </sheetData>
@@ -8707,9 +8722,9 @@
     <hyperlink ref="C20" r:id="rId14" xr:uid="{316E9202-338F-4301-AEBE-A9FA398A76CC}"/>
     <hyperlink ref="C6" r:id="rId15" xr:uid="{0888F4DA-9569-4326-990C-43015A33BD61}"/>
     <hyperlink ref="C19" r:id="rId16" xr:uid="{C2959A9B-7367-43D7-934F-562A915DC4DD}"/>
-    <hyperlink ref="C27" r:id="rId17" xr:uid="{A069369A-FB97-4A4A-A581-321FA79E4250}"/>
+    <hyperlink ref="C28" r:id="rId17" xr:uid="{A069369A-FB97-4A4A-A581-321FA79E4250}"/>
     <hyperlink ref="C48" r:id="rId18" xr:uid="{6EF35D30-7113-4CE8-9077-C5BE97F74D36}"/>
-    <hyperlink ref="C28" r:id="rId19" xr:uid="{1F769FA7-6B90-4B6B-9BCC-7D6679675B06}"/>
+    <hyperlink ref="C27" r:id="rId19" xr:uid="{1F769FA7-6B90-4B6B-9BCC-7D6679675B06}"/>
     <hyperlink ref="C50" r:id="rId20" xr:uid="{10922C8B-4C13-4E76-B998-3ADD8CC60E47}"/>
     <hyperlink ref="C25" r:id="rId21" xr:uid="{61277D68-67DC-475B-9B61-B7E2F3017110}"/>
     <hyperlink ref="C162" r:id="rId22" xr:uid="{14A63DAF-63A6-4B91-A2AF-AE28EA251457}"/>

</xml_diff>

<commit_message>
various updates: SBNY, TEAM, SAGE, GME, FRC, ASND
</commit_message>
<xml_diff>
--- a/Biopharma.xlsx
+++ b/Biopharma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803D3465-5000-4BCF-80F7-0B303EC90A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A1E152-671C-4995-A5B7-87D5E77B563C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15915" yWindow="195" windowWidth="25875" windowHeight="20685" activeTab="3" xr2:uid="{17641224-F2C3-441B-B85B-BB32567FE633}"/>
+    <workbookView xWindow="10515" yWindow="0" windowWidth="41190" windowHeight="20985" xr2:uid="{17641224-F2C3-441B-B85B-BB32567FE633}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -102,6 +102,7 @@
     <externalReference r:id="rId85"/>
     <externalReference r:id="rId86"/>
     <externalReference r:id="rId87"/>
+    <externalReference r:id="rId88"/>
   </externalReferences>
   <definedNames>
     <definedName name="AUD">FX!$C$5</definedName>
@@ -158,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="647">
   <si>
     <t>Exarta</t>
   </si>
@@ -2051,6 +2052,54 @@
   </si>
   <si>
     <t>Cambridge, MA</t>
+  </si>
+  <si>
+    <t>Antiverse</t>
+  </si>
+  <si>
+    <t>GPCR antibodies</t>
+  </si>
+  <si>
+    <t>Radiopharma</t>
+  </si>
+  <si>
+    <t>Series D</t>
+  </si>
+  <si>
+    <t>160m</t>
+  </si>
+  <si>
+    <t>108m</t>
+  </si>
+  <si>
+    <t>105m</t>
+  </si>
+  <si>
+    <t>venBio, Versant</t>
+  </si>
+  <si>
+    <t>Venrock</t>
+  </si>
+  <si>
+    <t>Sofinnova, Viking, Wellington</t>
+  </si>
+  <si>
+    <t>Ensoma</t>
+  </si>
+  <si>
+    <t>70m</t>
+  </si>
+  <si>
+    <t>85m</t>
+  </si>
+  <si>
+    <t>Catalio, Solasta, QIA, 5AM, Cormorant</t>
+  </si>
+  <si>
+    <t>SetPoint Medical</t>
+  </si>
+  <si>
+    <t>42m</t>
   </si>
 </sst>
 </file>
@@ -5729,6 +5778,42 @@
           </cell>
         </row>
       </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink83.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="KarXT"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="L3">
+            <v>34.515033000000003</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="L5">
+            <v>1124.0440000000001</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="L6">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6096,11 +6181,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AC227"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <pane xSplit="3" ySplit="3" topLeftCell="D44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="L65" sqref="L65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6122,7 +6207,7 @@
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B1" s="1">
         <f ca="1">RANDBETWEEN(1,B167)</f>
-        <v>41</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
@@ -8668,7 +8753,7 @@
         <v>459.06500000000005</v>
       </c>
       <c r="H62" s="6">
-        <f t="shared" ref="H62:H68" si="7">+F62-G62</f>
+        <f t="shared" ref="H62:H69" si="7">+F62-G62</f>
         <v>5854.9390000000003</v>
       </c>
       <c r="I62" s="3" t="s">
@@ -8684,8 +8769,8 @@
     </row>
     <row r="63" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B63" s="1">
-        <f>B102+1</f>
-        <v>92</v>
+        <f t="shared" si="5"/>
+        <v>54</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>139</v>
@@ -8718,8 +8803,8 @@
     </row>
     <row r="64" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B64" s="1">
-        <f>B62+1</f>
-        <v>54</v>
+        <f t="shared" si="5"/>
+        <v>55</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>303</v>
@@ -8753,356 +8838,375 @@
     <row r="65" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B65" s="1">
         <f t="shared" si="5"/>
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E65" s="3">
-        <v>35.26</v>
+        <v>619</v>
+      </c>
+      <c r="D65" t="s">
+        <v>620</v>
+      </c>
+      <c r="E65" s="7">
+        <v>176</v>
       </c>
       <c r="F65" s="6">
-        <f>+E65*J65</f>
-        <v>5008.6948473599996</v>
+        <f>E65*J65</f>
+        <v>6074.6458080000002</v>
       </c>
       <c r="G65" s="6">
-        <f>+[55]Main!$L$5-[55]Main!$L$6</f>
-        <v>816.24800000000005</v>
+        <f>[83]Main!$L$5-[83]Main!$L$6</f>
+        <v>1124.0440000000001</v>
       </c>
       <c r="H65" s="6">
-        <f t="shared" si="7"/>
-        <v>4192.4468473599991</v>
-      </c>
-      <c r="I65" s="9" t="s">
-        <v>432</v>
+        <f>F65-G65</f>
+        <v>4950.6018080000003</v>
+      </c>
+      <c r="I65" s="3" t="s">
+        <v>536</v>
       </c>
       <c r="J65" s="6">
-        <f>+[55]Main!$L$3</f>
-        <v>142.05033599999999</v>
+        <f>[83]Main!$L$3</f>
+        <v>34.515033000000003</v>
       </c>
       <c r="K65" s="9">
-        <v>44959</v>
+        <v>45008</v>
       </c>
     </row>
     <row r="66" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B66" s="1">
         <f t="shared" si="5"/>
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>137</v>
+        <v>102</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
       <c r="E66" s="3">
-        <v>28.03</v>
+        <v>35.26</v>
       </c>
       <c r="F66" s="6">
-        <f>+J66*E66</f>
-        <v>4604.0473282500006</v>
+        <f>+E66*J66</f>
+        <v>5008.6948473599996</v>
       </c>
       <c r="G66" s="6">
-        <f>+[56]Main!$L$5-[56]Main!$L$6</f>
-        <v>465.44</v>
+        <f>+[55]Main!$L$5-[55]Main!$L$6</f>
+        <v>816.24800000000005</v>
       </c>
       <c r="H66" s="6">
         <f t="shared" si="7"/>
-        <v>4138.607328250001</v>
-      </c>
-      <c r="I66" s="3" t="s">
-        <v>308</v>
+        <v>4192.4468473599991</v>
+      </c>
+      <c r="I66" s="9" t="s">
+        <v>432</v>
       </c>
       <c r="J66" s="6">
-        <f>+[56]Main!$L$3</f>
-        <v>164.25427500000001</v>
+        <f>+[55]Main!$L$3</f>
+        <v>142.05033599999999</v>
       </c>
       <c r="K66" s="9">
-        <v>44782</v>
+        <v>44959</v>
       </c>
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B67" s="1">
         <f t="shared" si="5"/>
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="E67" s="3">
-        <v>18.559999999999999</v>
+        <v>28.03</v>
       </c>
       <c r="F67" s="6">
-        <f>+E67*J67</f>
-        <v>6012.5305600000002</v>
+        <f>+J67*E67</f>
+        <v>4604.0473282500006</v>
       </c>
       <c r="G67" s="6">
-        <f>+[57]Main!$M$5-[57]Main!$M$6</f>
-        <v>2065.1990000000001</v>
+        <f>+[56]Main!$L$5-[56]Main!$L$6</f>
+        <v>465.44</v>
       </c>
       <c r="H67" s="6">
         <f t="shared" si="7"/>
-        <v>3947.3315600000001</v>
+        <v>4138.607328250001</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>536</v>
+        <v>308</v>
       </c>
       <c r="J67" s="6">
-        <f>+[57]Main!$M$3</f>
-        <v>323.95100000000002</v>
+        <f>+[56]Main!$L$3</f>
+        <v>164.25427500000001</v>
       </c>
       <c r="K67" s="9">
-        <v>44971</v>
+        <v>44782</v>
       </c>
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B68" s="1">
         <f t="shared" si="5"/>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>445</v>
-      </c>
-      <c r="D68" t="s">
-        <v>446</v>
-      </c>
-      <c r="E68" s="7">
-        <v>73.790000000000006</v>
+        <v>124</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E68" s="3">
+        <v>18.559999999999999</v>
       </c>
       <c r="F68" s="6">
         <f>+E68*J68</f>
-        <v>3204.4164939800003</v>
+        <v>6012.5305600000002</v>
       </c>
       <c r="G68" s="6">
-        <f>+[58]Main!$L$5-[58]Main!$L$6</f>
-        <v>133.33705900000001</v>
+        <f>+[57]Main!$M$5-[57]Main!$M$6</f>
+        <v>2065.1990000000001</v>
       </c>
       <c r="H68" s="6">
         <f t="shared" si="7"/>
-        <v>3071.0794349800003</v>
+        <v>3947.3315600000001</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>432</v>
+        <v>536</v>
       </c>
       <c r="J68" s="6">
-        <f>+[58]Main!$L$3</f>
-        <v>43.426161999999998</v>
+        <f>+[57]Main!$M$3</f>
+        <v>323.95100000000002</v>
       </c>
       <c r="K68" s="9">
-        <v>44920</v>
+        <v>44971</v>
       </c>
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B69" s="1">
         <f t="shared" si="5"/>
-        <v>59</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>391</v>
+        <v>60</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>445</v>
       </c>
       <c r="D69" t="s">
-        <v>392</v>
+        <v>446</v>
+      </c>
+      <c r="E69" s="7">
+        <v>73.790000000000006</v>
+      </c>
+      <c r="F69" s="6">
+        <f>+E69*J69</f>
+        <v>3204.4164939800003</v>
+      </c>
+      <c r="G69" s="6">
+        <f>+[58]Main!$L$5-[58]Main!$L$6</f>
+        <v>133.33705900000001</v>
+      </c>
+      <c r="H69" s="6">
+        <f t="shared" si="7"/>
+        <v>3071.0794349800003</v>
+      </c>
+      <c r="I69" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="J69" s="6">
+        <f>+[58]Main!$L$3</f>
+        <v>43.426161999999998</v>
+      </c>
+      <c r="K69" s="9">
+        <v>44920</v>
       </c>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B70" s="1">
-        <f>+B69</f>
-        <v>59</v>
+        <f t="shared" si="5"/>
+        <v>61</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>391</v>
       </c>
       <c r="D70" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B71" s="1">
-        <f t="shared" si="5"/>
-        <v>60</v>
-      </c>
-      <c r="C71" t="s">
-        <v>277</v>
+        <f>+B70</f>
+        <v>61</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>391</v>
       </c>
       <c r="D71" t="s">
-        <v>277</v>
-      </c>
-      <c r="E71" s="15">
-        <v>73.56</v>
+        <v>393</v>
       </c>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B72" s="1">
         <f t="shared" si="5"/>
-        <v>61</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E72" s="3">
-        <v>7.71</v>
-      </c>
-      <c r="F72" s="3">
-        <v>9880</v>
+        <v>62</v>
+      </c>
+      <c r="C72" t="s">
+        <v>277</v>
+      </c>
+      <c r="D72" t="s">
+        <v>277</v>
+      </c>
+      <c r="E72" s="15">
+        <v>73.56</v>
       </c>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B73" s="1">
-        <f>B99+1</f>
-        <v>88</v>
+        <f t="shared" si="5"/>
+        <v>63</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="E73" s="3">
-        <v>46.23</v>
+        <v>7.71</v>
       </c>
       <c r="F73" s="3">
-        <v>7850</v>
+        <v>9880</v>
       </c>
     </row>
     <row r="74" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B74" s="1">
-        <f>B72+1</f>
-        <v>62</v>
-      </c>
-      <c r="C74" t="s">
-        <v>378</v>
-      </c>
-      <c r="D74" t="s">
-        <v>379</v>
+        <f>B99+1</f>
+        <v>73</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E74" s="3">
+        <v>46.23</v>
+      </c>
+      <c r="F74" s="3">
+        <v>7850</v>
       </c>
     </row>
     <row r="75" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B75" s="1">
-        <f t="shared" si="5"/>
-        <v>63</v>
+        <f>B73+1</f>
+        <v>64</v>
       </c>
       <c r="C75" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D75" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="76" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B76" s="1">
         <f t="shared" si="5"/>
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C76" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D76" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="77" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B77" s="1">
         <f t="shared" si="5"/>
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C77" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="D77" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
     </row>
     <row r="78" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B78" s="1">
         <f t="shared" si="5"/>
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C78" t="s">
-        <v>282</v>
+        <v>376</v>
       </c>
       <c r="D78" t="s">
-        <v>283</v>
+        <v>377</v>
       </c>
     </row>
     <row r="79" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B79" s="1">
         <f t="shared" si="5"/>
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C79" t="s">
-        <v>364</v>
+        <v>282</v>
       </c>
       <c r="D79" t="s">
-        <v>365</v>
+        <v>283</v>
       </c>
     </row>
     <row r="80" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B80" s="1">
         <f t="shared" si="5"/>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C80" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="D80" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="81" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B81" s="1">
         <f t="shared" si="5"/>
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C81" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="D81" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
     </row>
     <row r="82" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B82" s="1">
         <f t="shared" si="5"/>
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C82" t="s">
-        <v>278</v>
+        <v>366</v>
       </c>
       <c r="D82" t="s">
-        <v>279</v>
+        <v>367</v>
       </c>
     </row>
     <row r="83" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B83" s="1">
         <f t="shared" si="5"/>
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C83" t="s">
-        <v>619</v>
+        <v>278</v>
       </c>
       <c r="D83" t="s">
-        <v>620</v>
-      </c>
-      <c r="E83" s="7">
-        <v>187</v>
-      </c>
-      <c r="F83" s="6">
-        <v>6460</v>
+        <v>279</v>
       </c>
     </row>
     <row r="84" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B84" s="1">
-        <f t="shared" si="5"/>
-        <v>72</v>
+        <f>B65+1</f>
+        <v>57</v>
       </c>
       <c r="C84" t="s">
         <v>621</v>
@@ -9120,7 +9224,7 @@
     <row r="85" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B85" s="1">
         <f t="shared" si="5"/>
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C85" t="s">
         <v>275</v>
@@ -9132,7 +9236,7 @@
     <row r="86" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B86" s="1">
         <f t="shared" si="5"/>
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="C86" t="s">
         <v>372</v>
@@ -9144,7 +9248,7 @@
     <row r="87" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B87" s="1">
         <f t="shared" si="5"/>
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C87" t="s">
         <v>387</v>
@@ -9159,7 +9263,7 @@
     <row r="88" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B88" s="1">
         <f t="shared" si="5"/>
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>106</v>
@@ -9174,7 +9278,7 @@
     <row r="89" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B89" s="1">
         <f t="shared" si="5"/>
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>108</v>
@@ -9189,7 +9293,7 @@
     <row r="90" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B90" s="1">
         <f t="shared" si="5"/>
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>110</v>
@@ -9204,7 +9308,7 @@
     <row r="91" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B91" s="1">
         <f t="shared" si="5"/>
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="C91" t="s">
         <v>617</v>
@@ -9216,7 +9320,7 @@
     <row r="92" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B92" s="1">
         <f t="shared" si="5"/>
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>112</v>
@@ -9234,7 +9338,7 @@
     <row r="93" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B93" s="1">
         <f t="shared" si="5"/>
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="C93" t="s">
         <v>531</v>
@@ -9252,7 +9356,7 @@
     <row r="94" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B94" s="1">
         <f t="shared" si="5"/>
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="C94" s="5" t="s">
         <v>114</v>
@@ -9289,7 +9393,7 @@
     <row r="95" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B95" s="1">
         <f t="shared" si="5"/>
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="C95" s="5" t="s">
         <v>122</v>
@@ -9326,7 +9430,7 @@
     <row r="96" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B96" s="1">
         <f t="shared" si="5"/>
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="C96" s="5" t="s">
         <v>98</v>
@@ -9363,7 +9467,7 @@
     <row r="97" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B97" s="1">
         <f t="shared" si="5"/>
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="C97" t="s">
         <v>451</v>
@@ -9382,7 +9486,7 @@
     <row r="98" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B98" s="1">
         <f t="shared" si="5"/>
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>116</v>
@@ -9397,7 +9501,7 @@
     <row r="99" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B99" s="1">
         <f t="shared" si="5"/>
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>118</v>
@@ -9411,8 +9515,8 @@
     </row>
     <row r="100" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B100" s="1">
-        <f>B73+1</f>
-        <v>89</v>
+        <f>B74+1</f>
+        <v>74</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>127</v>
@@ -9430,7 +9534,7 @@
     <row r="101" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B101" s="1">
         <f t="shared" si="5"/>
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>131</v>
@@ -9448,7 +9552,7 @@
     <row r="102" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B102" s="1">
         <f t="shared" si="5"/>
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>133</v>
@@ -9463,7 +9567,7 @@
     <row r="103" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B103" s="1">
         <f>B63+1</f>
-        <v>93</v>
+        <v>55</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>141</v>
@@ -9478,7 +9582,7 @@
     <row r="104" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B104" s="1">
         <f t="shared" si="5"/>
-        <v>94</v>
+        <v>56</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>143</v>
@@ -9493,7 +9597,7 @@
     <row r="105" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B105" s="1">
         <f t="shared" ref="B105:B172" si="8">B104+1</f>
-        <v>95</v>
+        <v>57</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>145</v>
@@ -9508,7 +9612,7 @@
     <row r="106" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B106" s="1">
         <f t="shared" si="8"/>
-        <v>96</v>
+        <v>58</v>
       </c>
       <c r="C106" t="s">
         <v>314</v>
@@ -9526,7 +9630,7 @@
     <row r="107" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B107" s="1">
         <f t="shared" si="8"/>
-        <v>97</v>
+        <v>59</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>149</v>
@@ -9541,7 +9645,7 @@
     <row r="108" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B108" s="1">
         <f t="shared" si="8"/>
-        <v>98</v>
+        <v>60</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>151</v>
@@ -9556,7 +9660,7 @@
     <row r="109" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B109" s="1">
         <f t="shared" si="8"/>
-        <v>99</v>
+        <v>61</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>167</v>
@@ -9574,7 +9678,7 @@
     <row r="110" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B110" s="1">
         <f t="shared" si="8"/>
-        <v>100</v>
+        <v>62</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>169</v>
@@ -9592,7 +9696,7 @@
     <row r="111" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B111" s="1">
         <f t="shared" si="8"/>
-        <v>101</v>
+        <v>63</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>155</v>
@@ -9610,7 +9714,7 @@
     <row r="112" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B112" s="1">
         <f t="shared" si="8"/>
-        <v>102</v>
+        <v>64</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>157</v>
@@ -9628,7 +9732,7 @@
     <row r="113" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B113" s="1">
         <f t="shared" si="8"/>
-        <v>103</v>
+        <v>65</v>
       </c>
       <c r="C113" s="5" t="s">
         <v>147</v>
@@ -9665,7 +9769,7 @@
     <row r="114" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B114" s="1">
         <f t="shared" si="8"/>
-        <v>104</v>
+        <v>66</v>
       </c>
       <c r="C114" s="5" t="s">
         <v>161</v>
@@ -9702,7 +9806,7 @@
     <row r="115" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B115" s="1">
         <f t="shared" si="8"/>
-        <v>105</v>
+        <v>67</v>
       </c>
       <c r="C115" s="5" t="s">
         <v>159</v>
@@ -9732,7 +9836,7 @@
     <row r="116" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B116" s="1">
         <f>B128+1</f>
-        <v>119</v>
+        <v>81</v>
       </c>
       <c r="C116" s="5" t="s">
         <v>185</v>
@@ -9769,7 +9873,7 @@
     <row r="117" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B117" s="1">
         <f>B115+1</f>
-        <v>106</v>
+        <v>68</v>
       </c>
       <c r="C117" s="5" t="s">
         <v>385</v>
@@ -9806,7 +9910,7 @@
     <row r="118" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B118" s="1">
         <f t="shared" si="8"/>
-        <v>107</v>
+        <v>69</v>
       </c>
       <c r="C118" s="5" t="s">
         <v>358</v>
@@ -9843,7 +9947,7 @@
     <row r="119" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B119" s="1">
         <f t="shared" si="8"/>
-        <v>108</v>
+        <v>70</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>165</v>
@@ -9861,7 +9965,7 @@
     <row r="120" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B120" s="1">
         <f t="shared" si="8"/>
-        <v>109</v>
+        <v>71</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>542</v>
@@ -9874,7 +9978,7 @@
     <row r="121" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B121" s="1">
         <f t="shared" si="8"/>
-        <v>110</v>
+        <v>72</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>177</v>
@@ -9892,7 +9996,7 @@
     <row r="122" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B122" s="25">
         <f t="shared" si="8"/>
-        <v>111</v>
+        <v>73</v>
       </c>
       <c r="C122" s="25" t="s">
         <v>527</v>
@@ -9910,7 +10014,7 @@
     <row r="123" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B123" s="1">
         <f t="shared" si="8"/>
-        <v>112</v>
+        <v>74</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>525</v>
@@ -9928,7 +10032,7 @@
     <row r="124" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B124" s="1">
         <f>B151+1</f>
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>179</v>
@@ -9946,7 +10050,7 @@
     <row r="125" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B125" s="1">
         <f t="shared" si="8"/>
-        <v>115</v>
+        <v>77</v>
       </c>
       <c r="C125" t="s">
         <v>351</v>
@@ -9964,7 +10068,7 @@
     <row r="126" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B126" s="1">
         <f t="shared" si="8"/>
-        <v>116</v>
+        <v>78</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>208</v>
@@ -9982,7 +10086,7 @@
     <row r="127" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B127" s="1">
         <f t="shared" si="8"/>
-        <v>117</v>
+        <v>79</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>183</v>
@@ -10000,7 +10104,7 @@
     <row r="128" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B128" s="1">
         <f t="shared" si="8"/>
-        <v>118</v>
+        <v>80</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>196</v>
@@ -10018,7 +10122,7 @@
     <row r="129" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B129" s="1">
         <f>B116+1</f>
-        <v>120</v>
+        <v>82</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>299</v>
@@ -10036,7 +10140,7 @@
     <row r="130" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B130" s="1">
         <f t="shared" si="8"/>
-        <v>121</v>
+        <v>83</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>218</v>
@@ -10054,7 +10158,7 @@
     <row r="131" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B131" s="1">
         <f t="shared" si="8"/>
-        <v>122</v>
+        <v>84</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>216</v>
@@ -10072,7 +10176,7 @@
     <row r="132" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B132" s="1">
         <f t="shared" si="8"/>
-        <v>123</v>
+        <v>85</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>204</v>
@@ -10090,7 +10194,7 @@
     <row r="133" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B133" s="1">
         <f t="shared" si="8"/>
-        <v>124</v>
+        <v>86</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>222</v>
@@ -10108,7 +10212,7 @@
     <row r="134" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B134" s="1">
         <f t="shared" si="8"/>
-        <v>125</v>
+        <v>87</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>192</v>
@@ -10126,7 +10230,7 @@
     <row r="135" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B135" s="1">
         <f t="shared" si="8"/>
-        <v>126</v>
+        <v>88</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>173</v>
@@ -10144,7 +10248,7 @@
     <row r="136" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B136" s="1">
         <f t="shared" si="8"/>
-        <v>127</v>
+        <v>89</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>187</v>
@@ -10162,7 +10266,7 @@
     <row r="137" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B137" s="1">
         <f t="shared" si="8"/>
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>181</v>
@@ -10180,7 +10284,7 @@
     <row r="138" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B138" s="1">
         <f t="shared" si="8"/>
-        <v>129</v>
+        <v>91</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>210</v>
@@ -10198,7 +10302,7 @@
     <row r="139" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B139" s="1">
         <f t="shared" si="8"/>
-        <v>130</v>
+        <v>92</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>212</v>
@@ -10216,7 +10320,7 @@
     <row r="140" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B140" s="1">
         <f t="shared" si="8"/>
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>163</v>
@@ -10234,7 +10338,7 @@
     <row r="141" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B141" s="1">
         <f t="shared" si="8"/>
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>171</v>
@@ -10252,7 +10356,7 @@
     <row r="142" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B142" s="1">
         <f t="shared" si="8"/>
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="C142" t="s">
         <v>454</v>
@@ -10270,7 +10374,7 @@
     <row r="143" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B143" s="1">
         <f t="shared" si="8"/>
-        <v>134</v>
+        <v>96</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>175</v>
@@ -10288,7 +10392,7 @@
     <row r="144" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B144" s="1">
         <f t="shared" si="8"/>
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>220</v>
@@ -10306,7 +10410,7 @@
     <row r="145" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B145" s="1">
         <f t="shared" si="8"/>
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>88</v>
@@ -10324,7 +10428,7 @@
     <row r="146" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B146" s="1">
         <f t="shared" si="8"/>
-        <v>137</v>
+        <v>99</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>202</v>
@@ -10342,7 +10446,7 @@
     <row r="147" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B147" s="1">
         <f t="shared" si="8"/>
-        <v>138</v>
+        <v>100</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>200</v>
@@ -10360,7 +10464,7 @@
     <row r="148" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B148" s="1">
         <f t="shared" si="8"/>
-        <v>139</v>
+        <v>101</v>
       </c>
       <c r="C148" t="s">
         <v>311</v>
@@ -10378,7 +10482,7 @@
     <row r="149" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B149" s="1">
         <f t="shared" si="8"/>
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>206</v>
@@ -10396,7 +10500,7 @@
     <row r="150" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B150" s="1">
         <f t="shared" si="8"/>
-        <v>141</v>
+        <v>103</v>
       </c>
       <c r="C150" t="s">
         <v>297</v>
@@ -10415,7 +10519,7 @@
     <row r="151" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B151" s="1">
         <f>B123+1</f>
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="C151" t="s">
         <v>529</v>
@@ -10433,7 +10537,7 @@
     <row r="152" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B152" s="1">
         <f>B150+1</f>
-        <v>142</v>
+        <v>104</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>214</v>
@@ -10451,7 +10555,7 @@
     <row r="153" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B153" s="1">
         <f t="shared" si="8"/>
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="C153" s="5" t="s">
         <v>294</v>
@@ -10481,7 +10585,7 @@
     <row r="154" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B154" s="1">
         <f t="shared" si="8"/>
-        <v>144</v>
+        <v>106</v>
       </c>
       <c r="C154" s="5" t="s">
         <v>230</v>
@@ -10521,7 +10625,7 @@
     <row r="155" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B155" s="1">
         <f t="shared" si="8"/>
-        <v>145</v>
+        <v>107</v>
       </c>
       <c r="C155" s="5" t="s">
         <v>305</v>
@@ -10559,7 +10663,7 @@
     <row r="156" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B156" s="1">
         <f t="shared" si="8"/>
-        <v>146</v>
+        <v>108</v>
       </c>
       <c r="C156" s="5" t="s">
         <v>198</v>
@@ -10596,7 +10700,7 @@
     <row r="157" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B157" s="1">
         <f t="shared" si="8"/>
-        <v>147</v>
+        <v>109</v>
       </c>
       <c r="C157" t="s">
         <v>309</v>
@@ -10614,7 +10718,7 @@
     <row r="158" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B158" s="1">
         <f t="shared" si="8"/>
-        <v>148</v>
+        <v>110</v>
       </c>
       <c r="C158" t="s">
         <v>316</v>
@@ -10632,7 +10736,7 @@
     <row r="159" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B159" s="1">
         <f t="shared" si="8"/>
-        <v>149</v>
+        <v>111</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>224</v>
@@ -10650,7 +10754,7 @@
     <row r="160" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B160" s="1">
         <f t="shared" si="8"/>
-        <v>150</v>
+        <v>112</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>226</v>
@@ -10668,7 +10772,7 @@
     <row r="161" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B161" s="1">
         <f t="shared" si="8"/>
-        <v>151</v>
+        <v>113</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>228</v>
@@ -10686,7 +10790,7 @@
     <row r="162" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B162" s="1">
         <f t="shared" si="8"/>
-        <v>152</v>
+        <v>114</v>
       </c>
       <c r="C162" s="5" t="s">
         <v>329</v>
@@ -10723,7 +10827,7 @@
     <row r="163" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B163" s="1">
         <f t="shared" si="8"/>
-        <v>153</v>
+        <v>115</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>232</v>
@@ -10741,7 +10845,7 @@
     <row r="164" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B164" s="1">
         <f t="shared" si="8"/>
-        <v>154</v>
+        <v>116</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>234</v>
@@ -10759,7 +10863,7 @@
     <row r="165" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B165" s="1">
         <f t="shared" si="8"/>
-        <v>155</v>
+        <v>117</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>236</v>
@@ -10777,7 +10881,7 @@
     <row r="166" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B166" s="1">
         <f t="shared" si="8"/>
-        <v>156</v>
+        <v>118</v>
       </c>
       <c r="C166" s="5" t="s">
         <v>238</v>
@@ -10807,7 +10911,7 @@
     <row r="167" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B167" s="1">
         <f t="shared" si="8"/>
-        <v>157</v>
+        <v>119</v>
       </c>
       <c r="C167" s="5" t="s">
         <v>360</v>
@@ -10847,7 +10951,7 @@
     <row r="168" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B168" s="1">
         <f t="shared" si="8"/>
-        <v>158</v>
+        <v>120</v>
       </c>
       <c r="C168" s="5" t="s">
         <v>240</v>
@@ -10877,7 +10981,7 @@
     <row r="169" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B169" s="1">
         <f t="shared" si="8"/>
-        <v>159</v>
+        <v>121</v>
       </c>
       <c r="C169" s="5" t="s">
         <v>242</v>
@@ -10907,7 +11011,7 @@
     <row r="170" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B170" s="1">
         <f t="shared" si="8"/>
-        <v>160</v>
+        <v>122</v>
       </c>
       <c r="C170" s="5" t="s">
         <v>244</v>
@@ -10937,7 +11041,7 @@
     <row r="171" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B171" s="1">
         <f t="shared" si="8"/>
-        <v>161</v>
+        <v>123</v>
       </c>
       <c r="C171" s="5" t="s">
         <v>246</v>
@@ -10967,7 +11071,7 @@
     <row r="172" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B172" s="1">
         <f t="shared" si="8"/>
-        <v>162</v>
+        <v>124</v>
       </c>
       <c r="C172" s="5" t="s">
         <v>248</v>
@@ -10997,7 +11101,7 @@
     <row r="173" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B173" s="1">
         <f t="shared" ref="B173:B213" si="11">B172+1</f>
-        <v>163</v>
+        <v>125</v>
       </c>
       <c r="C173" s="5" t="s">
         <v>250</v>
@@ -11027,7 +11131,7 @@
     <row r="174" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B174" s="1">
         <f t="shared" si="11"/>
-        <v>164</v>
+        <v>126</v>
       </c>
       <c r="C174" s="5" t="s">
         <v>252</v>
@@ -11057,7 +11161,7 @@
     <row r="175" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B175" s="1">
         <f t="shared" si="11"/>
-        <v>165</v>
+        <v>127</v>
       </c>
       <c r="C175" s="5" t="s">
         <v>254</v>
@@ -11087,7 +11191,7 @@
     <row r="176" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B176" s="1">
         <f t="shared" si="11"/>
-        <v>166</v>
+        <v>128</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>256</v>
@@ -11102,7 +11206,7 @@
     <row r="177" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B177" s="1">
         <f t="shared" si="11"/>
-        <v>167</v>
+        <v>129</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>258</v>
@@ -11117,7 +11221,7 @@
     <row r="178" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B178" s="1">
         <f t="shared" si="11"/>
-        <v>168</v>
+        <v>130</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>356</v>
@@ -11132,7 +11236,7 @@
     <row r="179" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B179" s="1">
         <f t="shared" si="11"/>
-        <v>169</v>
+        <v>131</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>340</v>
@@ -11147,7 +11251,7 @@
     <row r="180" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B180" s="1">
         <f t="shared" si="11"/>
-        <v>170</v>
+        <v>132</v>
       </c>
       <c r="C180" t="s">
         <v>344</v>
@@ -11162,7 +11266,7 @@
     <row r="181" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B181" s="1">
         <f t="shared" si="11"/>
-        <v>171</v>
+        <v>133</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>389</v>
@@ -11177,7 +11281,7 @@
     <row r="182" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B182" s="1">
         <f t="shared" si="11"/>
-        <v>172</v>
+        <v>134</v>
       </c>
       <c r="C182" t="s">
         <v>395</v>
@@ -11195,7 +11299,7 @@
     <row r="183" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B183" s="1">
         <f t="shared" si="11"/>
-        <v>173</v>
+        <v>135</v>
       </c>
       <c r="C183" t="s">
         <v>442</v>
@@ -11207,7 +11311,7 @@
     <row r="184" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B184" s="1">
         <f t="shared" si="11"/>
-        <v>174</v>
+        <v>136</v>
       </c>
       <c r="C184" t="s">
         <v>443</v>
@@ -11219,7 +11323,7 @@
     <row r="185" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B185" s="1">
         <f t="shared" si="11"/>
-        <v>175</v>
+        <v>137</v>
       </c>
       <c r="C185" s="1" t="s">
         <v>406</v>
@@ -11231,7 +11335,7 @@
     <row r="186" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B186" s="1">
         <f t="shared" si="11"/>
-        <v>176</v>
+        <v>138</v>
       </c>
       <c r="C186" t="s">
         <v>436</v>
@@ -11246,7 +11350,7 @@
     <row r="187" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B187" s="1">
         <f t="shared" si="11"/>
-        <v>177</v>
+        <v>139</v>
       </c>
       <c r="C187" s="1" t="s">
         <v>516</v>
@@ -11258,7 +11362,7 @@
     <row r="188" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B188" s="1">
         <f t="shared" si="11"/>
-        <v>178</v>
+        <v>140</v>
       </c>
       <c r="C188" t="s">
         <v>523</v>
@@ -11270,7 +11374,7 @@
     <row r="189" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B189" s="1">
         <f t="shared" si="11"/>
-        <v>179</v>
+        <v>141</v>
       </c>
       <c r="C189" s="1" t="s">
         <v>534</v>
@@ -11282,7 +11386,7 @@
     <row r="190" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B190" s="1">
         <f t="shared" si="11"/>
-        <v>180</v>
+        <v>142</v>
       </c>
       <c r="C190" t="s">
         <v>539</v>
@@ -11294,7 +11398,7 @@
     <row r="191" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B191" s="1">
         <f t="shared" si="11"/>
-        <v>181</v>
+        <v>143</v>
       </c>
       <c r="C191" s="1" t="s">
         <v>543</v>
@@ -11306,7 +11410,7 @@
     <row r="192" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B192" s="1">
         <f t="shared" si="11"/>
-        <v>182</v>
+        <v>144</v>
       </c>
       <c r="C192" t="s">
         <v>546</v>
@@ -11318,7 +11422,7 @@
     <row r="193" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B193" s="1">
         <f t="shared" si="11"/>
-        <v>183</v>
+        <v>145</v>
       </c>
       <c r="C193" t="s">
         <v>547</v>
@@ -11330,7 +11434,7 @@
     <row r="194" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B194" s="1">
         <f t="shared" si="11"/>
-        <v>184</v>
+        <v>146</v>
       </c>
       <c r="C194" t="s">
         <v>549</v>
@@ -11342,7 +11446,7 @@
     <row r="195" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B195" s="1">
         <f t="shared" si="11"/>
-        <v>185</v>
+        <v>147</v>
       </c>
       <c r="C195" t="s">
         <v>551</v>
@@ -11354,7 +11458,7 @@
     <row r="196" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B196" s="1">
         <f t="shared" si="11"/>
-        <v>186</v>
+        <v>148</v>
       </c>
       <c r="C196" t="s">
         <v>553</v>
@@ -11366,7 +11470,7 @@
     <row r="197" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B197" s="1">
         <f t="shared" si="11"/>
-        <v>187</v>
+        <v>149</v>
       </c>
       <c r="C197" t="s">
         <v>555</v>
@@ -11378,7 +11482,7 @@
     <row r="198" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B198" s="1">
         <f t="shared" si="11"/>
-        <v>188</v>
+        <v>150</v>
       </c>
       <c r="C198" t="s">
         <v>557</v>
@@ -11390,7 +11494,7 @@
     <row r="199" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B199" s="1">
         <f t="shared" si="11"/>
-        <v>189</v>
+        <v>151</v>
       </c>
       <c r="C199" t="s">
         <v>559</v>
@@ -11402,7 +11506,7 @@
     <row r="200" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B200" s="1">
         <f t="shared" si="11"/>
-        <v>190</v>
+        <v>152</v>
       </c>
       <c r="C200" t="s">
         <v>561</v>
@@ -11414,7 +11518,7 @@
     <row r="201" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B201" s="1">
         <f t="shared" si="11"/>
-        <v>191</v>
+        <v>153</v>
       </c>
       <c r="C201" t="s">
         <v>563</v>
@@ -11426,7 +11530,7 @@
     <row r="202" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B202" s="1">
         <f t="shared" si="11"/>
-        <v>192</v>
+        <v>154</v>
       </c>
       <c r="C202" t="s">
         <v>565</v>
@@ -11438,7 +11542,7 @@
     <row r="203" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B203" s="1">
         <f t="shared" si="11"/>
-        <v>193</v>
+        <v>155</v>
       </c>
       <c r="C203" t="s">
         <v>567</v>
@@ -11450,7 +11554,7 @@
     <row r="204" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B204" s="1">
         <f t="shared" si="11"/>
-        <v>194</v>
+        <v>156</v>
       </c>
       <c r="C204" t="s">
         <v>569</v>
@@ -11462,7 +11566,7 @@
     <row r="205" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B205" s="1">
         <f t="shared" si="11"/>
-        <v>195</v>
+        <v>157</v>
       </c>
       <c r="C205" t="s">
         <v>571</v>
@@ -11474,7 +11578,7 @@
     <row r="206" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B206" s="1">
         <f t="shared" si="11"/>
-        <v>196</v>
+        <v>158</v>
       </c>
       <c r="C206" t="s">
         <v>573</v>
@@ -11486,7 +11590,7 @@
     <row r="207" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B207" s="1">
         <f t="shared" si="11"/>
-        <v>197</v>
+        <v>159</v>
       </c>
       <c r="C207" t="s">
         <v>575</v>
@@ -11498,7 +11602,7 @@
     <row r="208" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B208" s="1">
         <f t="shared" si="11"/>
-        <v>198</v>
+        <v>160</v>
       </c>
       <c r="C208" t="s">
         <v>577</v>
@@ -11510,7 +11614,7 @@
     <row r="209" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B209" s="1">
         <f t="shared" si="11"/>
-        <v>199</v>
+        <v>161</v>
       </c>
       <c r="C209" t="s">
         <v>579</v>
@@ -11522,7 +11626,7 @@
     <row r="210" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B210" s="1">
         <f t="shared" si="11"/>
-        <v>200</v>
+        <v>162</v>
       </c>
       <c r="C210" t="s">
         <v>581</v>
@@ -11534,7 +11638,7 @@
     <row r="211" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B211" s="1">
         <f t="shared" si="11"/>
-        <v>201</v>
+        <v>163</v>
       </c>
       <c r="C211" t="s">
         <v>583</v>
@@ -11546,7 +11650,7 @@
     <row r="212" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B212" s="1">
         <f t="shared" si="11"/>
-        <v>202</v>
+        <v>164</v>
       </c>
       <c r="C212" t="s">
         <v>585</v>
@@ -11558,7 +11662,7 @@
     <row r="213" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B213" s="1">
         <f t="shared" si="11"/>
-        <v>203</v>
+        <v>165</v>
       </c>
       <c r="C213" t="s">
         <v>587</v>
@@ -11571,7 +11675,7 @@
     <row r="214" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B214" s="1">
         <f t="shared" ref="B214:B227" si="12">B213+1</f>
-        <v>204</v>
+        <v>166</v>
       </c>
       <c r="C214" t="s">
         <v>590</v>
@@ -11583,7 +11687,7 @@
     <row r="215" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B215" s="1">
         <f t="shared" si="12"/>
-        <v>205</v>
+        <v>167</v>
       </c>
       <c r="C215" t="s">
         <v>591</v>
@@ -11595,7 +11699,7 @@
     <row r="216" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B216" s="1">
         <f t="shared" si="12"/>
-        <v>206</v>
+        <v>168</v>
       </c>
       <c r="C216" t="s">
         <v>356</v>
@@ -11607,7 +11711,7 @@
     <row r="217" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B217" s="1">
         <f t="shared" si="12"/>
-        <v>207</v>
+        <v>169</v>
       </c>
       <c r="C217" t="s">
         <v>593</v>
@@ -11619,7 +11723,7 @@
     <row r="218" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B218" s="1">
         <f t="shared" si="12"/>
-        <v>208</v>
+        <v>170</v>
       </c>
       <c r="C218" t="s">
         <v>595</v>
@@ -11631,7 +11735,7 @@
     <row r="219" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B219" s="1">
         <f t="shared" si="12"/>
-        <v>209</v>
+        <v>171</v>
       </c>
       <c r="C219" t="s">
         <v>597</v>
@@ -11643,7 +11747,7 @@
     <row r="220" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B220" s="1">
         <f t="shared" si="12"/>
-        <v>210</v>
+        <v>172</v>
       </c>
       <c r="C220" t="s">
         <v>599</v>
@@ -11655,7 +11759,7 @@
     <row r="221" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B221" s="1">
         <f t="shared" si="12"/>
-        <v>211</v>
+        <v>173</v>
       </c>
       <c r="C221" t="s">
         <v>601</v>
@@ -11667,7 +11771,7 @@
     <row r="222" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B222" s="1">
         <f t="shared" si="12"/>
-        <v>212</v>
+        <v>174</v>
       </c>
       <c r="C222" t="s">
         <v>603</v>
@@ -11679,7 +11783,7 @@
     <row r="223" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B223" s="1">
         <f t="shared" si="12"/>
-        <v>213</v>
+        <v>175</v>
       </c>
       <c r="C223" t="s">
         <v>605</v>
@@ -11691,7 +11795,7 @@
     <row r="224" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B224" s="1">
         <f t="shared" si="12"/>
-        <v>214</v>
+        <v>176</v>
       </c>
       <c r="C224" t="s">
         <v>607</v>
@@ -11703,7 +11807,7 @@
     <row r="225" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B225" s="1">
         <f t="shared" si="12"/>
-        <v>215</v>
+        <v>177</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>609</v>
@@ -11715,7 +11819,7 @@
     <row r="226" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B226" s="1">
         <f t="shared" si="12"/>
-        <v>216</v>
+        <v>178</v>
       </c>
       <c r="C226" t="s">
         <v>611</v>
@@ -11727,7 +11831,7 @@
     <row r="227" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B227" s="1">
         <f t="shared" si="12"/>
-        <v>217</v>
+        <v>179</v>
       </c>
       <c r="C227" t="s">
         <v>613</v>
@@ -11782,7 +11886,7 @@
     <hyperlink ref="C115" r:id="rId35" xr:uid="{B83625D8-44D2-4842-9139-F29C8D5F2D8E}"/>
     <hyperlink ref="C155" r:id="rId36" xr:uid="{5FF32E6A-C6C7-4793-8271-BD230B9C7641}"/>
     <hyperlink ref="C64" r:id="rId37" xr:uid="{E5739E03-9FE4-4D05-90C8-36ABF7D078CB}"/>
-    <hyperlink ref="C66" r:id="rId38" xr:uid="{25285F59-771C-40DB-8B78-E1E454C61406}"/>
+    <hyperlink ref="C67" r:id="rId38" xr:uid="{25285F59-771C-40DB-8B78-E1E454C61406}"/>
     <hyperlink ref="C162" r:id="rId39" xr:uid="{C000061C-001D-4088-90A4-B672D181D3C5}"/>
     <hyperlink ref="C30" r:id="rId40" xr:uid="{6A1F812B-EA91-4B3C-B4DC-88F792A7D0DE}"/>
     <hyperlink ref="C46" r:id="rId41" xr:uid="{6930A656-C59A-465F-8634-B30B4FEF47BC}"/>
@@ -11810,7 +11914,7 @@
     <hyperlink ref="C36" r:id="rId63" xr:uid="{BC97A7B7-8716-48D0-BA90-60A75E6A24CE}"/>
     <hyperlink ref="C45" r:id="rId64" xr:uid="{AD16E898-B1E4-4F25-8E21-E2BC1C6FE9AD}"/>
     <hyperlink ref="C52" r:id="rId65" xr:uid="{E9207892-DA1F-48D2-B2C3-EFA59FCA8A47}"/>
-    <hyperlink ref="C68" r:id="rId66" xr:uid="{DE2D1DDB-B5B7-4055-B885-0CD9E7670070}"/>
+    <hyperlink ref="C69" r:id="rId66" xr:uid="{DE2D1DDB-B5B7-4055-B885-0CD9E7670070}"/>
     <hyperlink ref="C38" r:id="rId67" xr:uid="{9DD12163-063E-4F73-89A5-34D8E8AC0534}"/>
     <hyperlink ref="C39" r:id="rId68" xr:uid="{30732F31-0D9B-4774-8215-75872BFC9B96}"/>
     <hyperlink ref="C61" r:id="rId69" xr:uid="{1D3A6A47-22C9-4CC1-94BD-20DE3BB08016}"/>
@@ -11818,7 +11922,7 @@
     <hyperlink ref="C54" r:id="rId71" xr:uid="{144D13FD-59BD-499B-A0B4-B06985623C68}"/>
     <hyperlink ref="C154" r:id="rId72" xr:uid="{E48CD1EB-CFA1-47B1-BD8B-09F09CDD4FA4}"/>
     <hyperlink ref="C113" r:id="rId73" xr:uid="{6E9AFF81-F520-4A86-9FC2-D5CFE68E7EB7}"/>
-    <hyperlink ref="C65" r:id="rId74" xr:uid="{ED527D70-0B51-4151-8378-8C40B68FF19D}"/>
+    <hyperlink ref="C66" r:id="rId74" xr:uid="{ED527D70-0B51-4151-8378-8C40B68FF19D}"/>
     <hyperlink ref="C51" r:id="rId75" xr:uid="{A902B26E-CA39-4DC5-9F23-4459D8D315E8}"/>
     <hyperlink ref="C56" r:id="rId76" xr:uid="{5F0313F8-3376-4F67-9822-E1412CAA5959}"/>
     <hyperlink ref="C94" r:id="rId77" xr:uid="{AE3A3FD9-E651-4A72-81DB-B29CC61B516B}"/>
@@ -11826,7 +11930,7 @@
     <hyperlink ref="C96" r:id="rId79" xr:uid="{C6F461C3-F385-4BE1-8914-0B22F9A9FF52}"/>
     <hyperlink ref="C44" r:id="rId80" xr:uid="{98D02B7D-F218-457E-B156-7FE773CF515A}"/>
     <hyperlink ref="C43" r:id="rId81" xr:uid="{02CB6FD9-C55D-44A1-9F2E-6A96A222EE6B}"/>
-    <hyperlink ref="C67" r:id="rId82" xr:uid="{C691BA46-1169-4CAF-84E5-2A83E1B5404A}"/>
+    <hyperlink ref="C68" r:id="rId82" xr:uid="{C691BA46-1169-4CAF-84E5-2A83E1B5404A}"/>
     <hyperlink ref="C50" r:id="rId83" xr:uid="{425EA3DE-2A59-4B96-B380-B688A4EDE233}"/>
     <hyperlink ref="C49" r:id="rId84" xr:uid="{1F24E207-02BC-4A1F-B083-69F8E95AC067}"/>
     <hyperlink ref="C59" r:id="rId85" xr:uid="{CE56D1ED-1CAA-4667-A3D9-82426599D26C}"/>
@@ -11834,9 +11938,10 @@
     <hyperlink ref="C95" r:id="rId87" xr:uid="{ED810682-5208-4265-9E0E-6746A399EA34}"/>
     <hyperlink ref="C116" r:id="rId88" xr:uid="{44DEB74A-F098-4876-A279-D1E6237DF8DB}"/>
     <hyperlink ref="C63" r:id="rId89" xr:uid="{ADF59BEC-B8D8-4144-ADEB-041425B69409}"/>
+    <hyperlink ref="C65" r:id="rId90" xr:uid="{5448F263-AB4A-41FB-B7B9-A94746C9D9E1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId90"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId91"/>
 </worksheet>
 </file>
 
@@ -12131,8 +12236,8 @@
     </row>
     <row r="8" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
-        <f>Main!B80+1</f>
-        <v>69</v>
+        <f>Main!B81+1</f>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
         <v>370</v>
@@ -12277,13 +12382,13 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED149DB-8F62-4CB2-88E6-87DDBD9316FC}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:I86"/>
+  <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C56" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C70" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H85" sqref="H85"/>
+      <selection pane="bottomRight" activeCell="E94" sqref="E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12291,6 +12396,7 @@
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -12415,471 +12521,604 @@
       <c r="B15" t="s">
         <v>505</v>
       </c>
+      <c r="C15">
+        <v>2018</v>
+      </c>
+      <c r="E15" t="s">
+        <v>634</v>
+      </c>
+      <c r="F15" t="s">
+        <v>635</v>
+      </c>
+      <c r="G15" t="s">
+        <v>640</v>
+      </c>
+      <c r="H15" s="13">
+        <v>44817</v>
+      </c>
+      <c r="I15" t="s">
+        <v>633</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
+        <v>505</v>
+      </c>
+      <c r="C16">
+        <v>2018</v>
+      </c>
+      <c r="E16" t="s">
+        <v>403</v>
+      </c>
+      <c r="F16" t="s">
+        <v>636</v>
+      </c>
+      <c r="G16" t="s">
+        <v>639</v>
+      </c>
+      <c r="H16" s="13">
+        <v>44362</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>505</v>
+      </c>
+      <c r="C17">
+        <v>2018</v>
+      </c>
+      <c r="E17" t="s">
+        <v>623</v>
+      </c>
+      <c r="F17" t="s">
+        <v>637</v>
+      </c>
+      <c r="G17" t="s">
+        <v>639</v>
+      </c>
+      <c r="H17" s="13">
+        <v>44173</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>505</v>
+      </c>
+      <c r="C18">
+        <v>2018</v>
+      </c>
+      <c r="E18" t="s">
+        <v>333</v>
+      </c>
+      <c r="F18" t="s">
+        <v>625</v>
+      </c>
+      <c r="G18" t="s">
+        <v>638</v>
+      </c>
+      <c r="H18" s="13">
+        <v>44118</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
         <v>465</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>491</v>
+        <v>472</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>492</v>
+        <v>473</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>494</v>
+        <v>474</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>475</v>
+        <v>492</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>476</v>
+        <v>494</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>477</v>
+        <v>493</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B49" t="s">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B50" t="s">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B51" t="s">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B52" t="s">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B53" t="s">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B54" t="s">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B55" t="s">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B56" t="s">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B57" t="s">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B58" t="s">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B59" t="s">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B60" t="s">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B61" t="s">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
         <v>286</v>
-      </c>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B62" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B63" t="s">
-        <v>288</v>
-      </c>
-      <c r="C63">
-        <v>2019</v>
-      </c>
-      <c r="D63" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B64" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
-        <v>296</v>
+        <v>288</v>
+      </c>
+      <c r="C66">
+        <v>2019</v>
+      </c>
+      <c r="D66" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
-        <v>331</v>
-      </c>
-      <c r="C67">
-        <v>2019</v>
-      </c>
-      <c r="D67" t="s">
-        <v>339</v>
-      </c>
-      <c r="E67" t="s">
-        <v>333</v>
-      </c>
-      <c r="F67" t="s">
-        <v>337</v>
-      </c>
-      <c r="G67" t="s">
-        <v>336</v>
-      </c>
-      <c r="H67" s="13">
-        <v>44599</v>
+        <v>291</v>
       </c>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
-        <v>346</v>
-      </c>
-      <c r="E68" t="s">
-        <v>333</v>
-      </c>
-      <c r="F68" t="s">
-        <v>347</v>
+        <v>293</v>
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
-        <v>348</v>
+        <v>296</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
-        <v>349</v>
-      </c>
-      <c r="I70" t="s">
-        <v>350</v>
+        <v>331</v>
+      </c>
+      <c r="C70">
+        <v>2019</v>
+      </c>
+      <c r="D70" t="s">
+        <v>339</v>
+      </c>
+      <c r="E70" t="s">
+        <v>333</v>
+      </c>
+      <c r="F70" t="s">
+        <v>337</v>
+      </c>
+      <c r="G70" t="s">
+        <v>336</v>
+      </c>
+      <c r="H70" s="13">
+        <v>44599</v>
       </c>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
-        <v>394</v>
+        <v>346</v>
+      </c>
+      <c r="E71" t="s">
+        <v>333</v>
+      </c>
+      <c r="F71" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
-        <v>397</v>
-      </c>
-      <c r="C72" t="s">
-        <v>398</v>
-      </c>
-      <c r="E72" t="s">
-        <v>333</v>
-      </c>
-      <c r="F72" t="s">
-        <v>399</v>
-      </c>
-      <c r="H72" s="13">
-        <v>43466</v>
-      </c>
-      <c r="I72" t="s">
-        <v>400</v>
+        <v>348</v>
       </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
-        <v>401</v>
+        <v>349</v>
+      </c>
+      <c r="I73" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
-        <v>402</v>
-      </c>
-      <c r="E74" t="s">
-        <v>403</v>
-      </c>
-      <c r="F74" t="s">
-        <v>404</v>
-      </c>
-      <c r="I74" t="s">
-        <v>405</v>
+        <v>394</v>
       </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
-        <v>409</v>
+        <v>397</v>
+      </c>
+      <c r="C75" t="s">
+        <v>398</v>
       </c>
       <c r="E75" t="s">
-        <v>403</v>
+        <v>333</v>
       </c>
       <c r="F75" t="s">
-        <v>410</v>
+        <v>399</v>
+      </c>
+      <c r="H75" s="13">
+        <v>43466</v>
+      </c>
+      <c r="I75" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
-        <v>427</v>
+        <v>401</v>
       </c>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
-        <v>431</v>
+        <v>402</v>
+      </c>
+      <c r="E77" t="s">
+        <v>403</v>
+      </c>
+      <c r="F77" t="s">
+        <v>404</v>
+      </c>
+      <c r="I77" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
-        <v>433</v>
+        <v>409</v>
+      </c>
+      <c r="E78" t="s">
+        <v>403</v>
+      </c>
+      <c r="F78" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
-        <v>438</v>
-      </c>
-      <c r="I79" t="s">
-        <v>439</v>
+        <v>427</v>
       </c>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
-        <v>457</v>
+        <v>431</v>
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
-        <v>521</v>
+        <v>433</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
-        <v>537</v>
+        <v>438</v>
       </c>
       <c r="I82" t="s">
-        <v>538</v>
+        <v>439</v>
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
-        <v>541</v>
-      </c>
-      <c r="I83" t="s">
-        <v>538</v>
+        <v>457</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
-        <v>627</v>
-      </c>
-      <c r="C84">
-        <v>2018</v>
-      </c>
-      <c r="D84" t="s">
-        <v>630</v>
-      </c>
-      <c r="E84" t="s">
-        <v>628</v>
-      </c>
-      <c r="F84" t="s">
-        <v>629</v>
-      </c>
-      <c r="H84" s="13">
-        <v>43251</v>
+        <v>521</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
-        <v>627</v>
-      </c>
-      <c r="C85">
-        <v>2018</v>
-      </c>
-      <c r="D85" t="s">
-        <v>630</v>
-      </c>
-      <c r="E85" t="s">
-        <v>626</v>
-      </c>
-      <c r="F85" t="s">
-        <v>625</v>
+        <v>537</v>
+      </c>
+      <c r="I85" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
+        <v>541</v>
+      </c>
+      <c r="I86" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B87" t="s">
         <v>627</v>
       </c>
-      <c r="C86">
+      <c r="C87">
         <v>2018</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D87" t="s">
         <v>630</v>
       </c>
-      <c r="E86" t="s">
+      <c r="E87" t="s">
+        <v>628</v>
+      </c>
+      <c r="F87" t="s">
+        <v>629</v>
+      </c>
+      <c r="H87" s="13">
+        <v>43251</v>
+      </c>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B88" t="s">
+        <v>627</v>
+      </c>
+      <c r="C88">
+        <v>2018</v>
+      </c>
+      <c r="D88" t="s">
+        <v>630</v>
+      </c>
+      <c r="E88" t="s">
+        <v>626</v>
+      </c>
+      <c r="F88" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B89" t="s">
+        <v>627</v>
+      </c>
+      <c r="C89">
+        <v>2018</v>
+      </c>
+      <c r="D89" t="s">
+        <v>630</v>
+      </c>
+      <c r="E89" t="s">
         <v>623</v>
       </c>
-      <c r="F86" t="s">
+      <c r="F89" t="s">
         <v>624</v>
+      </c>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B90" t="s">
+        <v>631</v>
+      </c>
+      <c r="I90" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="91" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B91" t="s">
+        <v>641</v>
+      </c>
+      <c r="E91" t="s">
+        <v>623</v>
+      </c>
+      <c r="F91" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B92" t="s">
+        <v>641</v>
+      </c>
+      <c r="E92" t="s">
+        <v>333</v>
+      </c>
+      <c r="F92" t="s">
+        <v>642</v>
+      </c>
+      <c r="G92" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="93" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B93" t="s">
+        <v>645</v>
+      </c>
+      <c r="E93" t="s">
+        <v>403</v>
+      </c>
+      <c r="F93" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="94" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B94" t="s">
+        <v>645</v>
+      </c>
+      <c r="E94" t="s">
+        <v>634</v>
+      </c>
+      <c r="F94" t="s">
+        <v>629</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated AAPL, created PYPL shell
</commit_message>
<xml_diff>
--- a/Biopharma.xlsx
+++ b/Biopharma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5238C581-CA6D-4EEF-B19B-2FCEFB0CD2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310841A5-438B-4177-8AC2-19F890824BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8655" yWindow="5085" windowWidth="38700" windowHeight="15345" xr2:uid="{17641224-F2C3-441B-B85B-BB32567FE633}"/>
+    <workbookView xWindow="11415" yWindow="1290" windowWidth="38700" windowHeight="15345" xr2:uid="{17641224-F2C3-441B-B85B-BB32567FE633}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -143,7 +143,7 @@
     <author>Martin</author>
   </authors>
   <commentList>
-    <comment ref="AE4" authorId="0" shapeId="0" xr:uid="{B2BE9396-5825-4BE7-B3C2-AD4180B21E1E}">
+    <comment ref="AE6" authorId="0" shapeId="0" xr:uid="{B2BE9396-5825-4BE7-B3C2-AD4180B21E1E}">
       <text>
         <r>
           <rPr>
@@ -167,7 +167,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG8" authorId="0" shapeId="0" xr:uid="{E932D832-A0D4-461F-9F84-E6D0EDCD4316}">
+    <comment ref="AG12" authorId="0" shapeId="0" xr:uid="{E932D832-A0D4-461F-9F84-E6D0EDCD4316}">
       <text>
         <r>
           <rPr>
@@ -218,7 +218,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="674">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="679">
   <si>
     <t>Exarta</t>
   </si>
@@ -2240,6 +2240,21 @@
   </si>
   <si>
     <t>Q123</t>
+  </si>
+  <si>
+    <t>Remicade</t>
+  </si>
+  <si>
+    <t>Zytiga</t>
+  </si>
+  <si>
+    <t>Imbruvica</t>
+  </si>
+  <si>
+    <t>Darzalex</t>
+  </si>
+  <si>
+    <t>Tremfya</t>
   </si>
 </sst>
 </file>
@@ -2326,7 +2341,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2407,6 +2422,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2487,73 +2503,73 @@
       <sheetName val="Duragesic"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
       <sheetData sheetId="6">
         <row r="3">
           <cell r="Q3">
-            <v>2661</v>
+            <v>2598</v>
           </cell>
         </row>
         <row r="5">
           <cell r="Q5">
-            <v>34079</v>
+            <v>32308</v>
           </cell>
         </row>
         <row r="6">
           <cell r="Q6">
-            <v>32027</v>
+            <v>52907</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="30" refreshError="1"/>
+      <sheetData sheetId="31" refreshError="1"/>
+      <sheetData sheetId="32" refreshError="1"/>
+      <sheetData sheetId="33" refreshError="1"/>
+      <sheetData sheetId="34" refreshError="1"/>
+      <sheetData sheetId="35" refreshError="1"/>
+      <sheetData sheetId="36" refreshError="1"/>
+      <sheetData sheetId="37" refreshError="1"/>
+      <sheetData sheetId="38" refreshError="1"/>
+      <sheetData sheetId="39" refreshError="1"/>
+      <sheetData sheetId="40" refreshError="1"/>
+      <sheetData sheetId="41" refreshError="1"/>
+      <sheetData sheetId="42" refreshError="1"/>
+      <sheetData sheetId="43" refreshError="1"/>
+      <sheetData sheetId="44" refreshError="1"/>
+      <sheetData sheetId="45" refreshError="1"/>
+      <sheetData sheetId="46" refreshError="1"/>
+      <sheetData sheetId="47" refreshError="1"/>
+      <sheetData sheetId="48" refreshError="1"/>
+      <sheetData sheetId="49" refreshError="1"/>
+      <sheetData sheetId="50" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3698,7 +3714,7 @@
       <sheetName val="Skyrizi"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="3">
           <cell r="K3">
@@ -3716,12 +3732,12 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6361,7 +6377,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K4" sqref="K4"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6383,7 +6399,7 @@
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B1" s="1">
         <f ca="1">RANDBETWEEN(1,B168)</f>
-        <v>18</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
@@ -6509,25 +6525,25 @@
       </c>
       <c r="F4" s="6">
         <f>E4*[1]Main!$Q$3</f>
-        <v>431481.15</v>
+        <v>421265.7</v>
       </c>
       <c r="G4" s="6">
         <f>+[1]Main!$Q$5-[1]Main!$Q$6</f>
-        <v>2052</v>
+        <v>-20599</v>
       </c>
       <c r="H4" s="6">
         <f t="shared" ref="H4:H19" si="0">F4-G4</f>
-        <v>429429.15</v>
+        <v>441864.7</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>673</v>
       </c>
       <c r="J4" s="6">
         <f>+[1]Main!$Q$3</f>
-        <v>2661</v>
+        <v>2598</v>
       </c>
       <c r="K4" s="9">
-        <v>45039</v>
+        <v>45048</v>
       </c>
       <c r="L4" s="9"/>
       <c r="M4" s="9"/>
@@ -12144,28 +12160,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A489F4D5-421B-432D-9B8B-67BB999210AF}">
-  <dimension ref="A1:CC17"/>
+  <dimension ref="A1:CW23"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L17" sqref="L17"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" customWidth="1"/>
     <col min="5" max="7" width="9.140625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="2" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:101" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>659</v>
       </c>
@@ -12191,7 +12208,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="3" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>655</v>
       </c>
@@ -12214,1456 +12231,2199 @@
         <v>568.5</v>
       </c>
     </row>
-    <row r="4" spans="1:81" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
+        <v>678</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="30">
+        <v>47</v>
+      </c>
+      <c r="F4" s="30">
+        <v>72</v>
+      </c>
+      <c r="G4" s="30">
+        <v>126</v>
+      </c>
+      <c r="H4" s="30">
+        <v>171</v>
+      </c>
+      <c r="I4" s="30">
+        <v>175</v>
+      </c>
+      <c r="J4" s="30">
+        <v>217</v>
+      </c>
+      <c r="K4" s="30">
+        <v>235</v>
+      </c>
+      <c r="L4" s="30">
+        <v>290</v>
+      </c>
+      <c r="M4" s="30">
+        <v>270</v>
+      </c>
+      <c r="N4" s="30">
+        <v>296</v>
+      </c>
+      <c r="O4" s="30">
+        <v>342</v>
+      </c>
+      <c r="P4" s="30">
+        <v>327</v>
+      </c>
+      <c r="Q4" s="30">
+        <v>382</v>
+      </c>
+      <c r="R4" s="30">
+        <v>418</v>
+      </c>
+      <c r="S4" s="30">
+        <v>479</v>
+      </c>
+      <c r="T4" s="30">
+        <v>537</v>
+      </c>
+      <c r="U4" s="30">
+        <v>693</v>
+      </c>
+      <c r="V4" s="30">
+        <v>590</v>
+      </c>
+      <c r="W4" s="30">
+        <v>597</v>
+      </c>
+      <c r="X4" s="30">
+        <v>729</v>
+      </c>
+      <c r="Y4" s="30">
+        <v>752</v>
+      </c>
+      <c r="Z4" s="30">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="5" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>677</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="28">
+        <v>20</v>
+      </c>
+      <c r="F5" s="28">
+        <v>101</v>
+      </c>
+      <c r="G5" s="28">
+        <v>108</v>
+      </c>
+      <c r="I5">
+        <v>200</v>
+      </c>
+      <c r="J5">
+        <v>255</v>
+      </c>
+      <c r="K5">
+        <v>299</v>
+      </c>
+      <c r="L5">
+        <v>317</v>
+      </c>
+      <c r="M5">
+        <v>371</v>
+      </c>
+      <c r="N5">
+        <v>432</v>
+      </c>
+      <c r="O5">
+        <v>511</v>
+      </c>
+      <c r="P5">
+        <v>498</v>
+      </c>
+      <c r="Q5">
+        <v>584</v>
+      </c>
+      <c r="R5">
+        <v>629</v>
+      </c>
+      <c r="S5">
+        <v>774</v>
+      </c>
+      <c r="T5">
+        <v>765</v>
+      </c>
+      <c r="U5">
+        <v>830</v>
+      </c>
+      <c r="V5">
+        <v>937</v>
+      </c>
+      <c r="W5">
+        <v>901</v>
+      </c>
+      <c r="X5">
+        <v>1099</v>
+      </c>
+      <c r="Y5">
+        <v>1253</v>
+      </c>
+      <c r="Z5">
+        <v>1365</v>
+      </c>
+      <c r="AA5">
+        <v>1433</v>
+      </c>
+      <c r="AB5">
+        <v>1580</v>
+      </c>
+      <c r="AC5">
+        <v>1645</v>
+      </c>
+      <c r="AD5">
+        <v>1856</v>
+      </c>
+      <c r="AE5">
+        <v>1986</v>
+      </c>
+      <c r="AF5">
+        <v>2052</v>
+      </c>
+      <c r="AG5">
+        <v>2083</v>
+      </c>
+      <c r="AH5">
+        <v>2264</v>
+      </c>
+    </row>
+    <row r="6" spans="1:101" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
         <v>672</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="30">
-        <v>32.5</v>
-      </c>
-      <c r="F4" s="30">
-        <v>61.3</v>
-      </c>
-      <c r="G4" s="30">
-        <v>106.8</v>
-      </c>
-      <c r="H4" s="30">
-        <v>161.4</v>
-      </c>
-      <c r="I4" s="30">
-        <v>182.8</v>
-      </c>
-      <c r="J4" s="30">
-        <v>228.8</v>
-      </c>
-      <c r="K4" s="30">
-        <v>233</v>
-      </c>
-      <c r="L4" s="30">
-        <v>310</v>
-      </c>
-      <c r="M4" s="30">
-        <v>349</v>
-      </c>
-      <c r="N4" s="30">
-        <v>424.1</v>
-      </c>
-      <c r="O4" s="30">
-        <v>441.8</v>
-      </c>
-      <c r="P4" s="30">
-        <v>519.5</v>
-      </c>
-      <c r="Q4" s="30">
-        <v>513.20000000000005</v>
-      </c>
-      <c r="R4" s="30">
-        <v>628.29999999999995</v>
-      </c>
-      <c r="S4" s="30">
-        <v>605.1</v>
-      </c>
-      <c r="T4" s="30">
-        <v>654.4</v>
-      </c>
-      <c r="U4" s="30">
-        <v>716.4</v>
-      </c>
-      <c r="V4" s="30">
-        <v>721.2</v>
-      </c>
-      <c r="W4" s="30">
-        <v>709.3</v>
-      </c>
-      <c r="X4" s="30">
-        <v>744.4</v>
-      </c>
-      <c r="Y4" s="30">
-        <v>790.2</v>
-      </c>
-      <c r="Z4" s="30">
-        <v>830.8</v>
-      </c>
-      <c r="AA4" s="30">
-        <v>803.2</v>
-      </c>
-      <c r="AB4" s="30">
-        <v>867.7</v>
-      </c>
-      <c r="AC4" s="30">
-        <v>825.3</v>
-      </c>
-      <c r="AD4" s="30">
-        <v>984.6</v>
-      </c>
-      <c r="AE4" s="30">
-        <v>908.8</v>
-      </c>
-      <c r="AF4" s="30">
-        <v>1003.4</v>
-      </c>
-      <c r="AG4" s="30">
-        <v>1068.5999999999999</v>
-      </c>
-      <c r="AH4" s="30">
-        <v>1180.7</v>
-      </c>
-      <c r="AI4" s="30">
-        <v>1114.9000000000001</v>
-      </c>
-      <c r="AJ4" s="30">
-        <v>1223.0999999999999</v>
-      </c>
-      <c r="AK4" s="30">
-        <v>1235.8</v>
-      </c>
-      <c r="AL4" s="30">
-        <v>1420.4</v>
-      </c>
-      <c r="AM4" s="30">
-        <v>1328.2</v>
-      </c>
-      <c r="AN4" s="30">
-        <v>1497.2</v>
-      </c>
-      <c r="AO4" s="30">
-        <v>1375.8</v>
-      </c>
-      <c r="AP4" s="30">
-        <v>883.2</v>
-      </c>
-      <c r="AQ4" s="30">
-        <v>478.2</v>
-      </c>
-      <c r="AR4" s="30">
-        <v>401.3</v>
-      </c>
-      <c r="AS4" s="30">
-        <v>368</v>
-      </c>
-      <c r="AT4" s="30">
-        <v>367.3</v>
-      </c>
-      <c r="AU4" s="30">
-        <v>287</v>
-      </c>
-      <c r="AV4" s="30">
-        <v>274.10000000000002</v>
-      </c>
-      <c r="AW4" s="30">
-        <v>242.9</v>
-      </c>
-      <c r="AX4" s="30">
-        <v>223.6</v>
-      </c>
-      <c r="AY4" s="30">
-        <v>198.7</v>
-      </c>
-      <c r="AZ4" s="30">
-        <v>236.5</v>
-      </c>
-      <c r="BA4" s="30">
-        <v>313.5</v>
-      </c>
-      <c r="BB4" s="30">
-        <v>181.8</v>
-      </c>
-      <c r="BC4" s="30">
-        <v>174.6</v>
-      </c>
-      <c r="BD4" s="30">
-        <v>206.6</v>
-      </c>
-      <c r="BE4" s="30">
-        <v>183.2</v>
-      </c>
-      <c r="BF4" s="30">
-        <v>192.8</v>
-      </c>
-      <c r="BG4" s="30">
-        <v>169.6</v>
-      </c>
-      <c r="BH4" s="30">
-        <v>181.9</v>
-      </c>
-      <c r="BI4" s="30">
-        <v>172</v>
-      </c>
-      <c r="BJ4" s="30">
-        <v>184.5</v>
-      </c>
-      <c r="BK4" s="30">
-        <v>164.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:81" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>664</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="29">
-        <v>19.3</v>
-      </c>
-      <c r="F5" s="29">
-        <v>32.5</v>
-      </c>
-      <c r="G5" s="29">
-        <v>61.3</v>
-      </c>
-      <c r="H5" s="29">
-        <v>96.6</v>
-      </c>
-      <c r="I5" s="29">
-        <v>138.69999999999999</v>
-      </c>
-      <c r="J5" s="29">
-        <v>151.30000000000001</v>
-      </c>
-      <c r="K5" s="29">
-        <v>172.5</v>
-      </c>
-      <c r="L5" s="29">
-        <v>146.5</v>
-      </c>
-      <c r="M5" s="29">
-        <v>220.1</v>
-      </c>
-      <c r="N5" s="29">
-        <v>263.89999999999998</v>
-      </c>
-      <c r="O5" s="29">
-        <v>307</v>
-      </c>
-      <c r="P5" s="29">
-        <v>252.5</v>
-      </c>
-      <c r="Q5" s="29">
-        <v>353.8</v>
-      </c>
-      <c r="R5" s="29">
-        <v>340</v>
-      </c>
-      <c r="S5" s="29">
-        <v>420.1</v>
-      </c>
-      <c r="T5" s="29">
-        <v>443.5</v>
-      </c>
-      <c r="U5" s="29">
-        <v>395.2</v>
-      </c>
-      <c r="V5" s="29">
-        <v>454.5</v>
-      </c>
-      <c r="W5" s="29">
-        <v>495.3</v>
-      </c>
-      <c r="X5" s="29">
-        <v>403.2</v>
-      </c>
-      <c r="Y5" s="29">
-        <v>569.1</v>
-      </c>
-      <c r="Z5" s="29">
-        <v>593.1</v>
-      </c>
-      <c r="AA5" s="29">
-        <v>647.4</v>
-      </c>
-      <c r="AB5" s="29">
-        <v>488.1</v>
-      </c>
-      <c r="AC5" s="29">
-        <v>606.20000000000005</v>
-      </c>
-      <c r="AD5" s="29">
-        <v>679.9</v>
-      </c>
-      <c r="AE5" s="29">
-        <v>707.8</v>
-      </c>
-      <c r="AF5" s="29">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="6" spans="1:81" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>660</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
       </c>
       <c r="E6" s="30">
-        <v>21</v>
+        <v>32.5</v>
       </c>
       <c r="F6" s="30">
-        <v>29.7</v>
+        <v>61.3</v>
       </c>
       <c r="G6" s="30">
-        <v>57.7</v>
+        <v>106.8</v>
       </c>
       <c r="H6" s="30">
-        <v>84.5</v>
+        <v>161.4</v>
       </c>
       <c r="I6" s="30">
-        <v>83.1</v>
+        <v>182.8</v>
       </c>
       <c r="J6" s="30">
-        <v>109.4</v>
+        <v>228.8</v>
       </c>
       <c r="K6" s="30">
-        <v>133.9</v>
+        <v>233</v>
       </c>
       <c r="L6" s="30">
-        <v>157.19999999999999</v>
+        <v>310</v>
       </c>
       <c r="M6" s="30">
-        <v>179.1</v>
+        <v>349</v>
       </c>
       <c r="N6" s="30">
-        <v>188</v>
+        <v>424.1</v>
       </c>
       <c r="O6" s="30">
-        <v>208.6</v>
+        <v>441.8</v>
       </c>
       <c r="P6" s="30">
-        <v>234.4</v>
+        <v>519.5</v>
       </c>
       <c r="Q6" s="30">
-        <v>281.60000000000002</v>
+        <v>513.20000000000005</v>
       </c>
       <c r="R6" s="30">
-        <v>269</v>
+        <v>628.29999999999995</v>
       </c>
       <c r="S6" s="30">
-        <v>341.3</v>
+        <v>605.1</v>
       </c>
       <c r="T6" s="30">
-        <v>335.5</v>
+        <v>654.4</v>
       </c>
       <c r="U6" s="30">
-        <v>404.1</v>
+        <v>716.4</v>
       </c>
       <c r="V6" s="30">
-        <v>469.4</v>
+        <v>721.2</v>
       </c>
       <c r="W6" s="30">
-        <v>588.5</v>
+        <v>709.3</v>
       </c>
       <c r="X6" s="30">
-        <v>617.70000000000005</v>
+        <v>744.4</v>
       </c>
       <c r="Y6" s="30">
-        <v>808</v>
+        <v>790.2</v>
       </c>
       <c r="Z6" s="30">
-        <v>750.9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:81" x14ac:dyDescent="0.2">
+        <v>830.8</v>
+      </c>
+      <c r="AA6" s="30">
+        <v>803.2</v>
+      </c>
+      <c r="AB6" s="30">
+        <v>867.7</v>
+      </c>
+      <c r="AC6" s="30">
+        <v>825.3</v>
+      </c>
+      <c r="AD6" s="30">
+        <v>984.6</v>
+      </c>
+      <c r="AE6" s="30">
+        <v>908.8</v>
+      </c>
+      <c r="AF6" s="30">
+        <v>1003.4</v>
+      </c>
+      <c r="AG6" s="30">
+        <v>1068.5999999999999</v>
+      </c>
+      <c r="AH6" s="30">
+        <v>1180.7</v>
+      </c>
+      <c r="AI6" s="30">
+        <v>1114.9000000000001</v>
+      </c>
+      <c r="AJ6" s="30">
+        <v>1223.0999999999999</v>
+      </c>
+      <c r="AK6" s="30">
+        <v>1235.8</v>
+      </c>
+      <c r="AL6" s="30">
+        <v>1420.4</v>
+      </c>
+      <c r="AM6" s="30">
+        <v>1328.2</v>
+      </c>
+      <c r="AN6" s="30">
+        <v>1497.2</v>
+      </c>
+      <c r="AO6" s="30">
+        <v>1375.8</v>
+      </c>
+      <c r="AP6" s="30">
+        <v>883.2</v>
+      </c>
+      <c r="AQ6" s="30">
+        <v>478.2</v>
+      </c>
+      <c r="AR6" s="30">
+        <v>401.3</v>
+      </c>
+      <c r="AS6" s="30">
+        <v>368</v>
+      </c>
+      <c r="AT6" s="30">
+        <v>367.3</v>
+      </c>
+      <c r="AU6" s="30">
+        <v>287</v>
+      </c>
+      <c r="AV6" s="30">
+        <v>274.10000000000002</v>
+      </c>
+      <c r="AW6" s="30">
+        <v>242.9</v>
+      </c>
+      <c r="AX6" s="30">
+        <v>223.6</v>
+      </c>
+      <c r="AY6" s="30">
+        <v>198.7</v>
+      </c>
+      <c r="AZ6" s="30">
+        <v>236.5</v>
+      </c>
+      <c r="BA6" s="30">
+        <v>313.5</v>
+      </c>
+      <c r="BB6" s="30">
+        <v>181.8</v>
+      </c>
+      <c r="BC6" s="30">
+        <v>174.6</v>
+      </c>
+      <c r="BD6" s="30">
+        <v>206.6</v>
+      </c>
+      <c r="BE6" s="30">
+        <v>183.2</v>
+      </c>
+      <c r="BF6" s="30">
+        <v>192.8</v>
+      </c>
+      <c r="BG6" s="30">
+        <v>169.6</v>
+      </c>
+      <c r="BH6" s="30">
+        <v>181.9</v>
+      </c>
+      <c r="BI6" s="30">
+        <v>172</v>
+      </c>
+      <c r="BJ6" s="30">
+        <v>184.5</v>
+      </c>
+      <c r="BK6" s="30">
+        <v>164.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>666</v>
+        <v>675</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="29">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="F7" s="29">
-        <v>18.3</v>
-      </c>
-      <c r="G7" s="29">
-        <v>44.3</v>
-      </c>
-      <c r="H7" s="29">
-        <v>73.7</v>
-      </c>
-      <c r="I7" s="29">
-        <v>112.5</v>
-      </c>
-      <c r="J7" s="29">
-        <v>143.6</v>
-      </c>
-      <c r="K7" s="29">
-        <v>201.3</v>
-      </c>
-      <c r="L7" s="29">
-        <v>243.6</v>
-      </c>
-      <c r="M7" s="29">
-        <v>337</v>
-      </c>
-      <c r="N7" s="29">
-        <v>372.9</v>
-      </c>
-      <c r="O7" s="29">
-        <v>480.2</v>
-      </c>
-      <c r="P7" s="29">
-        <v>527.70000000000005</v>
-      </c>
-      <c r="Q7" s="29">
-        <v>649</v>
-      </c>
-      <c r="R7" s="29">
-        <v>678.3</v>
-      </c>
-      <c r="S7" s="29">
-        <v>779.8</v>
-      </c>
-      <c r="T7" s="29">
-        <v>816.2</v>
-      </c>
-      <c r="U7" s="29">
-        <v>924.7</v>
-      </c>
-      <c r="V7" s="29">
-        <v>879.7</v>
-      </c>
-      <c r="W7" s="29">
-        <v>1028.5</v>
-      </c>
-      <c r="X7" s="29">
-        <v>1011.5</v>
-      </c>
-      <c r="Y7" s="29">
-        <v>1208.0999999999999</v>
-      </c>
-      <c r="Z7" s="29">
-        <v>1229.4000000000001</v>
-      </c>
-      <c r="AA7" s="29">
-        <v>1229.8</v>
-      </c>
-      <c r="AB7" s="29">
-        <v>1106.5999999999999</v>
-      </c>
-      <c r="AC7" s="29">
-        <v>1502.4</v>
-      </c>
-      <c r="AD7" s="29">
-        <v>1452.4</v>
-      </c>
-      <c r="AE7" s="29">
-        <v>1535.6</v>
-      </c>
-      <c r="AF7" s="29">
-        <v>1600.1</v>
-      </c>
-      <c r="AG7" s="29">
-        <v>1883.7</v>
-      </c>
-      <c r="AH7" s="29">
-        <v>1741.3</v>
-      </c>
-      <c r="AI7" s="29">
-        <v>1911.9</v>
-      </c>
-      <c r="AJ7" s="29">
-        <v>1850.4</v>
-      </c>
-      <c r="AK7" s="29">
-        <v>1936.2</v>
-      </c>
-      <c r="AL7" s="29">
-        <v>1977.1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:81" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="E7" s="28">
+        <v>5</v>
+      </c>
+      <c r="G7" s="28">
+        <v>95</v>
+      </c>
+      <c r="I7">
+        <v>200</v>
+      </c>
+      <c r="J7">
+        <v>232</v>
+      </c>
+      <c r="K7">
+        <v>265</v>
+      </c>
+      <c r="L7">
+        <v>264</v>
+      </c>
+      <c r="M7">
+        <v>344</v>
+      </c>
+      <c r="N7">
+        <v>395</v>
+      </c>
+      <c r="O7">
+        <v>464</v>
+      </c>
+      <c r="P7">
+        <v>495</v>
+      </c>
+      <c r="Q7">
+        <v>512</v>
+      </c>
+      <c r="R7">
+        <v>562</v>
+      </c>
+      <c r="S7">
+        <v>568</v>
+      </c>
+      <c r="T7">
+        <v>595</v>
+      </c>
+      <c r="U7">
+        <v>556</v>
+      </c>
+      <c r="V7">
+        <v>546</v>
+      </c>
+      <c r="W7">
+        <v>548</v>
+      </c>
+      <c r="X7">
+        <v>581</v>
+      </c>
+      <c r="Y7">
+        <v>558</v>
+      </c>
+      <c r="Z7">
+        <v>601</v>
+      </c>
+      <c r="AA7">
+        <v>582</v>
+      </c>
+      <c r="AB7">
+        <v>519</v>
+      </c>
+      <c r="AC7">
+        <v>523</v>
+      </c>
+      <c r="AD7">
+        <v>558</v>
+      </c>
+      <c r="AE7">
+        <v>669</v>
+      </c>
+      <c r="AF7">
+        <v>755</v>
+      </c>
+      <c r="AG7">
+        <v>845</v>
+      </c>
+      <c r="AH7">
+        <v>909</v>
+      </c>
+      <c r="AI7">
+        <v>958</v>
+      </c>
+      <c r="AJ7">
+        <v>786</v>
+      </c>
+      <c r="AK7">
+        <v>679</v>
+      </c>
+      <c r="AL7">
+        <v>698</v>
+      </c>
+      <c r="AM7">
+        <v>741</v>
+      </c>
+      <c r="AN7">
+        <v>677</v>
+      </c>
+      <c r="AO7">
+        <v>690</v>
+      </c>
+      <c r="AP7">
+        <v>568</v>
+      </c>
+      <c r="AQ7">
+        <v>590</v>
+      </c>
+      <c r="AR7">
+        <v>622</v>
+      </c>
+      <c r="AS7">
+        <v>638</v>
+      </c>
+      <c r="AT7">
+        <v>563</v>
+      </c>
+      <c r="AU7">
+        <v>548</v>
+      </c>
+      <c r="AV7">
+        <v>548</v>
+      </c>
+      <c r="AW7">
+        <v>539</v>
+      </c>
+      <c r="AX7">
+        <v>505</v>
+      </c>
+      <c r="AY7">
+        <v>456</v>
+      </c>
+      <c r="AZ7">
+        <v>270</v>
+      </c>
+      <c r="BA7">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="8" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>671</v>
+        <v>664</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="30">
-        <v>11.6</v>
-      </c>
-      <c r="F8" s="30">
-        <v>17.8</v>
-      </c>
-      <c r="G8" s="30">
-        <v>40</v>
-      </c>
-      <c r="H8" s="30">
-        <v>73.099999999999994</v>
-      </c>
-      <c r="I8" s="30">
-        <v>93.9</v>
-      </c>
-      <c r="J8" s="30">
-        <v>111.2</v>
-      </c>
-      <c r="K8" s="30">
-        <v>122.3</v>
-      </c>
-      <c r="L8" s="30">
-        <v>135.80000000000001</v>
-      </c>
-      <c r="M8" s="30">
-        <v>130</v>
-      </c>
-      <c r="N8" s="30">
-        <v>153</v>
-      </c>
-      <c r="O8" s="30">
-        <v>157</v>
-      </c>
-      <c r="P8" s="30">
-        <v>171.4</v>
-      </c>
-      <c r="Q8" s="30">
-        <v>187.8</v>
-      </c>
-      <c r="R8" s="30">
-        <v>207.1</v>
-      </c>
-      <c r="S8" s="30">
-        <v>215</v>
-      </c>
-      <c r="T8" s="30">
-        <v>244.1</v>
-      </c>
-      <c r="U8" s="30">
-        <v>247.2</v>
-      </c>
-      <c r="V8" s="30">
-        <v>275</v>
-      </c>
-      <c r="W8" s="30">
-        <v>313.89999999999998</v>
-      </c>
-      <c r="X8" s="30">
-        <v>318.7</v>
-      </c>
-      <c r="Y8" s="30">
-        <v>335.3</v>
-      </c>
-      <c r="Z8" s="30">
-        <v>385.3</v>
-      </c>
-      <c r="AA8" s="30">
-        <v>461.9</v>
-      </c>
-      <c r="AB8" s="30">
-        <v>523.6</v>
-      </c>
-      <c r="AC8" s="30">
-        <v>527.4</v>
-      </c>
-      <c r="AD8" s="30">
-        <v>551.79999999999995</v>
-      </c>
-      <c r="AE8" s="30">
-        <v>560.29999999999995</v>
-      </c>
-      <c r="AF8" s="30">
-        <v>569</v>
-      </c>
-      <c r="AG8" s="30">
-        <v>579.9</v>
-      </c>
-      <c r="AH8" s="30">
-        <v>613.4</v>
-      </c>
-      <c r="AI8" s="30">
-        <v>629.70000000000005</v>
-      </c>
-      <c r="AJ8" s="30">
-        <v>638.1</v>
-      </c>
-      <c r="AK8" s="30">
-        <v>606.79999999999995</v>
-      </c>
-      <c r="AL8" s="30">
-        <v>659.5</v>
-      </c>
-      <c r="AM8" s="30">
-        <v>643.6</v>
-      </c>
-      <c r="AN8" s="30">
-        <v>684.3</v>
-      </c>
-      <c r="AO8" s="30">
-        <v>616.79999999999995</v>
-      </c>
-      <c r="AP8" s="30">
-        <v>669.4</v>
-      </c>
-      <c r="AQ8" s="30">
-        <v>690.5</v>
-      </c>
-      <c r="AR8" s="30">
-        <v>726.2</v>
-      </c>
-      <c r="AS8" s="30">
-        <v>632</v>
-      </c>
-      <c r="AT8" s="30">
-        <v>711.6</v>
-      </c>
-      <c r="AU8" s="30">
-        <v>723.4</v>
-      </c>
-      <c r="AV8" s="30">
-        <v>725</v>
-      </c>
-      <c r="AW8" s="30">
-        <v>573</v>
-      </c>
-      <c r="AX8" s="30">
-        <v>664.3</v>
-      </c>
-      <c r="AY8" s="30">
-        <v>628.5</v>
-      </c>
-      <c r="AZ8" s="30">
-        <v>627.20000000000005</v>
-      </c>
-      <c r="BA8" s="30">
-        <v>564.20000000000005</v>
-      </c>
-      <c r="BB8" s="30">
-        <v>607.1</v>
-      </c>
-      <c r="BC8" s="30">
-        <v>570.4</v>
-      </c>
-      <c r="BD8" s="30">
-        <v>541.6</v>
-      </c>
-      <c r="BE8" s="30">
-        <v>489.9</v>
-      </c>
-      <c r="BF8" s="30">
-        <v>532.9</v>
-      </c>
-      <c r="BG8" s="30">
-        <v>514.5</v>
-      </c>
-      <c r="BH8" s="30">
-        <v>525.20000000000005</v>
-      </c>
-      <c r="BI8" s="30">
-        <v>499.6</v>
-      </c>
-      <c r="BJ8" s="30">
-        <v>555.9</v>
-      </c>
-      <c r="BK8" s="30">
-        <v>520.5</v>
-      </c>
-      <c r="BL8" s="30">
-        <v>556.9</v>
-      </c>
-      <c r="BM8" s="30">
-        <v>499.2</v>
-      </c>
-      <c r="BN8" s="30">
-        <v>577.79999999999995</v>
-      </c>
-      <c r="BO8" s="30">
-        <v>508.2</v>
-      </c>
-      <c r="BP8" s="30">
-        <v>530.70000000000005</v>
-      </c>
-      <c r="BQ8" s="30">
-        <v>560.1</v>
-      </c>
-      <c r="BR8" s="30">
-        <v>539.1</v>
-      </c>
-      <c r="BS8" s="30">
-        <v>578</v>
-      </c>
-      <c r="BT8" s="30">
-        <v>652.70000000000005</v>
-      </c>
-      <c r="BU8" s="30">
-        <v>559</v>
-      </c>
-      <c r="BV8" s="30">
-        <v>610.6</v>
-      </c>
-      <c r="BW8" s="30">
-        <v>457</v>
-      </c>
-      <c r="BX8" s="30">
-        <v>434.9</v>
-      </c>
-      <c r="BY8" s="30">
-        <v>343.9</v>
-      </c>
-      <c r="BZ8" s="30">
-        <v>227.7</v>
-      </c>
-      <c r="CA8" s="30">
-        <v>119.4</v>
-      </c>
-      <c r="CB8" s="30">
-        <v>236.6</v>
-      </c>
-      <c r="CC8" s="30">
-        <v>58.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="E8" s="29">
+        <v>19.3</v>
+      </c>
+      <c r="F8" s="29">
+        <v>32.5</v>
+      </c>
+      <c r="G8" s="29">
+        <v>61.3</v>
+      </c>
+      <c r="H8" s="29">
+        <v>96.6</v>
+      </c>
+      <c r="I8" s="29">
+        <v>138.69999999999999</v>
+      </c>
+      <c r="J8" s="29">
+        <v>151.30000000000001</v>
+      </c>
+      <c r="K8" s="29">
+        <v>172.5</v>
+      </c>
+      <c r="L8" s="29">
+        <v>146.5</v>
+      </c>
+      <c r="M8" s="29">
+        <v>220.1</v>
+      </c>
+      <c r="N8" s="29">
+        <v>263.89999999999998</v>
+      </c>
+      <c r="O8" s="29">
+        <v>307</v>
+      </c>
+      <c r="P8" s="29">
+        <v>252.5</v>
+      </c>
+      <c r="Q8" s="29">
+        <v>353.8</v>
+      </c>
+      <c r="R8" s="29">
+        <v>340</v>
+      </c>
+      <c r="S8" s="29">
+        <v>420.1</v>
+      </c>
+      <c r="T8" s="29">
+        <v>443.5</v>
+      </c>
+      <c r="U8" s="29">
+        <v>395.2</v>
+      </c>
+      <c r="V8" s="29">
+        <v>454.5</v>
+      </c>
+      <c r="W8" s="29">
+        <v>495.3</v>
+      </c>
+      <c r="X8" s="29">
+        <v>403.2</v>
+      </c>
+      <c r="Y8" s="29">
+        <v>569.1</v>
+      </c>
+      <c r="Z8" s="29">
+        <v>593.1</v>
+      </c>
+      <c r="AA8" s="29">
+        <v>647.4</v>
+      </c>
+      <c r="AB8" s="29">
+        <v>488.1</v>
+      </c>
+      <c r="AC8" s="29">
+        <v>606.20000000000005</v>
+      </c>
+      <c r="AD8" s="29">
+        <v>679.9</v>
+      </c>
+      <c r="AE8" s="29">
+        <v>707.8</v>
+      </c>
+      <c r="AF8" s="29">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="9" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>668</v>
+        <v>676</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="30">
-        <v>13.7</v>
-      </c>
-      <c r="F9" s="30">
-        <v>28.4</v>
-      </c>
-      <c r="G9" s="30">
-        <v>33.6</v>
-      </c>
-      <c r="H9" s="30">
-        <v>67.5</v>
-      </c>
-      <c r="I9" s="30">
-        <v>87.7</v>
-      </c>
-      <c r="J9" s="30">
-        <v>111.2</v>
-      </c>
-      <c r="K9" s="30">
-        <v>117.5</v>
-      </c>
-      <c r="L9" s="30">
-        <v>131</v>
-      </c>
-      <c r="M9" s="30">
-        <v>147</v>
-      </c>
-      <c r="N9" s="30">
-        <v>159</v>
-      </c>
-      <c r="O9" s="30">
-        <v>177.1</v>
-      </c>
-      <c r="P9" s="30">
-        <v>171.2</v>
-      </c>
-      <c r="Q9" s="30">
-        <v>186.3</v>
-      </c>
-      <c r="R9" s="30">
-        <v>196</v>
-      </c>
-      <c r="S9" s="30">
-        <v>204.8</v>
-      </c>
-      <c r="T9" s="30">
-        <v>183.6</v>
-      </c>
-      <c r="U9" s="30">
-        <v>218.8</v>
-      </c>
-      <c r="V9" s="30">
-        <v>198.4</v>
-      </c>
-      <c r="W9" s="30">
-        <v>220.6</v>
-      </c>
-      <c r="X9" s="30">
-        <v>198.3</v>
-      </c>
-      <c r="Y9" s="30">
-        <v>241.8</v>
-      </c>
-      <c r="Z9" s="30">
-        <v>240</v>
-      </c>
-      <c r="AA9" s="30">
-        <v>245.1</v>
-      </c>
-      <c r="AB9" s="30">
-        <v>239</v>
-      </c>
-      <c r="AC9" s="30">
-        <v>256.7</v>
-      </c>
-      <c r="AD9" s="30">
-        <v>252.7</v>
-      </c>
-      <c r="AE9" s="30">
-        <v>284.2</v>
-      </c>
-      <c r="AF9" s="30">
-        <v>240.5</v>
-      </c>
-      <c r="AG9" s="30">
-        <v>268.7</v>
-      </c>
-      <c r="AH9" s="30">
-        <v>253.4</v>
-      </c>
-      <c r="AI9" s="30">
-        <v>270.39999999999998</v>
-      </c>
-      <c r="AJ9" s="30">
-        <v>230.3</v>
-      </c>
-      <c r="AK9" s="30">
-        <v>231.3</v>
-      </c>
-      <c r="AL9" s="30">
-        <v>232.1</v>
-      </c>
-      <c r="AM9" s="30">
-        <v>277.8</v>
-      </c>
-      <c r="AN9" s="30">
-        <v>236.8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:81" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="E9" s="28">
+        <v>10</v>
+      </c>
+      <c r="F9" s="28">
+        <v>42</v>
+      </c>
+      <c r="G9" s="28">
+        <v>56</v>
+      </c>
+      <c r="H9">
+        <v>92</v>
+      </c>
+      <c r="I9">
+        <v>116</v>
+      </c>
+      <c r="J9">
+        <v>154</v>
+      </c>
+      <c r="K9">
+        <v>184</v>
+      </c>
+      <c r="L9">
+        <v>235</v>
+      </c>
+      <c r="M9">
+        <v>261</v>
+      </c>
+      <c r="N9">
+        <v>295</v>
+      </c>
+      <c r="O9">
+        <v>349</v>
+      </c>
+      <c r="P9">
+        <v>346</v>
+      </c>
+      <c r="Q9">
+        <v>409</v>
+      </c>
+      <c r="R9">
+        <v>450</v>
+      </c>
+      <c r="S9">
+        <v>512</v>
+      </c>
+      <c r="T9">
+        <v>522</v>
+      </c>
+      <c r="U9">
+        <v>587</v>
+      </c>
+      <c r="V9">
+        <v>620</v>
+      </c>
+      <c r="W9">
+        <v>705</v>
+      </c>
+      <c r="X9">
+        <v>703</v>
+      </c>
+      <c r="Y9">
+        <v>784</v>
+      </c>
+      <c r="Z9">
+        <v>831</v>
+      </c>
+      <c r="AA9">
+        <v>921</v>
+      </c>
+      <c r="AB9">
+        <v>875</v>
+      </c>
+      <c r="AC9">
+        <v>1031</v>
+      </c>
+      <c r="AD9">
+        <v>949</v>
+      </c>
+      <c r="AE9">
+        <v>1031</v>
+      </c>
+      <c r="AF9">
+        <v>1117</v>
+      </c>
+      <c r="AG9">
+        <v>1125</v>
+      </c>
+      <c r="AH9">
+        <v>1116</v>
+      </c>
+      <c r="AI9">
+        <v>1066</v>
+      </c>
+      <c r="AJ9">
+        <v>1062</v>
+      </c>
+      <c r="AK9">
+        <v>1038</v>
+      </c>
+      <c r="AL9">
+        <v>970</v>
+      </c>
+      <c r="AM9">
+        <v>911</v>
+      </c>
+      <c r="AN9">
+        <v>866</v>
+      </c>
+      <c r="AO9">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="10" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>670</v>
+        <v>660</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
       </c>
       <c r="E10" s="30">
-        <v>25.7</v>
+        <v>21</v>
       </c>
       <c r="F10" s="30">
-        <v>36</v>
+        <v>29.7</v>
       </c>
       <c r="G10" s="30">
-        <v>52</v>
+        <v>57.7</v>
       </c>
       <c r="H10" s="30">
-        <v>62</v>
+        <v>84.5</v>
       </c>
       <c r="I10" s="30">
-        <f>M10/1.34</f>
-        <v>68.731343283582078</v>
+        <v>83.1</v>
       </c>
       <c r="J10" s="30">
-        <v>72</v>
+        <v>109.4</v>
       </c>
       <c r="K10" s="30">
-        <v>152.1</v>
+        <v>133.9</v>
       </c>
       <c r="L10" s="30">
-        <v>87.1</v>
+        <v>157.19999999999999</v>
       </c>
       <c r="M10" s="30">
-        <v>92.1</v>
+        <v>179.1</v>
       </c>
       <c r="N10" s="30">
-        <v>82.7</v>
+        <v>188</v>
       </c>
       <c r="O10" s="30">
-        <v>101.2</v>
+        <v>208.6</v>
       </c>
       <c r="P10" s="30">
-        <v>109.2</v>
+        <v>234.4</v>
       </c>
       <c r="Q10" s="30">
-        <v>103</v>
+        <v>281.60000000000002</v>
       </c>
       <c r="R10" s="30">
-        <v>97.5</v>
+        <v>269</v>
       </c>
       <c r="S10" s="30">
-        <v>114.6</v>
+        <v>341.3</v>
       </c>
       <c r="T10" s="30">
-        <v>115.8</v>
+        <v>335.5</v>
       </c>
       <c r="U10" s="30">
-        <v>120.5</v>
+        <v>404.1</v>
       </c>
       <c r="V10" s="30">
-        <v>115.7</v>
+        <v>469.4</v>
       </c>
       <c r="W10" s="30">
-        <v>106.9</v>
+        <v>588.5</v>
       </c>
       <c r="X10" s="30">
-        <v>102.7</v>
+        <v>617.70000000000005</v>
       </c>
       <c r="Y10" s="30">
-        <v>105.3</v>
+        <v>808</v>
       </c>
       <c r="Z10" s="30">
-        <v>101.8</v>
-      </c>
-      <c r="AA10" s="30">
-        <v>103.9</v>
-      </c>
-      <c r="AB10" s="30">
-        <v>106.7</v>
-      </c>
-      <c r="AC10" s="30">
-        <v>110.3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:81" x14ac:dyDescent="0.2">
+        <v>750.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>658</v>
+        <v>666</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
       </c>
       <c r="E11" s="29">
-        <v>4.9000000000000004</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="F11" s="29">
-        <v>14.2</v>
+        <v>18.3</v>
       </c>
       <c r="G11" s="29">
-        <v>34.299999999999997</v>
+        <v>44.3</v>
       </c>
       <c r="H11" s="29">
-        <v>47.7</v>
+        <v>73.7</v>
       </c>
       <c r="I11" s="29">
-        <v>66.3</v>
+        <v>112.5</v>
       </c>
       <c r="J11" s="29">
-        <v>74</v>
+        <v>143.6</v>
       </c>
       <c r="K11" s="29">
-        <v>87.4</v>
+        <v>201.3</v>
       </c>
       <c r="L11" s="29">
-        <v>91.5</v>
+        <v>243.6</v>
       </c>
       <c r="M11" s="29">
-        <v>109.9</v>
+        <v>337</v>
       </c>
       <c r="N11" s="29">
-        <v>119.5</v>
+        <v>372.9</v>
       </c>
       <c r="O11" s="29">
-        <v>156.30000000000001</v>
+        <v>480.2</v>
       </c>
       <c r="P11" s="29">
-        <v>140</v>
+        <v>527.70000000000005</v>
       </c>
       <c r="Q11" s="29">
-        <v>161.5</v>
+        <v>649</v>
       </c>
       <c r="R11" s="29">
-        <v>149.30000000000001</v>
+        <v>678.3</v>
       </c>
       <c r="S11" s="29">
-        <v>157.5</v>
+        <v>779.8</v>
       </c>
       <c r="T11" s="29">
-        <v>168.5</v>
+        <v>816.2</v>
       </c>
       <c r="U11" s="29">
-        <v>175.6</v>
+        <v>924.7</v>
       </c>
       <c r="V11" s="29">
-        <v>154.30000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:81" x14ac:dyDescent="0.2">
+        <v>879.7</v>
+      </c>
+      <c r="W11" s="29">
+        <v>1028.5</v>
+      </c>
+      <c r="X11" s="29">
+        <v>1011.5</v>
+      </c>
+      <c r="Y11" s="29">
+        <v>1208.0999999999999</v>
+      </c>
+      <c r="Z11" s="29">
+        <v>1229.4000000000001</v>
+      </c>
+      <c r="AA11" s="29">
+        <v>1229.8</v>
+      </c>
+      <c r="AB11" s="29">
+        <v>1106.5999999999999</v>
+      </c>
+      <c r="AC11" s="29">
+        <v>1502.4</v>
+      </c>
+      <c r="AD11" s="29">
+        <v>1452.4</v>
+      </c>
+      <c r="AE11" s="29">
+        <v>1535.6</v>
+      </c>
+      <c r="AF11" s="29">
+        <v>1600.1</v>
+      </c>
+      <c r="AG11" s="29">
+        <v>1883.7</v>
+      </c>
+      <c r="AH11" s="29">
+        <v>1741.3</v>
+      </c>
+      <c r="AI11" s="29">
+        <v>1911.9</v>
+      </c>
+      <c r="AJ11" s="29">
+        <v>1850.4</v>
+      </c>
+      <c r="AK11" s="29">
+        <v>1936.2</v>
+      </c>
+      <c r="AL11" s="29">
+        <v>1977.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>662</v>
+        <v>671</v>
       </c>
       <c r="C12" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="29">
-        <v>9.9</v>
-      </c>
-      <c r="F12" s="29">
-        <v>40.1</v>
-      </c>
-      <c r="G12" s="29">
-        <v>46.6</v>
-      </c>
-      <c r="H12" s="29">
-        <v>37.4</v>
-      </c>
-      <c r="I12" s="29">
-        <v>57.4</v>
-      </c>
-      <c r="J12" s="29">
-        <v>64.099999999999994</v>
-      </c>
-      <c r="K12" s="29">
-        <v>84.4</v>
-      </c>
-      <c r="L12" s="29">
-        <v>102.8</v>
-      </c>
-      <c r="M12" s="29">
-        <v>109.7</v>
-      </c>
-      <c r="N12" s="29">
-        <v>105</v>
-      </c>
-      <c r="O12" s="29">
-        <v>125.6</v>
-      </c>
-      <c r="P12" s="29">
-        <v>77.8</v>
-      </c>
-      <c r="Q12" s="29">
-        <v>85.5</v>
-      </c>
-      <c r="R12" s="29">
-        <v>73.599999999999994</v>
-      </c>
-      <c r="S12" s="29">
-        <v>76.8</v>
-      </c>
-      <c r="T12" s="29">
-        <v>57.5</v>
-      </c>
-      <c r="U12" s="29">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="E12" s="30">
+        <v>11.6</v>
+      </c>
+      <c r="F12" s="30">
+        <v>17.8</v>
+      </c>
+      <c r="G12" s="30">
+        <v>40</v>
+      </c>
+      <c r="H12" s="30">
+        <v>73.099999999999994</v>
+      </c>
+      <c r="I12" s="30">
+        <v>93.9</v>
+      </c>
+      <c r="J12" s="30">
+        <v>111.2</v>
+      </c>
+      <c r="K12" s="30">
+        <v>122.3</v>
+      </c>
+      <c r="L12" s="30">
+        <v>135.80000000000001</v>
+      </c>
+      <c r="M12" s="30">
+        <v>130</v>
+      </c>
+      <c r="N12" s="30">
+        <v>153</v>
+      </c>
+      <c r="O12" s="30">
+        <v>157</v>
+      </c>
+      <c r="P12" s="30">
+        <v>171.4</v>
+      </c>
+      <c r="Q12" s="30">
+        <v>187.8</v>
+      </c>
+      <c r="R12" s="30">
+        <v>207.1</v>
+      </c>
+      <c r="S12" s="30">
+        <v>215</v>
+      </c>
+      <c r="T12" s="30">
+        <v>244.1</v>
+      </c>
+      <c r="U12" s="30">
+        <v>247.2</v>
+      </c>
+      <c r="V12" s="30">
+        <v>275</v>
+      </c>
+      <c r="W12" s="30">
+        <v>313.89999999999998</v>
+      </c>
+      <c r="X12" s="30">
+        <v>318.7</v>
+      </c>
+      <c r="Y12" s="30">
+        <v>335.3</v>
+      </c>
+      <c r="Z12" s="30">
+        <v>385.3</v>
+      </c>
+      <c r="AA12" s="30">
+        <v>461.9</v>
+      </c>
+      <c r="AB12" s="30">
+        <v>523.6</v>
+      </c>
+      <c r="AC12" s="30">
+        <v>527.4</v>
+      </c>
+      <c r="AD12" s="30">
+        <v>551.79999999999995</v>
+      </c>
+      <c r="AE12" s="30">
+        <v>560.29999999999995</v>
+      </c>
+      <c r="AF12" s="30">
+        <v>569</v>
+      </c>
+      <c r="AG12" s="30">
+        <v>579.9</v>
+      </c>
+      <c r="AH12" s="30">
+        <v>613.4</v>
+      </c>
+      <c r="AI12" s="30">
+        <v>629.70000000000005</v>
+      </c>
+      <c r="AJ12" s="30">
+        <v>638.1</v>
+      </c>
+      <c r="AK12" s="30">
+        <v>606.79999999999995</v>
+      </c>
+      <c r="AL12" s="30">
+        <v>659.5</v>
+      </c>
+      <c r="AM12" s="30">
+        <v>643.6</v>
+      </c>
+      <c r="AN12" s="30">
+        <v>684.3</v>
+      </c>
+      <c r="AO12" s="30">
+        <v>616.79999999999995</v>
+      </c>
+      <c r="AP12" s="30">
+        <v>669.4</v>
+      </c>
+      <c r="AQ12" s="30">
+        <v>690.5</v>
+      </c>
+      <c r="AR12" s="30">
+        <v>726.2</v>
+      </c>
+      <c r="AS12" s="30">
+        <v>632</v>
+      </c>
+      <c r="AT12" s="30">
+        <v>711.6</v>
+      </c>
+      <c r="AU12" s="30">
+        <v>723.4</v>
+      </c>
+      <c r="AV12" s="30">
+        <v>725</v>
+      </c>
+      <c r="AW12" s="30">
+        <v>573</v>
+      </c>
+      <c r="AX12" s="30">
+        <v>664.3</v>
+      </c>
+      <c r="AY12" s="30">
+        <v>628.5</v>
+      </c>
+      <c r="AZ12" s="30">
+        <v>627.20000000000005</v>
+      </c>
+      <c r="BA12" s="30">
+        <v>564.20000000000005</v>
+      </c>
+      <c r="BB12" s="30">
+        <v>607.1</v>
+      </c>
+      <c r="BC12" s="30">
+        <v>570.4</v>
+      </c>
+      <c r="BD12" s="30">
+        <v>541.6</v>
+      </c>
+      <c r="BE12" s="30">
+        <v>489.9</v>
+      </c>
+      <c r="BF12" s="30">
+        <v>532.9</v>
+      </c>
+      <c r="BG12" s="30">
+        <v>514.5</v>
+      </c>
+      <c r="BH12" s="30">
+        <v>525.20000000000005</v>
+      </c>
+      <c r="BI12" s="30">
+        <v>499.6</v>
+      </c>
+      <c r="BJ12" s="30">
+        <v>555.9</v>
+      </c>
+      <c r="BK12" s="30">
+        <v>520.5</v>
+      </c>
+      <c r="BL12" s="30">
+        <v>556.9</v>
+      </c>
+      <c r="BM12" s="30">
+        <v>499.2</v>
+      </c>
+      <c r="BN12" s="30">
+        <v>577.79999999999995</v>
+      </c>
+      <c r="BO12" s="30">
+        <v>508.2</v>
+      </c>
+      <c r="BP12" s="30">
+        <v>530.70000000000005</v>
+      </c>
+      <c r="BQ12" s="30">
+        <v>560.1</v>
+      </c>
+      <c r="BR12" s="30">
+        <v>539.1</v>
+      </c>
+      <c r="BS12" s="30">
+        <v>578</v>
+      </c>
+      <c r="BT12" s="30">
+        <v>652.70000000000005</v>
+      </c>
+      <c r="BU12" s="30">
+        <v>559</v>
+      </c>
+      <c r="BV12" s="30">
+        <v>610.6</v>
+      </c>
+      <c r="BW12" s="30">
+        <v>457</v>
+      </c>
+      <c r="BX12" s="30">
+        <v>434.9</v>
+      </c>
+      <c r="BY12" s="30">
+        <v>343.9</v>
+      </c>
+      <c r="BZ12" s="30">
+        <v>227.7</v>
+      </c>
+      <c r="CA12" s="30">
+        <v>119.4</v>
+      </c>
+      <c r="CB12" s="30">
+        <v>236.6</v>
+      </c>
+      <c r="CC12" s="30">
+        <v>58.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>661</v>
+        <v>668</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="29">
-        <v>1.9</v>
-      </c>
-      <c r="F13" s="29">
-        <v>4.8</v>
-      </c>
-      <c r="G13" s="29">
-        <v>16.2</v>
-      </c>
-      <c r="H13" s="29">
-        <v>23</v>
-      </c>
-      <c r="I13" s="29">
-        <v>32.200000000000003</v>
-      </c>
-      <c r="J13" s="29">
-        <v>44.7</v>
-      </c>
-      <c r="K13" s="29">
-        <v>55.6</v>
-      </c>
-      <c r="L13" s="29">
-        <v>70.099999999999994</v>
-      </c>
-      <c r="M13" s="29">
-        <v>82.1</v>
-      </c>
-      <c r="N13" s="29">
-        <v>102.4</v>
-      </c>
-      <c r="O13" s="29">
-        <v>114.6</v>
-      </c>
-      <c r="P13" s="29">
-        <v>127.8</v>
-      </c>
-      <c r="Q13" s="29">
-        <v>139.69999999999999</v>
-      </c>
-      <c r="R13" s="29">
-        <v>145</v>
-      </c>
-      <c r="S13" s="29">
-        <v>162</v>
-      </c>
-      <c r="T13" s="29">
-        <v>192.2</v>
-      </c>
-      <c r="U13" s="29">
-        <v>193.8</v>
-      </c>
-      <c r="V13" s="29">
-        <v>208.4</v>
-      </c>
-      <c r="W13" s="29">
-        <v>406.9</v>
-      </c>
-      <c r="X13" s="29">
-        <v>306</v>
-      </c>
-      <c r="Y13" s="29">
-        <v>255.6</v>
-      </c>
-      <c r="Z13" s="29">
-        <v>186.2</v>
-      </c>
-      <c r="AA13" s="29">
-        <v>182.9</v>
-      </c>
-      <c r="AB13" s="29">
-        <v>205.8</v>
-      </c>
-      <c r="AC13" s="29">
-        <v>228.9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="E13" s="30">
+        <v>13.7</v>
+      </c>
+      <c r="F13" s="30">
+        <v>28.4</v>
+      </c>
+      <c r="G13" s="30">
+        <v>33.6</v>
+      </c>
+      <c r="H13" s="30">
+        <v>67.5</v>
+      </c>
+      <c r="I13" s="30">
+        <v>87.7</v>
+      </c>
+      <c r="J13" s="30">
+        <v>111.2</v>
+      </c>
+      <c r="K13" s="30">
+        <v>117.5</v>
+      </c>
+      <c r="L13" s="30">
+        <v>131</v>
+      </c>
+      <c r="M13" s="30">
+        <v>147</v>
+      </c>
+      <c r="N13" s="30">
+        <v>159</v>
+      </c>
+      <c r="O13" s="30">
+        <v>177.1</v>
+      </c>
+      <c r="P13" s="30">
+        <v>171.2</v>
+      </c>
+      <c r="Q13" s="30">
+        <v>186.3</v>
+      </c>
+      <c r="R13" s="30">
+        <v>196</v>
+      </c>
+      <c r="S13" s="30">
+        <v>204.8</v>
+      </c>
+      <c r="T13" s="30">
+        <v>183.6</v>
+      </c>
+      <c r="U13" s="30">
+        <v>218.8</v>
+      </c>
+      <c r="V13" s="30">
+        <v>198.4</v>
+      </c>
+      <c r="W13" s="30">
+        <v>220.6</v>
+      </c>
+      <c r="X13" s="30">
+        <v>198.3</v>
+      </c>
+      <c r="Y13" s="30">
+        <v>241.8</v>
+      </c>
+      <c r="Z13" s="30">
+        <v>240</v>
+      </c>
+      <c r="AA13" s="30">
+        <v>245.1</v>
+      </c>
+      <c r="AB13" s="30">
+        <v>239</v>
+      </c>
+      <c r="AC13" s="30">
+        <v>256.7</v>
+      </c>
+      <c r="AD13" s="30">
+        <v>252.7</v>
+      </c>
+      <c r="AE13" s="30">
+        <v>284.2</v>
+      </c>
+      <c r="AF13" s="30">
+        <v>240.5</v>
+      </c>
+      <c r="AG13" s="30">
+        <v>268.7</v>
+      </c>
+      <c r="AH13" s="30">
+        <v>253.4</v>
+      </c>
+      <c r="AI13" s="30">
+        <v>270.39999999999998</v>
+      </c>
+      <c r="AJ13" s="30">
+        <v>230.3</v>
+      </c>
+      <c r="AK13" s="30">
+        <v>231.3</v>
+      </c>
+      <c r="AL13" s="30">
+        <v>232.1</v>
+      </c>
+      <c r="AM13" s="30">
+        <v>277.8</v>
+      </c>
+      <c r="AN13" s="30">
+        <v>236.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="C14" t="s">
         <v>20</v>
       </c>
       <c r="E14" s="30">
-        <v>6.3</v>
+        <v>25.7</v>
       </c>
       <c r="F14" s="30">
-        <v>11.6</v>
+        <v>36</v>
       </c>
       <c r="G14" s="30">
-        <v>18.7</v>
+        <v>52</v>
       </c>
       <c r="H14" s="30">
-        <v>16.8</v>
+        <v>62</v>
       </c>
       <c r="I14" s="30">
-        <v>25.7</v>
+        <f>M14/1.34</f>
+        <v>68.731343283582078</v>
       </c>
       <c r="J14" s="30">
-        <v>33.6</v>
+        <v>72</v>
       </c>
       <c r="K14" s="30">
-        <v>38.6</v>
+        <v>152.1</v>
       </c>
       <c r="L14" s="30">
-        <v>41.8</v>
+        <v>87.1</v>
       </c>
       <c r="M14" s="30">
-        <v>45</v>
+        <v>92.1</v>
       </c>
       <c r="N14" s="30">
-        <v>40.5</v>
+        <v>82.7</v>
       </c>
       <c r="O14" s="30">
-        <v>64.599999999999994</v>
+        <v>101.2</v>
       </c>
       <c r="P14" s="30">
-        <v>51.4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:81" x14ac:dyDescent="0.2">
+        <v>109.2</v>
+      </c>
+      <c r="Q14" s="30">
+        <v>103</v>
+      </c>
+      <c r="R14" s="30">
+        <v>97.5</v>
+      </c>
+      <c r="S14" s="30">
+        <v>114.6</v>
+      </c>
+      <c r="T14" s="30">
+        <v>115.8</v>
+      </c>
+      <c r="U14" s="30">
+        <v>120.5</v>
+      </c>
+      <c r="V14" s="30">
+        <v>115.7</v>
+      </c>
+      <c r="W14" s="30">
+        <v>106.9</v>
+      </c>
+      <c r="X14" s="30">
+        <v>102.7</v>
+      </c>
+      <c r="Y14" s="30">
+        <v>105.3</v>
+      </c>
+      <c r="Z14" s="30">
+        <v>101.8</v>
+      </c>
+      <c r="AA14" s="30">
+        <v>103.9</v>
+      </c>
+      <c r="AB14" s="30">
+        <v>106.7</v>
+      </c>
+      <c r="AC14" s="30">
+        <v>110.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>665</v>
+        <v>658</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="30">
-        <v>3.8</v>
-      </c>
-      <c r="F15" s="30">
-        <v>7.3</v>
-      </c>
-      <c r="G15" s="30">
-        <v>10.9</v>
-      </c>
-      <c r="H15" s="30">
-        <v>16.3</v>
-      </c>
-      <c r="I15" s="30">
-        <v>19.399999999999999</v>
-      </c>
-      <c r="J15" s="30">
-        <v>39.5</v>
-      </c>
-      <c r="K15" s="30">
-        <v>46</v>
-      </c>
-      <c r="L15" s="30">
-        <v>86.6</v>
-      </c>
-      <c r="M15" s="30">
-        <v>145.69999999999999</v>
-      </c>
-      <c r="N15" s="30">
-        <v>153.80000000000001</v>
-      </c>
-      <c r="O15" s="30">
-        <v>166</v>
-      </c>
-      <c r="P15" s="30">
-        <v>201.8</v>
-      </c>
-      <c r="Q15" s="30">
-        <v>201.2</v>
-      </c>
-      <c r="R15" s="30">
-        <v>232.2</v>
-      </c>
-      <c r="S15" s="30">
-        <v>251.4</v>
-      </c>
-      <c r="T15" s="30">
-        <v>290.7</v>
-      </c>
-      <c r="U15" s="30">
-        <v>263.2</v>
-      </c>
-      <c r="V15" s="30">
-        <v>307.2</v>
-      </c>
-      <c r="W15" s="30">
-        <v>303.7</v>
-      </c>
-      <c r="X15" s="30">
-        <v>290.39999999999998</v>
-      </c>
-      <c r="Y15" s="30">
-        <v>248.2</v>
-      </c>
-      <c r="Z15" s="30">
-        <v>282.10000000000002</v>
-      </c>
-      <c r="AA15" s="30">
-        <v>246.6</v>
-      </c>
-      <c r="AB15" s="30">
-        <v>210.7</v>
-      </c>
-      <c r="AC15" s="30">
-        <v>192.8</v>
-      </c>
-      <c r="AD15" s="30">
-        <v>242.4</v>
-      </c>
-      <c r="AE15" s="30">
-        <v>191.5</v>
-      </c>
-      <c r="AF15" s="30">
-        <v>174.2</v>
-      </c>
-      <c r="AG15" s="30">
-        <v>193</v>
-      </c>
-      <c r="AH15" s="30">
-        <v>201.7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:81" x14ac:dyDescent="0.2">
+      <c r="E15" s="29">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F15" s="29">
+        <v>14.2</v>
+      </c>
+      <c r="G15" s="29">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="H15" s="29">
+        <v>47.7</v>
+      </c>
+      <c r="I15" s="29">
+        <v>66.3</v>
+      </c>
+      <c r="J15" s="29">
+        <v>74</v>
+      </c>
+      <c r="K15" s="29">
+        <v>87.4</v>
+      </c>
+      <c r="L15" s="29">
+        <v>91.5</v>
+      </c>
+      <c r="M15" s="29">
+        <v>109.9</v>
+      </c>
+      <c r="N15" s="29">
+        <v>119.5</v>
+      </c>
+      <c r="O15" s="29">
+        <v>156.30000000000001</v>
+      </c>
+      <c r="P15" s="29">
+        <v>140</v>
+      </c>
+      <c r="Q15" s="29">
+        <v>161.5</v>
+      </c>
+      <c r="R15" s="29">
+        <v>149.30000000000001</v>
+      </c>
+      <c r="S15" s="29">
+        <v>157.5</v>
+      </c>
+      <c r="T15" s="29">
+        <v>168.5</v>
+      </c>
+      <c r="U15" s="29">
+        <v>175.6</v>
+      </c>
+      <c r="V15" s="29">
+        <v>154.30000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>667</v>
+        <v>674</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="30">
-        <v>19.3</v>
-      </c>
-      <c r="F16" s="30">
-        <v>11.1</v>
-      </c>
-      <c r="G16" s="30">
-        <v>15.4</v>
-      </c>
-      <c r="H16" s="30">
-        <v>14.6</v>
-      </c>
-      <c r="I16" s="30">
-        <v>38.200000000000003</v>
-      </c>
-      <c r="J16" s="30">
-        <v>40.1</v>
-      </c>
-      <c r="K16" s="30">
-        <v>47.5</v>
-      </c>
-      <c r="L16" s="30">
-        <v>76.099999999999994</v>
-      </c>
-      <c r="M16" s="30">
-        <v>74</v>
-      </c>
-      <c r="N16" s="30">
-        <v>103.2</v>
-      </c>
-      <c r="O16" s="30">
-        <v>127.2</v>
-      </c>
-      <c r="P16" s="30">
-        <v>143.19999999999999</v>
-      </c>
-      <c r="Q16" s="30">
-        <v>151</v>
-      </c>
-      <c r="R16" s="30">
-        <v>147.19999999999999</v>
-      </c>
-      <c r="S16" s="30">
-        <v>166.9</v>
-      </c>
-      <c r="T16" s="30">
-        <v>193.2</v>
-      </c>
-      <c r="U16" s="30">
-        <v>203.6</v>
-      </c>
-      <c r="V16" s="30">
-        <v>231.9</v>
-      </c>
-      <c r="W16" s="30">
-        <v>240.7</v>
-      </c>
-      <c r="X16" s="30">
-        <v>268</v>
-      </c>
-      <c r="Y16" s="30">
-        <v>267.5</v>
-      </c>
-      <c r="Z16" s="30">
-        <v>262</v>
-      </c>
-      <c r="AA16" s="30">
-        <v>310.8</v>
-      </c>
-      <c r="AB16" s="30">
-        <v>313.60000000000002</v>
-      </c>
-      <c r="AC16" s="30">
-        <v>312</v>
-      </c>
-      <c r="AD16" s="30">
-        <v>356.5</v>
-      </c>
-      <c r="AE16" s="30">
-        <v>390.4</v>
-      </c>
-      <c r="AF16" s="30">
-        <v>431.9</v>
-      </c>
-      <c r="AG16" s="30">
-        <v>419.4</v>
-      </c>
-      <c r="AH16" s="30">
-        <v>461</v>
-      </c>
-      <c r="AI16" s="30">
-        <v>573.29999999999995</v>
-      </c>
-      <c r="AJ16" s="30">
-        <v>612.29999999999995</v>
-      </c>
-      <c r="AK16" s="30">
-        <v>577.5</v>
-      </c>
-    </row>
-    <row r="17" spans="2:34" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="E16" s="28">
+        <v>21</v>
+      </c>
+      <c r="F16" s="28">
+        <v>26</v>
+      </c>
+      <c r="G16" s="28">
+        <v>27</v>
+      </c>
+      <c r="H16">
+        <v>41</v>
+      </c>
+      <c r="I16">
+        <v>49</v>
+      </c>
+      <c r="J16" s="32">
+        <v>91.2</v>
+      </c>
+      <c r="K16" s="32">
+        <v>90.8</v>
+      </c>
+      <c r="L16" s="32">
+        <v>139</v>
+      </c>
+      <c r="M16" s="32">
+        <v>131</v>
+      </c>
+      <c r="N16" s="32">
+        <v>171</v>
+      </c>
+      <c r="O16">
+        <v>209</v>
+      </c>
+      <c r="P16">
+        <v>210</v>
+      </c>
+      <c r="Q16">
+        <v>245</v>
+      </c>
+      <c r="R16">
+        <v>332</v>
+      </c>
+      <c r="S16">
+        <v>341</v>
+      </c>
+      <c r="T16">
+        <v>379</v>
+      </c>
+      <c r="U16">
+        <v>409</v>
+      </c>
+      <c r="V16">
+        <v>421</v>
+      </c>
+      <c r="W16">
+        <v>444</v>
+      </c>
+      <c r="X16">
+        <v>456</v>
+      </c>
+      <c r="Y16">
+        <v>464</v>
+      </c>
+      <c r="Z16">
+        <v>539</v>
+      </c>
+      <c r="AA16">
+        <v>545</v>
+      </c>
+      <c r="AB16">
+        <v>598</v>
+      </c>
+      <c r="AC16">
+        <v>577</v>
+      </c>
+      <c r="AD16">
+        <v>642</v>
+      </c>
+      <c r="AE16">
+        <v>624</v>
+      </c>
+      <c r="AF16">
+        <v>692</v>
+      </c>
+      <c r="AG16">
+        <v>681</v>
+      </c>
+      <c r="AH16">
+        <v>777</v>
+      </c>
+      <c r="AI16">
+        <v>776</v>
+      </c>
+      <c r="AJ16">
+        <v>780</v>
+      </c>
+      <c r="AK16">
+        <v>731</v>
+      </c>
+      <c r="AL16">
+        <v>869</v>
+      </c>
+      <c r="AM16">
+        <v>819</v>
+      </c>
+      <c r="AN16">
+        <v>908</v>
+      </c>
+      <c r="AO16">
+        <v>998</v>
+      </c>
+      <c r="AP16">
+        <v>886</v>
+      </c>
+      <c r="AQ16">
+        <v>978</v>
+      </c>
+      <c r="AR16">
+        <v>886</v>
+      </c>
+      <c r="AS16">
+        <v>1028</v>
+      </c>
+      <c r="AT16">
+        <v>1102</v>
+      </c>
+      <c r="AU16">
+        <v>1036</v>
+      </c>
+      <c r="AV16">
+        <v>1138</v>
+      </c>
+      <c r="AW16">
+        <v>1186</v>
+      </c>
+      <c r="AX16">
+        <v>1130</v>
+      </c>
+      <c r="AY16">
+        <v>1229</v>
+      </c>
+      <c r="AZ16">
+        <v>1065</v>
+      </c>
+      <c r="BA16">
+        <v>1285</v>
+      </c>
+      <c r="BB16">
+        <v>1371</v>
+      </c>
+      <c r="BC16">
+        <v>1408</v>
+      </c>
+      <c r="BD16">
+        <v>1428</v>
+      </c>
+      <c r="BE16">
+        <v>1521</v>
+      </c>
+      <c r="BF16">
+        <v>1523</v>
+      </c>
+      <c r="BG16">
+        <v>1591</v>
+      </c>
+      <c r="BH16">
+        <v>1504</v>
+      </c>
+      <c r="BI16">
+        <v>1600</v>
+      </c>
+      <c r="BJ16">
+        <v>1672</v>
+      </c>
+      <c r="BK16">
+        <v>1689</v>
+      </c>
+      <c r="BL16">
+        <v>1712</v>
+      </c>
+      <c r="BM16">
+        <v>1610</v>
+      </c>
+      <c r="BN16">
+        <v>1804</v>
+      </c>
+      <c r="BO16">
+        <v>1782</v>
+      </c>
+      <c r="BP16">
+        <v>1672</v>
+      </c>
+      <c r="BQ16">
+        <v>1600</v>
+      </c>
+      <c r="BR16">
+        <v>1668</v>
+      </c>
+      <c r="BS16">
+        <v>1613</v>
+      </c>
+      <c r="BT16">
+        <v>1680</v>
+      </c>
+      <c r="BU16">
+        <v>1779</v>
+      </c>
+      <c r="BV16">
+        <v>1780</v>
+      </c>
+      <c r="BW16">
+        <v>1783</v>
+      </c>
+      <c r="BX16">
+        <v>1624</v>
+      </c>
+      <c r="BY16">
+        <v>1672</v>
+      </c>
+      <c r="BZ16">
+        <v>1530</v>
+      </c>
+      <c r="CA16">
+        <v>1647</v>
+      </c>
+      <c r="CB16">
+        <v>1466</v>
+      </c>
+      <c r="CC16">
+        <v>1389</v>
+      </c>
+      <c r="CD16">
+        <v>1320</v>
+      </c>
+      <c r="CE16">
+        <v>1379</v>
+      </c>
+      <c r="CF16">
+        <v>1238</v>
+      </c>
+      <c r="CG16">
+        <v>1102</v>
+      </c>
+      <c r="CH16">
+        <v>1107</v>
+      </c>
+      <c r="CI16">
+        <v>1136</v>
+      </c>
+      <c r="CJ16">
+        <v>1035</v>
+      </c>
+      <c r="CK16">
+        <v>990</v>
+      </c>
+      <c r="CL16">
+        <v>935</v>
+      </c>
+      <c r="CM16">
+        <v>921</v>
+      </c>
+      <c r="CN16">
+        <v>901</v>
+      </c>
+      <c r="CO16">
+        <v>777</v>
+      </c>
+      <c r="CP16">
+        <v>888</v>
+      </c>
+      <c r="CQ16">
+        <v>761</v>
+      </c>
+      <c r="CR16">
+        <v>764</v>
+      </c>
+      <c r="CS16">
+        <v>663</v>
+      </c>
+      <c r="CT16">
+        <v>647</v>
+      </c>
+      <c r="CU16">
+        <v>558</v>
+      </c>
+      <c r="CV16">
+        <v>475</v>
+      </c>
+      <c r="CW16">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="17" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>669</v>
+        <v>662</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
       </c>
       <c r="E17" s="29">
+        <v>9.9</v>
+      </c>
+      <c r="F17" s="29">
+        <v>40.1</v>
+      </c>
+      <c r="G17" s="29">
+        <v>46.6</v>
+      </c>
+      <c r="H17" s="29">
+        <v>37.4</v>
+      </c>
+      <c r="I17" s="29">
+        <v>57.4</v>
+      </c>
+      <c r="J17" s="29">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="K17" s="29">
+        <v>84.4</v>
+      </c>
+      <c r="L17" s="29">
+        <v>102.8</v>
+      </c>
+      <c r="M17" s="29">
+        <v>109.7</v>
+      </c>
+      <c r="N17" s="29">
+        <v>105</v>
+      </c>
+      <c r="O17" s="29">
+        <v>125.6</v>
+      </c>
+      <c r="P17" s="29">
+        <v>77.8</v>
+      </c>
+      <c r="Q17" s="29">
+        <v>85.5</v>
+      </c>
+      <c r="R17" s="29">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="S17" s="29">
+        <v>76.8</v>
+      </c>
+      <c r="T17" s="29">
+        <v>57.5</v>
+      </c>
+      <c r="U17" s="29">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>661</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="29">
+        <v>1.9</v>
+      </c>
+      <c r="F18" s="29">
+        <v>4.8</v>
+      </c>
+      <c r="G18" s="29">
+        <v>16.2</v>
+      </c>
+      <c r="H18" s="29">
+        <v>23</v>
+      </c>
+      <c r="I18" s="29">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="J18" s="29">
+        <v>44.7</v>
+      </c>
+      <c r="K18" s="29">
+        <v>55.6</v>
+      </c>
+      <c r="L18" s="29">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="M18" s="29">
+        <v>82.1</v>
+      </c>
+      <c r="N18" s="29">
+        <v>102.4</v>
+      </c>
+      <c r="O18" s="29">
+        <v>114.6</v>
+      </c>
+      <c r="P18" s="29">
+        <v>127.8</v>
+      </c>
+      <c r="Q18" s="29">
+        <v>139.69999999999999</v>
+      </c>
+      <c r="R18" s="29">
+        <v>145</v>
+      </c>
+      <c r="S18" s="29">
+        <v>162</v>
+      </c>
+      <c r="T18" s="29">
+        <v>192.2</v>
+      </c>
+      <c r="U18" s="29">
+        <v>193.8</v>
+      </c>
+      <c r="V18" s="29">
+        <v>208.4</v>
+      </c>
+      <c r="W18" s="29">
+        <v>406.9</v>
+      </c>
+      <c r="X18" s="29">
+        <v>306</v>
+      </c>
+      <c r="Y18" s="29">
+        <v>255.6</v>
+      </c>
+      <c r="Z18" s="29">
+        <v>186.2</v>
+      </c>
+      <c r="AA18" s="29">
+        <v>182.9</v>
+      </c>
+      <c r="AB18" s="29">
+        <v>205.8</v>
+      </c>
+      <c r="AC18" s="29">
+        <v>228.9</v>
+      </c>
+    </row>
+    <row r="19" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>663</v>
+      </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="30">
+        <v>6.3</v>
+      </c>
+      <c r="F19" s="30">
+        <v>11.6</v>
+      </c>
+      <c r="G19" s="30">
+        <v>18.7</v>
+      </c>
+      <c r="H19" s="30">
+        <v>16.8</v>
+      </c>
+      <c r="I19" s="30">
+        <v>25.7</v>
+      </c>
+      <c r="J19" s="30">
+        <v>33.6</v>
+      </c>
+      <c r="K19" s="30">
+        <v>38.6</v>
+      </c>
+      <c r="L19" s="30">
+        <v>41.8</v>
+      </c>
+      <c r="M19" s="30">
+        <v>45</v>
+      </c>
+      <c r="N19" s="30">
+        <v>40.5</v>
+      </c>
+      <c r="O19" s="30">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="P19" s="30">
+        <v>51.4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>665</v>
+      </c>
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="30">
+        <v>3.8</v>
+      </c>
+      <c r="F20" s="30">
+        <v>7.3</v>
+      </c>
+      <c r="G20" s="30">
+        <v>10.9</v>
+      </c>
+      <c r="H20" s="30">
+        <v>16.3</v>
+      </c>
+      <c r="I20" s="30">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="J20" s="30">
+        <v>39.5</v>
+      </c>
+      <c r="K20" s="30">
+        <v>46</v>
+      </c>
+      <c r="L20" s="30">
+        <v>86.6</v>
+      </c>
+      <c r="M20" s="30">
+        <v>145.69999999999999</v>
+      </c>
+      <c r="N20" s="30">
+        <v>153.80000000000001</v>
+      </c>
+      <c r="O20" s="30">
+        <v>166</v>
+      </c>
+      <c r="P20" s="30">
+        <v>201.8</v>
+      </c>
+      <c r="Q20" s="30">
+        <v>201.2</v>
+      </c>
+      <c r="R20" s="30">
+        <v>232.2</v>
+      </c>
+      <c r="S20" s="30">
+        <v>251.4</v>
+      </c>
+      <c r="T20" s="30">
+        <v>290.7</v>
+      </c>
+      <c r="U20" s="30">
+        <v>263.2</v>
+      </c>
+      <c r="V20" s="30">
+        <v>307.2</v>
+      </c>
+      <c r="W20" s="30">
+        <v>303.7</v>
+      </c>
+      <c r="X20" s="30">
+        <v>290.39999999999998</v>
+      </c>
+      <c r="Y20" s="30">
+        <v>248.2</v>
+      </c>
+      <c r="Z20" s="30">
+        <v>282.10000000000002</v>
+      </c>
+      <c r="AA20" s="30">
+        <v>246.6</v>
+      </c>
+      <c r="AB20" s="30">
+        <v>210.7</v>
+      </c>
+      <c r="AC20" s="30">
+        <v>192.8</v>
+      </c>
+      <c r="AD20" s="30">
+        <v>242.4</v>
+      </c>
+      <c r="AE20" s="30">
+        <v>191.5</v>
+      </c>
+      <c r="AF20" s="30">
+        <v>174.2</v>
+      </c>
+      <c r="AG20" s="30">
+        <v>193</v>
+      </c>
+      <c r="AH20" s="30">
+        <v>201.7</v>
+      </c>
+    </row>
+    <row r="21" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>667</v>
+      </c>
+      <c r="C21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="30">
+        <v>19.3</v>
+      </c>
+      <c r="F21" s="30">
+        <v>11.1</v>
+      </c>
+      <c r="G21" s="30">
+        <v>15.4</v>
+      </c>
+      <c r="H21" s="30">
+        <v>14.6</v>
+      </c>
+      <c r="I21" s="30">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="J21" s="30">
+        <v>40.1</v>
+      </c>
+      <c r="K21" s="30">
+        <v>47.5</v>
+      </c>
+      <c r="L21" s="30">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="M21" s="30">
+        <v>74</v>
+      </c>
+      <c r="N21" s="30">
+        <v>103.2</v>
+      </c>
+      <c r="O21" s="30">
+        <v>127.2</v>
+      </c>
+      <c r="P21" s="30">
+        <v>143.19999999999999</v>
+      </c>
+      <c r="Q21" s="30">
+        <v>151</v>
+      </c>
+      <c r="R21" s="30">
+        <v>147.19999999999999</v>
+      </c>
+      <c r="S21" s="30">
+        <v>166.9</v>
+      </c>
+      <c r="T21" s="30">
+        <v>193.2</v>
+      </c>
+      <c r="U21" s="30">
+        <v>203.6</v>
+      </c>
+      <c r="V21" s="30">
+        <v>231.9</v>
+      </c>
+      <c r="W21" s="30">
+        <v>240.7</v>
+      </c>
+      <c r="X21" s="30">
+        <v>268</v>
+      </c>
+      <c r="Y21" s="30">
+        <v>267.5</v>
+      </c>
+      <c r="Z21" s="30">
+        <v>262</v>
+      </c>
+      <c r="AA21" s="30">
+        <v>310.8</v>
+      </c>
+      <c r="AB21" s="30">
+        <v>313.60000000000002</v>
+      </c>
+      <c r="AC21" s="30">
+        <v>312</v>
+      </c>
+      <c r="AD21" s="30">
+        <v>356.5</v>
+      </c>
+      <c r="AE21" s="30">
+        <v>390.4</v>
+      </c>
+      <c r="AF21" s="30">
+        <v>431.9</v>
+      </c>
+      <c r="AG21" s="30">
+        <v>419.4</v>
+      </c>
+      <c r="AH21" s="30">
+        <v>461</v>
+      </c>
+      <c r="AI21" s="30">
+        <v>573.29999999999995</v>
+      </c>
+      <c r="AJ21" s="30">
+        <v>612.29999999999995</v>
+      </c>
+      <c r="AK21" s="30">
+        <v>577.5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>669</v>
+      </c>
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="29">
         <v>22.6</v>
       </c>
-      <c r="F17" s="29">
+      <c r="F22" s="29">
         <v>4</v>
       </c>
-      <c r="G17" s="29">
+      <c r="G22" s="29">
         <v>8.8000000000000007</v>
       </c>
-      <c r="H17" s="29">
+      <c r="H22" s="29">
         <v>22.9</v>
       </c>
-      <c r="I17" s="29">
+      <c r="I22" s="29">
         <v>36.299999999999997</v>
       </c>
-      <c r="J17" s="29">
+      <c r="J22" s="29">
         <v>47</v>
       </c>
-      <c r="K17" s="29">
+      <c r="K22" s="29">
         <v>56.3</v>
       </c>
-      <c r="L17" s="29">
+      <c r="L22" s="29">
         <v>71.7</v>
       </c>
-      <c r="M17" s="29">
+      <c r="M22" s="29">
         <v>83.5</v>
       </c>
-      <c r="N17" s="29">
+      <c r="N22" s="29">
         <v>90.9</v>
       </c>
-      <c r="O17" s="29">
+      <c r="O22" s="29">
         <v>115.8</v>
       </c>
-      <c r="P17" s="29">
+      <c r="P22" s="29">
         <v>111</v>
       </c>
-      <c r="Q17" s="29">
+      <c r="Q22" s="29">
         <v>109.7</v>
       </c>
-      <c r="R17" s="29">
+      <c r="R22" s="29">
         <v>120.6</v>
       </c>
-      <c r="S17" s="29">
+      <c r="S22" s="29">
         <v>115.9</v>
       </c>
-      <c r="T17" s="29">
+      <c r="T22" s="29">
         <v>137.4</v>
       </c>
-      <c r="U17" s="29">
+      <c r="U22" s="29">
         <v>124.9</v>
       </c>
-      <c r="V17" s="29">
+      <c r="V22" s="29">
         <v>130.6</v>
       </c>
-      <c r="W17" s="29">
+      <c r="W22" s="29">
         <v>119.3</v>
       </c>
-      <c r="X17" s="29">
+      <c r="X22" s="29">
         <v>133.6</v>
       </c>
-      <c r="Y17" s="29">
+      <c r="Y22" s="29">
         <v>131.5</v>
       </c>
-      <c r="Z17" s="29">
+      <c r="Z22" s="29">
         <v>137.80000000000001</v>
       </c>
-      <c r="AA17" s="29">
+      <c r="AA22" s="29">
         <v>121.8</v>
       </c>
-      <c r="AB17" s="29">
+      <c r="AB22" s="29">
         <v>128.80000000000001</v>
       </c>
-      <c r="AC17" s="29">
+      <c r="AC22" s="29">
         <v>132.1</v>
       </c>
-      <c r="AD17" s="29">
+      <c r="AD22" s="29">
         <v>140.30000000000001</v>
       </c>
-      <c r="AE17" s="29">
+      <c r="AE22" s="29">
         <v>131.5</v>
       </c>
-      <c r="AF17" s="29">
+      <c r="AF22" s="29">
         <v>135.1</v>
       </c>
-      <c r="AG17" s="29">
+      <c r="AG22" s="29">
         <v>127.7</v>
       </c>
-      <c r="AH17" s="29">
+      <c r="AH22" s="29">
         <v>140.9</v>
       </c>
+    </row>
+    <row r="23" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="J23" s="32"/>
+      <c r="K23" s="32"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="32"/>
+      <c r="N23" s="32"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
updates on BIIB and others
</commit_message>
<xml_diff>
--- a/Biopharma.xlsx
+++ b/Biopharma.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5DC7FA-D05A-4E70-A47D-97A223B5E838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2E0E53-A5DF-4F37-97A9-AD8095BB003D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="465" windowWidth="24480" windowHeight="20415" xr2:uid="{17641224-F2C3-441B-B85B-BB32567FE633}"/>
+    <workbookView xWindow="18000" yWindow="1680" windowWidth="32370" windowHeight="18030" xr2:uid="{17641224-F2C3-441B-B85B-BB32567FE633}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -226,7 +226,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1589" uniqueCount="1056">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="1058">
   <si>
     <t>Exarta</t>
   </si>
@@ -3394,6 +3394,12 @@
   </si>
   <si>
     <t>12m</t>
+  </si>
+  <si>
+    <t>Verseon</t>
+  </si>
+  <si>
+    <t>Current Price</t>
   </si>
 </sst>
 </file>
@@ -4566,7 +4572,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4641,6 +4647,9 @@
 <file path=xl/externalLinks/externalLink24.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
@@ -4654,16 +4663,16 @@
         </row>
         <row r="5">
           <cell r="J5">
-            <v>7384</v>
+            <v>7400</v>
           </cell>
         </row>
         <row r="6">
           <cell r="J6">
-            <v>6279</v>
+            <v>6283</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4740,6 +4749,58 @@
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="K3">
+            <v>185.66490099999999</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="K5">
+            <v>1763.7020000000002</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="K6">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="23">
+          <cell r="AO23">
+            <v>0.08</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="AO24">
+            <v>-0.01</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="AO25">
+            <v>0.03</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="AO27">
+            <v>119.56497461195261</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink28.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
       <sheetName val="Viagra"/>
       <sheetName val="Norvasc"/>
       <sheetName val="Lyrica"/>
@@ -4777,7 +4838,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink29.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -4803,40 +4864,6 @@
         </row>
       </sheetData>
       <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink29.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Main"/>
-      <sheetName val="Model"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="J3">
-            <v>4263.5283170000002</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="J5">
-            <v>10082.542000000001</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="J6">
-            <v>2347.1640000000002</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4888,6 +4915,9 @@
 <file path=xl/externalLinks/externalLink30.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
@@ -4896,7 +4926,17 @@
       <sheetData sheetId="0">
         <row r="3">
           <cell r="J3">
-            <v>2399</v>
+            <v>4263.5283170000002</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="J5">
+            <v>10082.542000000001</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="J6">
+            <v>2347.1640000000002</v>
           </cell>
         </row>
       </sheetData>
@@ -4911,25 +4951,17 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
+      <sheetName val="Model"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="L3">
-            <v>226.621465</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="L5">
-            <v>2130.527</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="L6">
-            <v>2565.14</v>
+          <cell r="J3">
+            <v>2399</v>
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4940,45 +4972,22 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
-      <sheetName val="Model"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="K3">
-            <v>185.66490099999999</v>
+          <cell r="L3">
+            <v>226.621465</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="K5">
-            <v>1763.7020000000002</v>
+          <cell r="L5">
+            <v>2130.527</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="K6">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1">
-        <row r="23">
-          <cell r="AO23">
-            <v>0.08</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="AO24">
-            <v>-0.01</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="AO25">
-            <v>0.03</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="AO27">
-            <v>119.56497461195261</v>
+          <cell r="L6">
+            <v>2565.14</v>
           </cell>
         </row>
       </sheetData>
@@ -7008,6 +7017,36 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
+      <sheetName val="Master"/>
+      <sheetName val="Model"/>
+      <sheetName val="Enbrel"/>
+      <sheetName val="Lumakras"/>
+      <sheetName val="Neulasta"/>
+      <sheetName val="Neupogen"/>
+      <sheetName val="Epogen"/>
+      <sheetName val="EPO safety"/>
+      <sheetName val="Aranesp"/>
+      <sheetName val="G-CSF"/>
+      <sheetName val="Sensipar"/>
+      <sheetName val="Vectibix"/>
+      <sheetName val="Denosumab"/>
+      <sheetName val="Denosumab trials"/>
+      <sheetName val="Kineret"/>
+      <sheetName val="706"/>
+      <sheetName val="531"/>
+      <sheetName val="108"/>
+      <sheetName val="114"/>
+      <sheetName val="223"/>
+      <sheetName val="386"/>
+      <sheetName val="479"/>
+      <sheetName val="102"/>
+      <sheetName val="655"/>
+      <sheetName val="785"/>
+      <sheetName val="811"/>
+      <sheetName val="208"/>
+      <sheetName val="714"/>
+      <sheetName val="Failures"/>
+      <sheetName val="Kepivance"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
@@ -7027,6 +7066,36 @@
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="30" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7217,6 +7286,23 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
+      <sheetName val="Master"/>
+      <sheetName val="Model"/>
+      <sheetName val="Lovenox"/>
+      <sheetName val="Lantus"/>
+      <sheetName val="Aubagio"/>
+      <sheetName val="Plavix"/>
+      <sheetName val="Multaq"/>
+      <sheetName val="idraparinux"/>
+      <sheetName val="SR 58611"/>
+      <sheetName val="Eplivanserin"/>
+      <sheetName val="SSR 591813"/>
+      <sheetName val="Xaliproden"/>
+      <sheetName val="Alvocidib"/>
+      <sheetName val="SR 121463"/>
+      <sheetName val="BSI-201"/>
+      <sheetName val="Zimulti"/>
+      <sheetName val="Failures"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
@@ -7236,6 +7322,23 @@
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7658,11 +7761,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AD397"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <pane xSplit="3" ySplit="3" topLeftCell="D19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J34" sqref="J34"/>
+      <selection pane="bottomRight" activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7684,7 +7787,7 @@
     <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B1" s="1">
         <f ca="1">RANDBETWEEN(1,B208)</f>
-        <v>89</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
@@ -9046,29 +9149,29 @@
         <v>269</v>
       </c>
       <c r="E32" s="7">
-        <v>279</v>
+        <v>294.36</v>
       </c>
       <c r="F32" s="6">
         <f>+E32*J32</f>
-        <v>40455</v>
+        <v>42682.200000000004</v>
       </c>
       <c r="G32" s="6">
         <f>+[24]Main!$J$5-[24]Main!$J$6</f>
-        <v>1105</v>
+        <v>1117</v>
       </c>
       <c r="H32" s="6">
         <f>+F32-G32</f>
-        <v>39350</v>
+        <v>41565.200000000004</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>429</v>
+        <v>669</v>
       </c>
       <c r="J32" s="6">
         <f>+[24]Main!$J$3</f>
         <v>145</v>
       </c>
       <c r="K32" s="9">
-        <v>44922</v>
+        <v>45098</v>
       </c>
       <c r="AC32" s="1">
         <v>1978</v>
@@ -9182,7 +9285,7 @@
         <v>36501.719536599994</v>
       </c>
       <c r="G35" s="6">
-        <f>+[32]Main!$K$5-[32]Main!$K$6</f>
+        <f>+[27]Main!$K$5-[27]Main!$K$6</f>
         <v>1763.7020000000002</v>
       </c>
       <c r="H35" s="6">
@@ -9193,14 +9296,14 @@
         <v>429</v>
       </c>
       <c r="J35" s="6">
-        <f>+[32]Main!$K$3</f>
+        <f>+[27]Main!$K$3</f>
         <v>185.66490099999999</v>
       </c>
       <c r="K35" s="9">
         <v>44919</v>
       </c>
       <c r="L35" s="7">
-        <f>+[32]Model!$AO$27</f>
+        <f>+[27]Model!$AO$27</f>
         <v>119.56497461195261</v>
       </c>
       <c r="M35" s="10">
@@ -9208,15 +9311,15 @@
         <v>-0.39183634480186869</v>
       </c>
       <c r="N35" s="10">
-        <f>+[32]Model!$AO$25</f>
+        <f>+[27]Model!$AO$25</f>
         <v>0.03</v>
       </c>
       <c r="O35" s="10">
-        <f>+[32]Model!$AO$24</f>
+        <f>+[27]Model!$AO$24</f>
         <v>-0.01</v>
       </c>
       <c r="P35" s="10">
-        <f>+[32]Model!$AO$23</f>
+        <f>+[27]Model!$AO$23</f>
         <v>0.08</v>
       </c>
       <c r="AC35" s="1">
@@ -9241,11 +9344,11 @@
         <v>11</v>
       </c>
       <c r="F36" s="6">
-        <f>E36*[27]Main!$M$3</f>
+        <f>E36*[28]Main!$M$3</f>
         <v>13164.953549000002</v>
       </c>
       <c r="G36" s="6">
-        <f>[27]Main!$M$5-[27]Main!$M$6</f>
+        <f>[28]Main!$M$5-[28]Main!$M$6</f>
         <v>-19342.3</v>
       </c>
       <c r="H36" s="6">
@@ -9256,7 +9359,7 @@
         <v>429</v>
       </c>
       <c r="J36" s="6">
-        <f>+[27]Main!$M$3</f>
+        <f>+[28]Main!$M$3</f>
         <v>1196.8139590000001</v>
       </c>
       <c r="K36" s="9">
@@ -9288,7 +9391,7 @@
         <v>21659.668701269999</v>
       </c>
       <c r="G37" s="6">
-        <f>+[28]Main!$L$5-[28]Main!$L$6</f>
+        <f>+[29]Main!$L$5-[29]Main!$L$6</f>
         <v>-4644</v>
       </c>
       <c r="H37" s="6">
@@ -9299,7 +9402,7 @@
         <v>532</v>
       </c>
       <c r="J37" s="6">
-        <f>+[28]Main!$L$3</f>
+        <f>+[29]Main!$L$3</f>
         <v>607.22368099999994</v>
       </c>
       <c r="K37" s="9">
@@ -9331,7 +9434,7 @@
         <v>24359.139492668794</v>
       </c>
       <c r="G38" s="6">
-        <f>([29]Main!$J$5-[29]Main!$J$6)/HKD</f>
+        <f>([30]Main!$J$5-[30]Main!$J$6)/HKD</f>
         <v>985.39847133757974</v>
       </c>
       <c r="H38" s="6">
@@ -9342,7 +9445,7 @@
         <v>307</v>
       </c>
       <c r="J38" s="6">
-        <f>+[29]Main!$J$3</f>
+        <f>+[30]Main!$J$3</f>
         <v>4263.5283170000002</v>
       </c>
       <c r="K38" s="9">
@@ -9381,7 +9484,7 @@
         <v>429</v>
       </c>
       <c r="J39" s="6">
-        <f>+[30]Main!$J$3</f>
+        <f>+[31]Main!$J$3</f>
         <v>2399</v>
       </c>
       <c r="K39" s="9">
@@ -9412,7 +9515,7 @@
         <v>25650</v>
       </c>
       <c r="G40" s="6">
-        <f>+[31]Main!$L$5-[31]Main!$L$6</f>
+        <f>+[32]Main!$L$5-[32]Main!$L$6</f>
         <v>-434.61299999999983</v>
       </c>
       <c r="H40" s="6">
@@ -9423,7 +9526,7 @@
         <v>429</v>
       </c>
       <c r="J40" s="6">
-        <f>+[31]Main!$L$3</f>
+        <f>+[32]Main!$L$3</f>
         <v>226.621465</v>
       </c>
       <c r="K40" s="9">
@@ -16726,27 +16829,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB2359B-6F3C-4B5E-BAEA-85D9BCFEA817}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>1047</v>
       </c>
@@ -16762,13 +16866,16 @@
       <c r="F2" t="s">
         <v>1049</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>1048</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>148</v>
       </c>
@@ -16784,8 +16891,11 @@
       <c r="F4">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>41.85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>1045</v>
       </c>
@@ -16801,8 +16911,11 @@
       <c r="F5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>19.21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>1046</v>
       </c>
@@ -16818,8 +16931,11 @@
       <c r="F6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <v>68.19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>806</v>
       </c>
@@ -16834,6 +16950,9 @@
       </c>
       <c r="F7">
         <v>3</v>
+      </c>
+      <c r="G7">
+        <v>25.09</v>
       </c>
     </row>
   </sheetData>
@@ -20897,13 +21016,13 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED149DB-8F62-4CB2-88E6-87DDBD9316FC}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:I104"/>
+  <dimension ref="A1:I105"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C66" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B105" sqref="B105"/>
+      <selection pane="bottomRight" activeCell="E105" sqref="E105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -21763,6 +21882,11 @@
       </c>
       <c r="F104" t="s">
         <v>1055</v>
+      </c>
+    </row>
+    <row r="105" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B105" t="s">
+        <v>1056</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
various enterprise software updates
</commit_message>
<xml_diff>
--- a/Biopharma.xlsx
+++ b/Biopharma.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296F3570-D688-4562-9AD9-4A65B8FF6D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3175F5C5-0D03-4A35-BE4B-4341F27B3823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26010" yWindow="1410" windowWidth="22575" windowHeight="18825" xr2:uid="{17641224-F2C3-441B-B85B-BB32567FE633}"/>
+    <workbookView xWindow="-35220" yWindow="1995" windowWidth="23265" windowHeight="17910" xr2:uid="{17641224-F2C3-441B-B85B-BB32567FE633}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -3628,7 +3628,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -3729,7 +3729,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -7923,7 +7922,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="D112" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E135" sqref="E135"/>
+      <selection pane="bottomRight" activeCell="E121" sqref="E121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7945,7 +7944,7 @@
     <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B1" s="1">
         <f ca="1">RANDBETWEEN(1,B204)</f>
-        <v>156</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
@@ -12164,10 +12163,10 @@
         <f t="shared" si="8"/>
         <v>127</v>
       </c>
-      <c r="C135" s="42" t="s">
+      <c r="C135" t="s">
         <v>1099</v>
       </c>
-      <c r="D135" s="42" t="s">
+      <c r="D135" t="s">
         <v>1100</v>
       </c>
       <c r="E135" s="7">

</xml_diff>

<commit_message>
update NVDA and GSK
</commit_message>
<xml_diff>
--- a/Biopharma.xlsx
+++ b/Biopharma.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3DF6ACC-7222-4FA0-8E87-E5E3AB7675C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D78561E-1420-4661-9BA1-8D636063F254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30465" yWindow="975" windowWidth="30015" windowHeight="18480" xr2:uid="{17641224-F2C3-441B-B85B-BB32567FE633}"/>
+    <workbookView xWindow="-51465" yWindow="0" windowWidth="20970" windowHeight="15480" xr2:uid="{17641224-F2C3-441B-B85B-BB32567FE633}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -4580,35 +4580,6 @@
       <xxl21:absoluteUrl r:id="rId2"/>
     </xxl21:alternateUrls>
     <sheetNames>
-      <sheetName val="Main"/>
-      <sheetName val="Model"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="5">
-          <cell r="J5">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="J6">
-            <v>7950</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink19.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
       <sheetName val="Master"/>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
@@ -4638,73 +4609,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Master"/>
-      <sheetName val="Main"/>
-      <sheetName val="Model"/>
-      <sheetName val="Ozempic"/>
-      <sheetName val="Wegovy"/>
-      <sheetName val="Rybelsus"/>
-      <sheetName val="Type 2 Diabetes"/>
-      <sheetName val="Victoza"/>
-      <sheetName val="NovoLog"/>
-      <sheetName val="Levemir"/>
-      <sheetName val="Sogroya"/>
-      <sheetName val="insulin icodec"/>
-      <sheetName val="NLRP3"/>
-      <sheetName val="ziltivekimab"/>
-      <sheetName val="amycretin"/>
-      <sheetName val="GLP-1-GIP"/>
-      <sheetName val="cagrilintide"/>
-      <sheetName val="CDR132L"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="3">
-          <cell r="J3">
-            <v>4471</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="J5">
-            <v>12315</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="J6">
-            <v>29038</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink19.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -4768,21 +4673,124 @@
       <sheetName val="Avandia"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1">
         <row r="4">
           <cell r="J4">
-            <v>4069</v>
+            <v>4079</v>
           </cell>
         </row>
         <row r="6">
           <cell r="J6">
-            <v>0</v>
+            <v>4219</v>
           </cell>
         </row>
         <row r="7">
           <cell r="J7">
-            <v>14961</v>
+            <v>16943</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="30" refreshError="1"/>
+      <sheetData sheetId="31" refreshError="1"/>
+      <sheetData sheetId="32" refreshError="1"/>
+      <sheetData sheetId="33" refreshError="1"/>
+      <sheetData sheetId="34" refreshError="1"/>
+      <sheetData sheetId="35" refreshError="1"/>
+      <sheetData sheetId="36" refreshError="1"/>
+      <sheetData sheetId="37" refreshError="1"/>
+      <sheetData sheetId="38" refreshError="1"/>
+      <sheetData sheetId="39" refreshError="1"/>
+      <sheetData sheetId="40" refreshError="1"/>
+      <sheetData sheetId="41" refreshError="1"/>
+      <sheetData sheetId="42" refreshError="1"/>
+      <sheetData sheetId="43" refreshError="1"/>
+      <sheetData sheetId="44" refreshError="1"/>
+      <sheetData sheetId="45" refreshError="1"/>
+      <sheetData sheetId="46" refreshError="1"/>
+      <sheetData sheetId="47" refreshError="1"/>
+      <sheetData sheetId="48" refreshError="1"/>
+      <sheetData sheetId="49" refreshError="1"/>
+      <sheetData sheetId="50" refreshError="1"/>
+      <sheetData sheetId="51" refreshError="1"/>
+      <sheetData sheetId="52" refreshError="1"/>
+      <sheetData sheetId="53" refreshError="1"/>
+      <sheetData sheetId="54" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Master"/>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+      <sheetName val="Ozempic"/>
+      <sheetName val="Wegovy"/>
+      <sheetName val="Rybelsus"/>
+      <sheetName val="Type 2 Diabetes"/>
+      <sheetName val="Victoza"/>
+      <sheetName val="NovoLog"/>
+      <sheetName val="Levemir"/>
+      <sheetName val="Sogroya"/>
+      <sheetName val="insulin icodec"/>
+      <sheetName val="NLRP3"/>
+      <sheetName val="ziltivekimab"/>
+      <sheetName val="amycretin"/>
+      <sheetName val="GLP-1-GIP"/>
+      <sheetName val="cagrilintide"/>
+      <sheetName val="CDR132L"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="3">
+          <cell r="J3">
+            <v>4471</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="J5">
+            <v>12315</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="J6">
+            <v>29038</v>
           </cell>
         </row>
       </sheetData>
@@ -4802,43 +4810,35 @@
       <sheetData sheetId="15"/>
       <sheetData sheetId="16"/>
       <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-      <sheetData sheetId="54"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink20.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="5">
+          <cell r="J5">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="J6">
+            <v>7950</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -8355,7 +8355,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H26" sqref="H26"/>
+      <selection pane="bottomRight" activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8377,7 +8377,7 @@
     <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B1" s="1">
         <f ca="1">RANDBETWEEN(1,B209)</f>
-        <v>60</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
@@ -8926,7 +8926,7 @@
     <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14"/>
       <c r="B14" s="1">
-        <f t="shared" ref="B14:B24" si="2">+B13+1</f>
+        <f t="shared" ref="B14:B22" si="2">+B13+1</f>
         <v>8</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -9283,116 +9283,116 @@
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23"/>
       <c r="B23" s="1">
-        <f>+B26+1</f>
-        <v>17</v>
+        <f>+B25+1</f>
+        <v>18</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="D23" t="s">
-        <v>260</v>
-      </c>
-      <c r="E23" s="15">
-        <v>53.42</v>
+        <v>40</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="7">
+        <v>41</v>
       </c>
       <c r="F23" s="6">
-        <f>+E23*J23*EUR</f>
-        <v>58253.772804000007</v>
+        <f>+E23*J23/2</f>
+        <v>83619.5</v>
       </c>
       <c r="G23" s="6">
-        <f>([19]Main!$J$5-[19]Main!$J$6)</f>
-        <v>-36077</v>
+        <f>([19]Main!$J$6-[19]Main!$J$7)*GBP</f>
+        <v>-16541.2</v>
       </c>
       <c r="H23" s="6">
-        <f>+F23-G23</f>
-        <v>94330.772804000007</v>
+        <f>F23-G23</f>
+        <v>100160.7</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>661</v>
+        <v>1069</v>
       </c>
       <c r="J23" s="6">
-        <f>+[19]Main!$J$3</f>
-        <v>982.42</v>
+        <f>+[19]Main!$J$4</f>
+        <v>4079</v>
       </c>
       <c r="K23" s="9">
-        <v>45076</v>
+        <v>45532</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24"/>
       <c r="B24" s="1">
-        <f t="shared" si="2"/>
+        <f>+B23</f>
         <v>18</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>40</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" s="7">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="E24" s="16">
+        <v>1598</v>
       </c>
       <c r="F24" s="6">
-        <f>+E24*J24/2</f>
-        <v>83414.5</v>
+        <f>+E24*J24/100*GBP</f>
+        <v>84737.145999999993</v>
       </c>
       <c r="G24" s="6">
-        <f>+[20]Main!$J$6-[20]Main!$J$7</f>
-        <v>-14961</v>
+        <f>([19]Main!$J$6-[19]Main!$J$7)*GBP</f>
+        <v>-16541.2</v>
       </c>
       <c r="H24" s="6">
         <f>F24-G24</f>
-        <v>98375.5</v>
+        <v>101278.34599999999</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>306</v>
+        <v>1069</v>
       </c>
       <c r="J24" s="6">
-        <f>+[20]Main!$J$4</f>
-        <v>4069</v>
+        <f>+J23</f>
+        <v>4079</v>
       </c>
       <c r="K24" s="9">
-        <v>44987</v>
+        <f>+K23</f>
+        <v>45532</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25"/>
       <c r="B25" s="1">
-        <f>+B24</f>
-        <v>18</v>
+        <f>+B26+1</f>
+        <v>17</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E25" s="16">
-        <v>1598</v>
+        <v>259</v>
+      </c>
+      <c r="D25" t="s">
+        <v>260</v>
+      </c>
+      <c r="E25" s="15">
+        <v>53.42</v>
       </c>
       <c r="F25" s="6">
-        <f>+E25*J25/100*GBP</f>
-        <v>84529.406000000003</v>
+        <f>+E25*J25*EUR</f>
+        <v>58253.772804000007</v>
       </c>
       <c r="G25" s="6">
-        <f>+[20]Main!$J$6-[20]Main!$J$7</f>
-        <v>-14961</v>
+        <f>([18]Main!$J$5-[18]Main!$J$6)</f>
+        <v>-36077</v>
       </c>
       <c r="H25" s="6">
-        <f>F25-G25</f>
-        <v>99490.406000000003</v>
+        <f>+F25-G25</f>
+        <v>94330.772804000007</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>306</v>
+        <v>661</v>
       </c>
       <c r="J25" s="6">
-        <f>+J24</f>
-        <v>4069</v>
+        <f>+[18]Main!$J$3</f>
+        <v>982.42</v>
       </c>
       <c r="K25" s="9">
-        <f>+K24</f>
-        <v>44987</v>
+        <v>45076</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -9415,7 +9415,7 @@
         <v>74733</v>
       </c>
       <c r="G26" s="6">
-        <f>([18]Main!$J$5-[18]Main!$J$6)*EUR</f>
+        <f>([20]Main!$J$5-[20]Main!$J$6)*EUR</f>
         <v>-8824.5</v>
       </c>
       <c r="H26" s="6">
@@ -9435,7 +9435,7 @@
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27"/>
       <c r="B27" s="1">
-        <f>+B25+1</f>
+        <f>+B24+1</f>
         <v>19</v>
       </c>
       <c r="C27" s="5" t="s">
@@ -16890,12 +16890,12 @@
     <hyperlink ref="C80" r:id="rId40" xr:uid="{559FAD8A-D620-4B93-BE14-CC22630BD57E}"/>
     <hyperlink ref="C6" r:id="rId41" xr:uid="{467EEBCD-6BD7-4E71-B2C9-FCF3DB57F059}"/>
     <hyperlink ref="C209" r:id="rId42" xr:uid="{6A576FDB-A573-4A00-8381-4BECF13B35A1}"/>
-    <hyperlink ref="C25" r:id="rId43" xr:uid="{994E2867-C411-41E7-8332-43A0B3B0CC2B}"/>
+    <hyperlink ref="C24" r:id="rId43" xr:uid="{994E2867-C411-41E7-8332-43A0B3B0CC2B}"/>
     <hyperlink ref="C118" r:id="rId44" xr:uid="{51C9506E-5D60-43F8-BADA-7F72A25DAFF6}"/>
     <hyperlink ref="C107" r:id="rId45" xr:uid="{9E4325F2-98CF-4735-96D0-66A9DC5A8E86}"/>
     <hyperlink ref="C188" r:id="rId46" xr:uid="{6D062383-838D-42C7-BFCD-E5C9DC258548}"/>
     <hyperlink ref="C35" r:id="rId47" xr:uid="{3F36D809-73FC-441C-88D2-EEB42A40734A}"/>
-    <hyperlink ref="C23" r:id="rId48" xr:uid="{5D73AAA9-EBCA-4613-83CF-E75D37F58B6D}"/>
+    <hyperlink ref="C25" r:id="rId48" xr:uid="{5D73AAA9-EBCA-4613-83CF-E75D37F58B6D}"/>
     <hyperlink ref="C32" r:id="rId49" xr:uid="{203E18C7-425E-49E1-9AA5-204AFBE41E2D}"/>
     <hyperlink ref="C30" r:id="rId50" xr:uid="{5670E9A9-D014-4D7B-962A-54CBDC766969}"/>
     <hyperlink ref="C56" r:id="rId51" xr:uid="{04E7711A-AB14-45D0-B73B-7EA804EC5564}"/>

</xml_diff>

<commit_message>
TSLA, SMCI, F, BRZE, AMC, HD updates
</commit_message>
<xml_diff>
--- a/Biopharma.xlsx
+++ b/Biopharma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48199F4-8B15-4EC8-BB94-37CD89F070AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D34FED-F7DD-465F-BE07-5D31A7DCEBB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28500" yWindow="1680" windowWidth="28230" windowHeight="17955" xr2:uid="{17641224-F2C3-441B-B85B-BB32567FE633}"/>
+    <workbookView xWindow="-40665" yWindow="2580" windowWidth="27405" windowHeight="15345" xr2:uid="{17641224-F2C3-441B-B85B-BB32567FE633}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -8884,7 +8884,7 @@
       <sheetName val="Kepivance"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="5">
           <cell r="J5">
@@ -8897,35 +8897,35 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -9582,10 +9582,10 @@
   <dimension ref="A1:AD412"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D79" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K15" sqref="K15"/>
+      <selection pane="bottomRight" activeCell="I83" sqref="H83:I83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9608,7 +9608,7 @@
     <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B1" s="1">
         <f ca="1">RANDBETWEEN(1,B221)</f>
-        <v>73</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
RDDT and other updates
</commit_message>
<xml_diff>
--- a/Biopharma.xlsx
+++ b/Biopharma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823F1959-D8C5-49EA-BE17-1E86FBE1790D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54CEEDBA-DA79-4431-8BE0-3175DC5F0A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51390" yWindow="255" windowWidth="25650" windowHeight="19635" xr2:uid="{17641224-F2C3-441B-B85B-BB32567FE633}"/>
+    <workbookView xWindow="18165" yWindow="1935" windowWidth="25650" windowHeight="19635" xr2:uid="{17641224-F2C3-441B-B85B-BB32567FE633}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -5436,6 +5436,7 @@
       <sheetName val="Mounjaro-Zepbound"/>
       <sheetName val="Kisunla"/>
       <sheetName val="insulin efsitora"/>
+      <sheetName val="imlunestrant"/>
       <sheetName val="Ebglyss"/>
       <sheetName val="Jayprica"/>
       <sheetName val="Verzenio"/>
@@ -5501,6 +5502,7 @@
       <sheetData sheetId="26"/>
       <sheetData sheetId="27"/>
       <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -5661,23 +5663,23 @@
     </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
-      <sheetName val="REC-2282"/>
+      <sheetName val="RP-A501"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
           <cell r="K3">
-            <v>242.19640899999999</v>
+            <v>90.956000000000003</v>
           </cell>
         </row>
         <row r="5">
           <cell r="K5">
-            <v>473.4</v>
+            <v>278.82499999999999</v>
           </cell>
         </row>
         <row r="6">
           <cell r="K6">
-            <v>31.03</v>
+            <v>0</v>
           </cell>
         </row>
       </sheetData>
@@ -5695,6 +5697,40 @@
     </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
+      <sheetName val="REC-2282"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="K3">
+            <v>242.19640899999999</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="K5">
+            <v>473.4</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="K6">
+            <v>31.03</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink104.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Main"/>
       <sheetName val="BEAM-101"/>
       <sheetName val="BEAM-302"/>
     </sheetNames>
@@ -5723,7 +5759,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink104.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink105.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -5763,7 +5799,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink105.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink106.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -5797,7 +5833,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink106.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink107.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -5829,40 +5865,6 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink107.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Main"/>
-      <sheetName val="RP-A501"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="K3">
-            <v>90.956000000000003</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="K5">
-            <v>278.82499999999999</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="K6">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/externalLinks/externalLink108.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -5871,18 +5873,23 @@
     </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
-      <sheetName val="vusolimogene"/>
+      <sheetName val="SC291"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
+        <row r="3">
+          <cell r="I3">
+            <v>222.5</v>
+          </cell>
+        </row>
         <row r="5">
-          <cell r="K5">
-            <v>469.12400000000002</v>
+          <cell r="I5">
+            <v>251.643</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="K6">
-            <v>45.192</v>
+          <cell r="I6">
+            <v>0</v>
           </cell>
         </row>
       </sheetData>
@@ -5900,23 +5907,18 @@
     </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
-      <sheetName val="taletrectinib"/>
+      <sheetName val="vusolimogene"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="3">
-          <cell r="K3">
-            <v>249.24512899999999</v>
-          </cell>
-        </row>
         <row r="5">
           <cell r="K5">
-            <v>577.16899999999998</v>
+            <v>469.12400000000002</v>
           </cell>
         </row>
         <row r="6">
           <cell r="K6">
-            <v>11.634</v>
+            <v>45.192</v>
           </cell>
         </row>
       </sheetData>
@@ -6046,23 +6048,23 @@
     </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
-      <sheetName val="Model"/>
+      <sheetName val="taletrectinib"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="L3">
-            <v>294.66553199999998</v>
+          <cell r="K3">
+            <v>249.24512899999999</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="L5">
-            <v>851.52300000000002</v>
+          <cell r="K5">
+            <v>577.16899999999998</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="L6">
-            <v>0</v>
+          <cell r="K6">
+            <v>11.634</v>
           </cell>
         </row>
       </sheetData>
@@ -6073,6 +6075,40 @@
 </file>
 
 <file path=xl/externalLinks/externalLink111.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="L3">
+            <v>294.66553199999998</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="L5">
+            <v>851.52300000000002</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="L6">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink112.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -6103,7 +6139,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink112.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink113.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -6137,7 +6173,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink113.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink114.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -6170,7 +6206,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink114.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink115.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -6203,7 +6239,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink115.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink116.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -6253,7 +6289,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink116.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink117.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -6284,7 +6320,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink117.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink118.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -6318,7 +6354,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink118.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink119.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -6335,40 +6371,6 @@
         <row r="5">
           <cell r="K5">
             <v>449.76100000000002</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="K6">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink119.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Main"/>
-      <sheetName val="Model"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="K3">
-            <v>87.760456000000005</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="K5">
-            <v>361.86599999999999</v>
           </cell>
         </row>
         <row r="6">
@@ -6444,6 +6446,40 @@
     </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="K3">
+            <v>87.760456000000005</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="K5">
+            <v>361.86599999999999</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="K6">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink121.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Main"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
@@ -6468,7 +6504,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink121.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink122.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -6509,7 +6545,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink122.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink123.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -6538,7 +6574,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink123.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink124.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -6563,40 +6599,6 @@
         <row r="6">
           <cell r="K6">
             <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink124.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Main"/>
-      <sheetName val="seralutinib"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="K3">
-            <v>226.227259</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="K5">
-            <v>354.488</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="K6">
-            <v>197.05099999999999</v>
           </cell>
         </row>
       </sheetData>
@@ -6614,6 +6616,40 @@
     </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
+      <sheetName val="seralutinib"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="K3">
+            <v>226.227259</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="K5">
+            <v>354.488</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="K6">
+            <v>197.05099999999999</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink126.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Main"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
@@ -6638,7 +6674,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink126.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink127.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -6674,7 +6710,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink127.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink128.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -6717,7 +6753,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink128.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink129.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -6746,7 +6782,68 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink129.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink13.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Master"/>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+      <sheetName val="Lovenox"/>
+      <sheetName val="Lantus"/>
+      <sheetName val="Aubagio"/>
+      <sheetName val="Plavix"/>
+      <sheetName val="Multaq"/>
+      <sheetName val="idraparinux"/>
+      <sheetName val="SR 58611"/>
+      <sheetName val="Eplivanserin"/>
+      <sheetName val="SSR 591813"/>
+      <sheetName val="Xaliproden"/>
+      <sheetName val="Alvocidib"/>
+      <sheetName val="SR 121463"/>
+      <sheetName val="BSI-201"/>
+      <sheetName val="Zimulti"/>
+      <sheetName val="Failures"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="5">
+          <cell r="K5">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="K6">
+            <v>15112</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink130.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -6835,68 +6932,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink13.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Master"/>
-      <sheetName val="Main"/>
-      <sheetName val="Model"/>
-      <sheetName val="Lovenox"/>
-      <sheetName val="Lantus"/>
-      <sheetName val="Aubagio"/>
-      <sheetName val="Plavix"/>
-      <sheetName val="Multaq"/>
-      <sheetName val="idraparinux"/>
-      <sheetName val="SR 58611"/>
-      <sheetName val="Eplivanserin"/>
-      <sheetName val="SSR 591813"/>
-      <sheetName val="Xaliproden"/>
-      <sheetName val="Alvocidib"/>
-      <sheetName val="SR 121463"/>
-      <sheetName val="BSI-201"/>
-      <sheetName val="Zimulti"/>
-      <sheetName val="Failures"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="5">
-          <cell r="K5">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="K6">
-            <v>15112</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink130.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink131.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -6926,35 +6962,6 @@
       <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink131.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Main"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="M3">
-            <v>44.710678000000001</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="M5">
-            <v>120.43700000000001</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="M6">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6970,17 +6977,17 @@
       <sheetData sheetId="0">
         <row r="3">
           <cell r="M3">
-            <v>184.19892899999999</v>
+            <v>44.710678000000001</v>
           </cell>
         </row>
         <row r="5">
           <cell r="M5">
-            <v>67.233999999999995</v>
+            <v>120.43700000000001</v>
           </cell>
         </row>
         <row r="6">
           <cell r="M6">
-            <v>126.736</v>
+            <v>0</v>
           </cell>
         </row>
       </sheetData>
@@ -6990,6 +6997,35 @@
 </file>
 
 <file path=xl/externalLinks/externalLink133.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="M3">
+            <v>184.19892899999999</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="M5">
+            <v>67.233999999999995</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="M6">
+            <v>126.736</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink134.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -7013,35 +7049,6 @@
         <row r="6">
           <cell r="K6">
             <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink134.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Main"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="N3">
-            <v>9.4141049999999993</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="N5">
-            <v>11.249000000000001</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="N6">
-            <v>18.713000000000001</v>
           </cell>
         </row>
       </sheetData>
@@ -7060,17 +7067,17 @@
       <sheetData sheetId="0">
         <row r="3">
           <cell r="N3">
-            <v>20.079526999999999</v>
+            <v>9.4141049999999993</v>
           </cell>
         </row>
         <row r="5">
           <cell r="N5">
-            <v>16.64</v>
+            <v>11.249000000000001</v>
           </cell>
         </row>
         <row r="6">
           <cell r="N6">
-            <v>0.69799999999999995</v>
+            <v>18.713000000000001</v>
           </cell>
         </row>
       </sheetData>
@@ -7088,18 +7095,18 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="L3">
-            <v>48.69059</v>
+          <cell r="N3">
+            <v>20.079526999999999</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="L5">
-            <v>18.687999999999999</v>
+          <cell r="N5">
+            <v>16.64</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="L6">
-            <v>5.4249999999999998</v>
+          <cell r="N6">
+            <v>0.69799999999999995</v>
           </cell>
         </row>
       </sheetData>
@@ -7117,18 +7124,18 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="M3">
-            <v>20.500177000000001</v>
+          <cell r="L3">
+            <v>48.69059</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="M5">
-            <v>131.17699999999999</v>
+          <cell r="L5">
+            <v>18.687999999999999</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="M6">
-            <v>0</v>
+          <cell r="L6">
+            <v>5.4249999999999998</v>
           </cell>
         </row>
       </sheetData>
@@ -7138,6 +7145,35 @@
 </file>
 
 <file path=xl/externalLinks/externalLink138.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="M3">
+            <v>20.500177000000001</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="M5">
+            <v>131.17699999999999</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="M6">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink139.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -7195,40 +7231,6 @@
       <sheetData sheetId="15" refreshError="1"/>
       <sheetData sheetId="16" refreshError="1"/>
       <sheetData sheetId="17" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink139.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Main"/>
-      <sheetName val="ATEV"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="J3">
-            <v>119.351122</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="J5">
-            <v>95.563000000000002</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="J6">
-            <v>60.078000000000003</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7318,6 +7320,40 @@
     </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
+      <sheetName val="ATEV"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="J3">
+            <v>119.351122</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="J5">
+            <v>95.563000000000002</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="J6">
+            <v>60.078000000000003</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink141.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Main"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
@@ -7342,7 +7378,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink141.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink142.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -7376,7 +7412,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink142.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink143.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -7410,7 +7446,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink143.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink144.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -7439,7 +7475,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink144.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink145.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -7475,7 +7511,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink145.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink146.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -7499,40 +7535,6 @@
         </row>
         <row r="6">
           <cell r="J6">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink146.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Main"/>
-      <sheetName val="CLS-AX"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="K3">
-            <v>74.745571999999996</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="K5">
-            <v>29.36</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="K6">
             <v>0</v>
           </cell>
         </row>
@@ -7551,60 +7553,33 @@
     </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
+      <sheetName val="CLS-AX"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="L3">
-            <v>35.424388</v>
+          <cell r="K3">
+            <v>74.745571999999996</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="L5">
-            <v>33.298999999999999</v>
+          <cell r="K5">
+            <v>29.36</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="L6">
+          <cell r="K6">
             <v>0</v>
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
 <file path=xl/externalLinks/externalLink148.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Main"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="K3">
-            <v>35.751956</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="K5">
-            <v>66.650000000000006</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="K6">
-            <v>11.667</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink149.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -7616,18 +7591,47 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
+          <cell r="L3">
+            <v>35.424388</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="L5">
+            <v>33.298999999999999</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="L6">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink149.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
           <cell r="K3">
-            <v>70.558753999999993</v>
+            <v>35.751956</v>
           </cell>
         </row>
         <row r="5">
           <cell r="K5">
-            <v>426.65000000000003</v>
+            <v>66.650000000000006</v>
           </cell>
         </row>
         <row r="6">
           <cell r="K6">
-            <v>0</v>
+            <v>11.667</v>
           </cell>
         </row>
       </sheetData>
@@ -7692,27 +7696,25 @@
     </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
-      <sheetName val="pz-cel"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="J3">
-            <v>43.314397</v>
+          <cell r="K3">
+            <v>70.558753999999993</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="J5">
-            <v>122.708</v>
+          <cell r="K5">
+            <v>426.65000000000003</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="J6">
-            <v>18.355</v>
+          <cell r="K6">
+            <v>0</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7726,23 +7728,23 @@
     </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
-      <sheetName val="Model"/>
+      <sheetName val="pz-cel"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="K3">
-            <v>27.999521999999999</v>
+          <cell r="J3">
+            <v>43.314397</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="K5">
-            <v>19.905999999999999</v>
+          <cell r="J5">
+            <v>122.708</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="K6">
-            <v>4.4909999999999997</v>
+          <cell r="J6">
+            <v>18.355</v>
           </cell>
         </row>
       </sheetData>
@@ -7760,25 +7762,27 @@
     </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
+      <sheetName val="Model"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="L3">
-            <v>36.819809999999997</v>
+          <cell r="K3">
+            <v>27.999521999999999</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="L5">
-            <v>57.733724000000002</v>
+          <cell r="K5">
+            <v>19.905999999999999</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="L6">
-            <v>24.225999999999999</v>
+          <cell r="K6">
+            <v>4.4909999999999997</v>
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7792,27 +7796,25 @@
     </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
-      <sheetName val="Model"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="P3">
-            <v>22.004159000000001</v>
+          <cell r="L3">
+            <v>36.819809999999997</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="P5">
-            <v>4.1559999999999997</v>
+          <cell r="L5">
+            <v>57.733724000000002</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="P6">
-            <v>8.4879999999999995</v>
+          <cell r="L6">
+            <v>24.225999999999999</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7831,18 +7833,18 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="J3">
-            <v>4263.5283170000002</v>
+          <cell r="P3">
+            <v>22.004159000000001</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="J5">
-            <v>10082.542000000001</v>
+          <cell r="P5">
+            <v>4.1559999999999997</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="J6">
-            <v>2347.1640000000002</v>
+          <cell r="P6">
+            <v>8.4879999999999995</v>
           </cell>
         </row>
       </sheetData>
@@ -7860,27 +7862,27 @@
     </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
-      <sheetName val="SC291"/>
+      <sheetName val="Model"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="I3">
-            <v>222.5</v>
+          <cell r="J3">
+            <v>4263.5283170000002</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="I5">
-            <v>251.643</v>
+          <cell r="J5">
+            <v>10082.542000000001</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="I6">
-            <v>0</v>
+          <cell r="J6">
+            <v>2347.1640000000002</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7925,7 +7927,7 @@
       <sheetName val="Tamiflu"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="3">
           <cell r="J3">
@@ -7943,34 +7945,34 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -8721,12 +8723,12 @@
       <sheetName val="Duragesic"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
       <sheetData sheetId="6">
         <row r="3">
           <cell r="R3">
@@ -8744,50 +8746,50 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
-      <sheetData sheetId="33" refreshError="1"/>
-      <sheetData sheetId="34" refreshError="1"/>
-      <sheetData sheetId="35" refreshError="1"/>
-      <sheetData sheetId="36" refreshError="1"/>
-      <sheetData sheetId="37" refreshError="1"/>
-      <sheetData sheetId="38" refreshError="1"/>
-      <sheetData sheetId="39" refreshError="1"/>
-      <sheetData sheetId="40" refreshError="1"/>
-      <sheetData sheetId="41" refreshError="1"/>
-      <sheetData sheetId="42" refreshError="1"/>
-      <sheetData sheetId="43" refreshError="1"/>
-      <sheetData sheetId="44" refreshError="1"/>
-      <sheetData sheetId="45" refreshError="1"/>
-      <sheetData sheetId="46" refreshError="1"/>
-      <sheetData sheetId="47" refreshError="1"/>
-      <sheetData sheetId="48" refreshError="1"/>
-      <sheetData sheetId="49" refreshError="1"/>
-      <sheetData sheetId="50" refreshError="1"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+      <sheetData sheetId="37"/>
+      <sheetData sheetId="38"/>
+      <sheetData sheetId="39"/>
+      <sheetData sheetId="40"/>
+      <sheetData sheetId="41"/>
+      <sheetData sheetId="42"/>
+      <sheetData sheetId="43"/>
+      <sheetData sheetId="44"/>
+      <sheetData sheetId="45"/>
+      <sheetData sheetId="46"/>
+      <sheetData sheetId="47"/>
+      <sheetData sheetId="48"/>
+      <sheetData sheetId="49"/>
+      <sheetData sheetId="50"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -10213,26 +10215,28 @@
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
+      <sheetName val="VK2735"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="L3">
-            <v>146.21109100000001</v>
+          <cell r="K3">
+            <v>104</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="L5">
-            <v>2078.6860000000001</v>
+          <cell r="K5">
+            <v>711</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="L6">
-            <v>1768.7780000000002</v>
+          <cell r="K6">
+            <v>0</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -10246,25 +10250,27 @@
     </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
+      <sheetName val="Model"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="K3">
-            <v>221.74757500000001</v>
+          <cell r="L3">
+            <v>146.21109100000001</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="K5">
-            <v>236</v>
+          <cell r="L5">
+            <v>2078.6860000000001</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="K6">
-            <v>1512</v>
+          <cell r="L6">
+            <v>1768.7780000000002</v>
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -10278,27 +10284,25 @@
     </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
-      <sheetName val="Model"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="L3">
-            <v>533.87796600000001</v>
+          <cell r="K3">
+            <v>221.74757500000001</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="L5">
-            <v>365009</v>
+          <cell r="K5">
+            <v>236</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="L6">
-            <v>0</v>
+          <cell r="K6">
+            <v>1512</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -10317,18 +10321,18 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="N3">
-            <v>136.41541799999999</v>
+          <cell r="L3">
+            <v>533.87796600000001</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="N5">
-            <v>542.79999999999995</v>
+          <cell r="L5">
+            <v>365009</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="N6">
-            <v>4057.6000000000004</v>
+          <cell r="L6">
+            <v>0</v>
           </cell>
         </row>
       </sheetData>
@@ -10351,18 +10355,18 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="L3">
-            <v>105.66692500000001</v>
+          <cell r="N3">
+            <v>136.41541799999999</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="L5">
-            <v>1024.6570000000002</v>
+          <cell r="N5">
+            <v>542.79999999999995</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="L6">
-            <v>0</v>
+          <cell r="N6">
+            <v>4057.6000000000004</v>
           </cell>
         </row>
       </sheetData>
@@ -10381,28 +10385,26 @@
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
-      <sheetName val="aficamten"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="K3">
-            <v>117.659578</v>
+          <cell r="L3">
+            <v>105.66692500000001</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="K5">
-            <v>1362.136</v>
+          <cell r="L5">
+            <v>1024.6570000000002</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="K6">
-            <v>654.95100000000002</v>
+          <cell r="L6">
+            <v>0</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -10417,23 +10419,23 @@
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
-      <sheetName val="VK2735"/>
+      <sheetName val="aficamten"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
           <cell r="K3">
-            <v>104</v>
+            <v>117.659578</v>
           </cell>
         </row>
         <row r="5">
           <cell r="K5">
-            <v>711</v>
+            <v>1362.136</v>
           </cell>
         </row>
         <row r="6">
           <cell r="K6">
-            <v>0</v>
+            <v>654.95100000000002</v>
           </cell>
         </row>
       </sheetData>
@@ -11750,6 +11752,8 @@
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
+      <sheetName val="navacaprant"/>
+      <sheetName val="Options"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
@@ -11769,7 +11773,9 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -12122,10 +12128,10 @@
   <dimension ref="A1:AD436"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D91" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K21" sqref="K21"/>
+      <selection pane="bottomRight" activeCell="L97" sqref="L97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12148,13 +12154,13 @@
     <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B1" s="1">
         <f ca="1">RANDBETWEEN(1,B240)</f>
-        <v>120</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="F2" s="6">
         <f>SUM(F4:F454)-F5-F10-F12-F17-F24-F27-F47-F55</f>
-        <v>5644504.5401696106</v>
+        <v>5644045.0764096109</v>
       </c>
       <c r="K2" s="9">
         <f>MIN(K4:K91)</f>
@@ -15005,7 +15011,7 @@
         <v>8112</v>
       </c>
       <c r="G71" s="26">
-        <f>+[68]Main!$K$5-[68]Main!$K$6</f>
+        <f>+[62]Main!$K$5-[62]Main!$K$6</f>
         <v>711</v>
       </c>
       <c r="H71" s="27">
@@ -15016,7 +15022,7 @@
         <v>1117</v>
       </c>
       <c r="J71" s="26">
-        <f>+[68]Main!$K$3</f>
+        <f>+[62]Main!$K$3</f>
         <v>104</v>
       </c>
       <c r="K71" s="45">
@@ -15059,7 +15065,7 @@
         <v>7284.2365536200004</v>
       </c>
       <c r="G72" s="6">
-        <f>+[62]Main!$L$5-[62]Main!$L$6</f>
+        <f>+[63]Main!$L$5-[63]Main!$L$6</f>
         <v>309.9079999999999</v>
       </c>
       <c r="H72" s="6">
@@ -15070,7 +15076,7 @@
         <v>1074</v>
       </c>
       <c r="J72" s="6">
-        <f>+[62]Main!$L$3</f>
+        <f>+[63]Main!$L$3</f>
         <v>146.21109100000001</v>
       </c>
       <c r="K72" s="9">
@@ -15099,7 +15105,7 @@
         <v>5742.3752022000008</v>
       </c>
       <c r="G73" s="6">
-        <f>+[63]Main!$K$5-[63]Main!$K$6</f>
+        <f>+[64]Main!$K$5-[64]Main!$K$6</f>
         <v>-1276</v>
       </c>
       <c r="H73" s="6">
@@ -15110,7 +15116,7 @@
         <v>1074</v>
       </c>
       <c r="J73" s="6">
-        <f>+[63]Main!$K$3</f>
+        <f>+[64]Main!$K$3</f>
         <v>221.74757500000001</v>
       </c>
       <c r="K73" s="9">
@@ -15136,7 +15142,7 @@
         <v>9510.5627333907069</v>
       </c>
       <c r="G74" s="6">
-        <f>([64]Main!$L$5-[64]Main!$L$6)/JPY</f>
+        <f>([65]Main!$L$5-[65]Main!$L$6)/JPY</f>
         <v>2512.9707401032701</v>
       </c>
       <c r="H74" s="6">
@@ -15147,7 +15153,7 @@
         <v>1074</v>
       </c>
       <c r="J74" s="6">
-        <f>+[64]Main!$L$3</f>
+        <f>+[65]Main!$L$3</f>
         <v>533.87796600000001</v>
       </c>
       <c r="K74" s="9">
@@ -15176,7 +15182,7 @@
         <v>3477.2290048199993</v>
       </c>
       <c r="G75" s="6">
-        <f>+[65]Main!$N$5-[65]Main!$N$6</f>
+        <f>+[66]Main!$N$5-[66]Main!$N$6</f>
         <v>-3514.8</v>
       </c>
       <c r="H75" s="6">
@@ -15187,7 +15193,7 @@
         <v>1074</v>
       </c>
       <c r="J75" s="6">
-        <f>+[65]Main!$N$3</f>
+        <f>+[66]Main!$N$3</f>
         <v>136.41541799999999</v>
       </c>
       <c r="K75" s="9">
@@ -15216,7 +15222,7 @@
         <v>7619.6419617500005</v>
       </c>
       <c r="G76" s="6">
-        <f>+[66]Main!$L$5-[66]Main!$L$6</f>
+        <f>+[67]Main!$L$5-[67]Main!$L$6</f>
         <v>1024.6570000000002</v>
       </c>
       <c r="H76" s="6">
@@ -15227,7 +15233,7 @@
         <v>1074</v>
       </c>
       <c r="J76" s="6">
-        <f>+[66]Main!$L$3</f>
+        <f>+[67]Main!$L$3</f>
         <v>105.66692500000001</v>
       </c>
       <c r="K76" s="9">
@@ -15253,7 +15259,7 @@
         <v>6668.9448810399999</v>
       </c>
       <c r="G77" s="6">
-        <f>+[67]Main!$K$5-[67]Main!$K$6</f>
+        <f>+[68]Main!$K$5-[68]Main!$K$6</f>
         <v>707.18499999999995</v>
       </c>
       <c r="H77" s="6">
@@ -15264,7 +15270,7 @@
         <v>1074</v>
       </c>
       <c r="J77" s="6">
-        <f>+[67]Main!$K$3</f>
+        <f>+[68]Main!$K$3</f>
         <v>117.659578</v>
       </c>
       <c r="K77" s="9">
@@ -16423,11 +16429,11 @@
         <v>1300</v>
       </c>
       <c r="E107" s="7">
-        <v>14.6</v>
+        <v>11.71</v>
       </c>
       <c r="F107" s="6">
         <f>+E107*[98]Main!$K$3</f>
-        <v>2321.1664000000001</v>
+        <v>1861.7026400000002</v>
       </c>
       <c r="G107" s="6">
         <f>+[98]Main!$K$5-[98]Main!$K$6</f>
@@ -16435,10 +16441,17 @@
       </c>
       <c r="H107" s="6">
         <f>+F107-G107</f>
-        <v>1949.5273999999999</v>
+        <v>1490.0636400000003</v>
       </c>
       <c r="I107" s="3" t="s">
         <v>1074</v>
+      </c>
+      <c r="J107" s="6">
+        <f>+[98]Main!$K$3</f>
+        <v>158.98400000000001</v>
+      </c>
+      <c r="K107" s="9">
+        <v>45600</v>
       </c>
     </row>
     <row r="108" spans="1:29" x14ac:dyDescent="0.2">
@@ -16600,7 +16613,7 @@
         <v>1559.8953999999999</v>
       </c>
       <c r="G111" s="6">
-        <f>+[107]Main!$K$5-[107]Main!$K$6</f>
+        <f>+[102]Main!$K$5-[102]Main!$K$6</f>
         <v>278.82499999999999</v>
       </c>
       <c r="H111" s="6">
@@ -16611,7 +16624,7 @@
         <v>1074</v>
       </c>
       <c r="J111" s="6">
-        <f>+[107]Main!$K$3</f>
+        <f>+[102]Main!$K$3</f>
         <v>90.956000000000003</v>
       </c>
       <c r="K111" s="9">
@@ -16640,7 +16653,7 @@
         <v>1487.0859512599998</v>
       </c>
       <c r="G112" s="6">
-        <f>[102]Main!$K$5-[102]Main!$K$6</f>
+        <f>[103]Main!$K$5-[103]Main!$K$6</f>
         <v>442.37</v>
       </c>
       <c r="H112" s="6">
@@ -16651,7 +16664,7 @@
         <v>1074</v>
       </c>
       <c r="J112" s="6">
-        <f>[102]Main!$K$3</f>
+        <f>[103]Main!$K$3</f>
         <v>242.19640899999999</v>
       </c>
       <c r="K112" s="9">
@@ -16680,7 +16693,7 @@
         <v>2019.1826655000002</v>
       </c>
       <c r="G113" s="6">
-        <f>+[103]Main!$K$5-[103]Main!$K$6</f>
+        <f>+[104]Main!$K$5-[104]Main!$K$6</f>
         <v>1008.165</v>
       </c>
       <c r="H113" s="6">
@@ -16691,7 +16704,7 @@
         <v>1074</v>
       </c>
       <c r="J113" s="6">
-        <f>+[103]Main!$K$3</f>
+        <f>+[104]Main!$K$3</f>
         <v>82.415619000000007</v>
       </c>
       <c r="K113" s="9">
@@ -16720,7 +16733,7 @@
         <v>1929.5</v>
       </c>
       <c r="G114" s="6">
-        <f>+[104]Main!$J$5-[104]Main!$J$6</f>
+        <f>+[105]Main!$J$5-[105]Main!$J$6</f>
         <v>939.9</v>
       </c>
       <c r="H114" s="6">
@@ -16731,7 +16744,7 @@
         <v>1044</v>
       </c>
       <c r="J114" s="6">
-        <f>+[104]Main!$J$3</f>
+        <f>+[105]Main!$J$3</f>
         <v>96.474999999999994</v>
       </c>
       <c r="K114" s="9">
@@ -16760,7 +16773,7 @@
         <v>1352.1643102179487</v>
       </c>
       <c r="G115" s="6">
-        <f>([105]Main!$J$6-[105]Main!$J$7)/HKD</f>
+        <f>([106]Main!$J$6-[106]Main!$J$7)/HKD</f>
         <v>376.08884615384613</v>
       </c>
       <c r="H115" s="6">
@@ -16771,7 +16784,7 @@
         <v>1117</v>
       </c>
       <c r="J115" s="6">
-        <f>+[105]Main!$J$4</f>
+        <f>+[106]Main!$J$4</f>
         <v>985.68987100000004</v>
       </c>
       <c r="K115" s="9">
@@ -16829,7 +16842,7 @@
         <v>1252.1289825000001</v>
       </c>
       <c r="G117" s="6">
-        <f>+[106]Main!$O$5-[106]Main!$O$6</f>
+        <f>+[107]Main!$O$5-[107]Main!$O$6</f>
         <v>637.79299999999989</v>
       </c>
       <c r="H117" s="6">
@@ -16840,7 +16853,7 @@
         <v>1074</v>
       </c>
       <c r="J117" s="6">
-        <f>+[106]Main!$O$3</f>
+        <f>+[107]Main!$O$3</f>
         <v>61.833530000000003</v>
       </c>
       <c r="K117" s="9">
@@ -16866,7 +16879,7 @@
         <v>918.92499999999995</v>
       </c>
       <c r="G118" s="6">
-        <f>+[155]Main!$I$5-[155]Main!$I$6</f>
+        <f>+[108]Main!$I$5-[108]Main!$I$6</f>
         <v>251.643</v>
       </c>
       <c r="H118" s="6">
@@ -16877,7 +16890,7 @@
         <v>1074</v>
       </c>
       <c r="J118" s="6">
-        <f>+[155]Main!$I$3</f>
+        <f>+[108]Main!$I$3</f>
         <v>222.5</v>
       </c>
       <c r="K118" s="9">
@@ -16906,7 +16919,7 @@
         <v>760.17899999999997</v>
       </c>
       <c r="G119" s="6">
-        <f>+[108]Main!$K$5-[108]Main!$K$6</f>
+        <f>+[109]Main!$K$5-[109]Main!$K$6</f>
         <v>423.93200000000002</v>
       </c>
       <c r="H119" s="6">
@@ -16946,7 +16959,7 @@
         <v>757.70519216000002</v>
       </c>
       <c r="G120" s="6">
-        <f>+[109]Main!$K$5-[109]Main!$K$6</f>
+        <f>+[110]Main!$K$5-[110]Main!$K$6</f>
         <v>565.53499999999997</v>
       </c>
       <c r="H120" s="6">
@@ -16957,7 +16970,7 @@
         <v>1074</v>
       </c>
       <c r="J120" s="6">
-        <f>+[109]Main!$K$3</f>
+        <f>+[110]Main!$K$3</f>
         <v>249.24512899999999</v>
       </c>
       <c r="K120" s="9">
@@ -16989,7 +17002,7 @@
         <v>701.30396615999996</v>
       </c>
       <c r="G121" s="6">
-        <f>+[110]Main!$L$5-[110]Main!$L$6</f>
+        <f>+[111]Main!$L$5-[111]Main!$L$6</f>
         <v>851.52300000000002</v>
       </c>
       <c r="H121" s="6">
@@ -17000,7 +17013,7 @@
         <v>1074</v>
       </c>
       <c r="J121" s="6">
-        <f>+[110]Main!$L$3</f>
+        <f>+[111]Main!$L$3</f>
         <v>294.66553199999998</v>
       </c>
       <c r="K121" s="9">
@@ -17586,7 +17599,7 @@
         <v>1873.2795513199999</v>
       </c>
       <c r="G157" s="6">
-        <f>+[111]Main!$J$5-[111]Main!$J$6</f>
+        <f>+[112]Main!$J$5-[112]Main!$J$6</f>
         <v>566.44900000000007</v>
       </c>
       <c r="H157" s="6">
@@ -17597,7 +17610,7 @@
         <v>301</v>
       </c>
       <c r="J157" s="6">
-        <f>+[111]Main!$J$3</f>
+        <f>+[112]Main!$J$3</f>
         <v>58.068182</v>
       </c>
       <c r="K157" s="9">
@@ -17626,7 +17639,7 @@
         <v>686.11028007999994</v>
       </c>
       <c r="G158" s="6">
-        <f>[112]Main!$L$5-[112]Main!$L$6</f>
+        <f>[113]Main!$L$5-[113]Main!$L$6</f>
         <v>578</v>
       </c>
       <c r="H158" s="6">
@@ -17637,7 +17650,7 @@
         <v>649</v>
       </c>
       <c r="J158" s="6">
-        <f>[112]Main!$L$3</f>
+        <f>[113]Main!$L$3</f>
         <v>55.286887999999998</v>
       </c>
       <c r="K158" s="9">
@@ -17666,7 +17679,7 @@
         <v>205.55876502000001</v>
       </c>
       <c r="G159" s="6">
-        <f>[113]Main!$O$5-[113]Main!$O$6</f>
+        <f>[114]Main!$O$5-[114]Main!$O$6</f>
         <v>345.67399999999998</v>
       </c>
       <c r="H159" s="6">
@@ -17677,7 +17690,7 @@
         <v>649</v>
       </c>
       <c r="J159" s="6">
-        <f>[113]Main!$O$3</f>
+        <f>[114]Main!$O$3</f>
         <v>67.176067000000003</v>
       </c>
       <c r="K159" s="9">
@@ -17706,7 +17719,7 @@
         <v>434.74418623999998</v>
       </c>
       <c r="G160" s="6">
-        <f>[114]Main!$K$5-[114]Main!$K$6</f>
+        <f>[115]Main!$K$5-[115]Main!$K$6</f>
         <v>1272.4940000000001</v>
       </c>
       <c r="H160" s="6">
@@ -17717,7 +17730,7 @@
         <v>517</v>
       </c>
       <c r="J160" s="6">
-        <f>[114]Main!$K$3</f>
+        <f>[115]Main!$K$3</f>
         <v>59.717607999999998</v>
       </c>
       <c r="K160" s="9">
@@ -18629,7 +18642,7 @@
         <v>1364.9219226999999</v>
       </c>
       <c r="G210" s="27">
-        <f>+[115]Main!$J$5-[115]Main!$J$6</f>
+        <f>+[116]Main!$J$5-[116]Main!$J$6</f>
         <v>167.291</v>
       </c>
       <c r="H210" s="27">
@@ -18640,7 +18653,7 @@
         <v>1074</v>
       </c>
       <c r="J210" s="27">
-        <f>+[115]Main!$J$3</f>
+        <f>+[116]Main!$J$3</f>
         <v>47.976165999999999</v>
       </c>
       <c r="K210" s="45">
@@ -18665,11 +18678,11 @@
         <v>15.65</v>
       </c>
       <c r="F211" s="6">
-        <f>E211*[116]Main!$L$3</f>
+        <f>E211*[117]Main!$L$3</f>
         <v>1253.1559559500001</v>
       </c>
       <c r="G211" s="6">
-        <f>+[116]Main!$L$5-[116]Main!$L$6</f>
+        <f>+[117]Main!$L$5-[117]Main!$L$6</f>
         <v>112.015</v>
       </c>
       <c r="H211" s="6">
@@ -18700,7 +18713,7 @@
         <v>1318.30476669</v>
       </c>
       <c r="G212" s="6">
-        <f>+[117]Main!$K$5-[117]Main!$K$6</f>
+        <f>+[118]Main!$K$5-[118]Main!$K$6</f>
         <v>304.87299999999999</v>
       </c>
       <c r="H212" s="6">
@@ -18711,7 +18724,7 @@
         <v>1074</v>
       </c>
       <c r="J212" s="6">
-        <f>+[117]Main!$K$3</f>
+        <f>+[118]Main!$K$3</f>
         <v>38.899521</v>
       </c>
       <c r="K212" s="9">
@@ -18740,7 +18753,7 @@
         <v>1355.4004112499999</v>
       </c>
       <c r="G213" s="6">
-        <f>+[118]Main!$K$5-[118]Main!$K$6</f>
+        <f>+[119]Main!$K$5-[119]Main!$K$6</f>
         <v>449.76100000000002</v>
       </c>
       <c r="H213" s="6">
@@ -18751,7 +18764,7 @@
         <v>419</v>
       </c>
       <c r="J213" s="6">
-        <f>+[118]Main!$K$3</f>
+        <f>+[119]Main!$K$3</f>
         <v>57.069490999999999</v>
       </c>
       <c r="K213" s="9">
@@ -18783,7 +18796,7 @@
         <v>1258.48493904</v>
       </c>
       <c r="G214" s="6">
-        <f>+[119]Main!$K$5-[119]Main!$K$6</f>
+        <f>+[120]Main!$K$5-[120]Main!$K$6</f>
         <v>361.86599999999999</v>
       </c>
       <c r="H214" s="6">
@@ -18794,7 +18807,7 @@
         <v>1074</v>
       </c>
       <c r="J214" s="6">
-        <f>+[119]Main!$K$3</f>
+        <f>+[120]Main!$K$3</f>
         <v>87.760456000000005</v>
       </c>
       <c r="K214" s="9">
@@ -18820,7 +18833,7 @@
         <v>963.56021369000007</v>
       </c>
       <c r="G215" s="6">
-        <f>+[120]Main!$L$5-[120]Main!$L$6</f>
+        <f>+[121]Main!$L$5-[121]Main!$L$6</f>
         <v>122.197</v>
       </c>
       <c r="H215" s="6">
@@ -18831,7 +18844,7 @@
         <v>1074</v>
       </c>
       <c r="J215" s="6">
-        <f>+[120]Main!$L$3</f>
+        <f>+[121]Main!$L$3</f>
         <v>114.846271</v>
       </c>
       <c r="K215" s="9">
@@ -18856,11 +18869,11 @@
         <v>11</v>
       </c>
       <c r="F216" s="6">
-        <f>+E216*[121]Main!$L$3</f>
+        <f>+E216*[122]Main!$L$3</f>
         <v>798.23003700000004</v>
       </c>
       <c r="G216" s="6">
-        <f>+[121]Main!$L$5-[121]Main!$L$6</f>
+        <f>+[122]Main!$L$5-[122]Main!$L$6</f>
         <v>153.25991400000001</v>
       </c>
       <c r="H216" s="6">
@@ -18901,7 +18914,7 @@
         <v>897.18233664000002</v>
       </c>
       <c r="G217" s="6">
-        <f>+[122]Main!$J$5-[122]Main!$J$6</f>
+        <f>+[123]Main!$J$5-[123]Main!$J$6</f>
         <v>601.58999999999992</v>
       </c>
       <c r="H217" s="6">
@@ -18912,7 +18925,7 @@
         <v>16</v>
       </c>
       <c r="J217" s="6">
-        <f>+[122]Main!$J$3</f>
+        <f>+[123]Main!$J$3</f>
         <v>121.89977399999999</v>
       </c>
       <c r="K217" s="9">
@@ -18939,7 +18952,7 @@
         <v>357.16781451000003</v>
       </c>
       <c r="G218" s="6">
-        <f>+[123]Main!$K$5-[123]Main!$K$6</f>
+        <f>+[124]Main!$K$5-[124]Main!$K$6</f>
         <v>62.650000000000006</v>
       </c>
       <c r="H218" s="6">
@@ -18950,7 +18963,7 @@
         <v>1074</v>
       </c>
       <c r="J218" s="6">
-        <f>+[123]Main!$K$3</f>
+        <f>+[124]Main!$K$3</f>
         <v>62.551281000000003</v>
       </c>
       <c r="K218" s="9">
@@ -18980,7 +18993,7 @@
         <v>226.227259</v>
       </c>
       <c r="G219" s="6">
-        <f>+[124]Main!$K$5-[124]Main!$K$6</f>
+        <f>+[125]Main!$K$5-[125]Main!$K$6</f>
         <v>157.43700000000001</v>
       </c>
       <c r="H219" s="6">
@@ -18991,7 +19004,7 @@
         <v>1074</v>
       </c>
       <c r="J219" s="6">
-        <f>+[124]Main!$K$3</f>
+        <f>+[125]Main!$K$3</f>
         <v>226.227259</v>
       </c>
       <c r="K219" s="9">
@@ -19105,7 +19118,7 @@
         <v>289.28000241999996</v>
       </c>
       <c r="G223" s="6">
-        <f>+[125]Main!$J$5-[125]Main!$J$6</f>
+        <f>+[126]Main!$J$5-[126]Main!$J$6</f>
         <v>220.43200000000002</v>
       </c>
       <c r="H223" s="6">
@@ -19116,7 +19129,7 @@
         <v>1074</v>
       </c>
       <c r="J223" s="6">
-        <f>+[125]Main!$J$3</f>
+        <f>+[126]Main!$J$3</f>
         <v>30.972162999999998</v>
       </c>
       <c r="K223" s="9">
@@ -19199,7 +19212,7 @@
         <v>94.614233720000001</v>
       </c>
       <c r="G227" s="6">
-        <f>+[126]Main!$L$5-[126]Main!$L$6</f>
+        <f>+[127]Main!$L$5-[127]Main!$L$6</f>
         <v>30.146999999999998</v>
       </c>
       <c r="H227" s="6">
@@ -19210,7 +19223,7 @@
         <v>1074</v>
       </c>
       <c r="J227" s="6">
-        <f>+[126]Main!$L$3</f>
+        <f>+[127]Main!$L$3</f>
         <v>80.181554000000006</v>
       </c>
       <c r="K227" s="9">
@@ -19438,11 +19451,11 @@
         <v>7.06</v>
       </c>
       <c r="F239" s="6">
-        <f>E239*[127]Main!$J$3</f>
+        <f>E239*[128]Main!$J$3</f>
         <v>725.62786605999997</v>
       </c>
       <c r="G239" s="6">
-        <f>[127]Main!$J$5-[127]Main!$J$6</f>
+        <f>[128]Main!$J$5-[128]Main!$J$6</f>
         <v>197.79600000000002</v>
       </c>
       <c r="H239" s="8">
@@ -19475,7 +19488,7 @@
         <v>486.43225439999998</v>
       </c>
       <c r="G240" s="6">
-        <f>+[128]Main!$K$5-[128]Main!$K$6</f>
+        <f>+[129]Main!$K$5-[129]Main!$K$6</f>
         <v>-37.984000000000002</v>
       </c>
       <c r="H240" s="8">
@@ -19486,7 +19499,7 @@
         <v>301</v>
       </c>
       <c r="J240" s="6">
-        <f>+[128]Main!$K$3</f>
+        <f>+[129]Main!$K$3</f>
         <v>810.72042399999998</v>
       </c>
       <c r="K240" s="9">
@@ -19514,11 +19527,11 @@
         <v>14.68</v>
       </c>
       <c r="F241" s="6">
-        <f>E241*[129]Main!$L$3</f>
+        <f>E241*[130]Main!$L$3</f>
         <v>587.26396075999992</v>
       </c>
       <c r="G241" s="6">
-        <f>[129]Main!$L$5-[129]Main!$L$6</f>
+        <f>[130]Main!$L$5-[130]Main!$L$6</f>
         <v>277.88299999999998</v>
       </c>
       <c r="H241" s="8">
@@ -19547,11 +19560,11 @@
         <v>4.8600000000000003</v>
       </c>
       <c r="F242" s="6">
-        <f>E242*[130]Main!$J$3</f>
+        <f>E242*[131]Main!$J$3</f>
         <v>312.71415336000001</v>
       </c>
       <c r="G242" s="8">
-        <f>+[130]Main!$J$5-[130]Main!$J$6</f>
+        <f>+[131]Main!$J$5-[131]Main!$J$6</f>
         <v>92.317999999999998</v>
       </c>
       <c r="H242" s="8">
@@ -19580,11 +19593,11 @@
         <v>5.8</v>
       </c>
       <c r="F243" s="6">
-        <f>E243*[131]Main!$M$3</f>
+        <f>E243*[132]Main!$M$3</f>
         <v>259.32193239999998</v>
       </c>
       <c r="G243" s="6">
-        <f>[131]Main!$M$5-[131]Main!$M$6</f>
+        <f>[132]Main!$M$5-[132]Main!$M$6</f>
         <v>120.43700000000001</v>
       </c>
       <c r="H243" s="8">
@@ -19610,11 +19623,11 @@
         <v>0.7</v>
       </c>
       <c r="F244" s="6">
-        <f>E244*[132]Main!$M$3</f>
+        <f>E244*[133]Main!$M$3</f>
         <v>128.9392503</v>
       </c>
       <c r="G244" s="6">
-        <f>[132]Main!$M$5-[132]Main!$M$6</f>
+        <f>[133]Main!$M$5-[133]Main!$M$6</f>
         <v>-59.50200000000001</v>
       </c>
       <c r="H244" s="8">
@@ -19644,7 +19657,7 @@
         <v>144.77073818</v>
       </c>
       <c r="G245" s="6">
-        <f>+[133]Main!$K$5-[133]Main!$K$6</f>
+        <f>+[134]Main!$K$5-[134]Main!$K$6</f>
         <v>78.481999999999999</v>
       </c>
       <c r="H245" s="6">
@@ -19655,7 +19668,7 @@
         <v>1074</v>
       </c>
       <c r="J245" s="6">
-        <f>+[133]Main!$K$3</f>
+        <f>+[134]Main!$K$3</f>
         <v>75.796198000000004</v>
       </c>
       <c r="K245" s="9">
@@ -19684,7 +19697,7 @@
         <v>30.407559149999997</v>
       </c>
       <c r="G246" s="6">
-        <f>+[134]Main!$N$5-[134]Main!$N$6</f>
+        <f>+[135]Main!$N$5-[135]Main!$N$6</f>
         <v>-7.4640000000000004</v>
       </c>
       <c r="H246" s="6">
@@ -19695,7 +19708,7 @@
         <v>301</v>
       </c>
       <c r="J246" s="6">
-        <f>+[134]Main!$N$3</f>
+        <f>+[135]Main!$N$3</f>
         <v>9.4141049999999993</v>
       </c>
       <c r="K246" s="9">
@@ -19720,11 +19733,11 @@
         <v>1.98</v>
       </c>
       <c r="F247" s="6">
-        <f>E247*[135]Main!$N$3</f>
+        <f>E247*[136]Main!$N$3</f>
         <v>39.757463459999997</v>
       </c>
       <c r="G247" s="6">
-        <f>[135]Main!$N$5-[135]Main!$N$6</f>
+        <f>[136]Main!$N$5-[136]Main!$N$6</f>
         <v>15.942</v>
       </c>
       <c r="H247" s="8">
@@ -19750,11 +19763,11 @@
         <v>0.62</v>
       </c>
       <c r="F248" s="6">
-        <f>E248*[136]Main!$L$3</f>
+        <f>E248*[137]Main!$L$3</f>
         <v>30.1881658</v>
       </c>
       <c r="G248" s="6">
-        <f>[136]Main!$L$5-[136]Main!$L$6</f>
+        <f>[137]Main!$L$5-[137]Main!$L$6</f>
         <v>13.262999999999998</v>
       </c>
       <c r="H248" s="8">
@@ -19780,11 +19793,11 @@
         <v>6.12</v>
       </c>
       <c r="F249" s="6">
-        <f>E249*[137]Main!$M$3</f>
+        <f>E249*[138]Main!$M$3</f>
         <v>125.46108324000001</v>
       </c>
       <c r="G249" s="6">
-        <f>[137]Main!$M$5-[137]Main!$M$6</f>
+        <f>[138]Main!$M$5-[138]Main!$M$6</f>
         <v>131.17699999999999</v>
       </c>
       <c r="H249" s="8">
@@ -19810,11 +19823,11 @@
         <v>0.98</v>
       </c>
       <c r="F250" s="6">
-        <f>E250*[138]Main!$M$3</f>
+        <f>E250*[139]Main!$M$3</f>
         <v>20.935517539999999</v>
       </c>
       <c r="G250" s="6">
-        <f>[138]Main!$M$5-[138]Main!$M$6</f>
+        <f>[139]Main!$M$5-[139]Main!$M$6</f>
         <v>55.28</v>
       </c>
       <c r="H250" s="8">
@@ -19844,7 +19857,7 @@
         <v>596.75561000000005</v>
       </c>
       <c r="G251" s="6">
-        <f>+[139]Main!$J$5-[139]Main!$J$6</f>
+        <f>+[140]Main!$J$5-[140]Main!$J$6</f>
         <v>35.484999999999999</v>
       </c>
       <c r="H251" s="8">
@@ -19855,7 +19868,7 @@
         <v>1074</v>
       </c>
       <c r="J251" s="6">
-        <f>+[139]Main!$J$3</f>
+        <f>+[140]Main!$J$3</f>
         <v>119.351122</v>
       </c>
     </row>
@@ -19878,7 +19891,7 @@
         <v>56.676359999999995</v>
       </c>
       <c r="G252" s="6">
-        <f>+[140]Main!$K$5-[140]Main!$K$6</f>
+        <f>+[141]Main!$K$5-[141]Main!$K$6</f>
         <v>136.64599999999999</v>
       </c>
       <c r="H252" s="6">
@@ -19889,7 +19902,7 @@
         <v>1074</v>
       </c>
       <c r="J252" s="6">
-        <f>+[140]Main!$K$3</f>
+        <f>+[141]Main!$K$3</f>
         <v>60.293999999999997</v>
       </c>
       <c r="K252" s="9">
@@ -20875,7 +20888,7 @@
         <v>588.73448214000007</v>
       </c>
       <c r="G316" s="6">
-        <f>+[141]Main!$M$5-[141]Main!$M$6</f>
+        <f>+[142]Main!$M$5-[142]Main!$M$6</f>
         <v>99.997</v>
       </c>
       <c r="H316" s="6">
@@ -20886,7 +20899,7 @@
         <v>1074</v>
       </c>
       <c r="J316" s="6">
-        <f>+[141]Main!$M$3</f>
+        <f>+[142]Main!$M$3</f>
         <v>44.567334000000002</v>
       </c>
       <c r="K316" s="9">
@@ -20915,7 +20928,7 @@
         <v>492.22422607999999</v>
       </c>
       <c r="G317" s="6">
-        <f>+[142]Main!$K$5-[142]Main!$K$6</f>
+        <f>+[143]Main!$K$5-[143]Main!$K$6</f>
         <v>174.27199999999999</v>
       </c>
       <c r="H317" s="6">
@@ -20926,7 +20939,7 @@
         <v>1074</v>
       </c>
       <c r="J317" s="6">
-        <f>+[142]Main!$K$3</f>
+        <f>+[143]Main!$K$3</f>
         <v>43.215471999999998</v>
       </c>
       <c r="K317" s="9">
@@ -20955,7 +20968,7 @@
         <v>653.378781</v>
       </c>
       <c r="G318" s="6">
-        <f>[143]Main!$M$5-[143]Main!$M$6</f>
+        <f>[144]Main!$M$5-[144]Main!$M$6</f>
         <v>236.422</v>
       </c>
       <c r="H318" s="6">
@@ -20966,7 +20979,7 @@
         <v>45063</v>
       </c>
       <c r="J318" s="6">
-        <f>[143]Main!$M$3</f>
+        <f>[144]Main!$M$3</f>
         <v>19.799357000000001</v>
       </c>
       <c r="AC318" s="1">
@@ -20993,7 +21006,7 @@
         <v>476.84725110000005</v>
       </c>
       <c r="G319" s="6">
-        <f>+[144]Main!$K$5-[144]Main!$K$6</f>
+        <f>+[145]Main!$K$5-[145]Main!$K$6</f>
         <v>280.24800000000005</v>
       </c>
       <c r="H319" s="6">
@@ -21004,7 +21017,7 @@
         <v>1074</v>
       </c>
       <c r="J319" s="6">
-        <f>+[144]Main!$K$3</f>
+        <f>+[145]Main!$K$3</f>
         <v>53.518210000000003</v>
       </c>
       <c r="K319" s="9">
@@ -21033,7 +21046,7 @@
         <v>242.45700277999998</v>
       </c>
       <c r="G320" s="6">
-        <f>+[145]Main!$J$5-[145]Main!$J$6</f>
+        <f>+[146]Main!$J$5-[146]Main!$J$6</f>
         <v>69.49499999999999</v>
       </c>
       <c r="H320" s="6">
@@ -21044,7 +21057,7 @@
         <v>1074</v>
       </c>
       <c r="J320" s="6">
-        <f>+[145]Main!$J$3</f>
+        <f>+[146]Main!$J$3</f>
         <v>72.591916999999995</v>
       </c>
       <c r="K320" s="9">
@@ -21071,7 +21084,7 @@
         <v>95.674332159999992</v>
       </c>
       <c r="G321" s="6">
-        <f>+[146]Main!$K$5-[146]Main!$K$6</f>
+        <f>+[147]Main!$K$5-[147]Main!$K$6</f>
         <v>29.36</v>
       </c>
       <c r="H321" s="6">
@@ -21082,7 +21095,7 @@
         <v>1074</v>
       </c>
       <c r="J321" s="6">
-        <f>+[146]Main!$K$3</f>
+        <f>+[147]Main!$K$3</f>
         <v>74.745571999999996</v>
       </c>
       <c r="K321" s="9">
@@ -21109,7 +21122,7 @@
         <v>30.110729799999998</v>
       </c>
       <c r="G322" s="6">
-        <f>+[147]Main!$L$5-[147]Main!$L$6</f>
+        <f>+[148]Main!$L$5-[148]Main!$L$6</f>
         <v>33.298999999999999</v>
       </c>
       <c r="H322" s="6">
@@ -21120,7 +21133,7 @@
         <v>1074</v>
       </c>
       <c r="J322" s="6">
-        <f>+[147]Main!$L$3</f>
+        <f>+[148]Main!$L$3</f>
         <v>35.424388</v>
       </c>
       <c r="K322" s="9">
@@ -21147,7 +21160,7 @@
         <v>12.513184599999999</v>
       </c>
       <c r="G323" s="6">
-        <f>[148]Main!$K$5-[148]Main!$K$6</f>
+        <f>[149]Main!$K$5-[149]Main!$K$6</f>
         <v>54.983000000000004</v>
       </c>
       <c r="H323" s="6">
@@ -21158,7 +21171,7 @@
         <v>45063</v>
       </c>
       <c r="J323" s="6">
-        <f>[148]Main!$K$3</f>
+        <f>[149]Main!$K$3</f>
         <v>35.751956</v>
       </c>
     </row>
@@ -21182,7 +21195,7 @@
         <v>326.68703101999995</v>
       </c>
       <c r="G324" s="6">
-        <f>+[149]Main!$K$5-[149]Main!$K$6</f>
+        <f>+[150]Main!$K$5-[150]Main!$K$6</f>
         <v>426.65000000000003</v>
       </c>
       <c r="H324" s="6">
@@ -21193,7 +21206,7 @@
         <v>1074</v>
       </c>
       <c r="J324" s="6">
-        <f>+[149]Main!$K$3</f>
+        <f>+[150]Main!$K$3</f>
         <v>70.558753999999993</v>
       </c>
       <c r="K324" s="9">
@@ -22701,7 +22714,7 @@
         <v>216.57198499999998</v>
       </c>
       <c r="G425" s="6">
-        <f>+[150]Main!$J$5-[150]Main!$J$6</f>
+        <f>+[151]Main!$J$5-[151]Main!$J$6</f>
         <v>104.35299999999999</v>
       </c>
       <c r="H425" s="6">
@@ -22712,7 +22725,7 @@
         <v>1074</v>
       </c>
       <c r="J425" s="6">
-        <f>+[150]Main!$J$3</f>
+        <f>+[151]Main!$J$3</f>
         <v>43.314397</v>
       </c>
       <c r="K425" s="9">
@@ -22738,7 +22751,7 @@
         <v>295.11496187999995</v>
       </c>
       <c r="G426" s="6">
-        <f>+[151]Main!$K$5-[151]Main!$K$6</f>
+        <f>+[152]Main!$K$5-[152]Main!$K$6</f>
         <v>15.414999999999999</v>
       </c>
       <c r="H426" s="6">
@@ -22749,7 +22762,7 @@
         <v>1074</v>
       </c>
       <c r="J426" s="6">
-        <f>+[151]Main!$K$3</f>
+        <f>+[152]Main!$K$3</f>
         <v>27.999521999999999</v>
       </c>
       <c r="K426" s="9">
@@ -22775,7 +22788,7 @@
         <v>132.55131599999999</v>
       </c>
       <c r="G427" s="6">
-        <f>+[152]Main!$L$5-[152]Main!$L$6</f>
+        <f>+[153]Main!$L$5-[153]Main!$L$6</f>
         <v>33.507724000000003</v>
       </c>
       <c r="H427" s="6">
@@ -22786,7 +22799,7 @@
         <v>1074</v>
       </c>
       <c r="J427" s="6">
-        <f>+[152]Main!$L$3</f>
+        <f>+[153]Main!$L$3</f>
         <v>36.819809999999997</v>
       </c>
       <c r="K427" s="9">
@@ -22812,7 +22825,7 @@
         <v>4.1807902100000005</v>
       </c>
       <c r="G428" s="6">
-        <f>+[153]Main!$P$5-[153]Main!$P$6</f>
+        <f>+[154]Main!$P$5-[154]Main!$P$6</f>
         <v>-4.3319999999999999</v>
       </c>
       <c r="H428" s="6">
@@ -22823,7 +22836,7 @@
         <v>1074</v>
       </c>
       <c r="J428" s="6">
-        <f>+[153]Main!$P$3</f>
+        <f>+[154]Main!$P$3</f>
         <v>22.004159000000001</v>
       </c>
       <c r="K428" s="9">
@@ -24311,7 +24324,7 @@
         <v>24515.28782275</v>
       </c>
       <c r="F76" s="6">
-        <f>([154]Main!$J$5-[154]Main!$J$6)/HKD</f>
+        <f>([155]Main!$J$5-[155]Main!$J$6)/HKD</f>
         <v>991.71512820512828</v>
       </c>
       <c r="G76" s="6">
@@ -24322,7 +24335,7 @@
         <v>301</v>
       </c>
       <c r="I76" s="6">
-        <f>+[154]Main!$J$3</f>
+        <f>+[155]Main!$J$3</f>
         <v>4263.5283170000002</v>
       </c>
       <c r="J76" s="9">

</xml_diff>

<commit_message>
JNJ and other updates
</commit_message>
<xml_diff>
--- a/Biopharma.xlsx
+++ b/Biopharma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin Shkreli - DL\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5A3D53-6461-46E1-ACA0-016C6A6D004C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0E2B47-4BEF-4B7D-AC30-DD11211602AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17180" yWindow="1070" windowWidth="20600" windowHeight="15370" xr2:uid="{17641224-F2C3-441B-B85B-BB32567FE633}"/>
+    <workbookView xWindow="6600" yWindow="2310" windowWidth="28840" windowHeight="15250" xr2:uid="{17641224-F2C3-441B-B85B-BB32567FE633}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -9063,7 +9063,7 @@
       <sheetName val="CDR132L"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="3">
           <cell r="J3">
@@ -9098,25 +9098,25 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -9543,73 +9543,73 @@
       <sheetName val="Duragesic"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
       <sheetData sheetId="6">
         <row r="3">
           <cell r="R3">
-            <v>2422</v>
+            <v>2407</v>
           </cell>
         </row>
         <row r="5">
           <cell r="R5">
-            <v>25475</v>
+            <v>20297</v>
           </cell>
         </row>
         <row r="6">
           <cell r="R6">
-            <v>41491</v>
+            <v>35751</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="30" refreshError="1"/>
+      <sheetData sheetId="31" refreshError="1"/>
+      <sheetData sheetId="32" refreshError="1"/>
+      <sheetData sheetId="33" refreshError="1"/>
+      <sheetData sheetId="34" refreshError="1"/>
+      <sheetData sheetId="35" refreshError="1"/>
+      <sheetData sheetId="36" refreshError="1"/>
+      <sheetData sheetId="37" refreshError="1"/>
+      <sheetData sheetId="38" refreshError="1"/>
+      <sheetData sheetId="39" refreshError="1"/>
+      <sheetData sheetId="40" refreshError="1"/>
+      <sheetData sheetId="41" refreshError="1"/>
+      <sheetData sheetId="42" refreshError="1"/>
+      <sheetData sheetId="43" refreshError="1"/>
+      <sheetData sheetId="44" refreshError="1"/>
+      <sheetData sheetId="45" refreshError="1"/>
+      <sheetData sheetId="46" refreshError="1"/>
+      <sheetData sheetId="47" refreshError="1"/>
+      <sheetData sheetId="48" refreshError="1"/>
+      <sheetData sheetId="49" refreshError="1"/>
+      <sheetData sheetId="50" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -12981,7 +12981,7 @@
       <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -13004,11 +13004,11 @@
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="D2" s="1">
         <f ca="1">RANDBETWEEN(1,D242)</f>
-        <v>198</v>
+        <v>8</v>
       </c>
       <c r="H2" s="6">
         <f>SUM(H4:H453)-H5-H13-H10-H17-H23-H27-H47-H55</f>
-        <v>5117397.5872115083</v>
+        <v>5115063.4372115079</v>
       </c>
       <c r="M2" s="9">
         <f>MIN(M4:M92)</f>
@@ -13301,25 +13301,25 @@
       </c>
       <c r="H7" s="6">
         <f>G7*[3]Main!$R$3</f>
-        <v>376887.42000000004</v>
+        <v>374553.27</v>
       </c>
       <c r="I7" s="6">
         <f>+[3]Main!$R$5-[3]Main!$R$6</f>
-        <v>-16016</v>
+        <v>-15454</v>
       </c>
       <c r="J7" s="6">
         <f>H7-I7</f>
-        <v>392903.42000000004</v>
+        <v>390007.27</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>1074</v>
+        <v>1280</v>
       </c>
       <c r="L7" s="6">
         <f>+[3]Main!$R$3</f>
-        <v>2422</v>
+        <v>2407</v>
       </c>
       <c r="M7" s="9">
-        <v>45593</v>
+        <v>45637</v>
       </c>
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>

</xml_diff>